<commit_message>
mas state high points
</commit_message>
<xml_diff>
--- a/Walter/TripReports/STATE HIGH POINTS.xlsx
+++ b/Walter/TripReports/STATE HIGH POINTS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>State</t>
   </si>
@@ -339,9 +339,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Attack On Mitchell was going on that day</t>
-  </si>
-  <si>
     <t>HP#1</t>
   </si>
   <si>
@@ -418,13 +415,53 @@
   </si>
   <si>
     <t>My HP Order</t>
+  </si>
+  <si>
+    <t>Estimated Cost</t>
+  </si>
+  <si>
+    <t>2nd time: 5/28/2005</t>
+  </si>
+  <si>
+    <t>Attack On Mitchell was going on that day, 2nd time: October 7, 2019</t>
+  </si>
+  <si>
+    <t>$650 with SD, and ND</t>
+  </si>
+  <si>
+    <t>$1900 with NH, Vermont, and MA</t>
+  </si>
+  <si>
+    <t>HP#25</t>
+  </si>
+  <si>
+    <t>HP#26</t>
+  </si>
+  <si>
+    <t>HP#27</t>
+  </si>
+  <si>
+    <t>HP#28</t>
+  </si>
+  <si>
+    <t>HP#29</t>
+  </si>
+  <si>
+    <t>$1005 with GA, TN, KY, VA, and NC</t>
+  </si>
+  <si>
+    <t>$5200 with trip to Denali NP</t>
+  </si>
+  <si>
+    <t>2nd time: 7/26/2008, 3rd: 9/4/11, 4th: 8/31/2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -479,7 +516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -534,6 +571,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -838,44 +879,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH104"/>
+  <dimension ref="A1:AG104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="14" customWidth="1"/>
-    <col min="7" max="34" width="8.88671875" style="14"/>
+    <col min="2" max="2" width="12" style="14" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="14" customWidth="1"/>
+    <col min="9" max="33" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>132</v>
-      </c>
       <c r="G1" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="20"/>
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
@@ -901,137 +946,138 @@
       <c r="AE1" s="20"/>
       <c r="AF1" s="20"/>
       <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-    </row>
-    <row r="2" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>6684</v>
       </c>
-      <c r="E2" s="15">
+      <c r="F2" s="15">
         <v>37030</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G2" s="13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>4861</v>
       </c>
-      <c r="E3" s="15">
+      <c r="F3" s="15">
         <v>37137</v>
       </c>
-      <c r="F3" s="21">
-        <v>38500</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G3" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>32</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="12">
+      <c r="E4" s="12">
         <v>3360</v>
       </c>
-      <c r="E4" s="16">
+      <c r="F4" s="16">
         <v>38501</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>5344</v>
       </c>
-      <c r="E5" s="15">
+      <c r="F5" s="15">
         <v>38537</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>13528</v>
       </c>
-      <c r="E6" s="15">
+      <c r="F6" s="15">
         <v>38962</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>13804</v>
       </c>
-      <c r="E7" s="15">
+      <c r="F7" s="15">
         <v>40044</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14" t="s">
-        <v>113</v>
-      </c>
+      <c r="G7" s="13"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -1058,238 +1104,240 @@
       <c r="AE7" s="14"/>
       <c r="AF7" s="14"/>
       <c r="AG7" s="14"/>
-      <c r="AH7" s="14"/>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>12662</v>
       </c>
-      <c r="E8" s="15">
+      <c r="F8" s="15">
         <v>40061</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>14433</v>
       </c>
-      <c r="E9" s="15">
+      <c r="F9" s="15">
         <v>40074</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>11239</v>
       </c>
-      <c r="E10" s="15">
+      <c r="F10" s="15">
         <v>40371</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>4</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>14411</v>
       </c>
-      <c r="E11" s="15">
+      <c r="F11" s="15">
         <v>40376</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>12633</v>
       </c>
-      <c r="E12" s="15">
+      <c r="F12" s="15">
         <v>40500</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="3">
+      <c r="E13" s="3">
         <v>14498</v>
       </c>
-      <c r="E13" s="15">
+      <c r="F13" s="15">
         <v>40809</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <v>12799</v>
       </c>
-      <c r="E14" s="15">
+      <c r="F14" s="15">
         <v>41139</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>8</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <v>13161</v>
       </c>
-      <c r="E15" s="15">
+      <c r="F15" s="15">
         <v>41391</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="4">
         <v>8749</v>
       </c>
-      <c r="E16" s="15">
+      <c r="F16" s="15">
         <v>41433</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="3">
+      <c r="E17" s="3">
         <v>20310</v>
       </c>
-      <c r="E17" s="15">
+      <c r="F17" s="15">
         <v>41797</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="13"/>
+      <c r="H17" s="22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>9</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="3">
+      <c r="E18" s="3">
         <v>13140</v>
       </c>
-      <c r="E18" s="15">
+      <c r="F18" s="15">
         <v>41918</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14" t="s">
-        <v>124</v>
-      </c>
+      <c r="G18" s="13"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -1316,29 +1364,30 @@
       <c r="AE18" s="14"/>
       <c r="AF18" s="14"/>
       <c r="AG18" s="14"/>
-      <c r="AH18" s="14"/>
-    </row>
-    <row r="19" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>20</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="4">
+      <c r="E19" s="4">
         <v>5426</v>
       </c>
-      <c r="E19" s="15">
+      <c r="F19" s="15">
         <v>42153</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H19" s="14"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14" t="s">
+        <v>136</v>
+      </c>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
@@ -1364,28 +1413,27 @@
       <c r="AE19" s="14"/>
       <c r="AF19" s="14"/>
       <c r="AG19" s="14"/>
-      <c r="AH19" s="14"/>
-    </row>
-    <row r="20" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>15</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="4">
+      <c r="E20" s="4">
         <v>7231</v>
       </c>
-      <c r="E20" s="15">
+      <c r="F20" s="15">
         <v>42154</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14" t="s">
-        <v>126</v>
-      </c>
+      <c r="G20" s="13"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -1412,353 +1460,263 @@
       <c r="AE20" s="14"/>
       <c r="AF20" s="14"/>
       <c r="AG20" s="14"/>
-      <c r="AH20" s="14"/>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>30</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="4">
+      <c r="E21" s="4">
         <v>3506</v>
       </c>
-      <c r="E21" s="15">
+      <c r="F21" s="15">
         <v>42155</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>22</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="12">
+      <c r="E22" s="12">
         <v>5268</v>
       </c>
-      <c r="E22" s="16">
+      <c r="F22" s="16">
         <v>43704</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:34" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="13"/>
+      <c r="H22" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>18</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="12">
+      <c r="E23" s="12">
         <v>6288</v>
       </c>
-      <c r="E23" s="16">
+      <c r="F23" s="16">
         <v>43705</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>26</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="12">
+      <c r="E24" s="12">
         <v>4393</v>
       </c>
-      <c r="E24" s="16">
+      <c r="F24" s="16">
         <v>43706</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>31</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="12">
+      <c r="E25" s="12">
         <v>3487</v>
       </c>
-      <c r="E25" s="16">
+      <c r="F25" s="16">
         <v>43707</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
+        <v>29</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="12">
+        <v>3554</v>
+      </c>
+      <c r="F26" s="16">
+        <v>43741</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
+        <v>25</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="12">
+        <v>4784</v>
+      </c>
+      <c r="F27" s="16">
+        <v>43741</v>
+      </c>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <v>17</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="12">
+        <v>6643</v>
+      </c>
+      <c r="F28" s="16">
+        <v>43742</v>
+      </c>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
+        <v>27</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="12">
+        <v>4139</v>
+      </c>
+      <c r="F29" s="16">
+        <v>43743</v>
+      </c>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10">
+        <v>19</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="12">
+        <v>5729</v>
+      </c>
+      <c r="F30" s="16">
+        <v>43744</v>
+      </c>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:33" s="14" customFormat="1" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
         <v>6</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="7">
+      <c r="E32" s="7">
         <v>13796</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
-        <v>17</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="9">
-        <v>6643</v>
-      </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
-      <c r="V27" s="14"/>
-      <c r="W27" s="14"/>
-      <c r="X27" s="14"/>
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="14"/>
-      <c r="AB27" s="14"/>
-      <c r="AC27" s="14"/>
-      <c r="AD27" s="14"/>
-      <c r="AE27" s="14"/>
-      <c r="AF27" s="14"/>
-      <c r="AG27" s="14"/>
-      <c r="AH27" s="14"/>
-    </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
-        <v>19</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="9">
-        <v>5729</v>
-      </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="13"/>
-    </row>
-    <row r="29" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
+      <c r="F32" s="17"/>
+      <c r="G32" s="13"/>
+    </row>
+    <row r="33" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
         <v>23</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B33" s="14"/>
+      <c r="C33" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="9">
+      <c r="E33" s="9">
         <v>4973</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="14"/>
-      <c r="V29" s="14"/>
-      <c r="W29" s="14"/>
-      <c r="X29" s="14"/>
-      <c r="Y29" s="14"/>
-      <c r="Z29" s="14"/>
-      <c r="AA29" s="14"/>
-      <c r="AB29" s="14"/>
-      <c r="AC29" s="14"/>
-      <c r="AD29" s="14"/>
-      <c r="AE29" s="14"/>
-      <c r="AF29" s="14"/>
-      <c r="AG29" s="14"/>
-      <c r="AH29" s="14"/>
-    </row>
-    <row r="30" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
-        <v>25</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="9">
-        <v>4784</v>
-      </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="U30" s="14"/>
-      <c r="V30" s="14"/>
-      <c r="W30" s="14"/>
-      <c r="X30" s="14"/>
-      <c r="Y30" s="14"/>
-      <c r="Z30" s="14"/>
-      <c r="AA30" s="14"/>
-      <c r="AB30" s="14"/>
-      <c r="AC30" s="14"/>
-      <c r="AD30" s="14"/>
-      <c r="AE30" s="14"/>
-      <c r="AF30" s="14"/>
-      <c r="AG30" s="14"/>
-      <c r="AH30" s="14"/>
-    </row>
-    <row r="31" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
-        <v>27</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="9">
-        <v>4139</v>
-      </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
-      <c r="U31" s="14"/>
-      <c r="V31" s="14"/>
-      <c r="W31" s="14"/>
-      <c r="X31" s="14"/>
-      <c r="Y31" s="14"/>
-      <c r="Z31" s="14"/>
-      <c r="AA31" s="14"/>
-      <c r="AB31" s="14"/>
-      <c r="AC31" s="14"/>
-      <c r="AD31" s="14"/>
-      <c r="AE31" s="14"/>
-      <c r="AF31" s="14"/>
-      <c r="AG31" s="14"/>
-      <c r="AH31" s="14"/>
-    </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
-        <v>28</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="9">
-        <v>4039</v>
-      </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="13"/>
-    </row>
-    <row r="33" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
-        <v>29</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33" s="9">
-        <v>3554</v>
-      </c>
-      <c r="E33" s="17"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="13"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
@@ -1785,68 +1743,39 @@
       <c r="AE33" s="14"/>
       <c r="AF33" s="14"/>
       <c r="AG33" s="14"/>
-      <c r="AH33" s="14"/>
-    </row>
-    <row r="34" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:33" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
+        <v>28</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="9">
+        <v>4039</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="13"/>
+    </row>
+    <row r="35" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
         <v>33</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B35" s="14"/>
+      <c r="C35" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="9">
+      <c r="E35" s="9">
         <v>3213</v>
       </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-      <c r="T34" s="14"/>
-      <c r="U34" s="14"/>
-      <c r="V34" s="14"/>
-      <c r="W34" s="14"/>
-      <c r="X34" s="14"/>
-      <c r="Y34" s="14"/>
-      <c r="Z34" s="14"/>
-      <c r="AA34" s="14"/>
-      <c r="AB34" s="14"/>
-      <c r="AC34" s="14"/>
-      <c r="AD34" s="14"/>
-      <c r="AE34" s="14"/>
-      <c r="AF34" s="14"/>
-      <c r="AG34" s="14"/>
-      <c r="AH34" s="14"/>
-    </row>
-    <row r="35" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="9">
-        <v>2753</v>
-      </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="14"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="13"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
@@ -1873,24 +1802,23 @@
       <c r="AE35" s="14"/>
       <c r="AF35" s="14"/>
       <c r="AG35" s="14"/>
-      <c r="AH35" s="14"/>
-    </row>
-    <row r="36" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
-        <v>35</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36" s="9">
-        <v>2405</v>
-      </c>
-      <c r="E36" s="17"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="9">
+        <v>2753</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="13"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
@@ -1917,24 +1845,23 @@
       <c r="AE36" s="14"/>
       <c r="AF36" s="14"/>
       <c r="AG36" s="14"/>
-      <c r="AH36" s="14"/>
-    </row>
-    <row r="37" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
-        <v>36</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D37" s="9">
-        <v>2380</v>
-      </c>
-      <c r="E37" s="17"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="14"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="14"/>
+      <c r="C37" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="9">
+        <v>2405</v>
+      </c>
+      <c r="F37" s="17"/>
+      <c r="G37" s="13"/>
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
@@ -1961,24 +1888,23 @@
       <c r="AE37" s="14"/>
       <c r="AF37" s="14"/>
       <c r="AG37" s="14"/>
-      <c r="AH37" s="14"/>
-    </row>
-    <row r="38" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
-        <v>37</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" s="9">
-        <v>2301</v>
-      </c>
-      <c r="E38" s="17"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="14"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="9">
+        <v>2380</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="G38" s="13"/>
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
@@ -2005,24 +1931,23 @@
       <c r="AE38" s="14"/>
       <c r="AF38" s="14"/>
       <c r="AG38" s="14"/>
-      <c r="AH38" s="14"/>
-    </row>
-    <row r="39" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D39" s="9">
-        <v>1979</v>
-      </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="14"/>
+        <v>37</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="9">
+        <v>2301</v>
+      </c>
+      <c r="F39" s="17"/>
+      <c r="G39" s="13"/>
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
@@ -2049,24 +1974,23 @@
       <c r="AE39" s="14"/>
       <c r="AF39" s="14"/>
       <c r="AG39" s="14"/>
-      <c r="AH39" s="14"/>
-    </row>
-    <row r="40" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
-        <v>39</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40" s="9">
-        <v>1951</v>
-      </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="14"/>
+        <v>38</v>
+      </c>
+      <c r="B40" s="14"/>
+      <c r="C40" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" s="9">
+        <v>1979</v>
+      </c>
+      <c r="F40" s="17"/>
+      <c r="G40" s="13"/>
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
@@ -2093,24 +2017,23 @@
       <c r="AE40" s="14"/>
       <c r="AF40" s="14"/>
       <c r="AG40" s="14"/>
-      <c r="AH40" s="14"/>
-    </row>
-    <row r="41" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D41" s="9">
-        <v>1803</v>
-      </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="14"/>
+        <v>39</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="9">
+        <v>1951</v>
+      </c>
+      <c r="F41" s="17"/>
+      <c r="G41" s="13"/>
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
@@ -2137,24 +2060,23 @@
       <c r="AE41" s="14"/>
       <c r="AF41" s="14"/>
       <c r="AG41" s="14"/>
-      <c r="AH41" s="14"/>
-    </row>
-    <row r="42" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" s="9">
-        <v>1772</v>
-      </c>
-      <c r="E42" s="17"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="14"/>
+        <v>40</v>
+      </c>
+      <c r="B42" s="14"/>
+      <c r="C42" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="9">
+        <v>1803</v>
+      </c>
+      <c r="F42" s="17"/>
+      <c r="G42" s="13"/>
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
@@ -2181,24 +2103,23 @@
       <c r="AE42" s="14"/>
       <c r="AF42" s="14"/>
       <c r="AG42" s="14"/>
-      <c r="AH42" s="14"/>
-    </row>
-    <row r="43" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="9">
-        <v>1670</v>
-      </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="14"/>
+        <v>41</v>
+      </c>
+      <c r="B43" s="14"/>
+      <c r="C43" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" s="9">
+        <v>1772</v>
+      </c>
+      <c r="F43" s="17"/>
+      <c r="G43" s="13"/>
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
@@ -2225,24 +2146,23 @@
       <c r="AE43" s="14"/>
       <c r="AF43" s="14"/>
       <c r="AG43" s="14"/>
-      <c r="AH43" s="14"/>
-    </row>
-    <row r="44" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
-        <v>43</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" s="9">
-        <v>1549</v>
-      </c>
-      <c r="E44" s="17"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="14"/>
+        <v>42</v>
+      </c>
+      <c r="B44" s="14"/>
+      <c r="C44" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44" s="9">
+        <v>1670</v>
+      </c>
+      <c r="F44" s="17"/>
+      <c r="G44" s="13"/>
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
@@ -2269,24 +2189,23 @@
       <c r="AE44" s="14"/>
       <c r="AF44" s="14"/>
       <c r="AG44" s="14"/>
-      <c r="AH44" s="14"/>
-    </row>
-    <row r="45" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="9">
-        <v>1257</v>
-      </c>
-      <c r="E45" s="17"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="14"/>
+        <v>43</v>
+      </c>
+      <c r="B45" s="14"/>
+      <c r="C45" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" s="9">
+        <v>1549</v>
+      </c>
+      <c r="F45" s="17"/>
+      <c r="G45" s="13"/>
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
@@ -2313,24 +2232,23 @@
       <c r="AE45" s="14"/>
       <c r="AF45" s="14"/>
       <c r="AG45" s="14"/>
-      <c r="AH45" s="14"/>
-    </row>
-    <row r="46" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D46" s="9">
-        <v>1235</v>
-      </c>
-      <c r="E46" s="17"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="14"/>
+        <v>44</v>
+      </c>
+      <c r="B46" s="14"/>
+      <c r="C46" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" s="9">
+        <v>1257</v>
+      </c>
+      <c r="F46" s="17"/>
+      <c r="G46" s="13"/>
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
@@ -2357,24 +2275,23 @@
       <c r="AE46" s="14"/>
       <c r="AF46" s="14"/>
       <c r="AG46" s="14"/>
-      <c r="AH46" s="14"/>
-    </row>
-    <row r="47" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47" s="9">
-        <v>812</v>
-      </c>
-      <c r="E47" s="17"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="14"/>
+        <v>45</v>
+      </c>
+      <c r="B47" s="14"/>
+      <c r="C47" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" s="9">
+        <v>1235</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="G47" s="13"/>
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
@@ -2401,24 +2318,23 @@
       <c r="AE47" s="14"/>
       <c r="AF47" s="14"/>
       <c r="AG47" s="14"/>
-      <c r="AH47" s="14"/>
-    </row>
-    <row r="48" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
-        <v>47</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" s="9">
-        <v>806</v>
-      </c>
-      <c r="E48" s="17"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="14"/>
+        <v>46</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="9">
+        <v>812</v>
+      </c>
+      <c r="F48" s="17"/>
+      <c r="G48" s="13"/>
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
@@ -2445,24 +2361,23 @@
       <c r="AE48" s="14"/>
       <c r="AF48" s="14"/>
       <c r="AG48" s="14"/>
-      <c r="AH48" s="14"/>
-    </row>
-    <row r="49" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D49" s="9">
-        <v>535</v>
-      </c>
-      <c r="E49" s="17"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="B49" s="14"/>
+      <c r="C49" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" s="9">
+        <v>806</v>
+      </c>
+      <c r="F49" s="17"/>
+      <c r="G49" s="13"/>
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
@@ -2489,24 +2404,23 @@
       <c r="AE49" s="14"/>
       <c r="AF49" s="14"/>
       <c r="AG49" s="14"/>
-      <c r="AH49" s="14"/>
-    </row>
-    <row r="50" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D50" s="9">
-        <v>450</v>
-      </c>
-      <c r="E50" s="17"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="14"/>
+        <v>48</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E50" s="9">
+        <v>535</v>
+      </c>
+      <c r="F50" s="17"/>
+      <c r="G50" s="13"/>
       <c r="H50" s="14"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
@@ -2533,40 +2447,66 @@
       <c r="AE50" s="14"/>
       <c r="AF50" s="14"/>
       <c r="AG50" s="14"/>
-      <c r="AH50" s="14"/>
-    </row>
-    <row r="51" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
-        <v>50</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51" s="4">
-        <v>415</v>
-      </c>
-      <c r="E51" s="15"/>
-      <c r="F51" s="13"/>
-    </row>
-    <row r="52" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5">
+        <v>49</v>
+      </c>
+      <c r="B51" s="14"/>
+      <c r="C51" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E51" s="9">
+        <v>450</v>
+      </c>
+      <c r="F51" s="17"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="14"/>
+      <c r="V51" s="14"/>
+      <c r="W51" s="14"/>
+      <c r="X51" s="14"/>
+      <c r="Y51" s="14"/>
+      <c r="Z51" s="14"/>
+      <c r="AA51" s="14"/>
+      <c r="AB51" s="14"/>
+      <c r="AC51" s="14"/>
+      <c r="AD51" s="14"/>
+      <c r="AE51" s="14"/>
+      <c r="AF51" s="14"/>
+      <c r="AG51" s="14"/>
+    </row>
+    <row r="52" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="14"/>
+      <c r="C52" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="D52" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D52" s="9">
+      <c r="E52" s="9">
         <v>345</v>
       </c>
-      <c r="E52" s="17"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="14"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="13"/>
       <c r="H52" s="14"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
@@ -2593,220 +2533,232 @@
       <c r="AE52" s="14"/>
       <c r="AF52" s="14"/>
       <c r="AG52" s="14"/>
-      <c r="AH52" s="14"/>
-    </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E53" s="15"/>
-    </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E54" s="15"/>
-    </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E55" s="15"/>
-    </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E56" s="15"/>
-    </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E57" s="15"/>
-    </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E58" s="15"/>
-    </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E59" s="15"/>
-    </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E60" s="15"/>
-    </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E61" s="15"/>
-    </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E62" s="15"/>
-    </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E63" s="15"/>
-    </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="E64" s="15"/>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E65" s="15"/>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E66" s="15"/>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E67" s="15"/>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E68" s="15"/>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E69" s="15"/>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E70" s="15"/>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E71" s="15"/>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E72" s="15"/>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E73" s="15"/>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E74" s="15"/>
-    </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E75" s="15"/>
-    </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E76" s="15"/>
-    </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E77" s="15"/>
-    </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E78" s="15"/>
-    </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E79" s="15"/>
-    </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E80" s="15"/>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E81" s="15"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E82" s="15"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E83" s="15"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E84" s="15"/>
-    </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E85" s="15"/>
-    </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E86" s="15"/>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E87" s="15"/>
-    </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E88" s="15"/>
-    </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E89" s="15"/>
-    </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E90" s="15"/>
-    </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E91" s="15"/>
-    </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E92" s="15"/>
-    </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E93" s="15"/>
-    </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E94" s="15"/>
-    </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E95" s="15"/>
-    </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E96" s="15"/>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E97" s="15"/>
-    </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E98" s="15"/>
-    </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E99" s="15"/>
-    </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E100" s="15"/>
-    </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E101" s="15"/>
-    </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E102" s="15"/>
-    </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E103" s="15"/>
-    </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E104" s="15"/>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F53" s="15"/>
+    </row>
+    <row r="54" spans="1:33" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="5">
+        <v>50</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E54" s="9">
+        <v>415</v>
+      </c>
+      <c r="F54" s="17"/>
+      <c r="G54" s="23"/>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F55" s="15"/>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F56" s="15"/>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F57" s="15"/>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F58" s="15"/>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F59" s="15"/>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F60" s="15"/>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F61" s="15"/>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F62" s="15"/>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F63" s="15"/>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F64" s="15"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F65" s="15"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F66" s="15"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F67" s="15"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F68" s="15"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F69" s="15"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F70" s="15"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F71" s="15"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F72" s="15"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F73" s="15"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F74" s="15"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F75" s="15"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F76" s="15"/>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F77" s="15"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F78" s="15"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F79" s="15"/>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F80" s="15"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F81" s="15"/>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F82" s="15"/>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F83" s="15"/>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F84" s="15"/>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F85" s="15"/>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F86" s="15"/>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F87" s="15"/>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F88" s="15"/>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F89" s="15"/>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F90" s="15"/>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F91" s="15"/>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F92" s="15"/>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F93" s="15"/>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F94" s="15"/>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F95" s="15"/>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F96" s="15"/>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F97" s="15"/>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F98" s="15"/>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F99" s="15"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F100" s="15"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F101" s="15"/>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F102" s="15"/>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F103" s="15"/>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F104" s="15"/>
     </row>
   </sheetData>
-  <sortState ref="A2:E98">
-    <sortCondition ref="E2"/>
+  <sortState ref="A2:F98">
+    <sortCondition ref="F2"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C17" r:id="rId1" display="https://www.peakbagger.com/peak.aspx?pid=271"/>
-    <hyperlink ref="C13" r:id="rId2" display="https://www.peakbagger.com/peak.aspx?pid=2829"/>
-    <hyperlink ref="C9" r:id="rId3" display="https://www.peakbagger.com/peak.aspx?pid=5736"/>
-    <hyperlink ref="C11" r:id="rId4" display="https://www.peakbagger.com/peak.aspx?pid=2296"/>
-    <hyperlink ref="C7" r:id="rId5" display="https://www.peakbagger.com/peak.aspx?pid=5352"/>
-    <hyperlink ref="C26" r:id="rId6" display="https://www.peakbagger.com/peak.aspx?pid=11909"/>
-    <hyperlink ref="C6" r:id="rId7" display="https://www.peakbagger.com/peak.aspx?pid=5507"/>
-    <hyperlink ref="C15" r:id="rId8" display="https://www.peakbagger.com/peak.aspx?pid=5937"/>
-    <hyperlink ref="C18" r:id="rId9" display="https://www.peakbagger.com/peak.aspx?pid=3625"/>
-    <hyperlink ref="C14" r:id="rId10" display="https://www.peakbagger.com/peak.aspx?pid=5258"/>
-    <hyperlink ref="C8" r:id="rId11" display="https://www.peakbagger.com/peak.aspx?pid=5142"/>
-    <hyperlink ref="C12" r:id="rId12" display="https://www.peakbagger.com/peak.aspx?pid=3938"/>
-    <hyperlink ref="C10" r:id="rId13" display="https://www.peakbagger.com/peak.aspx?pid=2382"/>
-    <hyperlink ref="C16" r:id="rId14" display="https://www.peakbagger.com/peak.aspx?pid=4297"/>
-    <hyperlink ref="C20" r:id="rId15" display="https://www.peakbagger.com/peak.aspx?pid=6236"/>
-    <hyperlink ref="C2" r:id="rId16" display="https://www.peakbagger.com/peak.aspx?pid=7822"/>
-    <hyperlink ref="C27" r:id="rId17" display="https://www.peakbagger.com/peak.aspx?pid=7764"/>
-    <hyperlink ref="C23" r:id="rId18" display="https://www.peakbagger.com/peak.aspx?pid=6960"/>
-    <hyperlink ref="C28" r:id="rId19" display="https://www.peakbagger.com/peak.aspx?pid=7796"/>
-    <hyperlink ref="C19" r:id="rId20" display="https://www.peakbagger.com/peak.aspx?pid=6284"/>
-    <hyperlink ref="C5" r:id="rId21" display="https://www.peakbagger.com/peak.aspx?pid=6048"/>
-    <hyperlink ref="C22" r:id="rId22" display="https://www.peakbagger.com/peak.aspx?pid=6820"/>
-    <hyperlink ref="C29" r:id="rId23" display="https://www.peakbagger.com/peak.aspx?pid=6322"/>
-    <hyperlink ref="C3" r:id="rId24" display="https://www.peakbagger.com/peak.aspx?pid=7376"/>
-    <hyperlink ref="C30" r:id="rId25" display="https://www.peakbagger.com/peak.aspx?pid=7730"/>
-    <hyperlink ref="C24" r:id="rId26" display="https://www.peakbagger.com/peak.aspx?pid=7013"/>
-    <hyperlink ref="C31" r:id="rId27" display="https://www.peakbagger.com/peak.aspx?pid=7464"/>
-    <hyperlink ref="C32" r:id="rId28" display="https://www.peakbagger.com/peak.aspx?pid=6307"/>
-    <hyperlink ref="C33" r:id="rId29" display="https://www.peakbagger.com/peak.aspx?pid=7720"/>
-    <hyperlink ref="C21" r:id="rId30" display="https://www.peakbagger.com/peak.aspx?pid=6192"/>
-    <hyperlink ref="C25" r:id="rId31" display="https://www.peakbagger.com/peak.aspx?pid=7065"/>
-    <hyperlink ref="C4" r:id="rId32" display="https://www.peakbagger.com/peak.aspx?pid=7354"/>
-    <hyperlink ref="C34" r:id="rId33" display="https://www.peakbagger.com/peak.aspx?pid=7351"/>
-    <hyperlink ref="C35" r:id="rId34" display="https://www.peakbagger.com/peak.aspx?pid=6606"/>
-    <hyperlink ref="C36" r:id="rId35" display="https://www.peakbagger.com/peak.aspx?pid=7542"/>
-    <hyperlink ref="C37" r:id="rId36" display="https://www.peakbagger.com/peak.aspx?pid=7083"/>
-    <hyperlink ref="C38" r:id="rId37" display="https://www.peakbagger.com/peak.aspx?pid=6440"/>
-    <hyperlink ref="C39" r:id="rId38" display="https://www.peakbagger.com/peak.aspx?pid=6474"/>
-    <hyperlink ref="C40" r:id="rId39" display="https://www.peakbagger.com/peak.aspx?pid=6466"/>
-    <hyperlink ref="C41" r:id="rId40" display="https://www.peakbagger.com/peak.aspx?pid=7553"/>
-    <hyperlink ref="C42" r:id="rId41" display="https://www.peakbagger.com/peak.aspx?pid=6575"/>
-    <hyperlink ref="C43" r:id="rId42" display="https://www.peakbagger.com/peak.aspx?pid=6217"/>
-    <hyperlink ref="C44" r:id="rId43" display="https://www.peakbagger.com/peak.aspx?pid=6532"/>
-    <hyperlink ref="C45" r:id="rId44" display="https://www.peakbagger.com/peak.aspx?pid=6535"/>
-    <hyperlink ref="C46" r:id="rId45" display="https://www.peakbagger.com/peak.aspx?pid=6426"/>
-    <hyperlink ref="C47" r:id="rId46" display="https://www.peakbagger.com/peak.aspx?pid=6771"/>
-    <hyperlink ref="C48" r:id="rId47" display="https://www.peakbagger.com/peak.aspx?pid=7505"/>
-    <hyperlink ref="C49" r:id="rId48" display="https://www.peakbagger.com/peak.aspx?pid=6630"/>
-    <hyperlink ref="C50" r:id="rId49" display="https://www.peakbagger.com/peak.aspx?pid=7156"/>
-    <hyperlink ref="C52" r:id="rId50" display="https://www.peakbagger.com/peak.aspx?pid=7917"/>
-    <hyperlink ref="C51" r:id="rId51" display="https://www.peakbagger.com/peak.aspx?pid=7637"/>
+    <hyperlink ref="D17" r:id="rId1" display="https://www.peakbagger.com/peak.aspx?pid=271"/>
+    <hyperlink ref="D13" r:id="rId2" display="https://www.peakbagger.com/peak.aspx?pid=2829"/>
+    <hyperlink ref="D9" r:id="rId3" display="https://www.peakbagger.com/peak.aspx?pid=5736"/>
+    <hyperlink ref="D11" r:id="rId4" display="https://www.peakbagger.com/peak.aspx?pid=2296"/>
+    <hyperlink ref="D7" r:id="rId5" display="https://www.peakbagger.com/peak.aspx?pid=5352"/>
+    <hyperlink ref="D32" r:id="rId6" display="https://www.peakbagger.com/peak.aspx?pid=11909"/>
+    <hyperlink ref="D6" r:id="rId7" display="https://www.peakbagger.com/peak.aspx?pid=5507"/>
+    <hyperlink ref="D15" r:id="rId8" display="https://www.peakbagger.com/peak.aspx?pid=5937"/>
+    <hyperlink ref="D18" r:id="rId9" display="https://www.peakbagger.com/peak.aspx?pid=3625"/>
+    <hyperlink ref="D14" r:id="rId10" display="https://www.peakbagger.com/peak.aspx?pid=5258"/>
+    <hyperlink ref="D8" r:id="rId11" display="https://www.peakbagger.com/peak.aspx?pid=5142"/>
+    <hyperlink ref="D12" r:id="rId12" display="https://www.peakbagger.com/peak.aspx?pid=3938"/>
+    <hyperlink ref="D10" r:id="rId13" display="https://www.peakbagger.com/peak.aspx?pid=2382"/>
+    <hyperlink ref="D16" r:id="rId14" display="https://www.peakbagger.com/peak.aspx?pid=4297"/>
+    <hyperlink ref="D20" r:id="rId15" display="https://www.peakbagger.com/peak.aspx?pid=6236"/>
+    <hyperlink ref="D2" r:id="rId16" display="https://www.peakbagger.com/peak.aspx?pid=7822"/>
+    <hyperlink ref="D28" r:id="rId17" display="https://www.peakbagger.com/peak.aspx?pid=7764"/>
+    <hyperlink ref="D23" r:id="rId18" display="https://www.peakbagger.com/peak.aspx?pid=6960"/>
+    <hyperlink ref="D30" r:id="rId19" display="https://www.peakbagger.com/peak.aspx?pid=7796"/>
+    <hyperlink ref="D19" r:id="rId20" display="https://www.peakbagger.com/peak.aspx?pid=6284"/>
+    <hyperlink ref="D5" r:id="rId21" display="https://www.peakbagger.com/peak.aspx?pid=6048"/>
+    <hyperlink ref="D22" r:id="rId22" display="https://www.peakbagger.com/peak.aspx?pid=6820"/>
+    <hyperlink ref="D33" r:id="rId23" display="https://www.peakbagger.com/peak.aspx?pid=6322"/>
+    <hyperlink ref="D3" r:id="rId24" display="https://www.peakbagger.com/peak.aspx?pid=7376"/>
+    <hyperlink ref="D27" r:id="rId25" display="https://www.peakbagger.com/peak.aspx?pid=7730"/>
+    <hyperlink ref="D24" r:id="rId26" display="https://www.peakbagger.com/peak.aspx?pid=7013"/>
+    <hyperlink ref="D29" r:id="rId27" display="https://www.peakbagger.com/peak.aspx?pid=7464"/>
+    <hyperlink ref="D34" r:id="rId28" display="https://www.peakbagger.com/peak.aspx?pid=6307"/>
+    <hyperlink ref="D26" r:id="rId29" display="https://www.peakbagger.com/peak.aspx?pid=7720"/>
+    <hyperlink ref="D21" r:id="rId30" display="https://www.peakbagger.com/peak.aspx?pid=6192"/>
+    <hyperlink ref="D25" r:id="rId31" display="https://www.peakbagger.com/peak.aspx?pid=7065"/>
+    <hyperlink ref="D4" r:id="rId32" display="https://www.peakbagger.com/peak.aspx?pid=7354"/>
+    <hyperlink ref="D35" r:id="rId33" display="https://www.peakbagger.com/peak.aspx?pid=7351"/>
+    <hyperlink ref="D36" r:id="rId34" display="https://www.peakbagger.com/peak.aspx?pid=6606"/>
+    <hyperlink ref="D37" r:id="rId35" display="https://www.peakbagger.com/peak.aspx?pid=7542"/>
+    <hyperlink ref="D38" r:id="rId36" display="https://www.peakbagger.com/peak.aspx?pid=7083"/>
+    <hyperlink ref="D39" r:id="rId37" display="https://www.peakbagger.com/peak.aspx?pid=6440"/>
+    <hyperlink ref="D40" r:id="rId38" display="https://www.peakbagger.com/peak.aspx?pid=6474"/>
+    <hyperlink ref="D41" r:id="rId39" display="https://www.peakbagger.com/peak.aspx?pid=6466"/>
+    <hyperlink ref="D42" r:id="rId40" display="https://www.peakbagger.com/peak.aspx?pid=7553"/>
+    <hyperlink ref="D43" r:id="rId41" display="https://www.peakbagger.com/peak.aspx?pid=6575"/>
+    <hyperlink ref="D44" r:id="rId42" display="https://www.peakbagger.com/peak.aspx?pid=6217"/>
+    <hyperlink ref="D45" r:id="rId43" display="https://www.peakbagger.com/peak.aspx?pid=6532"/>
+    <hyperlink ref="D46" r:id="rId44" display="https://www.peakbagger.com/peak.aspx?pid=6535"/>
+    <hyperlink ref="D47" r:id="rId45" display="https://www.peakbagger.com/peak.aspx?pid=6426"/>
+    <hyperlink ref="D48" r:id="rId46" display="https://www.peakbagger.com/peak.aspx?pid=6771"/>
+    <hyperlink ref="D49" r:id="rId47" display="https://www.peakbagger.com/peak.aspx?pid=7505"/>
+    <hyperlink ref="D50" r:id="rId48" display="https://www.peakbagger.com/peak.aspx?pid=6630"/>
+    <hyperlink ref="D51" r:id="rId49" display="https://www.peakbagger.com/peak.aspx?pid=7156"/>
+    <hyperlink ref="D52" r:id="rId50" display="https://www.peakbagger.com/peak.aspx?pid=7917"/>
+    <hyperlink ref="D54" r:id="rId51" display="https://www.peakbagger.com/peak.aspx?pid=7637"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId52"/>

</xml_diff>

<commit_message>
Walter Scale includes weather, and days
</commit_message>
<xml_diff>
--- a/Walter/TripReports/STATE HIGH POINTS.xlsx
+++ b/Walter/TripReports/STATE HIGH POINTS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="195">
   <si>
     <t>State</t>
   </si>
@@ -557,43 +557,58 @@
     <t>Truncating  the  ratio of 3/0.189394  the Walter scale estimates it to be 15 times more difficult to climb 1 mile then to walk 1 mile.</t>
   </si>
   <si>
-    <t>Effort points are a combination of total hiking mileage, vertical gain, and terrain difficulty.</t>
-  </si>
-  <si>
     <t>It is estimaed that 3 miles can be walked in 1 hour, and likewise 1000 vertical feet  (0.189394 miles) can be climbed in one hour.</t>
   </si>
   <si>
     <t>As such the Walter scale awards 1 point for each milage of walking, and 1 point for each 352 feet of gain.</t>
   </si>
   <si>
-    <t>If a highpoint involves scrambling or glacier travel an additional 5 bonus points are awarded.</t>
-  </si>
-  <si>
-    <t>Walter Scale:  Points = (mileage + 15*(vertical distance in miles) + bonus points)</t>
-  </si>
-  <si>
-    <t>Highpoints can be classified as Mountains, Hills, and Landmarks.  The Walter scale considers 33 of the 50 to be mountains and they require 96.65%</t>
-  </si>
-  <si>
-    <t>of the effort.  Another 10 are Hills requiring the balance of the effort.  The remaining 7 are grouped as Landmarks requiring no physical effort.</t>
-  </si>
-  <si>
     <t>The Walter Scale reflects the Pareto Principle which states that for most taskes roughly 80% of the results come from 20% of the effort.</t>
   </si>
   <si>
-    <t>According to the Walter Scale reaching 38 of the 50 highpoints (aka 76%) requires only 20.29% of the effort.</t>
-  </si>
-  <si>
-    <t>Denali alone requires 15.83% of the total effort.</t>
-  </si>
-  <si>
-    <t>The remaining 12 highpoints (aka remaining 24%) require 79.71% of the effort.</t>
-  </si>
-  <si>
     <t>The 29 highpoints I have reached, between May 2001 and October 2019 account for 94.45% of the physical effort.</t>
   </si>
   <si>
     <t>That said my remaining 21 highpoints might be physically easier, but they are typically more difficult to plan for due to distance and cost.</t>
+  </si>
+  <si>
+    <t>Number of Nights</t>
+  </si>
+  <si>
+    <t>Days below freezing</t>
+  </si>
+  <si>
+    <t>Raw Walter Scale</t>
+  </si>
+  <si>
+    <t>Highpoints can be classified as Mountains, Hills, and Landmarks.  The Walter scale considers 33 of the 50 to be mountains and they require 97.09%</t>
+  </si>
+  <si>
+    <t>of the effort.  Another 10 are Hills requiring 2.85% of the effort.  The remaining 7 are grouped as Landmarks requiring only 0.02% of the physical effort.</t>
+  </si>
+  <si>
+    <t>Denali alone requires 22.20% of the total effort.</t>
+  </si>
+  <si>
+    <t>According to the Walter Scale reaching 39 of the 50 highpoints (aka 78%) requires only 20.14% of the effort.</t>
+  </si>
+  <si>
+    <t>The remaining 11 highpoints (aka remaining 22%) require 79.86% of the effort.</t>
+  </si>
+  <si>
+    <t>Points are normalized to a 1 - 1000 scale, to allow easy comparisons.</t>
+  </si>
+  <si>
+    <t>Walter Scale:  Points = (mileage + 15*(vertical distance in miles) + difficulty + nights + 2*coldDays)/maxScore * 1000</t>
+  </si>
+  <si>
+    <t>Effort points are a combination of total hiking mileage, vertical gain, terrain difficulty, nights required, and days with temperature remaining below.</t>
+  </si>
+  <si>
+    <t>If a highpoint involves roped rock climbing or roped glacier travel an additional 12 bonus miles are awarded.</t>
+  </si>
+  <si>
+    <t>If a highpoint involves climbing with the use of both hands and feet, but not the protection of a rope, an additional 6 bonus miles are awarded.</t>
   </si>
 </sst>
 </file>
@@ -751,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -839,6 +854,13 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -848,9 +870,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0B8B29"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFFF00FF"/>
-      <color rgb="FF0B8B29"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3233,25 +3255,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14.21875" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" style="37" customWidth="1"/>
     <col min="4" max="4" width="19.109375" style="37" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" customWidth="1"/>
+    <col min="5" max="7" width="20.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.88671875" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" customWidth="1"/>
+    <col min="14" max="14" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>171</v>
       </c>
@@ -3265,27 +3287,37 @@
         <v>165</v>
       </c>
       <c r="E1" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="H1" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="I1" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="J1" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="K1" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="L1" s="40" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50">
-        <f>E2/618.99</f>
+      <c r="M1" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="N1" s="40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53">
+        <f>G2/$G$52</f>
         <v>0</v>
       </c>
       <c r="B2" s="44" t="s">
@@ -3298,28 +3330,38 @@
         <v>70</v>
       </c>
       <c r="E2" s="46">
-        <f>I2+F2+J2</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="44">
-        <v>0</v>
-      </c>
-      <c r="G2" s="44">
+        <f>K2+H2+L2 + M2*2 + N2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="46">
+        <f>E2/$E$51*1000</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="57">
+        <f t="shared" ref="G2:G16" si="0">ROUND(F2,0)</f>
         <v>0</v>
       </c>
       <c r="H2" s="44">
-        <f>G2/5280</f>
         <v>0</v>
       </c>
       <c r="I2" s="44">
-        <f>15*H2</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="46"/>
-    </row>
-    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="44">
+        <f>I2/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="44">
+        <f>15*J2</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+    </row>
+    <row r="3" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50">
-        <f>E3/618.99</f>
+        <f>G3/$G$52</f>
         <v>0</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -3332,28 +3374,36 @@
         <v>98</v>
       </c>
       <c r="E3" s="43">
-        <f>I3+F3+J3</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-      <c r="G3" s="12">
+        <f>K3+H3+L3 + M3*2 + N3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="43">
+        <f>E3/$E$51*1000</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="54">
+        <f>ROUND(F3,0)</f>
         <v>0</v>
       </c>
       <c r="H3" s="12">
-        <f>G3/5280</f>
         <v>0</v>
       </c>
       <c r="I3" s="12">
-        <f>15*H3</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="43"/>
-    </row>
-    <row r="4" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12">
+        <f>I3/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="12">
+        <f>15*J3</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="43"/>
+    </row>
+    <row r="4" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50">
-        <f>E4/618.99</f>
+        <f>G4/$G$52</f>
         <v>0</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -3366,403 +3416,499 @@
         <v>100</v>
       </c>
       <c r="E4" s="43">
-        <f>I4+F4+J4</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="12">
-        <v>0</v>
-      </c>
-      <c r="G4" s="12">
+        <f>K4+H4+L4 + M4*2 + N4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="43">
+        <f>E4/$E$51*1000</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="54">
+        <f>ROUND(F4,0)</f>
         <v>0</v>
       </c>
       <c r="H4" s="12">
-        <f>G4/5280</f>
         <v>0</v>
       </c>
       <c r="I4" s="12">
-        <f>15*H4</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="43"/>
-    </row>
-    <row r="5" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="12">
+        <f>I4/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="12">
+        <f>15*J4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="43"/>
+    </row>
+    <row r="5" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50">
-        <f>E5/618.99</f>
+        <f>G5/$G$52</f>
         <v>0</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E5" s="43">
-        <f>I5+F5+J5</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="12">
-        <v>0</v>
-      </c>
-      <c r="G5" s="12">
+        <f>K5+H5+L5 + M5*2 + N5</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="43">
+        <f>E5/$E$51*1000</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="54">
+        <f>ROUND(F5,0)</f>
         <v>0</v>
       </c>
       <c r="H5" s="12">
-        <f>G5/5280</f>
         <v>0</v>
       </c>
       <c r="I5" s="12">
-        <f>15*H5</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="43"/>
-    </row>
-    <row r="6" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="12">
+        <f>I5/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
+        <f>15*J5</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="43"/>
+    </row>
+    <row r="6" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="50">
-        <f>E6/618.99</f>
+        <f>G6/$G$52</f>
         <v>0</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>170</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E6" s="43">
-        <f>I6+F6+J6</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="12">
+        <f>K6+H6+L6 + M6*2 + N6</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="43">
+        <f>E6/$E$51*1000</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="54">
+        <f>ROUND(F6,0)</f>
         <v>0</v>
       </c>
       <c r="H6" s="12">
-        <f>G6/5280</f>
         <v>0</v>
       </c>
       <c r="I6" s="12">
-        <f>15*H6</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="43"/>
-    </row>
-    <row r="7" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12">
+        <f>I6/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <f>15*J6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="43"/>
+    </row>
+    <row r="7" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="50">
-        <f>E7/618.99</f>
+        <f>G7/$G$52</f>
         <v>0</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>170</v>
       </c>
       <c r="C7" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="43">
+        <f>K7+H7+L7 + M7*2 + N7</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="43">
+        <f>E7/$E$51*1000</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="54">
+        <f>ROUND(F7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0</v>
+      </c>
+      <c r="J7" s="12">
+        <f>I7/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <f>15*J7</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="43"/>
+    </row>
+    <row r="8" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="50">
+        <f>G8/$G$52</f>
+        <v>0</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D8" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="43">
-        <f>I7+F7+J7</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="12">
-        <v>0</v>
-      </c>
-      <c r="G7" s="12">
-        <v>0</v>
-      </c>
-      <c r="H7" s="12">
-        <f>G7/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="12">
-        <f>15*H7</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="43"/>
-    </row>
-    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50">
-        <f>E8/618.99</f>
-        <v>0</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="E8" s="43">
+        <f>K8+H8+L8 + M8*2 + N8</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="43">
+        <f>E8/$E$51*1000</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="54">
+        <f>ROUND(F8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+      <c r="J8" s="12">
+        <f>I8/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <f>15*J8</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="43"/>
+    </row>
+    <row r="9" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="50">
+        <f>G9/$G$52</f>
+        <v>0</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C8" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" s="43">
-        <f>I8+F8+J8</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="12">
-        <v>0</v>
-      </c>
-      <c r="G8" s="12">
-        <v>0</v>
-      </c>
-      <c r="H8" s="12">
-        <f>G8/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="12">
-        <f>15*H8</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="43"/>
-    </row>
-    <row r="9" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50">
-        <f>E9/618.99</f>
-        <v>0</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>170</v>
-      </c>
       <c r="C9" s="42" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="E9" s="43">
-        <f>I9+F9+J9</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="12">
-        <v>0</v>
-      </c>
-      <c r="G9" s="12">
+        <f>K9+H9+L9 + M9*2 + N9</f>
+        <v>2.8409090909090912E-2</v>
+      </c>
+      <c r="F9" s="43">
+        <f>E9/$E$51*1000</f>
+        <v>0.17983024025320102</v>
+      </c>
+      <c r="G9" s="54">
+        <f>ROUND(F9,0)</f>
         <v>0</v>
       </c>
       <c r="H9" s="12">
-        <f>G9/5280</f>
         <v>0</v>
       </c>
       <c r="I9" s="12">
-        <f>15*H9</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="43"/>
-    </row>
-    <row r="10" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="J9" s="12">
+        <f>I9/5280</f>
+        <v>1.893939393939394E-3</v>
+      </c>
+      <c r="K9" s="12">
+        <f>15*J9</f>
+        <v>2.8409090909090912E-2</v>
+      </c>
+      <c r="L9" s="43"/>
+    </row>
+    <row r="10" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="50">
-        <f>E10/618.99</f>
+        <f>G10/$G$52</f>
         <v>0</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>169</v>
       </c>
       <c r="C10" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="43">
+        <f>K10+H10+L10 + M10*2 + N10</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="43">
+        <f>E10/$E$51*1000</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="54">
+        <f>ROUND(F10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0</v>
+      </c>
+      <c r="I10" s="12">
+        <v>0</v>
+      </c>
+      <c r="J10" s="12">
+        <f>I10/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <f>15*J10</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="43"/>
+    </row>
+    <row r="11" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="50">
+        <f>G11/$G$52</f>
+        <v>0</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="43">
+        <f>K11+H11+L11 + M11*2 + N11</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="43">
+        <f>E11/$E$51*1000</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="54">
+        <f>ROUND(F11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12">
+        <v>0</v>
+      </c>
+      <c r="J11" s="12">
+        <f>I11/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
+        <f>15*J11</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="43"/>
+    </row>
+    <row r="12" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="50">
+        <f>G12/$G$52</f>
+        <v>0</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="43">
+        <f>K12+H12+L12 + M12*2 + N12</f>
+        <v>5.6818181818181823E-2</v>
+      </c>
+      <c r="F12" s="43">
+        <f>E12/$E$51*1000</f>
+        <v>0.35966048050640204</v>
+      </c>
+      <c r="G12" s="54">
+        <f>ROUND(F12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12">
+        <v>20</v>
+      </c>
+      <c r="J12" s="12">
+        <f>I12/5280</f>
+        <v>3.787878787878788E-3</v>
+      </c>
+      <c r="K12" s="12">
+        <f>15*J12</f>
+        <v>5.6818181818181823E-2</v>
+      </c>
+      <c r="L12" s="43"/>
+    </row>
+    <row r="13" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="50">
+        <f>G13/$G$52</f>
+        <v>0</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D13" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="43">
-        <f>I10+F10+J10</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="12">
-        <v>0</v>
-      </c>
-      <c r="G10" s="12">
-        <v>0</v>
-      </c>
-      <c r="H10" s="12">
-        <f>G10/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="12">
-        <f>15*H10</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="43"/>
-    </row>
-    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50">
-        <f>E11/618.99</f>
-        <v>0</v>
-      </c>
-      <c r="B11" s="12" t="s">
+      <c r="E13" s="43">
+        <f>K13+H13+L13 + M13*2 + N13</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="43">
+        <f>E13/$E$51*1000</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="54">
+        <f>ROUND(F13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12">
+        <v>0</v>
+      </c>
+      <c r="J13" s="12">
+        <f>I13/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="12">
+        <f>15*J13</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="43"/>
+    </row>
+    <row r="14" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="50">
+        <f>G14/$G$52</f>
+        <v>0</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C14" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D14" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="43">
-        <f>I11+F11+J11</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="12">
-        <v>0</v>
-      </c>
-      <c r="G11" s="12">
-        <v>0</v>
-      </c>
-      <c r="H11" s="12">
-        <f>G11/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="12">
-        <f>15*H11</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="43"/>
-    </row>
-    <row r="12" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50">
-        <f>E12/618.99</f>
-        <v>4.5895880238922943E-5</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="43">
-        <f>I12+F12+J12</f>
-        <v>2.8409090909090912E-2</v>
-      </c>
-      <c r="F12" s="12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="12">
-        <v>10</v>
-      </c>
-      <c r="H12" s="12">
-        <f>G12/5280</f>
-        <v>1.893939393939394E-3</v>
-      </c>
-      <c r="I12" s="12">
-        <f>15*H12</f>
-        <v>2.8409090909090912E-2</v>
-      </c>
-      <c r="J12" s="43"/>
-    </row>
-    <row r="13" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50">
-        <f>E13/618.99</f>
-        <v>9.1791760477845887E-5</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="43">
-        <f>I13+F13+J13</f>
-        <v>5.6818181818181823E-2</v>
-      </c>
-      <c r="F13" s="12">
-        <v>0</v>
-      </c>
-      <c r="G13" s="12">
-        <v>20</v>
-      </c>
-      <c r="H13" s="12">
-        <f>G13/5280</f>
-        <v>3.787878787878788E-3</v>
-      </c>
-      <c r="I13" s="12">
-        <f>15*H13</f>
-        <v>5.6818181818181823E-2</v>
-      </c>
-      <c r="J13" s="43"/>
-    </row>
-    <row r="14" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50">
-        <f>E14/618.99</f>
-        <v>1.6155349844100875E-4</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>54</v>
-      </c>
       <c r="E14" s="43">
-        <f>I14+F14+J14</f>
-        <v>0.1</v>
-      </c>
-      <c r="F14" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="G14" s="12">
+        <f>K14+H14+L14 + M14*2 + N14</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="43">
+        <f>E14/$E$51*1000</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="54">
+        <f>ROUND(F14,0)</f>
         <v>0</v>
       </c>
       <c r="H14" s="12">
-        <f>G14/5280</f>
         <v>0</v>
       </c>
       <c r="I14" s="12">
-        <f>15*H14</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="43"/>
-    </row>
-    <row r="15" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="12">
+        <f>I14/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <f>15*J14</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="43"/>
+    </row>
+    <row r="15" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="50">
-        <f>E15/618.99</f>
-        <v>1.6155349844100875E-4</v>
+        <f>G15/$G$52</f>
+        <v>2.2011886418666079E-4</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>168</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E15" s="43">
-        <f>I15+F15+J15</f>
+        <f>K15+H15+L15 + M15*2 + N15</f>
         <v>0.1</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="43">
+        <f>E15/$E$51*1000</f>
+        <v>0.63300244569126751</v>
+      </c>
+      <c r="G15" s="54">
+        <f>ROUND(F15,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="12">
         <v>0.1</v>
       </c>
-      <c r="G15" s="12">
-        <v>0</v>
-      </c>
-      <c r="H15" s="12">
-        <f>G15/5280</f>
-        <v>0</v>
-      </c>
       <c r="I15" s="12">
-        <f>15*H15</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="43"/>
-    </row>
-    <row r="16" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="12">
+        <f>I15/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="12">
+        <f>15*J15</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="43"/>
+    </row>
+    <row r="16" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="50">
-        <f>E16/618.99</f>
-        <v>2.5334525891885465E-4</v>
+        <f>G16/$G$52</f>
+        <v>2.2011886418666079E-4</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>168</v>
@@ -3774,29 +3920,37 @@
         <v>62</v>
       </c>
       <c r="E16" s="43">
-        <f>I16+F16+J16</f>
+        <f>K16+H16+L16 + M16*2 + N16</f>
         <v>0.15681818181818183</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="43">
+        <f>E16/$E$51*1000</f>
+        <v>0.9926629261976696</v>
+      </c>
+      <c r="G16" s="54">
+        <f>ROUND(F16,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="12">
         <v>0.1</v>
       </c>
-      <c r="G16" s="12">
+      <c r="I16" s="12">
         <v>20</v>
       </c>
-      <c r="H16" s="12">
-        <f>G16/5280</f>
+      <c r="J16" s="12">
+        <f>I16/5280</f>
         <v>3.787878787878788E-3</v>
       </c>
-      <c r="I16" s="12">
-        <f>15*H16</f>
+      <c r="K16" s="12">
+        <f>15*J16</f>
         <v>5.6818181818181823E-2</v>
       </c>
-      <c r="J16" s="43"/>
-    </row>
-    <row r="17" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="43"/>
+    </row>
+    <row r="17" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="50">
-        <f>E17/618.99</f>
-        <v>3.2310699688201751E-4</v>
+        <f>G17/$G$52</f>
+        <v>2.2011886418666079E-4</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>170</v>
@@ -3808,131 +3962,163 @@
         <v>92</v>
       </c>
       <c r="E17" s="43">
-        <f>I17+F17+J17</f>
+        <f>K17+H17+L17 + M17*2 + N17</f>
         <v>0.2</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="43">
+        <f>E17/$E$51*1000</f>
+        <v>1.266004891382535</v>
+      </c>
+      <c r="G17" s="54">
+        <f>ROUND(F17,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="12">
         <v>0.2</v>
       </c>
-      <c r="G17" s="12">
-        <v>0</v>
-      </c>
-      <c r="H17" s="12">
-        <f>G17/5280</f>
-        <v>0</v>
-      </c>
       <c r="I17" s="12">
-        <f>15*H17</f>
-        <v>0</v>
-      </c>
-      <c r="J17" s="43"/>
-    </row>
-    <row r="18" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="12">
+        <f>I17/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="12">
+        <f>15*J17</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="43"/>
+    </row>
+    <row r="18" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="50">
-        <f>E18/618.99</f>
-        <v>5.0669051783770931E-4</v>
+        <f>G18/$G$52</f>
+        <v>2.2011886418666079E-4</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="43">
+        <f>K18+H18+L18 + M18*2 + N18</f>
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="43">
+        <f>E18/$E$51*1000</f>
+        <v>0.63300244569126751</v>
+      </c>
+      <c r="G18" s="54">
+        <f>ROUND(F18,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0</v>
+      </c>
+      <c r="J18" s="12">
+        <f>I18/5280</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <f>15*J18</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="43"/>
+    </row>
+    <row r="19" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="50">
+        <f>G19/$G$52</f>
+        <v>4.4023772837332157E-4</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C19" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D19" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="43">
-        <f>I18+F18+J18</f>
+      <c r="E19" s="43">
+        <f>K19+H19+L19 + M19*2 + N19</f>
         <v>0.31363636363636366</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F19" s="43">
+        <f>E19/$E$51*1000</f>
+        <v>1.9853258523953392</v>
+      </c>
+      <c r="G19" s="54">
+        <f>ROUND(F19,0)</f>
+        <v>2</v>
+      </c>
+      <c r="H19" s="12">
         <v>0.2</v>
       </c>
-      <c r="G18" s="12">
+      <c r="I19" s="12">
         <v>40</v>
       </c>
-      <c r="H18" s="12">
-        <f>G18/5280</f>
+      <c r="J19" s="12">
+        <f>I19/5280</f>
         <v>7.575757575757576E-3</v>
       </c>
-      <c r="I18" s="12">
-        <f>15*H18</f>
+      <c r="K19" s="12">
+        <f>15*J19</f>
         <v>0.11363636363636365</v>
       </c>
-      <c r="J18" s="43"/>
-    </row>
-    <row r="19" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="50">
-        <f>E19/618.99</f>
-        <v>5.764522558008721E-4</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="43">
-        <f>I19+F19+J19</f>
-        <v>0.35681818181818181</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="G19" s="12">
-        <v>20</v>
-      </c>
-      <c r="H19" s="12">
-        <f>G19/5280</f>
-        <v>3.787878787878788E-3</v>
-      </c>
-      <c r="I19" s="12">
-        <f>15*H19</f>
-        <v>5.6818181818181823E-2</v>
-      </c>
-      <c r="J19" s="43"/>
-    </row>
-    <row r="20" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L19" s="43"/>
+    </row>
+    <row r="20" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="50">
-        <f>E20/618.99</f>
-        <v>7.8206579927124693E-4</v>
+        <f>G20/$G$52</f>
+        <v>4.4023772837332157E-4</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>168</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E20" s="43">
-        <f>I20+F20+J20</f>
-        <v>0.48409090909090913</v>
-      </c>
-      <c r="F20" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="G20" s="12">
-        <v>100</v>
+        <f>K20+H20+L20 + M20*2 + N20</f>
+        <v>0.35681818181818181</v>
+      </c>
+      <c r="F20" s="43">
+        <f>E20/$E$51*1000</f>
+        <v>2.2586678175802044</v>
+      </c>
+      <c r="G20" s="54">
+        <f>ROUND(F20,0)</f>
+        <v>2</v>
       </c>
       <c r="H20" s="12">
-        <f>G20/5280</f>
-        <v>1.893939393939394E-2</v>
+        <v>0.3</v>
       </c>
       <c r="I20" s="12">
-        <f>15*H20</f>
-        <v>0.28409090909090912</v>
-      </c>
-      <c r="J20" s="43"/>
-    </row>
-    <row r="21" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="J20" s="12">
+        <f>I20/5280</f>
+        <v>3.787878787878788E-3</v>
+      </c>
+      <c r="K20" s="12">
+        <f>15*J20</f>
+        <v>5.6818181818181823E-2</v>
+      </c>
+      <c r="L20" s="43"/>
+    </row>
+    <row r="21" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="50">
-        <f>E21/618.99</f>
-        <v>7.8390163448080377E-4</v>
+        <f>G21/$G$52</f>
+        <v>6.6035659255998238E-4</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>168</v>
@@ -3944,199 +4130,249 @@
         <v>82</v>
       </c>
       <c r="E21" s="43">
-        <f>I21+F21+J21</f>
+        <f>K21+H21+L21 + M21*2 + N21</f>
         <v>0.48522727272727273</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="43">
+        <f>E21/$E$51*1000</f>
+        <v>3.071500503524673</v>
+      </c>
+      <c r="G21" s="54">
+        <f>ROUND(F21,0)</f>
+        <v>3</v>
+      </c>
+      <c r="H21" s="12">
         <v>0.4</v>
       </c>
-      <c r="G21" s="12">
+      <c r="I21" s="12">
         <v>30</v>
       </c>
-      <c r="H21" s="12">
-        <f>G21/5280</f>
+      <c r="J21" s="12">
+        <f>I21/5280</f>
         <v>5.681818181818182E-3</v>
       </c>
-      <c r="I21" s="12">
-        <f>15*H21</f>
+      <c r="K21" s="12">
+        <f>15*J21</f>
         <v>8.5227272727272735E-2</v>
       </c>
-      <c r="J21" s="43"/>
-    </row>
-    <row r="22" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="43"/>
+    </row>
+    <row r="22" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="50">
-        <f>E22/618.99</f>
-        <v>1.1969645566311104E-3</v>
+        <f>G22/$G$52</f>
+        <v>6.6035659255998238E-4</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="43">
+        <f>K22+H22+L22 + M22*2 + N22</f>
+        <v>0.48409090909090913</v>
+      </c>
+      <c r="F22" s="43">
+        <f>E22/$E$51*1000</f>
+        <v>3.064307293914545</v>
+      </c>
+      <c r="G22" s="54">
+        <f>ROUND(F22,0)</f>
+        <v>3</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="I22" s="12">
+        <v>100</v>
+      </c>
+      <c r="J22" s="12">
+        <f>I22/5280</f>
+        <v>1.893939393939394E-2</v>
+      </c>
+      <c r="K22" s="12">
+        <f>15*J22</f>
+        <v>0.28409090909090912</v>
+      </c>
+      <c r="L22" s="43"/>
+    </row>
+    <row r="23" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="50">
+        <f>G23/$G$52</f>
+        <v>1.1005943209333039E-3</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C23" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D23" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="43">
-        <f>I22+F22+J22</f>
+      <c r="E23" s="43">
+        <f>K23+H23+L23 + M23*2 + N23</f>
         <v>0.74090909090909096</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F23" s="43">
+        <f>E23/$E$51*1000</f>
+        <v>4.6899726658034826</v>
+      </c>
+      <c r="G23" s="54">
+        <f>ROUND(F23,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H23" s="12">
         <v>0.4</v>
       </c>
-      <c r="G22" s="12">
+      <c r="I23" s="12">
         <v>120</v>
       </c>
-      <c r="H22" s="12">
-        <f>G22/5280</f>
+      <c r="J23" s="12">
+        <f>I23/5280</f>
         <v>2.2727272727272728E-2</v>
       </c>
-      <c r="I22" s="12">
-        <f>15*H22</f>
+      <c r="K23" s="12">
+        <f>15*J23</f>
         <v>0.34090909090909094</v>
       </c>
-      <c r="J22" s="43"/>
-    </row>
-    <row r="23" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="50">
-        <f>E23/618.99</f>
-        <v>1.7018192392592626E-3</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="43">
-        <f>I23+F23+J23</f>
-        <v>1.053409090909091</v>
-      </c>
-      <c r="F23" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="G23" s="12">
-        <v>230</v>
-      </c>
-      <c r="H23" s="12">
-        <f>G23/5280</f>
-        <v>4.3560606060606064E-2</v>
-      </c>
-      <c r="I23" s="12">
-        <f>15*H23</f>
-        <v>0.65340909090909094</v>
-      </c>
-      <c r="J23" s="43"/>
-    </row>
-    <row r="24" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L23" s="43"/>
+    </row>
+    <row r="24" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="50">
-        <f>E24/618.99</f>
-        <v>2.6481922897858535E-3</v>
+        <f>G24/$G$52</f>
+        <v>1.5408320493066256E-3</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>168</v>
       </c>
       <c r="C24" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="43">
+        <f>K24+H24+L24 + M24*2 + N24</f>
+        <v>1.053409090909091</v>
+      </c>
+      <c r="F24" s="43">
+        <f>E24/$E$51*1000</f>
+        <v>6.668105308588693</v>
+      </c>
+      <c r="G24" s="54">
+        <f>ROUND(F24,0)</f>
+        <v>7</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="I24" s="12">
+        <v>230</v>
+      </c>
+      <c r="J24" s="12">
+        <f>I24/5280</f>
+        <v>4.3560606060606064E-2</v>
+      </c>
+      <c r="K24" s="12">
+        <f>15*J24</f>
+        <v>0.65340909090909094</v>
+      </c>
+      <c r="L24" s="43"/>
+    </row>
+    <row r="25" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="50">
+        <f>G25/$G$52</f>
+        <v>2.2011886418666078E-3</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D25" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="43">
-        <f>I24+F24+J24</f>
+      <c r="E25" s="43">
+        <f>K25+H25+L25 + M25*2 + N25</f>
         <v>1.6392045454545454</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F25" s="43">
+        <f>E25/$E$51*1000</f>
+        <v>10.376204862609697</v>
+      </c>
+      <c r="G25" s="54">
+        <f>ROUND(F25,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H25" s="12">
         <v>1</v>
       </c>
-      <c r="G24" s="12">
+      <c r="I25" s="12">
         <v>225</v>
       </c>
-      <c r="H24" s="12">
-        <f>G24/5280</f>
+      <c r="J25" s="12">
+        <f>I25/5280</f>
         <v>4.261363636363636E-2</v>
       </c>
-      <c r="I24" s="12">
-        <f>15*H24</f>
+      <c r="K25" s="12">
+        <f>15*J25</f>
         <v>0.63920454545454541</v>
       </c>
-      <c r="J24" s="43"/>
-    </row>
-    <row r="25" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="50">
-        <f>E25/618.99</f>
-        <v>3.1300990322945441E-3</v>
-      </c>
-      <c r="B25" s="6" t="s">
+      <c r="L25" s="43"/>
+    </row>
+    <row r="26" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="52">
+        <f>G26/$G$52</f>
+        <v>2.6414263702399295E-3</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C26" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D26" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="38">
-        <f>I25+F25+J25</f>
+      <c r="E26" s="38">
+        <f>K26+H26+L26 + M26*2 + N26</f>
         <v>1.9375</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F26" s="38">
+        <f>E26/$E$51*1000</f>
+        <v>12.264422385268308</v>
+      </c>
+      <c r="G26" s="56">
+        <f>ROUND(F26,0)</f>
+        <v>12</v>
+      </c>
+      <c r="H26" s="6">
         <v>1</v>
       </c>
-      <c r="G25" s="6">
+      <c r="I26" s="6">
         <v>330</v>
       </c>
-      <c r="H25" s="6">
-        <f>G25/5280</f>
+      <c r="J26" s="6">
+        <f>I26/5280</f>
         <v>6.25E-2</v>
       </c>
-      <c r="I25" s="6">
-        <f>15*H25</f>
+      <c r="K26" s="6">
+        <f>15*J26</f>
         <v>0.9375</v>
       </c>
-      <c r="J25" s="38"/>
-    </row>
-    <row r="26" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50">
-        <f>E26/618.99</f>
-        <v>3.4513701939670053E-3</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="43">
-        <f>I26+F26+J26</f>
-        <v>2.1363636363636367</v>
-      </c>
-      <c r="F26" s="12">
-        <v>1</v>
-      </c>
-      <c r="G26" s="12">
-        <v>400</v>
-      </c>
-      <c r="H26" s="12">
-        <f>G26/5280</f>
-        <v>7.575757575757576E-2</v>
-      </c>
-      <c r="I26" s="12">
-        <f>15*H26</f>
-        <v>1.1363636363636365</v>
-      </c>
-      <c r="J26" s="43"/>
-    </row>
-    <row r="27" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+    </row>
+    <row r="27" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="50">
-        <f>E27/618.99</f>
-        <v>3.5964011755220014E-3</v>
+        <f>G27/$G$52</f>
+        <v>3.0816640986132513E-3</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>169</v>
@@ -4148,29 +4384,37 @@
         <v>96</v>
       </c>
       <c r="E27" s="43">
-        <f>I27+F27+J27</f>
+        <f>K27+H27+L27 + M27*2 + N27</f>
         <v>2.2261363636363636</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="43">
+        <f>E27/$E$51*1000</f>
+        <v>14.09149762624083</v>
+      </c>
+      <c r="G27" s="54">
+        <f>ROUND(F27,0)</f>
+        <v>14</v>
+      </c>
+      <c r="H27" s="12">
         <v>1.8</v>
       </c>
-      <c r="G27" s="12">
+      <c r="I27" s="12">
         <v>150</v>
       </c>
-      <c r="H27" s="12">
-        <f>G27/5280</f>
+      <c r="J27" s="12">
+        <f>I27/5280</f>
         <v>2.8409090909090908E-2</v>
       </c>
-      <c r="I27" s="12">
-        <f>15*H27</f>
+      <c r="K27" s="12">
+        <f>15*J27</f>
         <v>0.42613636363636365</v>
       </c>
-      <c r="J27" s="43"/>
-    </row>
-    <row r="28" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L27" s="43"/>
+    </row>
+    <row r="28" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="50">
-        <f>E28/618.99</f>
-        <v>5.0669051783770926E-3</v>
+        <f>G28/$G$52</f>
+        <v>4.4023772837332156E-3</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>169</v>
@@ -4182,29 +4426,37 @@
         <v>60</v>
       </c>
       <c r="E28" s="43">
-        <f>I28+F28+J28</f>
+        <f>K28+H28+L28 + M28*2 + N28</f>
         <v>3.1363636363636367</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="43">
+        <f>E28/$E$51*1000</f>
+        <v>19.853258523953389</v>
+      </c>
+      <c r="G28" s="54">
+        <f>ROUND(F28,0)</f>
+        <v>20</v>
+      </c>
+      <c r="H28" s="12">
         <v>2</v>
       </c>
-      <c r="G28" s="12">
+      <c r="I28" s="12">
         <v>400</v>
       </c>
-      <c r="H28" s="12">
-        <f>G28/5280</f>
+      <c r="J28" s="12">
+        <f>I28/5280</f>
         <v>7.575757575757576E-2</v>
       </c>
-      <c r="I28" s="12">
-        <f>15*H28</f>
+      <c r="K28" s="12">
+        <f>15*J28</f>
         <v>1.1363636363636365</v>
       </c>
-      <c r="J28" s="43"/>
-    </row>
-    <row r="29" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L28" s="43"/>
+    </row>
+    <row r="29" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="50">
-        <f>E29/618.99</f>
-        <v>5.3009741675955988E-3</v>
+        <f>G29/$G$52</f>
+        <v>4.6224961479198771E-3</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>169</v>
@@ -4216,29 +4468,37 @@
         <v>90</v>
       </c>
       <c r="E29" s="43">
-        <f>I29+F29+J29</f>
+        <f>K29+H29+L29 + M29*2 + N29</f>
         <v>3.28125</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="43">
+        <f>E29/$E$51*1000</f>
+        <v>20.770392749244714</v>
+      </c>
+      <c r="G29" s="54">
+        <f>ROUND(F29,0)</f>
+        <v>21</v>
+      </c>
+      <c r="H29" s="12">
         <v>2.5</v>
       </c>
-      <c r="G29" s="12">
+      <c r="I29" s="12">
         <v>275</v>
       </c>
-      <c r="H29" s="12">
-        <f>G29/5280</f>
+      <c r="J29" s="12">
+        <f>I29/5280</f>
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="I29" s="12">
-        <f>15*H29</f>
+      <c r="K29" s="12">
+        <f>15*J29</f>
         <v>0.78125</v>
       </c>
-      <c r="J29" s="43"/>
-    </row>
-    <row r="30" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L29" s="43"/>
+    </row>
+    <row r="30" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="50">
-        <f>E30/618.99</f>
-        <v>6.9963679836214134E-3</v>
+        <f>G30/$G$52</f>
+        <v>5.9432093330398419E-3</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>168</v>
@@ -4250,29 +4510,37 @@
         <v>64</v>
       </c>
       <c r="E30" s="43">
-        <f>I30+F30+J30</f>
+        <f>K30+H30+L30 + M30*2 + N30</f>
         <v>4.3306818181818185</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="43">
+        <f>E30/$E$51*1000</f>
+        <v>27.413321824197961</v>
+      </c>
+      <c r="G30" s="54">
+        <f>ROUND(F30,0)</f>
+        <v>27</v>
+      </c>
+      <c r="H30" s="12">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G30" s="12">
+      <c r="I30" s="12">
         <v>750</v>
       </c>
-      <c r="H30" s="12">
-        <f>G30/5280</f>
+      <c r="J30" s="12">
+        <f>I30/5280</f>
         <v>0.14204545454545456</v>
       </c>
-      <c r="I30" s="12">
-        <f>15*H30</f>
+      <c r="K30" s="12">
+        <f>15*J30</f>
         <v>2.1306818181818183</v>
       </c>
-      <c r="J30" s="43"/>
-    </row>
-    <row r="31" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L30" s="43"/>
+    </row>
+    <row r="31" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="50">
-        <f>E31/618.99</f>
-        <v>7.0477713694890058E-3</v>
+        <f>G31/$G$52</f>
+        <v>6.1633281972265025E-3</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>168</v>
@@ -4284,29 +4552,37 @@
         <v>52</v>
       </c>
       <c r="E31" s="43">
-        <f>I31+F31+J31</f>
+        <f>K31+H31+L31 + M31*2 + N31</f>
         <v>4.3624999999999998</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="43">
+        <f>E31/$E$51*1000</f>
+        <v>27.614731693281545</v>
+      </c>
+      <c r="G31" s="54">
+        <f>ROUND(F31,0)</f>
+        <v>28</v>
+      </c>
+      <c r="H31" s="12">
         <v>2.8</v>
       </c>
-      <c r="G31" s="12">
+      <c r="I31" s="12">
         <v>550</v>
       </c>
-      <c r="H31" s="12">
-        <f>G31/5280</f>
+      <c r="J31" s="12">
+        <f>I31/5280</f>
         <v>0.10416666666666667</v>
       </c>
-      <c r="I31" s="12">
-        <f>15*H31</f>
+      <c r="K31" s="12">
+        <f>15*J31</f>
         <v>1.5625</v>
       </c>
-      <c r="J31" s="43"/>
-    </row>
-    <row r="32" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L31" s="43"/>
+    </row>
+    <row r="32" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="50">
-        <f>E32/618.99</f>
-        <v>7.8812405546278483E-3</v>
+        <f>G32/$G$52</f>
+        <v>6.8236847897864845E-3</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>168</v>
@@ -4318,29 +4594,37 @@
         <v>72</v>
       </c>
       <c r="E32" s="43">
-        <f>I32+F32+J32</f>
+        <f>K32+H32+L32 + M32*2 + N32</f>
         <v>4.8784090909090914</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="43">
+        <f>E32/$E$51*1000</f>
+        <v>30.880448856279678</v>
+      </c>
+      <c r="G32" s="54">
+        <f>ROUND(F32,0)</f>
+        <v>31</v>
+      </c>
+      <c r="H32" s="12">
         <v>3.6</v>
       </c>
-      <c r="G32" s="12">
+      <c r="I32" s="12">
         <v>450</v>
       </c>
-      <c r="H32" s="12">
-        <f>G32/5280</f>
+      <c r="J32" s="12">
+        <f>I32/5280</f>
         <v>8.5227272727272721E-2</v>
       </c>
-      <c r="I32" s="12">
-        <f>15*H32</f>
+      <c r="K32" s="12">
+        <f>15*J32</f>
         <v>1.2784090909090908</v>
       </c>
-      <c r="J32" s="43"/>
-    </row>
-    <row r="33" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L32" s="43"/>
+    </row>
+    <row r="33" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="50">
-        <f>E33/618.99</f>
-        <v>1.4062497705205989E-2</v>
+        <f>G33/$G$52</f>
+        <v>1.2106537530266344E-2</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>168</v>
@@ -4352,29 +4636,37 @@
         <v>74</v>
       </c>
       <c r="E33" s="43">
-        <f>I33+F33+J33</f>
+        <f>K33+H33+L33 + M33*2 + N33</f>
         <v>8.704545454545455</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33" s="43">
+        <f>E33/$E$51*1000</f>
+        <v>55.099985613580785</v>
+      </c>
+      <c r="G33" s="54">
+        <f>ROUND(F33,0)</f>
+        <v>55</v>
+      </c>
+      <c r="H33" s="12">
         <v>7</v>
       </c>
-      <c r="G33" s="12">
+      <c r="I33" s="12">
         <v>600</v>
       </c>
-      <c r="H33" s="12">
-        <f>G33/5280</f>
+      <c r="J33" s="12">
+        <f>I33/5280</f>
         <v>0.11363636363636363</v>
       </c>
-      <c r="I33" s="12">
-        <f>15*H33</f>
+      <c r="K33" s="12">
+        <f>15*J33</f>
         <v>1.7045454545454546</v>
       </c>
-      <c r="J33" s="43"/>
-    </row>
-    <row r="34" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L33" s="43"/>
+    </row>
+    <row r="34" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="50">
-        <f>E34/618.99</f>
-        <v>1.6254484945416949E-2</v>
+        <f>G34/$G$52</f>
+        <v>1.408760730794629E-2</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>168</v>
@@ -4386,29 +4678,37 @@
         <v>30</v>
       </c>
       <c r="E34" s="43">
-        <f>I34+F34+J34</f>
+        <f>K34+H34+L34 + M34*2 + N34</f>
         <v>10.061363636363637</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="43">
+        <f>E34/$E$51*1000</f>
+        <v>63.68867788807367</v>
+      </c>
+      <c r="G34" s="54">
+        <f>ROUND(F34,0)</f>
+        <v>64</v>
+      </c>
+      <c r="H34" s="12">
         <v>5.8</v>
       </c>
-      <c r="G34" s="12">
+      <c r="I34" s="12">
         <v>1500</v>
       </c>
-      <c r="H34" s="12">
-        <f>G34/5280</f>
+      <c r="J34" s="12">
+        <f>I34/5280</f>
         <v>0.28409090909090912</v>
       </c>
-      <c r="I34" s="12">
-        <f>15*H34</f>
+      <c r="K34" s="12">
+        <f>15*J34</f>
         <v>4.2613636363636367</v>
       </c>
-      <c r="J34" s="43"/>
-    </row>
-    <row r="35" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L34" s="43"/>
+    </row>
+    <row r="35" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="50">
-        <f>E35/618.99</f>
-        <v>1.7450531584443277E-2</v>
+        <f>G35/$G$52</f>
+        <v>1.4968082764692935E-2</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>169</v>
@@ -4420,29 +4720,37 @@
         <v>46</v>
       </c>
       <c r="E35" s="43">
-        <f>I35+F35+J35</f>
+        <f>K35+H35+L35 + M35*2 + N35</f>
         <v>10.801704545454545</v>
       </c>
-      <c r="F35" s="12">
+      <c r="F35" s="43">
+        <f>E35/$E$51*1000</f>
+        <v>68.375053949072083</v>
+      </c>
+      <c r="G35" s="54">
+        <f>ROUND(F35,0)</f>
+        <v>68</v>
+      </c>
+      <c r="H35" s="12">
         <v>8.6</v>
       </c>
-      <c r="G35" s="12">
+      <c r="I35" s="12">
         <v>775</v>
       </c>
-      <c r="H35" s="12">
-        <f>G35/5280</f>
+      <c r="J35" s="12">
+        <f>I35/5280</f>
         <v>0.14678030303030304</v>
       </c>
-      <c r="I35" s="12">
-        <f>15*H35</f>
+      <c r="K35" s="12">
+        <f>15*J35</f>
         <v>2.2017045454545454</v>
       </c>
-      <c r="J35" s="43"/>
-    </row>
-    <row r="36" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L35" s="43"/>
+    </row>
+    <row r="36" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="50">
-        <f>E36/618.99</f>
-        <v>2.0777982901765191E-2</v>
+        <f>G36/$G$52</f>
+        <v>1.7829627999119524E-2</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>168</v>
@@ -4454,29 +4762,37 @@
         <v>38</v>
       </c>
       <c r="E36" s="43">
-        <f>I36+F36+J36</f>
+        <f>K36+H36+L36 + M36*2 + N36</f>
         <v>12.861363636363636</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36" s="43">
+        <f>E36/$E$51*1000</f>
+        <v>81.41274636742915</v>
+      </c>
+      <c r="G36" s="54">
+        <f>ROUND(F36,0)</f>
+        <v>81</v>
+      </c>
+      <c r="H36" s="12">
         <v>8.6</v>
       </c>
-      <c r="G36" s="12">
+      <c r="I36" s="12">
         <v>1500</v>
       </c>
-      <c r="H36" s="12">
-        <f>G36/5280</f>
+      <c r="J36" s="12">
+        <f>I36/5280</f>
         <v>0.28409090909090912</v>
       </c>
-      <c r="I36" s="12">
-        <f>15*H36</f>
+      <c r="K36" s="12">
+        <f>15*J36</f>
         <v>4.2613636363636367</v>
       </c>
-      <c r="J36" s="43"/>
-    </row>
-    <row r="37" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L36" s="43"/>
+    </row>
+    <row r="37" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="50">
-        <f>E37/618.99</f>
-        <v>2.4932477980992497E-2</v>
+        <f>G37/$G$52</f>
+        <v>2.1571648690292759E-2</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>168</v>
@@ -4488,29 +4804,37 @@
         <v>16</v>
       </c>
       <c r="E37" s="43">
-        <f>I37+F37+J37</f>
+        <f>K37+H37+L37 + M37*2 + N37</f>
         <v>15.432954545454546</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F37" s="43">
+        <f>E37/$E$51*1000</f>
+        <v>97.690979715148913</v>
+      </c>
+      <c r="G37" s="54">
+        <f>ROUND(F37,0)</f>
+        <v>98</v>
+      </c>
+      <c r="H37" s="12">
         <v>6.2</v>
       </c>
-      <c r="G37" s="12">
+      <c r="I37" s="12">
         <v>3250</v>
       </c>
-      <c r="H37" s="12">
-        <f>G37/5280</f>
+      <c r="J37" s="12">
+        <f>I37/5280</f>
         <v>0.61553030303030298</v>
       </c>
-      <c r="I37" s="12">
-        <f>15*H37</f>
+      <c r="K37" s="12">
+        <f>15*J37</f>
         <v>9.232954545454545</v>
       </c>
-      <c r="J37" s="43"/>
-    </row>
-    <row r="38" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L37" s="43"/>
+    </row>
+    <row r="38" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="50">
-        <f>E38/618.99</f>
-        <v>2.7109778539527001E-2</v>
+        <f>G38/$G$52</f>
+        <v>2.3332599603786044E-2</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>168</v>
@@ -4522,29 +4846,37 @@
         <v>28</v>
       </c>
       <c r="E38" s="43">
-        <f>I38+F38+J38</f>
+        <f>K38+H38+L38 + M38*2 + N38</f>
         <v>16.780681818181819</v>
       </c>
-      <c r="F38" s="12">
+      <c r="F38" s="43">
+        <f>E38/$E$51*1000</f>
+        <v>106.22212631276076</v>
+      </c>
+      <c r="G38" s="54">
+        <f>ROUND(F38,0)</f>
+        <v>106</v>
+      </c>
+      <c r="H38" s="12">
         <v>8.4</v>
       </c>
-      <c r="G38" s="12">
+      <c r="I38" s="12">
         <v>2950</v>
       </c>
-      <c r="H38" s="12">
-        <f>G38/5280</f>
+      <c r="J38" s="12">
+        <f>I38/5280</f>
         <v>0.55871212121212122</v>
       </c>
-      <c r="I38" s="12">
-        <f>15*H38</f>
+      <c r="K38" s="12">
+        <f>15*J38</f>
         <v>8.3806818181818183</v>
       </c>
-      <c r="J38" s="43"/>
-    </row>
-    <row r="39" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L38" s="43"/>
+    </row>
+    <row r="39" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="50">
-        <f>E39/618.99</f>
-        <v>3.0603372943313816E-2</v>
+        <f>G39/$G$52</f>
+        <v>2.6414263702399295E-2</v>
       </c>
       <c r="B39" s="42" t="s">
         <v>168</v>
@@ -4556,29 +4888,37 @@
         <v>24</v>
       </c>
       <c r="E39" s="43">
-        <f>I39+F39+J39</f>
+        <f>K39+H39+L39 + M39*2 + N39</f>
         <v>18.94318181818182</v>
       </c>
-      <c r="F39" s="12">
+      <c r="F39" s="43">
+        <f>E39/$E$51*1000</f>
+        <v>119.91080420083443</v>
+      </c>
+      <c r="G39" s="54">
+        <f>ROUND(F39,0)</f>
+        <v>120</v>
+      </c>
+      <c r="H39" s="12">
         <v>9</v>
       </c>
-      <c r="G39" s="12">
+      <c r="I39" s="12">
         <v>3500</v>
       </c>
-      <c r="H39" s="12">
-        <f>G39/5280</f>
+      <c r="J39" s="12">
+        <f>I39/5280</f>
         <v>0.66287878787878785</v>
       </c>
-      <c r="I39" s="12">
-        <f>15*H39</f>
+      <c r="K39" s="12">
+        <f>15*J39</f>
         <v>9.9431818181818183</v>
       </c>
-      <c r="J39" s="43"/>
-    </row>
-    <row r="40" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L39" s="43"/>
+    </row>
+    <row r="40" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="50">
-        <f>E40/618.99</f>
-        <v>3.2149146189760738E-2</v>
+        <f>G40/$G$52</f>
+        <v>2.7734976887519261E-2</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>168</v>
@@ -4590,29 +4930,37 @@
         <v>18</v>
       </c>
       <c r="E40" s="43">
-        <f>I40+F40+J40</f>
+        <f>K40+H40+L40 + M40*2 + N40</f>
         <v>19.899999999999999</v>
       </c>
-      <c r="F40" s="12">
+      <c r="F40" s="43">
+        <f>E40/$E$51*1000</f>
+        <v>125.96748669256222</v>
+      </c>
+      <c r="G40" s="54">
+        <f>ROUND(F40,0)</f>
+        <v>126</v>
+      </c>
+      <c r="H40" s="12">
         <v>7.4</v>
       </c>
-      <c r="G40" s="12">
+      <c r="I40" s="12">
         <v>4400</v>
       </c>
-      <c r="H40" s="12">
-        <f>G40/5280</f>
+      <c r="J40" s="12">
+        <f>I40/5280</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="I40" s="12">
-        <f>15*H40</f>
+      <c r="K40" s="12">
+        <f>15*J40</f>
         <v>12.5</v>
       </c>
-      <c r="J40" s="43"/>
-    </row>
-    <row r="41" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L40" s="43"/>
+    </row>
+    <row r="41" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="50">
-        <f>E41/618.99</f>
-        <v>3.6077833538212541E-2</v>
+        <f>G41/$G$52</f>
+        <v>3.1036759850319173E-2</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>168</v>
@@ -4624,29 +4972,37 @@
         <v>44</v>
       </c>
       <c r="E41" s="43">
-        <f>I41+F41+J41</f>
+        <f>K41+H41+L41 + M41*2 + N41</f>
         <v>22.331818181818182</v>
       </c>
-      <c r="F41" s="12">
+      <c r="F41" s="43">
+        <f>E41/$E$51*1000</f>
+        <v>141.36095525823623</v>
+      </c>
+      <c r="G41" s="54">
+        <f>ROUND(F41,0)</f>
+        <v>141</v>
+      </c>
+      <c r="H41" s="12">
         <v>10.4</v>
       </c>
-      <c r="G41" s="12">
+      <c r="I41" s="12">
         <v>4200</v>
       </c>
-      <c r="H41" s="12">
-        <f>G41/5280</f>
+      <c r="J41" s="12">
+        <f>I41/5280</f>
         <v>0.79545454545454541</v>
       </c>
-      <c r="I41" s="12">
-        <f>15*H41</f>
+      <c r="K41" s="12">
+        <f>15*J41</f>
         <v>11.931818181818182</v>
       </c>
-      <c r="J41" s="43"/>
-    </row>
-    <row r="42" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L41" s="43"/>
+    </row>
+    <row r="42" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="50">
-        <f>E42/618.99</f>
-        <v>3.748775497915225E-2</v>
+        <f>G42/$G$52</f>
+        <v>3.2357473035439135E-2</v>
       </c>
       <c r="B42" s="42" t="s">
         <v>168</v>
@@ -4658,29 +5014,37 @@
         <v>6</v>
       </c>
       <c r="E42" s="43">
-        <f>I42+F42+J42</f>
+        <f>K42+H42+L42 + M42*2 + N42</f>
         <v>23.204545454545453</v>
       </c>
-      <c r="F42" s="12">
+      <c r="F42" s="43">
+        <f>E42/$E$51*1000</f>
+        <v>146.88534023881456</v>
+      </c>
+      <c r="G42" s="54">
+        <f>ROUND(F42,0)</f>
+        <v>147</v>
+      </c>
+      <c r="H42" s="12">
         <v>9</v>
       </c>
-      <c r="G42" s="12">
+      <c r="I42" s="12">
         <v>5000</v>
       </c>
-      <c r="H42" s="12">
-        <f>G42/5280</f>
+      <c r="J42" s="12">
+        <f>I42/5280</f>
         <v>0.94696969696969702</v>
       </c>
-      <c r="I42" s="12">
-        <f>15*H42</f>
+      <c r="K42" s="12">
+        <f>15*J42</f>
         <v>14.204545454545455</v>
       </c>
-      <c r="J42" s="43"/>
-    </row>
-    <row r="43" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L42" s="43"/>
+    </row>
+    <row r="43" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="50">
-        <f>E43/618.99</f>
-        <v>3.8596599445724633E-2</v>
+        <f>G43/$G$52</f>
+        <v>3.3237948492185782E-2</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>168</v>
@@ -4692,29 +5056,37 @@
         <v>42</v>
       </c>
       <c r="E43" s="43">
-        <f>I43+F43+J43</f>
+        <f>K43+H43+L43 + M43*2 + N43</f>
         <v>23.890909090909091</v>
       </c>
-      <c r="F43" s="12">
+      <c r="F43" s="43">
+        <f>E43/$E$51*1000</f>
+        <v>151.2300388433319</v>
+      </c>
+      <c r="G43" s="54">
+        <f>ROUND(F43,0)</f>
+        <v>151</v>
+      </c>
+      <c r="H43" s="12">
         <v>14.8</v>
       </c>
-      <c r="G43" s="12">
+      <c r="I43" s="12">
         <v>3200</v>
       </c>
-      <c r="H43" s="12">
-        <f>G43/5280</f>
+      <c r="J43" s="12">
+        <f>I43/5280</f>
         <v>0.60606060606060608</v>
       </c>
-      <c r="I43" s="12">
-        <f>15*H43</f>
+      <c r="K43" s="12">
+        <f>15*J43</f>
         <v>9.0909090909090917</v>
       </c>
-      <c r="J43" s="43"/>
-    </row>
-    <row r="44" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L43" s="43"/>
+    </row>
+    <row r="44" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="50">
-        <f>E44/618.99</f>
-        <v>4.4535526348641261E-2</v>
+        <f>G44/$G$52</f>
+        <v>3.9841514417785606E-2</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>168</v>
@@ -4726,31 +5098,40 @@
         <v>22</v>
       </c>
       <c r="E44" s="43">
-        <f>I44+F44+J44</f>
-        <v>27.567045454545454</v>
-      </c>
-      <c r="F44" s="12">
+        <f>K44+H44+L44 + M44*2 + N44</f>
+        <v>28.567045454545454</v>
+      </c>
+      <c r="F44" s="43">
+        <f>E44/$E$51*1000</f>
+        <v>180.83009638900879</v>
+      </c>
+      <c r="G44" s="54">
+        <f>ROUND(F44,0)</f>
+        <v>181</v>
+      </c>
+      <c r="H44" s="12">
         <v>6.8</v>
       </c>
-      <c r="G44" s="12">
+      <c r="I44" s="12">
         <v>5550</v>
       </c>
-      <c r="H44" s="12">
-        <f>G44/5280</f>
+      <c r="J44" s="12">
+        <f>I44/5280</f>
         <v>1.0511363636363635</v>
       </c>
-      <c r="I44" s="12">
-        <f>15*H44</f>
+      <c r="K44" s="12">
+        <f>15*J44</f>
         <v>15.767045454545453</v>
       </c>
-      <c r="J44" s="43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L44" s="43">
+        <v>6</v>
+      </c>
+      <c r="M44" s="43"/>
+    </row>
+    <row r="45" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="50">
-        <f>E45/618.99</f>
-        <v>4.5326771323960298E-2</v>
+        <f>G45/$G$52</f>
+        <v>4.8866387849438697E-2</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>168</v>
@@ -4762,31 +5143,41 @@
         <v>26</v>
       </c>
       <c r="E45" s="43">
-        <f>I45+F45+J45</f>
-        <v>28.056818181818183</v>
-      </c>
-      <c r="F45" s="12">
+        <f>K45+H45+L45 + M45*2 + N45</f>
+        <v>35.056818181818187</v>
+      </c>
+      <c r="F45" s="43">
+        <f>E45/$E$51*1000</f>
+        <v>221.91051647245004</v>
+      </c>
+      <c r="G45" s="54">
+        <f>ROUND(F45,0)</f>
+        <v>222</v>
+      </c>
+      <c r="H45" s="12">
         <v>8</v>
       </c>
-      <c r="G45" s="12">
+      <c r="I45" s="12">
         <v>5300</v>
       </c>
-      <c r="H45" s="12">
-        <f>G45/5280</f>
+      <c r="J45" s="12">
+        <f>I45/5280</f>
         <v>1.0037878787878789</v>
       </c>
-      <c r="I45" s="12">
-        <f>15*H45</f>
+      <c r="K45" s="12">
+        <f>15*J45</f>
         <v>15.056818181818183</v>
       </c>
-      <c r="J45" s="43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L45" s="43">
+        <v>12</v>
+      </c>
+      <c r="M45" s="43"/>
+      <c r="N45" s="43"/>
+    </row>
+    <row r="46" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="50">
-        <f>E46/618.99</f>
-        <v>6.5552167827648861E-2</v>
+        <f>G46/$G$52</f>
+        <v>5.7891261281091788E-2</v>
       </c>
       <c r="B46" s="42" t="s">
         <v>168</v>
@@ -4798,29 +5189,41 @@
         <v>4</v>
       </c>
       <c r="E46" s="43">
-        <f>I46+F46+J46</f>
-        <v>40.576136363636365</v>
-      </c>
-      <c r="F46" s="12">
+        <f>K46+H46+L46 + M46*2 + N46</f>
+        <v>41.576136363636365</v>
+      </c>
+      <c r="F46" s="43">
+        <f>E46/$E$51*1000</f>
+        <v>263.17796000575458</v>
+      </c>
+      <c r="G46" s="54">
+        <f>ROUND(F46,0)</f>
+        <v>263</v>
+      </c>
+      <c r="H46" s="12">
         <v>21.4</v>
       </c>
-      <c r="G46" s="12">
+      <c r="I46" s="12">
         <v>6750</v>
       </c>
-      <c r="H46" s="12">
-        <f>G46/5280</f>
+      <c r="J46" s="12">
+        <f>I46/5280</f>
         <v>1.2784090909090908</v>
       </c>
-      <c r="I46" s="12">
-        <f>15*H46</f>
+      <c r="K46" s="12">
+        <f>15*J46</f>
         <v>19.176136363636363</v>
       </c>
-      <c r="J46" s="43"/>
-    </row>
-    <row r="47" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L46" s="43"/>
+      <c r="M46" s="43"/>
+      <c r="N46" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="50">
-        <f>E47/618.99</f>
-        <v>7.1081703478834288E-2</v>
+        <f>G47/$G$52</f>
+        <v>6.4054589478318297E-2</v>
       </c>
       <c r="B47" s="12" t="s">
         <v>168</v>
@@ -4832,101 +5235,139 @@
         <v>14</v>
       </c>
       <c r="E47" s="43">
-        <f>I47+F47+J47</f>
-        <v>43.998863636363637</v>
-      </c>
-      <c r="F47" s="12">
+        <f>K47+H47+L47 + M47*2 + N47</f>
+        <v>45.998863636363637</v>
+      </c>
+      <c r="F47" s="43">
+        <f>E47/$E$51*1000</f>
+        <v>291.17393180837291</v>
+      </c>
+      <c r="G47" s="54">
+        <f>ROUND(F47,0)</f>
+        <v>291</v>
+      </c>
+      <c r="H47" s="12">
         <v>28.8</v>
       </c>
-      <c r="G47" s="12">
+      <c r="I47" s="12">
         <v>5350</v>
       </c>
-      <c r="H47" s="12">
-        <f>G47/5280</f>
+      <c r="J47" s="12">
+        <f>I47/5280</f>
         <v>1.0132575757575757</v>
       </c>
-      <c r="I47" s="12">
-        <f>15*H47</f>
+      <c r="K47" s="12">
+        <f>15*J47</f>
         <v>15.198863636363635</v>
       </c>
-      <c r="J47" s="43"/>
-    </row>
-    <row r="48" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L47" s="43"/>
+      <c r="M47" s="43"/>
+      <c r="N47" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="50">
-        <f>E48/618.99</f>
-        <v>7.5691485690031701E-2</v>
+        <f>G48/$G$52</f>
+        <v>8.1003742020691175E-2</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>168</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D48" s="42" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E48" s="43">
-        <f>I48+F48+J48</f>
-        <v>46.852272727272727</v>
-      </c>
-      <c r="F48" s="12">
-        <v>16</v>
-      </c>
-      <c r="G48" s="12">
-        <v>9100</v>
+        <f>K48+H48+L48 + M48*2 + N48</f>
+        <v>58.075000000000003</v>
+      </c>
+      <c r="F48" s="43">
+        <f>E48/$E$51*1000</f>
+        <v>367.61617033520361</v>
+      </c>
+      <c r="G48" s="54">
+        <f>ROUND(F48,0)</f>
+        <v>368</v>
       </c>
       <c r="H48" s="12">
-        <f>G48/5280</f>
-        <v>1.7234848484848484</v>
+        <v>22.2</v>
       </c>
       <c r="I48" s="12">
-        <f>15*H48</f>
-        <v>25.852272727272727</v>
-      </c>
-      <c r="J48" s="43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>7700</v>
+      </c>
+      <c r="J48" s="12">
+        <f>I48/5280</f>
+        <v>1.4583333333333333</v>
+      </c>
+      <c r="K48" s="12">
+        <f>15*J48</f>
+        <v>21.875</v>
+      </c>
+      <c r="L48" s="43">
+        <v>12</v>
+      </c>
+      <c r="M48" s="43"/>
+      <c r="N48" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="50">
-        <f>E49/618.99</f>
-        <v>7.9282379359925048E-2</v>
+        <f>G49/$G$52</f>
+        <v>8.0563504292317858E-2</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>168</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D49" s="42" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E49" s="43">
-        <f>I49+F49+J49</f>
-        <v>49.075000000000003</v>
-      </c>
-      <c r="F49" s="12">
-        <v>22.2</v>
-      </c>
-      <c r="G49" s="12">
-        <v>7700</v>
+        <f>K49+H49+L49 + M49*2 + N49</f>
+        <v>57.852272727272727</v>
+      </c>
+      <c r="F49" s="43">
+        <f>E49/$E$51*1000</f>
+        <v>366.20630125161847</v>
+      </c>
+      <c r="G49" s="54">
+        <f>ROUND(F49,0)</f>
+        <v>366</v>
       </c>
       <c r="H49" s="12">
-        <f>G49/5280</f>
-        <v>1.4583333333333333</v>
+        <v>16</v>
       </c>
       <c r="I49" s="12">
-        <f>15*H49</f>
-        <v>21.875</v>
-      </c>
-      <c r="J49" s="43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>9100</v>
+      </c>
+      <c r="J49" s="12">
+        <f>I49/5280</f>
+        <v>1.7234848484848484</v>
+      </c>
+      <c r="K49" s="12">
+        <f>15*J49</f>
+        <v>25.852272727272727</v>
+      </c>
+      <c r="L49" s="43">
+        <v>12</v>
+      </c>
+      <c r="M49" s="43">
+        <v>1</v>
+      </c>
+      <c r="N49" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="50">
-        <f>E50/618.99</f>
-        <v>0.1130452246988863</v>
+        <f>G50/$G$52</f>
+        <v>0.11138014527845036</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>168</v>
@@ -4938,31 +5379,43 @@
         <v>10</v>
       </c>
       <c r="E50" s="43">
-        <f>I50+F50+J50</f>
-        <v>69.973863636363632</v>
-      </c>
-      <c r="F50" s="12">
+        <f>K50+H50+L50 + M50*2 + N50</f>
+        <v>79.973863636363632</v>
+      </c>
+      <c r="F50" s="43">
+        <f>E50/$E$51*1000</f>
+        <v>506.23651273198101</v>
+      </c>
+      <c r="G50" s="54">
+        <f>ROUND(F50,0)</f>
+        <v>506</v>
+      </c>
+      <c r="H50" s="12">
         <v>40.4</v>
       </c>
-      <c r="G50" s="12">
+      <c r="I50" s="12">
         <v>8650</v>
       </c>
-      <c r="H50" s="12">
-        <f>G50/5280</f>
+      <c r="J50" s="12">
+        <f>I50/5280</f>
         <v>1.6382575757575757</v>
       </c>
-      <c r="I50" s="12">
-        <f>15*H50</f>
+      <c r="K50" s="12">
+        <f>15*J50</f>
         <v>24.573863636363637</v>
       </c>
-      <c r="J50" s="43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="50">
-        <f>E51/618.99</f>
-        <v>0.15828571176799741</v>
+      <c r="L50" s="43">
+        <v>12</v>
+      </c>
+      <c r="M50" s="43"/>
+      <c r="N50" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="51">
+        <f>G51/$G$52</f>
+        <v>0.2201188641866608</v>
       </c>
       <c r="B51" s="47" t="s">
         <v>168</v>
@@ -4974,187 +5427,295 @@
         <v>2</v>
       </c>
       <c r="E51" s="49">
-        <f>I51+F51+J51</f>
-        <v>97.97727272727272</v>
-      </c>
-      <c r="F51" s="47">
+        <f>K51+H51+L51 + M51*2 + N51</f>
+        <v>157.97727272727272</v>
+      </c>
+      <c r="F51" s="49">
+        <f>E51/$E$51*1000</f>
+        <v>1000</v>
+      </c>
+      <c r="G51" s="55">
+        <f>ROUND(F51,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="H51" s="49">
         <v>39</v>
       </c>
-      <c r="G51" s="47">
+      <c r="I51" s="47">
         <v>19000</v>
       </c>
-      <c r="H51" s="47">
-        <f>G51/5280</f>
+      <c r="J51" s="47">
+        <f>I51/5280</f>
         <v>3.5984848484848486</v>
       </c>
-      <c r="I51" s="47">
-        <f>15*H51</f>
+      <c r="K51" s="47">
+        <f>15*J51</f>
         <v>53.977272727272727</v>
       </c>
-      <c r="J51" s="49">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L51" s="49">
+        <v>12</v>
+      </c>
+      <c r="M51" s="49">
+        <v>18</v>
+      </c>
+      <c r="N51" s="49">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E52" s="36">
         <f>SUM(E2:E51)</f>
-        <v>618.9948863636364</v>
-      </c>
-      <c r="J52" s="36"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C53" s="37" t="s">
+        <v>717.85852272727277</v>
+      </c>
+      <c r="F52" s="36">
+        <f>SUM(F2:F51)</f>
+        <v>4544.0620054668398</v>
+      </c>
+      <c r="G52" s="36">
+        <f>SUM(G2:G51)</f>
+        <v>4543</v>
+      </c>
+      <c r="L52" s="36"/>
+      <c r="M52" s="43"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="36"/>
+      <c r="L53" s="36"/>
+      <c r="M53" s="43"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C54" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="E53" s="36"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
+      <c r="E54" s="36"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="36"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
         <v>172</v>
       </c>
-      <c r="E54" s="36"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C55" s="37" t="s">
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="36"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C56" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="E55" s="36"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E56" s="36"/>
-      <c r="J56" s="36"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C57" s="37" t="s">
+      <c r="F56" s="36"/>
+      <c r="G56" s="36"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="36"/>
+      <c r="L57" s="36"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C58" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="E57" s="36"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C58" s="37" t="s">
+      <c r="E58" s="36"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="36"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C59" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C60" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="E58" s="36"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C59" s="37" t="s">
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
+      <c r="G60" s="36"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C61" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="E61" s="36"/>
+      <c r="F61" s="36"/>
+      <c r="G61" s="36"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C62" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="E59" s="36"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C60" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="E60" s="36"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C61" s="37" t="s">
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="36"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C63" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="E63" s="36"/>
+      <c r="F63" s="36"/>
+      <c r="G63" s="36"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C64" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="E64" s="36"/>
+      <c r="F64" s="36"/>
+      <c r="G64" s="36"/>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C65" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E65" s="36"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="36"/>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C66" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="E66" s="36"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="36"/>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E67" s="36"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="36"/>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C68" s="37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C69" s="37" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C71" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="E61" s="36"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C62" s="37" t="s">
+      <c r="E71" s="36"/>
+      <c r="F71" s="36"/>
+      <c r="G71" s="36"/>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C72" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
+      <c r="G72" s="36"/>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C73" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="E73" s="36"/>
+      <c r="F73" s="36"/>
+      <c r="G73" s="36"/>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C74" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="E74" s="36"/>
+      <c r="F74" s="36"/>
+      <c r="G74" s="36"/>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="36"/>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C76" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="E62" s="36"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C63" s="37" t="s">
+      <c r="E76" s="36"/>
+      <c r="F76" s="36"/>
+      <c r="G76" s="36"/>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E77" s="36"/>
+      <c r="F77" s="36"/>
+      <c r="G77" s="36"/>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C78" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="E63" s="36"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E64" s="36"/>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C65" s="37" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C66" s="37" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C68" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="E68" s="36"/>
-    </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C69" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="E69" s="36"/>
-    </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C70" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="E70" s="36"/>
-    </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C71" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="E71" s="36"/>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="E72" s="36"/>
-    </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C73" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="E73" s="36"/>
-    </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="E74" s="36"/>
-    </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C75" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="E75" s="36"/>
-    </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="E76" s="36"/>
-    </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="E77" s="36"/>
-    </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E78" s="36"/>
-    </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F78" s="36"/>
+      <c r="G78" s="36"/>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E79" s="36"/>
-    </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F79" s="36"/>
+      <c r="G79" s="36"/>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E80" s="36"/>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="F80" s="36"/>
+      <c r="G80" s="36"/>
+    </row>
+    <row r="81" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E81" s="36"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="F81" s="36"/>
+      <c r="G81" s="36"/>
+    </row>
+    <row r="82" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E82" s="36"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="F82" s="36"/>
+      <c r="G82" s="36"/>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E83" s="36"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="F83" s="36"/>
+      <c r="G83" s="36"/>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E84" s="36"/>
-    </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="F84" s="36"/>
+      <c r="G84" s="36"/>
+    </row>
+    <row r="85" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E85" s="36"/>
+      <c r="F85" s="36"/>
+      <c r="G85" s="36"/>
+    </row>
+    <row r="86" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E86" s="36"/>
+      <c r="F86" s="36"/>
+      <c r="G86" s="36"/>
+    </row>
+    <row r="87" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E87" s="36"/>
+      <c r="F87" s="36"/>
+      <c r="G87" s="36"/>
+    </row>
+    <row r="88" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E88" s="36"/>
+      <c r="F88" s="36"/>
+      <c r="G88" s="36"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K51">
-    <sortCondition ref="E2:E51"/>
+  <sortState ref="A3:N51">
+    <sortCondition ref="G3:G51"/>
+    <sortCondition ref="C3:C51"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Walter Scale write up
</commit_message>
<xml_diff>
--- a/Walter/TripReports/STATE HIGH POINTS.xlsx
+++ b/Walter/TripReports/STATE HIGH POINTS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="194">
   <si>
     <t>State</t>
   </si>
@@ -506,27 +506,12 @@
     <t>        2</t>
   </si>
   <si>
-    <t>mileage</t>
-  </si>
-  <si>
-    <t>&gt; class4 or glacier</t>
-  </si>
-  <si>
-    <t>vert as miles</t>
-  </si>
-  <si>
     <t>Walter Scale</t>
   </si>
   <si>
-    <t>vert converted to horizontal</t>
-  </si>
-  <si>
     <t>HP</t>
   </si>
   <si>
-    <t>vertical feet</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -575,9 +560,6 @@
     <t>Number of Nights</t>
   </si>
   <si>
-    <t>Days below freezing</t>
-  </si>
-  <si>
     <t>Raw Walter Scale</t>
   </si>
   <si>
@@ -609,6 +591,21 @@
   </si>
   <si>
     <t>If a highpoint involves climbing with the use of both hands and feet, but not the protection of a rope, an additional 6 bonus miles are awarded.</t>
+  </si>
+  <si>
+    <t>Vertical Points</t>
+  </si>
+  <si>
+    <t>Vertical Feet</t>
+  </si>
+  <si>
+    <t>Mileage</t>
+  </si>
+  <si>
+    <t>Terrain Points</t>
+  </si>
+  <si>
+    <t>Days Below Freezing in PM</t>
   </si>
 </sst>
 </file>
@@ -3255,7 +3252,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N88"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3264,2456 +3261,2018 @@
     <col min="1" max="2" width="14.21875" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" style="37" customWidth="1"/>
     <col min="4" max="4" width="19.109375" style="37" customWidth="1"/>
-    <col min="5" max="7" width="20.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="20.88671875" customWidth="1"/>
-    <col min="12" max="12" width="19.44140625" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" customWidth="1"/>
-    <col min="14" max="14" width="16.5546875" customWidth="1"/>
+    <col min="5" max="6" width="20.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C1" s="40" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="K1" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="L1" s="40" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51">
+        <f>F2/$F$52</f>
+        <v>0.2201188641866608</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="49">
+        <f>I2+H2+J2 + K2*2 + L2</f>
+        <v>157.97727272727272</v>
+      </c>
+      <c r="F2" s="55">
+        <f>ROUND(E2/$E$53*1000,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="G2" s="47">
+        <v>19000</v>
+      </c>
+      <c r="H2" s="49">
+        <v>39</v>
+      </c>
+      <c r="I2" s="47">
+        <f>15*G2/5280</f>
+        <v>53.977272727272727</v>
+      </c>
+      <c r="J2" s="55">
+        <v>12</v>
+      </c>
+      <c r="K2" s="55">
+        <v>18</v>
+      </c>
+      <c r="L2" s="55">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50">
+        <f>F3/$F$52</f>
+        <v>0.11138014527845036</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="43">
+        <f>I3+H3+J3 + K3*2 + L3</f>
+        <v>79.973863636363632</v>
+      </c>
+      <c r="F3" s="54">
+        <f>ROUND(E3/$E$53*1000,0)</f>
+        <v>506</v>
+      </c>
+      <c r="G3" s="12">
+        <v>8650</v>
+      </c>
+      <c r="H3" s="12">
+        <v>40.4</v>
+      </c>
+      <c r="I3" s="12">
+        <f>15*G3/5280</f>
+        <v>24.573863636363637</v>
+      </c>
+      <c r="J3" s="54">
+        <v>12</v>
+      </c>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50">
+        <f>F4/$F$52</f>
+        <v>8.1003742020691175E-2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="43">
+        <f>I4+H4+J4 + K4*2 + L4</f>
+        <v>58.075000000000003</v>
+      </c>
+      <c r="F4" s="54">
+        <f>ROUND(E4/$E$53*1000,0)</f>
+        <v>368</v>
+      </c>
+      <c r="G4" s="12">
+        <v>7700</v>
+      </c>
+      <c r="H4" s="12">
+        <v>22.2</v>
+      </c>
+      <c r="I4" s="12">
+        <f>15*G4/5280</f>
+        <v>21.875</v>
+      </c>
+      <c r="J4" s="54">
+        <v>12</v>
+      </c>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50">
+        <f>F5/$F$52</f>
+        <v>8.0563504292317858E-2</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="43">
+        <f>I5+H5+J5 + K5*2 + L5</f>
+        <v>57.852272727272727</v>
+      </c>
+      <c r="F5" s="54">
+        <f>ROUND(E5/$E$53*1000,0)</f>
+        <v>366</v>
+      </c>
+      <c r="G5" s="12">
+        <v>9100</v>
+      </c>
+      <c r="H5" s="12">
+        <v>16</v>
+      </c>
+      <c r="I5" s="12">
+        <f>15*G5/5280</f>
+        <v>25.852272727272727</v>
+      </c>
+      <c r="J5" s="54">
+        <v>12</v>
+      </c>
+      <c r="K5" s="54">
+        <v>1</v>
+      </c>
+      <c r="L5" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50">
+        <f>F6/$F$52</f>
+        <v>6.4054589478318297E-2</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="43">
+        <f>I6+H6+J6 + K6*2 + L6</f>
+        <v>45.998863636363637</v>
+      </c>
+      <c r="F6" s="54">
+        <f>ROUND(E6/$E$53*1000,0)</f>
+        <v>291</v>
+      </c>
+      <c r="G6" s="12">
+        <v>5350</v>
+      </c>
+      <c r="H6" s="12">
+        <v>28.8</v>
+      </c>
+      <c r="I6" s="12">
+        <f>15*G6/5280</f>
+        <v>15.198863636363637</v>
+      </c>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="50">
+        <f>F7/$F$52</f>
+        <v>5.7891261281091788E-2</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="43">
+        <f>I7+H7+J7 + K7*2 + L7</f>
+        <v>41.576136363636365</v>
+      </c>
+      <c r="F7" s="54">
+        <f>ROUND(E7/$E$53*1000,0)</f>
+        <v>263</v>
+      </c>
+      <c r="G7" s="12">
+        <v>6750</v>
+      </c>
+      <c r="H7" s="12">
+        <v>21.4</v>
+      </c>
+      <c r="I7" s="12">
+        <f>15*G7/5280</f>
+        <v>19.176136363636363</v>
+      </c>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="50">
+        <f>F8/$F$52</f>
+        <v>4.8866387849438697E-2</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="43">
+        <f>I8+H8+J8 + K8*2 + L8</f>
+        <v>35.05681818181818</v>
+      </c>
+      <c r="F8" s="54">
+        <f>ROUND(E8/$E$53*1000,0)</f>
+        <v>222</v>
+      </c>
+      <c r="G8" s="12">
+        <v>5300</v>
+      </c>
+      <c r="H8" s="12">
+        <v>8</v>
+      </c>
+      <c r="I8" s="12">
+        <f>15*G8/5280</f>
+        <v>15.056818181818182</v>
+      </c>
+      <c r="J8" s="54">
+        <v>12</v>
+      </c>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+    </row>
+    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="50">
+        <f>F9/$F$52</f>
+        <v>3.9841514417785606E-2</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="43">
+        <f>I9+H9+J9 + K9*2 + L9</f>
+        <v>28.567045454545454</v>
+      </c>
+      <c r="F9" s="54">
+        <f>ROUND(E9/$E$53*1000,0)</f>
+        <v>181</v>
+      </c>
+      <c r="G9" s="12">
+        <v>5550</v>
+      </c>
+      <c r="H9" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="I9" s="12">
+        <f>15*G9/5280</f>
+        <v>15.767045454545455</v>
+      </c>
+      <c r="J9" s="54">
+        <v>6</v>
+      </c>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+    </row>
+    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="50">
+        <f>F10/$F$52</f>
+        <v>3.3237948492185782E-2</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="43">
+        <f>I10+H10+J10 + K10*2 + L10</f>
+        <v>23.890909090909091</v>
+      </c>
+      <c r="F10" s="54">
+        <f>ROUND(E10/$E$53*1000,0)</f>
+        <v>151</v>
+      </c>
+      <c r="G10" s="12">
+        <v>3200</v>
+      </c>
+      <c r="H10" s="12">
+        <v>14.8</v>
+      </c>
+      <c r="I10" s="12">
+        <f>15*G10/5280</f>
+        <v>9.0909090909090917</v>
+      </c>
+      <c r="J10" s="43"/>
+    </row>
+    <row r="11" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="50">
+        <f>F11/$F$52</f>
+        <v>3.2357473035439135E-2</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="43">
+        <f>I11+H11+J11 + K11*2 + L11</f>
+        <v>23.204545454545453</v>
+      </c>
+      <c r="F11" s="54">
+        <f>ROUND(E11/$E$53*1000,0)</f>
+        <v>147</v>
+      </c>
+      <c r="G11" s="12">
+        <v>5000</v>
+      </c>
+      <c r="H11" s="12">
+        <v>9</v>
+      </c>
+      <c r="I11" s="12">
+        <f>15*G11/5280</f>
+        <v>14.204545454545455</v>
+      </c>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="50">
+        <f>F12/$F$52</f>
+        <v>3.1036759850319173E-2</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="43">
+        <f>I12+H12+J12 + K12*2 + L12</f>
+        <v>22.331818181818182</v>
+      </c>
+      <c r="F12" s="54">
+        <f>ROUND(E12/$E$53*1000,0)</f>
+        <v>141</v>
+      </c>
+      <c r="G12" s="12">
+        <v>4200</v>
+      </c>
+      <c r="H12" s="12">
+        <v>10.4</v>
+      </c>
+      <c r="I12" s="12">
+        <f>15*G12/5280</f>
+        <v>11.931818181818182</v>
+      </c>
+      <c r="J12" s="43"/>
+    </row>
+    <row r="13" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="50">
+        <f>F13/$F$52</f>
+        <v>2.7734976887519261E-2</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="43">
+        <f>I13+H13+J13 + K13*2 + L13</f>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F13" s="54">
+        <f>ROUND(E13/$E$53*1000,0)</f>
+        <v>126</v>
+      </c>
+      <c r="G13" s="12">
+        <v>4400</v>
+      </c>
+      <c r="H13" s="12">
+        <v>7.4</v>
+      </c>
+      <c r="I13" s="12">
+        <f>15*G13/5280</f>
+        <v>12.5</v>
+      </c>
+      <c r="J13" s="43"/>
+    </row>
+    <row r="14" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="50">
+        <f>F14/$F$52</f>
+        <v>2.6414263702399295E-2</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="43">
+        <f>I14+H14+J14 + K14*2 + L14</f>
+        <v>18.94318181818182</v>
+      </c>
+      <c r="F14" s="54">
+        <f>ROUND(E14/$E$53*1000,0)</f>
+        <v>120</v>
+      </c>
+      <c r="G14" s="12">
+        <v>3500</v>
+      </c>
+      <c r="H14" s="12">
+        <v>9</v>
+      </c>
+      <c r="I14" s="12">
+        <f>15*G14/5280</f>
+        <v>9.9431818181818183</v>
+      </c>
+      <c r="J14" s="43"/>
+    </row>
+    <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="50">
+        <f>F15/$F$52</f>
+        <v>2.3332599603786044E-2</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="43">
+        <f>I15+H15+J15 + K15*2 + L15</f>
+        <v>16.780681818181819</v>
+      </c>
+      <c r="F15" s="54">
+        <f>ROUND(E15/$E$53*1000,0)</f>
+        <v>106</v>
+      </c>
+      <c r="G15" s="12">
+        <v>2950</v>
+      </c>
+      <c r="H15" s="12">
+        <v>8.4</v>
+      </c>
+      <c r="I15" s="12">
+        <f>15*G15/5280</f>
+        <v>8.3806818181818183</v>
+      </c>
+      <c r="J15" s="43"/>
+    </row>
+    <row r="16" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="50">
+        <f>F16/$F$52</f>
+        <v>2.1571648690292759E-2</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="43">
+        <f>I16+H16+J16 + K16*2 + L16</f>
+        <v>15.432954545454546</v>
+      </c>
+      <c r="F16" s="54">
+        <f>ROUND(E16/$E$53*1000,0)</f>
+        <v>98</v>
+      </c>
+      <c r="G16" s="12">
+        <v>3250</v>
+      </c>
+      <c r="H16" s="12">
+        <v>6.2</v>
+      </c>
+      <c r="I16" s="12">
+        <f>15*G16/5280</f>
+        <v>9.232954545454545</v>
+      </c>
+      <c r="J16" s="43"/>
+    </row>
+    <row r="17" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="50">
+        <f>F17/$F$52</f>
+        <v>1.7829627999119524E-2</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="43">
+        <f>I17+H17+J17 + K17*2 + L17</f>
+        <v>12.861363636363636</v>
+      </c>
+      <c r="F17" s="54">
+        <f>ROUND(E17/$E$53*1000,0)</f>
+        <v>81</v>
+      </c>
+      <c r="G17" s="12">
+        <v>1500</v>
+      </c>
+      <c r="H17" s="12">
+        <v>8.6</v>
+      </c>
+      <c r="I17" s="12">
+        <f>15*G17/5280</f>
+        <v>4.2613636363636367</v>
+      </c>
+      <c r="J17" s="43"/>
+    </row>
+    <row r="18" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="50">
+        <f>F18/$F$52</f>
+        <v>1.408760730794629E-2</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="43">
+        <f>I18+H18+J18 + K18*2 + L18</f>
+        <v>10.061363636363637</v>
+      </c>
+      <c r="F18" s="54">
+        <f>ROUND(E18/$E$53*1000,0)</f>
+        <v>64</v>
+      </c>
+      <c r="G18" s="12">
+        <v>1500</v>
+      </c>
+      <c r="H18" s="12">
+        <v>5.8</v>
+      </c>
+      <c r="I18" s="12">
+        <f>15*G18/5280</f>
+        <v>4.2613636363636367</v>
+      </c>
+      <c r="J18" s="43"/>
+    </row>
+    <row r="19" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="50">
+        <f>F19/$F$52</f>
+        <v>1.2106537530266344E-2</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="43">
+        <f>I19+H19+J19 + K19*2 + L19</f>
+        <v>8.704545454545455</v>
+      </c>
+      <c r="F19" s="54">
+        <f>ROUND(E19/$E$53*1000,0)</f>
+        <v>55</v>
+      </c>
+      <c r="G19" s="12">
+        <v>600</v>
+      </c>
+      <c r="H19" s="12">
+        <v>7</v>
+      </c>
+      <c r="I19" s="12">
+        <f>15*G19/5280</f>
+        <v>1.7045454545454546</v>
+      </c>
+      <c r="J19" s="43"/>
+    </row>
+    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="50">
+        <f>F20/$F$52</f>
+        <v>6.8236847897864845E-3</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="43">
+        <f>I20+H20+J20 + K20*2 + L20</f>
+        <v>4.8784090909090914</v>
+      </c>
+      <c r="F20" s="54">
+        <f>ROUND(E20/$E$53*1000,0)</f>
+        <v>31</v>
+      </c>
+      <c r="G20" s="12">
+        <v>450</v>
+      </c>
+      <c r="H20" s="12">
+        <v>3.6</v>
+      </c>
+      <c r="I20" s="12">
+        <f>15*G20/5280</f>
+        <v>1.2784090909090908</v>
+      </c>
+      <c r="J20" s="43"/>
+    </row>
+    <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="50">
+        <f>F21/$F$52</f>
+        <v>6.1633281972265025E-3</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="43">
+        <f>I21+H21+J21 + K21*2 + L21</f>
+        <v>4.3624999999999998</v>
+      </c>
+      <c r="F21" s="54">
+        <f>ROUND(E21/$E$53*1000,0)</f>
+        <v>28</v>
+      </c>
+      <c r="G21" s="12">
+        <v>550</v>
+      </c>
+      <c r="H21" s="12">
+        <v>2.8</v>
+      </c>
+      <c r="I21" s="12">
+        <f>15*G21/5280</f>
+        <v>1.5625</v>
+      </c>
+      <c r="J21" s="43"/>
+    </row>
+    <row r="22" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="50">
+        <f>F22/$F$52</f>
+        <v>5.9432093330398419E-3</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="43">
+        <f>I22+H22+J22 + K22*2 + L22</f>
+        <v>4.3306818181818185</v>
+      </c>
+      <c r="F22" s="54">
+        <f>ROUND(E22/$E$53*1000,0)</f>
+        <v>27</v>
+      </c>
+      <c r="G22" s="12">
+        <v>750</v>
+      </c>
+      <c r="H22" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I22" s="12">
+        <f>15*G22/5280</f>
+        <v>2.1306818181818183</v>
+      </c>
+      <c r="J22" s="43"/>
+    </row>
+    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="52">
+        <f>F23/$F$52</f>
+        <v>2.6414263702399295E-3</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="38">
+        <f>I23+H23+J23 + K23*2 + L23</f>
+        <v>1.9375</v>
+      </c>
+      <c r="F23" s="56">
+        <f>ROUND(E23/$E$53*1000,0)</f>
+        <v>12</v>
+      </c>
+      <c r="G23" s="6">
+        <v>330</v>
+      </c>
+      <c r="H23" s="6">
+        <v>1</v>
+      </c>
+      <c r="I23" s="6">
+        <f>15*G23/5280</f>
+        <v>0.9375</v>
+      </c>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+    </row>
+    <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="50">
+        <f>F24/$F$52</f>
+        <v>2.2011886418666078E-3</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="43">
+        <f>I24+H24+J24 + K24*2 + L24</f>
+        <v>1.6392045454545454</v>
+      </c>
+      <c r="F24" s="54">
+        <f>ROUND(E24/$E$53*1000,0)</f>
+        <v>10</v>
+      </c>
+      <c r="G24" s="12">
+        <v>225</v>
+      </c>
+      <c r="H24" s="12">
+        <v>1</v>
+      </c>
+      <c r="I24" s="12">
+        <f>15*G24/5280</f>
+        <v>0.63920454545454541</v>
+      </c>
+      <c r="J24" s="43"/>
+    </row>
+    <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="50">
+        <f>F25/$F$52</f>
+        <v>1.5408320493066256E-3</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="43">
+        <f>I25+H25+J25 + K25*2 + L25</f>
+        <v>1.053409090909091</v>
+      </c>
+      <c r="F25" s="54">
+        <f>ROUND(E25/$E$53*1000,0)</f>
+        <v>7</v>
+      </c>
+      <c r="G25" s="12">
+        <v>230</v>
+      </c>
+      <c r="H25" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="I25" s="12">
+        <f>15*G25/5280</f>
+        <v>0.65340909090909094</v>
+      </c>
+      <c r="J25" s="43"/>
+    </row>
+    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="50">
+        <f>F26/$F$52</f>
+        <v>6.6035659255998238E-4</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="43">
+        <f>I26+H26+J26 + K26*2 + L26</f>
+        <v>0.48522727272727273</v>
+      </c>
+      <c r="F26" s="54">
+        <f>ROUND(E26/$E$53*1000,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G26" s="12">
+        <v>30</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="I26" s="12">
+        <f>15*G26/5280</f>
+        <v>8.5227272727272721E-2</v>
+      </c>
+      <c r="J26" s="43"/>
+    </row>
+    <row r="27" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="50">
+        <f>F27/$F$52</f>
+        <v>6.6035659255998238E-4</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="43">
+        <f>I27+H27+J27 + K27*2 + L27</f>
+        <v>0.48409090909090913</v>
+      </c>
+      <c r="F27" s="54">
+        <f>ROUND(E27/$E$53*1000,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G27" s="12">
+        <v>100</v>
+      </c>
+      <c r="H27" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="I27" s="12">
+        <f>15*G27/5280</f>
+        <v>0.28409090909090912</v>
+      </c>
+      <c r="J27" s="43"/>
+    </row>
+    <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="50">
+        <f>F28/$F$52</f>
+        <v>4.4023772837332157E-4</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="43">
+        <f>I28+H28+J28 + K28*2 + L28</f>
+        <v>0.35681818181818181</v>
+      </c>
+      <c r="F28" s="54">
+        <f>ROUND(E28/$E$53*1000,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G28" s="12">
+        <v>20</v>
+      </c>
+      <c r="H28" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="I28" s="12">
+        <f>15*G28/5280</f>
+        <v>5.6818181818181816E-2</v>
+      </c>
+      <c r="J28" s="43"/>
+    </row>
+    <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="50">
+        <f>F29/$F$52</f>
+        <v>2.2011886418666079E-4</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="43">
+        <f>I29+H29+J29 + K29*2 + L29</f>
+        <v>0.1</v>
+      </c>
+      <c r="F29" s="54">
+        <f>ROUND(E29/$E$53*1000,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G29" s="12">
+        <v>0</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I29" s="12">
+        <f>15*G29/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="43"/>
+    </row>
+    <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="50">
+        <f>F30/$F$52</f>
+        <v>2.2011886418666079E-4</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="43">
+        <f>I30+H30+J30 + K30*2 + L30</f>
+        <v>0.15681818181818183</v>
+      </c>
+      <c r="F30" s="54">
+        <f>ROUND(E30/$E$53*1000,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G30" s="12">
+        <v>20</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I30" s="12">
+        <f>15*G30/5280</f>
+        <v>5.6818181818181816E-2</v>
+      </c>
+      <c r="J30" s="43"/>
+    </row>
+    <row r="31" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="50">
+        <f>F31/$F$52</f>
+        <v>2.2011886418666079E-4</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="43">
+        <f>I31+H31+J31 + K31*2 + L31</f>
+        <v>0.1</v>
+      </c>
+      <c r="F31" s="54">
+        <f>ROUND(E31/$E$53*1000,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G31" s="12">
+        <v>0</v>
+      </c>
+      <c r="H31" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I31" s="12">
+        <f>15*G31/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="43"/>
+    </row>
+    <row r="32" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="53">
+        <f>F32/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="46">
+        <f>I32+H32+J32 + K32*2 + L32</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="57">
+        <f>ROUND(E32/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="44">
+        <v>0</v>
+      </c>
+      <c r="H32" s="44">
+        <v>0</v>
+      </c>
+      <c r="I32" s="44">
+        <f>15*G32/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+    </row>
+    <row r="33" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="50">
+        <f>F33/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="43">
+        <f>I33+H33+J33 + K33*2 + L33</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="54">
+        <f>ROUND(E33/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="12">
+        <v>0</v>
+      </c>
+      <c r="H33" s="12">
+        <v>0</v>
+      </c>
+      <c r="I33" s="12">
+        <f>15*G33/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="43"/>
+    </row>
+    <row r="34" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="50">
+        <f>F34/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="43">
+        <f>I34+H34+J34 + K34*2 + L34</f>
+        <v>5.6818181818181816E-2</v>
+      </c>
+      <c r="F34" s="54">
+        <f>ROUND(E34/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="12">
+        <v>20</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0</v>
+      </c>
+      <c r="I34" s="12">
+        <f>15*G34/5280</f>
+        <v>5.6818181818181816E-2</v>
+      </c>
+      <c r="J34" s="43"/>
+    </row>
+    <row r="35" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="50">
+        <f>F35/$F$52</f>
+        <v>2.2011886418666079E-4</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="E1" s="40" t="s">
-        <v>184</v>
-      </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="I1" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="J1" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="K1" s="40" t="s">
+      <c r="C35" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="43">
+        <f>I35+H35+J35 + K35*2 + L35</f>
+        <v>0.2</v>
+      </c>
+      <c r="F35" s="54">
+        <f>ROUND(E35/$E$53*1000,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G35" s="12">
+        <v>0</v>
+      </c>
+      <c r="H35" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="I35" s="12">
+        <f>15*G35/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="43"/>
+    </row>
+    <row r="36" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="50">
+        <f>F36/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="43">
+        <f>I36+H36+J36 + K36*2 + L36</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="54">
+        <f>ROUND(E36/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0</v>
+      </c>
+      <c r="I36" s="12">
+        <f>15*G36/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="43"/>
+    </row>
+    <row r="37" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="50">
+        <f>F37/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="43">
+        <f>I37+H37+J37 + K37*2 + L37</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="54">
+        <f>ROUND(E37/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="12">
+        <v>0</v>
+      </c>
+      <c r="H37" s="12">
+        <v>0</v>
+      </c>
+      <c r="I37" s="12">
+        <f>15*G37/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="43"/>
+    </row>
+    <row r="38" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="50">
+        <f>F38/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="43">
+        <f>I38+H38+J38 + K38*2 + L38</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="54">
+        <f>ROUND(E38/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="12">
+        <v>0</v>
+      </c>
+      <c r="H38" s="12">
+        <v>0</v>
+      </c>
+      <c r="I38" s="12">
+        <f>15*G38/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="43"/>
+    </row>
+    <row r="39" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="50">
+        <f>F39/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="43">
+        <f>I39+H39+J39 + K39*2 + L39</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="54">
+        <f>ROUND(E39/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="12">
+        <v>0</v>
+      </c>
+      <c r="H39" s="12">
+        <v>0</v>
+      </c>
+      <c r="I39" s="12">
+        <f>15*G39/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J39" s="43"/>
+    </row>
+    <row r="40" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="50">
+        <f>F40/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="43">
+        <f>I40+H40+J40 + K40*2 + L40</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="54">
+        <f>ROUND(E40/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="12">
+        <v>0</v>
+      </c>
+      <c r="H40" s="12">
+        <v>0</v>
+      </c>
+      <c r="I40" s="12">
+        <f>15*G40/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="43"/>
+    </row>
+    <row r="41" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="50">
+        <f>F41/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="43">
+        <f>I41+H41+J41 + K41*2 + L41</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="54">
+        <f>ROUND(E41/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="12">
+        <v>0</v>
+      </c>
+      <c r="H41" s="12">
+        <v>0</v>
+      </c>
+      <c r="I41" s="12">
+        <f>15*G41/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J41" s="43"/>
+    </row>
+    <row r="42" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="50">
+        <f>F42/$F$52</f>
+        <v>1.4968082764692935E-2</v>
+      </c>
+      <c r="B42" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="L1" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="M1" s="40" t="s">
-        <v>183</v>
-      </c>
-      <c r="N1" s="40" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53">
-        <f>G2/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>168</v>
-      </c>
-      <c r="C2" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="46">
-        <f>K2+H2+L2 + M2*2 + N2</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="46">
-        <f>E2/$E$51*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="57">
-        <f t="shared" ref="G2:G16" si="0">ROUND(F2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="44">
-        <v>0</v>
-      </c>
-      <c r="I2" s="44">
-        <v>0</v>
-      </c>
-      <c r="J2" s="44">
-        <f>I2/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="44">
-        <f>15*J2</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-    </row>
-    <row r="3" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50">
-        <f>G3/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="43">
-        <f>K3+H3+L3 + M3*2 + N3</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="43">
-        <f>E3/$E$51*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="54">
-        <f>ROUND(F3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="12">
-        <v>0</v>
-      </c>
-      <c r="I3" s="12">
-        <v>0</v>
-      </c>
-      <c r="J3" s="12">
-        <f>I3/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="12">
-        <f>15*J3</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="43"/>
-    </row>
-    <row r="4" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50">
-        <f>G4/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="43">
-        <f>K4+H4+L4 + M4*2 + N4</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="43">
-        <f>E4/$E$51*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="54">
-        <f>ROUND(F4,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="12">
-        <v>0</v>
-      </c>
-      <c r="I4" s="12">
-        <v>0</v>
-      </c>
-      <c r="J4" s="12">
-        <f>I4/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="12">
-        <f>15*J4</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="43"/>
-    </row>
-    <row r="5" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50">
-        <f>G5/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="43">
-        <f>K5+H5+L5 + M5*2 + N5</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="43">
-        <f>E5/$E$51*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="54">
-        <f>ROUND(F5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="12">
-        <v>0</v>
-      </c>
-      <c r="I5" s="12">
-        <v>0</v>
-      </c>
-      <c r="J5" s="12">
-        <f>I5/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="12">
-        <f>15*J5</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="43"/>
-    </row>
-    <row r="6" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50">
-        <f>G6/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="43">
-        <f>K6+H6+L6 + M6*2 + N6</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="43">
-        <f>E6/$E$51*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="54">
-        <f>ROUND(F6,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0</v>
-      </c>
-      <c r="I6" s="12">
-        <v>0</v>
-      </c>
-      <c r="J6" s="12">
-        <f>I6/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="12">
-        <f>15*J6</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="43"/>
-    </row>
-    <row r="7" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50">
-        <f>G7/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="43">
-        <f>K7+H7+L7 + M7*2 + N7</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="43">
-        <f>E7/$E$51*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="54">
-        <f>ROUND(F7,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="12">
-        <v>0</v>
-      </c>
-      <c r="I7" s="12">
-        <v>0</v>
-      </c>
-      <c r="J7" s="12">
-        <f>I7/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="12">
-        <f>15*J7</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="43"/>
-    </row>
-    <row r="8" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50">
-        <f>G8/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="43">
-        <f>K8+H8+L8 + M8*2 + N8</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="43">
-        <f>E8/$E$51*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="54">
-        <f>ROUND(F8,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="12">
-        <v>0</v>
-      </c>
-      <c r="I8" s="12">
-        <v>0</v>
-      </c>
-      <c r="J8" s="12">
-        <f>I8/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="12">
-        <f>15*J8</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="43"/>
-    </row>
-    <row r="9" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50">
-        <f>G9/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C9" s="42" t="s">
+      <c r="C42" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="43">
+        <f>I42+H42+J42 + K42*2 + L42</f>
+        <v>10.801704545454545</v>
+      </c>
+      <c r="F42" s="54">
+        <f>ROUND(E42/$E$53*1000,0)</f>
+        <v>68</v>
+      </c>
+      <c r="G42" s="12">
+        <v>775</v>
+      </c>
+      <c r="H42" s="12">
+        <v>8.6</v>
+      </c>
+      <c r="I42" s="12">
+        <f>15*G42/5280</f>
+        <v>2.2017045454545454</v>
+      </c>
+      <c r="J42" s="43"/>
+    </row>
+    <row r="43" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="50">
+        <f>F43/$F$52</f>
+        <v>4.6224961479198771E-3</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="43">
+        <f>I43+H43+J43 + K43*2 + L43</f>
+        <v>3.28125</v>
+      </c>
+      <c r="F43" s="54">
+        <f>ROUND(E43/$E$53*1000,0)</f>
+        <v>21</v>
+      </c>
+      <c r="G43" s="12">
+        <v>275</v>
+      </c>
+      <c r="H43" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="I43" s="12">
+        <f>15*G43/5280</f>
+        <v>0.78125</v>
+      </c>
+      <c r="J43" s="43"/>
+    </row>
+    <row r="44" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="50">
+        <f>F44/$F$52</f>
+        <v>4.4023772837332156E-3</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="43">
+        <f>I44+H44+J44 + K44*2 + L44</f>
+        <v>3.1363636363636367</v>
+      </c>
+      <c r="F44" s="54">
+        <f>ROUND(E44/$E$53*1000,0)</f>
+        <v>20</v>
+      </c>
+      <c r="G44" s="12">
+        <v>400</v>
+      </c>
+      <c r="H44" s="12">
+        <v>2</v>
+      </c>
+      <c r="I44" s="12">
+        <f>15*G44/5280</f>
+        <v>1.1363636363636365</v>
+      </c>
+      <c r="J44" s="43"/>
+    </row>
+    <row r="45" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="50">
+        <f>F45/$F$52</f>
+        <v>3.0816640986132513E-3</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" s="43">
+        <f>I45+H45+J45 + K45*2 + L45</f>
+        <v>2.2261363636363636</v>
+      </c>
+      <c r="F45" s="54">
+        <f>ROUND(E45/$E$53*1000,0)</f>
+        <v>14</v>
+      </c>
+      <c r="G45" s="12">
+        <v>150</v>
+      </c>
+      <c r="H45" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="I45" s="12">
+        <f>15*G45/5280</f>
+        <v>0.42613636363636365</v>
+      </c>
+      <c r="J45" s="43"/>
+    </row>
+    <row r="46" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="50">
+        <f>F46/$F$52</f>
+        <v>1.1005943209333039E-3</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" s="43">
+        <f>I46+H46+J46 + K46*2 + L46</f>
+        <v>0.74090909090909096</v>
+      </c>
+      <c r="F46" s="54">
+        <f>ROUND(E46/$E$53*1000,0)</f>
+        <v>5</v>
+      </c>
+      <c r="G46" s="12">
+        <v>120</v>
+      </c>
+      <c r="H46" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="I46" s="12">
+        <f>15*G46/5280</f>
+        <v>0.34090909090909088</v>
+      </c>
+      <c r="J46" s="43"/>
+    </row>
+    <row r="47" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="50">
+        <f>F47/$F$52</f>
+        <v>4.4023772837332157E-4</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="43">
+        <f>I47+H47+J47 + K47*2 + L47</f>
+        <v>0.31363636363636366</v>
+      </c>
+      <c r="F47" s="54">
+        <f>ROUND(E47/$E$53*1000,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G47" s="12">
+        <v>40</v>
+      </c>
+      <c r="H47" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="I47" s="12">
+        <f>15*G47/5280</f>
+        <v>0.11363636363636363</v>
+      </c>
+      <c r="J47" s="43"/>
+    </row>
+    <row r="48" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="50">
+        <f>F48/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D48" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="43">
-        <f>K9+H9+L9 + M9*2 + N9</f>
-        <v>2.8409090909090912E-2</v>
-      </c>
-      <c r="F9" s="43">
-        <f>E9/$E$51*1000</f>
-        <v>0.17983024025320102</v>
-      </c>
-      <c r="G9" s="54">
-        <f>ROUND(F9,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="12">
-        <v>0</v>
-      </c>
-      <c r="I9" s="12">
+      <c r="E48" s="43">
+        <f>I48+H48+J48 + K48*2 + L48</f>
+        <v>2.8409090909090908E-2</v>
+      </c>
+      <c r="F48" s="54">
+        <f>ROUND(E48/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="12">
         <v>10</v>
       </c>
-      <c r="J9" s="12">
-        <f>I9/5280</f>
-        <v>1.893939393939394E-3</v>
-      </c>
-      <c r="K9" s="12">
-        <f>15*J9</f>
-        <v>2.8409090909090912E-2</v>
-      </c>
-      <c r="L9" s="43"/>
-    </row>
-    <row r="10" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50">
-        <f>G10/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C10" s="42" t="s">
+      <c r="H48" s="12">
+        <v>0</v>
+      </c>
+      <c r="I48" s="12">
+        <f>15*G48/5280</f>
+        <v>2.8409090909090908E-2</v>
+      </c>
+      <c r="J48" s="43"/>
+    </row>
+    <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="50">
+        <f>F49/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C49" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D49" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="43">
-        <f>K10+H10+L10 + M10*2 + N10</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="43">
-        <f>E10/$E$51*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="54">
-        <f>ROUND(F10,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="12">
-        <v>0</v>
-      </c>
-      <c r="I10" s="12">
-        <v>0</v>
-      </c>
-      <c r="J10" s="12">
-        <f>I10/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="12">
-        <f>15*J10</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="43"/>
-    </row>
-    <row r="11" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50">
-        <f>G11/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="43">
-        <f>K11+H11+L11 + M11*2 + N11</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="43">
-        <f>E11/$E$51*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="54">
-        <f>ROUND(F11,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="12">
-        <v>0</v>
-      </c>
-      <c r="I11" s="12">
-        <v>0</v>
-      </c>
-      <c r="J11" s="12">
-        <f>I11/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="12">
-        <f>15*J11</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="43"/>
-    </row>
-    <row r="12" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50">
-        <f>G12/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="43">
-        <f>K12+H12+L12 + M12*2 + N12</f>
-        <v>5.6818181818181823E-2</v>
-      </c>
-      <c r="F12" s="43">
-        <f>E12/$E$51*1000</f>
-        <v>0.35966048050640204</v>
-      </c>
-      <c r="G12" s="54">
-        <f>ROUND(F12,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="12">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12">
-        <v>20</v>
-      </c>
-      <c r="J12" s="12">
-        <f>I12/5280</f>
-        <v>3.787878787878788E-3</v>
-      </c>
-      <c r="K12" s="12">
-        <f>15*J12</f>
-        <v>5.6818181818181823E-2</v>
-      </c>
-      <c r="L12" s="43"/>
-    </row>
-    <row r="13" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50">
-        <f>G13/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" s="42" t="s">
+      <c r="E49" s="43">
+        <f>I49+H49+J49 + K49*2 + L49</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="54">
+        <f>ROUND(E49/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G49" s="12">
+        <v>0</v>
+      </c>
+      <c r="H49" s="12">
+        <v>0</v>
+      </c>
+      <c r="I49" s="12">
+        <f>15*G49/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J49" s="43"/>
+    </row>
+    <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="50">
+        <f>F50/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D50" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="43">
-        <f>K13+H13+L13 + M13*2 + N13</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="43">
-        <f>E13/$E$51*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="54">
-        <f>ROUND(F13,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="12">
-        <v>0</v>
-      </c>
-      <c r="I13" s="12">
-        <v>0</v>
-      </c>
-      <c r="J13" s="12">
-        <f>I13/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="12">
-        <f>15*J13</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="43"/>
-    </row>
-    <row r="14" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50">
-        <f>G14/$G$52</f>
-        <v>0</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C14" s="42" t="s">
+      <c r="E50" s="43">
+        <f>I50+H50+J50 + K50*2 + L50</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="54">
+        <f>ROUND(E50/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="12">
+        <v>0</v>
+      </c>
+      <c r="H50" s="12">
+        <v>0</v>
+      </c>
+      <c r="I50" s="12">
+        <f>15*G50/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J50" s="43"/>
+    </row>
+    <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="50">
+        <f>F51/$F$52</f>
+        <v>0</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D51" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="43">
-        <f>K14+H14+L14 + M14*2 + N14</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="43">
-        <f>E14/$E$51*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="54">
-        <f>ROUND(F14,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="12">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12">
-        <v>0</v>
-      </c>
-      <c r="J14" s="12">
-        <f>I14/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="12">
-        <f>15*J14</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="43"/>
-    </row>
-    <row r="15" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50">
-        <f>G15/$G$52</f>
-        <v>2.2011886418666079E-4</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="43">
-        <f>K15+H15+L15 + M15*2 + N15</f>
-        <v>0.1</v>
-      </c>
-      <c r="F15" s="43">
-        <f>E15/$E$51*1000</f>
-        <v>0.63300244569126751</v>
-      </c>
-      <c r="G15" s="54">
-        <f>ROUND(F15,0)</f>
-        <v>1</v>
-      </c>
-      <c r="H15" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I15" s="12">
-        <v>0</v>
-      </c>
-      <c r="J15" s="12">
-        <f>I15/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="12">
-        <f>15*J15</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="43"/>
-    </row>
-    <row r="16" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50">
-        <f>G16/$G$52</f>
-        <v>2.2011886418666079E-4</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C16" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="43">
-        <f>K16+H16+L16 + M16*2 + N16</f>
-        <v>0.15681818181818183</v>
-      </c>
-      <c r="F16" s="43">
-        <f>E16/$E$51*1000</f>
-        <v>0.9926629261976696</v>
-      </c>
-      <c r="G16" s="54">
-        <f>ROUND(F16,0)</f>
-        <v>1</v>
-      </c>
-      <c r="H16" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I16" s="12">
-        <v>20</v>
-      </c>
-      <c r="J16" s="12">
-        <f>I16/5280</f>
-        <v>3.787878787878788E-3</v>
-      </c>
-      <c r="K16" s="12">
-        <f>15*J16</f>
-        <v>5.6818181818181823E-2</v>
-      </c>
-      <c r="L16" s="43"/>
-    </row>
-    <row r="17" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50">
-        <f>G17/$G$52</f>
-        <v>2.2011886418666079E-4</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C17" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" s="43">
-        <f>K17+H17+L17 + M17*2 + N17</f>
-        <v>0.2</v>
-      </c>
-      <c r="F17" s="43">
-        <f>E17/$E$51*1000</f>
-        <v>1.266004891382535</v>
-      </c>
-      <c r="G17" s="54">
-        <f>ROUND(F17,0)</f>
-        <v>1</v>
-      </c>
-      <c r="H17" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="I17" s="12">
-        <v>0</v>
-      </c>
-      <c r="J17" s="12">
-        <f>I17/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="12">
-        <f>15*J17</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="43"/>
-    </row>
-    <row r="18" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50">
-        <f>G18/$G$52</f>
-        <v>2.2011886418666079E-4</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="43">
-        <f>K18+H18+L18 + M18*2 + N18</f>
-        <v>0.1</v>
-      </c>
-      <c r="F18" s="43">
-        <f>E18/$E$51*1000</f>
-        <v>0.63300244569126751</v>
-      </c>
-      <c r="G18" s="54">
-        <f>ROUND(F18,0)</f>
-        <v>1</v>
-      </c>
-      <c r="H18" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I18" s="12">
-        <v>0</v>
-      </c>
-      <c r="J18" s="12">
-        <f>I18/5280</f>
-        <v>0</v>
-      </c>
-      <c r="K18" s="12">
-        <f>15*J18</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="43"/>
-    </row>
-    <row r="19" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="50">
-        <f>G19/$G$52</f>
-        <v>4.4023772837332157E-4</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="43">
-        <f>K19+H19+L19 + M19*2 + N19</f>
-        <v>0.31363636363636366</v>
-      </c>
-      <c r="F19" s="43">
-        <f>E19/$E$51*1000</f>
-        <v>1.9853258523953392</v>
-      </c>
-      <c r="G19" s="54">
-        <f>ROUND(F19,0)</f>
-        <v>2</v>
-      </c>
-      <c r="H19" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="I19" s="12">
-        <v>40</v>
-      </c>
-      <c r="J19" s="12">
-        <f>I19/5280</f>
-        <v>7.575757575757576E-3</v>
-      </c>
-      <c r="K19" s="12">
-        <f>15*J19</f>
-        <v>0.11363636363636365</v>
-      </c>
-      <c r="L19" s="43"/>
-    </row>
-    <row r="20" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50">
-        <f>G20/$G$52</f>
-        <v>4.4023772837332157E-4</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C20" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="43">
-        <f>K20+H20+L20 + M20*2 + N20</f>
-        <v>0.35681818181818181</v>
-      </c>
-      <c r="F20" s="43">
-        <f>E20/$E$51*1000</f>
-        <v>2.2586678175802044</v>
-      </c>
-      <c r="G20" s="54">
-        <f>ROUND(F20,0)</f>
-        <v>2</v>
-      </c>
-      <c r="H20" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="I20" s="12">
-        <v>20</v>
-      </c>
-      <c r="J20" s="12">
-        <f>I20/5280</f>
-        <v>3.787878787878788E-3</v>
-      </c>
-      <c r="K20" s="12">
-        <f>15*J20</f>
-        <v>5.6818181818181823E-2</v>
-      </c>
-      <c r="L20" s="43"/>
-    </row>
-    <row r="21" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50">
-        <f>G21/$G$52</f>
-        <v>6.6035659255998238E-4</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="43">
-        <f>K21+H21+L21 + M21*2 + N21</f>
-        <v>0.48522727272727273</v>
-      </c>
-      <c r="F21" s="43">
-        <f>E21/$E$51*1000</f>
-        <v>3.071500503524673</v>
-      </c>
-      <c r="G21" s="54">
-        <f>ROUND(F21,0)</f>
-        <v>3</v>
-      </c>
-      <c r="H21" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="I21" s="12">
-        <v>30</v>
-      </c>
-      <c r="J21" s="12">
-        <f>I21/5280</f>
-        <v>5.681818181818182E-3</v>
-      </c>
-      <c r="K21" s="12">
-        <f>15*J21</f>
-        <v>8.5227272727272735E-2</v>
-      </c>
-      <c r="L21" s="43"/>
-    </row>
-    <row r="22" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="50">
-        <f>G22/$G$52</f>
-        <v>6.6035659255998238E-4</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="43">
-        <f>K22+H22+L22 + M22*2 + N22</f>
-        <v>0.48409090909090913</v>
-      </c>
-      <c r="F22" s="43">
-        <f>E22/$E$51*1000</f>
-        <v>3.064307293914545</v>
-      </c>
-      <c r="G22" s="54">
-        <f>ROUND(F22,0)</f>
-        <v>3</v>
-      </c>
-      <c r="H22" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="I22" s="12">
-        <v>100</v>
-      </c>
-      <c r="J22" s="12">
-        <f>I22/5280</f>
-        <v>1.893939393939394E-2</v>
-      </c>
-      <c r="K22" s="12">
-        <f>15*J22</f>
-        <v>0.28409090909090912</v>
-      </c>
-      <c r="L22" s="43"/>
-    </row>
-    <row r="23" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="50">
-        <f>G23/$G$52</f>
-        <v>1.1005943209333039E-3</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="43">
-        <f>K23+H23+L23 + M23*2 + N23</f>
-        <v>0.74090909090909096</v>
-      </c>
-      <c r="F23" s="43">
-        <f>E23/$E$51*1000</f>
-        <v>4.6899726658034826</v>
-      </c>
-      <c r="G23" s="54">
-        <f>ROUND(F23,0)</f>
-        <v>5</v>
-      </c>
-      <c r="H23" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="I23" s="12">
-        <v>120</v>
-      </c>
-      <c r="J23" s="12">
-        <f>I23/5280</f>
-        <v>2.2727272727272728E-2</v>
-      </c>
-      <c r="K23" s="12">
-        <f>15*J23</f>
-        <v>0.34090909090909094</v>
-      </c>
-      <c r="L23" s="43"/>
-    </row>
-    <row r="24" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50">
-        <f>G24/$G$52</f>
-        <v>1.5408320493066256E-3</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C24" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="43">
-        <f>K24+H24+L24 + M24*2 + N24</f>
-        <v>1.053409090909091</v>
-      </c>
-      <c r="F24" s="43">
-        <f>E24/$E$51*1000</f>
-        <v>6.668105308588693</v>
-      </c>
-      <c r="G24" s="54">
-        <f>ROUND(F24,0)</f>
-        <v>7</v>
-      </c>
-      <c r="H24" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="I24" s="12">
-        <v>230</v>
-      </c>
-      <c r="J24" s="12">
-        <f>I24/5280</f>
-        <v>4.3560606060606064E-2</v>
-      </c>
-      <c r="K24" s="12">
-        <f>15*J24</f>
-        <v>0.65340909090909094</v>
-      </c>
-      <c r="L24" s="43"/>
-    </row>
-    <row r="25" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="50">
-        <f>G25/$G$52</f>
-        <v>2.2011886418666078E-3</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C25" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="43">
-        <f>K25+H25+L25 + M25*2 + N25</f>
-        <v>1.6392045454545454</v>
-      </c>
-      <c r="F25" s="43">
-        <f>E25/$E$51*1000</f>
-        <v>10.376204862609697</v>
-      </c>
-      <c r="G25" s="54">
-        <f>ROUND(F25,0)</f>
-        <v>10</v>
-      </c>
-      <c r="H25" s="12">
-        <v>1</v>
-      </c>
-      <c r="I25" s="12">
-        <v>225</v>
-      </c>
-      <c r="J25" s="12">
-        <f>I25/5280</f>
-        <v>4.261363636363636E-2</v>
-      </c>
-      <c r="K25" s="12">
-        <f>15*J25</f>
-        <v>0.63920454545454541</v>
-      </c>
-      <c r="L25" s="43"/>
-    </row>
-    <row r="26" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="52">
-        <f>G26/$G$52</f>
-        <v>2.6414263702399295E-3</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="38">
-        <f>K26+H26+L26 + M26*2 + N26</f>
-        <v>1.9375</v>
-      </c>
-      <c r="F26" s="38">
-        <f>E26/$E$51*1000</f>
-        <v>12.264422385268308</v>
-      </c>
-      <c r="G26" s="56">
-        <f>ROUND(F26,0)</f>
-        <v>12</v>
-      </c>
-      <c r="H26" s="6">
-        <v>1</v>
-      </c>
-      <c r="I26" s="6">
-        <v>330</v>
-      </c>
-      <c r="J26" s="6">
-        <f>I26/5280</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="K26" s="6">
-        <f>15*J26</f>
-        <v>0.9375</v>
-      </c>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-    </row>
-    <row r="27" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="50">
-        <f>G27/$G$52</f>
-        <v>3.0816640986132513E-3</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C27" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="E27" s="43">
-        <f>K27+H27+L27 + M27*2 + N27</f>
-        <v>2.2261363636363636</v>
-      </c>
-      <c r="F27" s="43">
-        <f>E27/$E$51*1000</f>
-        <v>14.09149762624083</v>
-      </c>
-      <c r="G27" s="54">
-        <f>ROUND(F27,0)</f>
-        <v>14</v>
-      </c>
-      <c r="H27" s="12">
-        <v>1.8</v>
-      </c>
-      <c r="I27" s="12">
-        <v>150</v>
-      </c>
-      <c r="J27" s="12">
-        <f>I27/5280</f>
-        <v>2.8409090909090908E-2</v>
-      </c>
-      <c r="K27" s="12">
-        <f>15*J27</f>
-        <v>0.42613636363636365</v>
-      </c>
-      <c r="L27" s="43"/>
-    </row>
-    <row r="28" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="50">
-        <f>G28/$G$52</f>
-        <v>4.4023772837332156E-3</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C28" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="43">
-        <f>K28+H28+L28 + M28*2 + N28</f>
-        <v>3.1363636363636367</v>
-      </c>
-      <c r="F28" s="43">
-        <f>E28/$E$51*1000</f>
-        <v>19.853258523953389</v>
-      </c>
-      <c r="G28" s="54">
-        <f>ROUND(F28,0)</f>
-        <v>20</v>
-      </c>
-      <c r="H28" s="12">
-        <v>2</v>
-      </c>
-      <c r="I28" s="12">
-        <v>400</v>
-      </c>
-      <c r="J28" s="12">
-        <f>I28/5280</f>
-        <v>7.575757575757576E-2</v>
-      </c>
-      <c r="K28" s="12">
-        <f>15*J28</f>
-        <v>1.1363636363636365</v>
-      </c>
-      <c r="L28" s="43"/>
-    </row>
-    <row r="29" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="50">
-        <f>G29/$G$52</f>
-        <v>4.6224961479198771E-3</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C29" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="43">
-        <f>K29+H29+L29 + M29*2 + N29</f>
-        <v>3.28125</v>
-      </c>
-      <c r="F29" s="43">
-        <f>E29/$E$51*1000</f>
-        <v>20.770392749244714</v>
-      </c>
-      <c r="G29" s="54">
-        <f>ROUND(F29,0)</f>
-        <v>21</v>
-      </c>
-      <c r="H29" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="I29" s="12">
-        <v>275</v>
-      </c>
-      <c r="J29" s="12">
-        <f>I29/5280</f>
-        <v>5.2083333333333336E-2</v>
-      </c>
-      <c r="K29" s="12">
-        <f>15*J29</f>
-        <v>0.78125</v>
-      </c>
-      <c r="L29" s="43"/>
-    </row>
-    <row r="30" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="50">
-        <f>G30/$G$52</f>
-        <v>5.9432093330398419E-3</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C30" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="43">
-        <f>K30+H30+L30 + M30*2 + N30</f>
-        <v>4.3306818181818185</v>
-      </c>
-      <c r="F30" s="43">
-        <f>E30/$E$51*1000</f>
-        <v>27.413321824197961</v>
-      </c>
-      <c r="G30" s="54">
-        <f>ROUND(F30,0)</f>
-        <v>27</v>
-      </c>
-      <c r="H30" s="12">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I30" s="12">
-        <v>750</v>
-      </c>
-      <c r="J30" s="12">
-        <f>I30/5280</f>
-        <v>0.14204545454545456</v>
-      </c>
-      <c r="K30" s="12">
-        <f>15*J30</f>
-        <v>2.1306818181818183</v>
-      </c>
-      <c r="L30" s="43"/>
-    </row>
-    <row r="31" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="50">
-        <f>G31/$G$52</f>
-        <v>6.1633281972265025E-3</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C31" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" s="43">
-        <f>K31+H31+L31 + M31*2 + N31</f>
-        <v>4.3624999999999998</v>
-      </c>
-      <c r="F31" s="43">
-        <f>E31/$E$51*1000</f>
-        <v>27.614731693281545</v>
-      </c>
-      <c r="G31" s="54">
-        <f>ROUND(F31,0)</f>
-        <v>28</v>
-      </c>
-      <c r="H31" s="12">
-        <v>2.8</v>
-      </c>
-      <c r="I31" s="12">
-        <v>550</v>
-      </c>
-      <c r="J31" s="12">
-        <f>I31/5280</f>
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="K31" s="12">
-        <f>15*J31</f>
-        <v>1.5625</v>
-      </c>
-      <c r="L31" s="43"/>
-    </row>
-    <row r="32" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="50">
-        <f>G32/$G$52</f>
-        <v>6.8236847897864845E-3</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C32" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="43">
-        <f>K32+H32+L32 + M32*2 + N32</f>
-        <v>4.8784090909090914</v>
-      </c>
-      <c r="F32" s="43">
-        <f>E32/$E$51*1000</f>
-        <v>30.880448856279678</v>
-      </c>
-      <c r="G32" s="54">
-        <f>ROUND(F32,0)</f>
-        <v>31</v>
-      </c>
-      <c r="H32" s="12">
-        <v>3.6</v>
-      </c>
-      <c r="I32" s="12">
-        <v>450</v>
-      </c>
-      <c r="J32" s="12">
-        <f>I32/5280</f>
-        <v>8.5227272727272721E-2</v>
-      </c>
-      <c r="K32" s="12">
-        <f>15*J32</f>
-        <v>1.2784090909090908</v>
-      </c>
-      <c r="L32" s="43"/>
-    </row>
-    <row r="33" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="50">
-        <f>G33/$G$52</f>
-        <v>1.2106537530266344E-2</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C33" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33" s="43">
-        <f>K33+H33+L33 + M33*2 + N33</f>
-        <v>8.704545454545455</v>
-      </c>
-      <c r="F33" s="43">
-        <f>E33/$E$51*1000</f>
-        <v>55.099985613580785</v>
-      </c>
-      <c r="G33" s="54">
-        <f>ROUND(F33,0)</f>
-        <v>55</v>
-      </c>
-      <c r="H33" s="12">
-        <v>7</v>
-      </c>
-      <c r="I33" s="12">
-        <v>600</v>
-      </c>
-      <c r="J33" s="12">
-        <f>I33/5280</f>
-        <v>0.11363636363636363</v>
-      </c>
-      <c r="K33" s="12">
-        <f>15*J33</f>
-        <v>1.7045454545454546</v>
-      </c>
-      <c r="L33" s="43"/>
-    </row>
-    <row r="34" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="50">
-        <f>G34/$G$52</f>
-        <v>1.408760730794629E-2</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34" s="43">
-        <f>K34+H34+L34 + M34*2 + N34</f>
-        <v>10.061363636363637</v>
-      </c>
-      <c r="F34" s="43">
-        <f>E34/$E$51*1000</f>
-        <v>63.68867788807367</v>
-      </c>
-      <c r="G34" s="54">
-        <f>ROUND(F34,0)</f>
-        <v>64</v>
-      </c>
-      <c r="H34" s="12">
-        <v>5.8</v>
-      </c>
-      <c r="I34" s="12">
-        <v>1500</v>
-      </c>
-      <c r="J34" s="12">
-        <f>I34/5280</f>
-        <v>0.28409090909090912</v>
-      </c>
-      <c r="K34" s="12">
-        <f>15*J34</f>
-        <v>4.2613636363636367</v>
-      </c>
-      <c r="L34" s="43"/>
-    </row>
-    <row r="35" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="50">
-        <f>G35/$G$52</f>
-        <v>1.4968082764692935E-2</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="43">
-        <f>K35+H35+L35 + M35*2 + N35</f>
-        <v>10.801704545454545</v>
-      </c>
-      <c r="F35" s="43">
-        <f>E35/$E$51*1000</f>
-        <v>68.375053949072083</v>
-      </c>
-      <c r="G35" s="54">
-        <f>ROUND(F35,0)</f>
-        <v>68</v>
-      </c>
-      <c r="H35" s="12">
-        <v>8.6</v>
-      </c>
-      <c r="I35" s="12">
-        <v>775</v>
-      </c>
-      <c r="J35" s="12">
-        <f>I35/5280</f>
-        <v>0.14678030303030304</v>
-      </c>
-      <c r="K35" s="12">
-        <f>15*J35</f>
-        <v>2.2017045454545454</v>
-      </c>
-      <c r="L35" s="43"/>
-    </row>
-    <row r="36" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="50">
-        <f>G36/$G$52</f>
-        <v>1.7829627999119524E-2</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="43">
-        <f>K36+H36+L36 + M36*2 + N36</f>
-        <v>12.861363636363636</v>
-      </c>
-      <c r="F36" s="43">
-        <f>E36/$E$51*1000</f>
-        <v>81.41274636742915</v>
-      </c>
-      <c r="G36" s="54">
-        <f>ROUND(F36,0)</f>
-        <v>81</v>
-      </c>
-      <c r="H36" s="12">
-        <v>8.6</v>
-      </c>
-      <c r="I36" s="12">
-        <v>1500</v>
-      </c>
-      <c r="J36" s="12">
-        <f>I36/5280</f>
-        <v>0.28409090909090912</v>
-      </c>
-      <c r="K36" s="12">
-        <f>15*J36</f>
-        <v>4.2613636363636367</v>
-      </c>
-      <c r="L36" s="43"/>
-    </row>
-    <row r="37" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="50">
-        <f>G37/$G$52</f>
-        <v>2.1571648690292759E-2</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C37" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="43">
-        <f>K37+H37+L37 + M37*2 + N37</f>
-        <v>15.432954545454546</v>
-      </c>
-      <c r="F37" s="43">
-        <f>E37/$E$51*1000</f>
-        <v>97.690979715148913</v>
-      </c>
-      <c r="G37" s="54">
-        <f>ROUND(F37,0)</f>
-        <v>98</v>
-      </c>
-      <c r="H37" s="12">
-        <v>6.2</v>
-      </c>
-      <c r="I37" s="12">
-        <v>3250</v>
-      </c>
-      <c r="J37" s="12">
-        <f>I37/5280</f>
-        <v>0.61553030303030298</v>
-      </c>
-      <c r="K37" s="12">
-        <f>15*J37</f>
-        <v>9.232954545454545</v>
-      </c>
-      <c r="L37" s="43"/>
-    </row>
-    <row r="38" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="50">
-        <f>G38/$G$52</f>
-        <v>2.3332599603786044E-2</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C38" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="43">
-        <f>K38+H38+L38 + M38*2 + N38</f>
-        <v>16.780681818181819</v>
-      </c>
-      <c r="F38" s="43">
-        <f>E38/$E$51*1000</f>
-        <v>106.22212631276076</v>
-      </c>
-      <c r="G38" s="54">
-        <f>ROUND(F38,0)</f>
-        <v>106</v>
-      </c>
-      <c r="H38" s="12">
-        <v>8.4</v>
-      </c>
-      <c r="I38" s="12">
-        <v>2950</v>
-      </c>
-      <c r="J38" s="12">
-        <f>I38/5280</f>
-        <v>0.55871212121212122</v>
-      </c>
-      <c r="K38" s="12">
-        <f>15*J38</f>
-        <v>8.3806818181818183</v>
-      </c>
-      <c r="L38" s="43"/>
-    </row>
-    <row r="39" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="50">
-        <f>G39/$G$52</f>
-        <v>2.6414263702399295E-2</v>
-      </c>
-      <c r="B39" s="42" t="s">
-        <v>168</v>
-      </c>
-      <c r="C39" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="E39" s="43">
-        <f>K39+H39+L39 + M39*2 + N39</f>
-        <v>18.94318181818182</v>
-      </c>
-      <c r="F39" s="43">
-        <f>E39/$E$51*1000</f>
-        <v>119.91080420083443</v>
-      </c>
-      <c r="G39" s="54">
-        <f>ROUND(F39,0)</f>
-        <v>120</v>
-      </c>
-      <c r="H39" s="12">
-        <v>9</v>
-      </c>
-      <c r="I39" s="12">
-        <v>3500</v>
-      </c>
-      <c r="J39" s="12">
-        <f>I39/5280</f>
-        <v>0.66287878787878785</v>
-      </c>
-      <c r="K39" s="12">
-        <f>15*J39</f>
-        <v>9.9431818181818183</v>
-      </c>
-      <c r="L39" s="43"/>
-    </row>
-    <row r="40" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="50">
-        <f>G40/$G$52</f>
-        <v>2.7734976887519261E-2</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C40" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="43">
-        <f>K40+H40+L40 + M40*2 + N40</f>
-        <v>19.899999999999999</v>
-      </c>
-      <c r="F40" s="43">
-        <f>E40/$E$51*1000</f>
-        <v>125.96748669256222</v>
-      </c>
-      <c r="G40" s="54">
-        <f>ROUND(F40,0)</f>
-        <v>126</v>
-      </c>
-      <c r="H40" s="12">
-        <v>7.4</v>
-      </c>
-      <c r="I40" s="12">
-        <v>4400</v>
-      </c>
-      <c r="J40" s="12">
-        <f>I40/5280</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="K40" s="12">
-        <f>15*J40</f>
-        <v>12.5</v>
-      </c>
-      <c r="L40" s="43"/>
-    </row>
-    <row r="41" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="50">
-        <f>G41/$G$52</f>
-        <v>3.1036759850319173E-2</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C41" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="43">
-        <f>K41+H41+L41 + M41*2 + N41</f>
-        <v>22.331818181818182</v>
-      </c>
-      <c r="F41" s="43">
-        <f>E41/$E$51*1000</f>
-        <v>141.36095525823623</v>
-      </c>
-      <c r="G41" s="54">
-        <f>ROUND(F41,0)</f>
-        <v>141</v>
-      </c>
-      <c r="H41" s="12">
-        <v>10.4</v>
-      </c>
-      <c r="I41" s="12">
-        <v>4200</v>
-      </c>
-      <c r="J41" s="12">
-        <f>I41/5280</f>
-        <v>0.79545454545454541</v>
-      </c>
-      <c r="K41" s="12">
-        <f>15*J41</f>
-        <v>11.931818181818182</v>
-      </c>
-      <c r="L41" s="43"/>
-    </row>
-    <row r="42" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="50">
-        <f>G42/$G$52</f>
-        <v>3.2357473035439135E-2</v>
-      </c>
-      <c r="B42" s="42" t="s">
-        <v>168</v>
-      </c>
-      <c r="C42" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" s="43">
-        <f>K42+H42+L42 + M42*2 + N42</f>
-        <v>23.204545454545453</v>
-      </c>
-      <c r="F42" s="43">
-        <f>E42/$E$51*1000</f>
-        <v>146.88534023881456</v>
-      </c>
-      <c r="G42" s="54">
-        <f>ROUND(F42,0)</f>
-        <v>147</v>
-      </c>
-      <c r="H42" s="12">
-        <v>9</v>
-      </c>
-      <c r="I42" s="12">
-        <v>5000</v>
-      </c>
-      <c r="J42" s="12">
-        <f>I42/5280</f>
-        <v>0.94696969696969702</v>
-      </c>
-      <c r="K42" s="12">
-        <f>15*J42</f>
-        <v>14.204545454545455</v>
-      </c>
-      <c r="L42" s="43"/>
-    </row>
-    <row r="43" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="50">
-        <f>G43/$G$52</f>
-        <v>3.3237948492185782E-2</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C43" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E43" s="43">
-        <f>K43+H43+L43 + M43*2 + N43</f>
-        <v>23.890909090909091</v>
-      </c>
-      <c r="F43" s="43">
-        <f>E43/$E$51*1000</f>
-        <v>151.2300388433319</v>
-      </c>
-      <c r="G43" s="54">
-        <f>ROUND(F43,0)</f>
-        <v>151</v>
-      </c>
-      <c r="H43" s="12">
-        <v>14.8</v>
-      </c>
-      <c r="I43" s="12">
-        <v>3200</v>
-      </c>
-      <c r="J43" s="12">
-        <f>I43/5280</f>
-        <v>0.60606060606060608</v>
-      </c>
-      <c r="K43" s="12">
-        <f>15*J43</f>
-        <v>9.0909090909090917</v>
-      </c>
-      <c r="L43" s="43"/>
-    </row>
-    <row r="44" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="50">
-        <f>G44/$G$52</f>
-        <v>3.9841514417785606E-2</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C44" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" s="43">
-        <f>K44+H44+L44 + M44*2 + N44</f>
-        <v>28.567045454545454</v>
-      </c>
-      <c r="F44" s="43">
-        <f>E44/$E$51*1000</f>
-        <v>180.83009638900879</v>
-      </c>
-      <c r="G44" s="54">
-        <f>ROUND(F44,0)</f>
-        <v>181</v>
-      </c>
-      <c r="H44" s="12">
-        <v>6.8</v>
-      </c>
-      <c r="I44" s="12">
-        <v>5550</v>
-      </c>
-      <c r="J44" s="12">
-        <f>I44/5280</f>
-        <v>1.0511363636363635</v>
-      </c>
-      <c r="K44" s="12">
-        <f>15*J44</f>
-        <v>15.767045454545453</v>
-      </c>
-      <c r="L44" s="43">
-        <v>6</v>
-      </c>
-      <c r="M44" s="43"/>
-    </row>
-    <row r="45" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="50">
-        <f>G45/$G$52</f>
-        <v>4.8866387849438697E-2</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C45" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="D45" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" s="43">
-        <f>K45+H45+L45 + M45*2 + N45</f>
-        <v>35.056818181818187</v>
-      </c>
-      <c r="F45" s="43">
-        <f>E45/$E$51*1000</f>
-        <v>221.91051647245004</v>
-      </c>
-      <c r="G45" s="54">
-        <f>ROUND(F45,0)</f>
-        <v>222</v>
-      </c>
-      <c r="H45" s="12">
-        <v>8</v>
-      </c>
-      <c r="I45" s="12">
-        <v>5300</v>
-      </c>
-      <c r="J45" s="12">
-        <f>I45/5280</f>
-        <v>1.0037878787878789</v>
-      </c>
-      <c r="K45" s="12">
-        <f>15*J45</f>
-        <v>15.056818181818183</v>
-      </c>
-      <c r="L45" s="43">
-        <v>12</v>
-      </c>
-      <c r="M45" s="43"/>
-      <c r="N45" s="43"/>
-    </row>
-    <row r="46" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="50">
-        <f>G46/$G$52</f>
-        <v>5.7891261281091788E-2</v>
-      </c>
-      <c r="B46" s="42" t="s">
-        <v>168</v>
-      </c>
-      <c r="C46" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" s="43">
-        <f>K46+H46+L46 + M46*2 + N46</f>
-        <v>41.576136363636365</v>
-      </c>
-      <c r="F46" s="43">
-        <f>E46/$E$51*1000</f>
-        <v>263.17796000575458</v>
-      </c>
-      <c r="G46" s="54">
-        <f>ROUND(F46,0)</f>
-        <v>263</v>
-      </c>
-      <c r="H46" s="12">
-        <v>21.4</v>
-      </c>
-      <c r="I46" s="12">
-        <v>6750</v>
-      </c>
-      <c r="J46" s="12">
-        <f>I46/5280</f>
-        <v>1.2784090909090908</v>
-      </c>
-      <c r="K46" s="12">
-        <f>15*J46</f>
-        <v>19.176136363636363</v>
-      </c>
-      <c r="L46" s="43"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="50">
-        <f>G47/$G$52</f>
-        <v>6.4054589478318297E-2</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C47" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="E47" s="43">
-        <f>K47+H47+L47 + M47*2 + N47</f>
-        <v>45.998863636363637</v>
-      </c>
-      <c r="F47" s="43">
-        <f>E47/$E$51*1000</f>
-        <v>291.17393180837291</v>
-      </c>
-      <c r="G47" s="54">
-        <f>ROUND(F47,0)</f>
-        <v>291</v>
-      </c>
-      <c r="H47" s="12">
-        <v>28.8</v>
-      </c>
-      <c r="I47" s="12">
-        <v>5350</v>
-      </c>
-      <c r="J47" s="12">
-        <f>I47/5280</f>
-        <v>1.0132575757575757</v>
-      </c>
-      <c r="K47" s="12">
-        <f>15*J47</f>
-        <v>15.198863636363635</v>
-      </c>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43"/>
-      <c r="N47" s="43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="50">
-        <f>G48/$G$52</f>
-        <v>8.1003742020691175E-2</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C48" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" s="43">
-        <f>K48+H48+L48 + M48*2 + N48</f>
-        <v>58.075000000000003</v>
-      </c>
-      <c r="F48" s="43">
-        <f>E48/$E$51*1000</f>
-        <v>367.61617033520361</v>
-      </c>
-      <c r="G48" s="54">
-        <f>ROUND(F48,0)</f>
-        <v>368</v>
-      </c>
-      <c r="H48" s="12">
-        <v>22.2</v>
-      </c>
-      <c r="I48" s="12">
-        <v>7700</v>
-      </c>
-      <c r="J48" s="12">
-        <f>I48/5280</f>
-        <v>1.4583333333333333</v>
-      </c>
-      <c r="K48" s="12">
-        <f>15*J48</f>
-        <v>21.875</v>
-      </c>
-      <c r="L48" s="43">
-        <v>12</v>
-      </c>
-      <c r="M48" s="43"/>
-      <c r="N48" s="43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="50">
-        <f>G49/$G$52</f>
-        <v>8.0563504292317858E-2</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C49" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="43">
-        <f>K49+H49+L49 + M49*2 + N49</f>
-        <v>57.852272727272727</v>
-      </c>
-      <c r="F49" s="43">
-        <f>E49/$E$51*1000</f>
-        <v>366.20630125161847</v>
-      </c>
-      <c r="G49" s="54">
-        <f>ROUND(F49,0)</f>
-        <v>366</v>
-      </c>
-      <c r="H49" s="12">
-        <v>16</v>
-      </c>
-      <c r="I49" s="12">
-        <v>9100</v>
-      </c>
-      <c r="J49" s="12">
-        <f>I49/5280</f>
-        <v>1.7234848484848484</v>
-      </c>
-      <c r="K49" s="12">
-        <f>15*J49</f>
-        <v>25.852272727272727</v>
-      </c>
-      <c r="L49" s="43">
-        <v>12</v>
-      </c>
-      <c r="M49" s="43">
-        <v>1</v>
-      </c>
-      <c r="N49" s="43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="50">
-        <f>G50/$G$52</f>
-        <v>0.11138014527845036</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C50" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="43">
-        <f>K50+H50+L50 + M50*2 + N50</f>
-        <v>79.973863636363632</v>
-      </c>
-      <c r="F50" s="43">
-        <f>E50/$E$51*1000</f>
-        <v>506.23651273198101</v>
-      </c>
-      <c r="G50" s="54">
-        <f>ROUND(F50,0)</f>
-        <v>506</v>
-      </c>
-      <c r="H50" s="12">
-        <v>40.4</v>
-      </c>
-      <c r="I50" s="12">
-        <v>8650</v>
-      </c>
-      <c r="J50" s="12">
-        <f>I50/5280</f>
-        <v>1.6382575757575757</v>
-      </c>
-      <c r="K50" s="12">
-        <f>15*J50</f>
-        <v>24.573863636363637</v>
-      </c>
-      <c r="L50" s="43">
-        <v>12</v>
-      </c>
-      <c r="M50" s="43"/>
-      <c r="N50" s="43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="51">
-        <f>G51/$G$52</f>
-        <v>0.2201188641866608</v>
-      </c>
-      <c r="B51" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="C51" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D51" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="E51" s="49">
-        <f>K51+H51+L51 + M51*2 + N51</f>
-        <v>157.97727272727272</v>
-      </c>
-      <c r="F51" s="49">
-        <f>E51/$E$51*1000</f>
-        <v>1000</v>
-      </c>
-      <c r="G51" s="55">
-        <f>ROUND(F51,0)</f>
-        <v>1000</v>
-      </c>
-      <c r="H51" s="49">
-        <v>39</v>
-      </c>
-      <c r="I51" s="47">
-        <v>19000</v>
-      </c>
-      <c r="J51" s="47">
-        <f>I51/5280</f>
-        <v>3.5984848484848486</v>
-      </c>
-      <c r="K51" s="47">
-        <f>15*J51</f>
-        <v>53.977272727272727</v>
-      </c>
-      <c r="L51" s="49">
-        <v>12</v>
-      </c>
-      <c r="M51" s="49">
-        <v>18</v>
-      </c>
-      <c r="N51" s="49">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E51" s="43">
+        <f>I51+H51+J51 + K51*2 + L51</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="54">
+        <f>ROUND(E51/$E$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="12">
+        <v>0</v>
+      </c>
+      <c r="H51" s="12">
+        <v>0</v>
+      </c>
+      <c r="I51" s="12">
+        <f>15*G51/5280</f>
+        <v>0</v>
+      </c>
+      <c r="J51" s="43"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E52" s="36">
         <f>SUM(E2:E51)</f>
-        <v>717.85852272727277</v>
+        <v>717.85852272727288</v>
       </c>
       <c r="F52" s="36">
         <f>SUM(F2:F51)</f>
-        <v>4544.0620054668398</v>
-      </c>
-      <c r="G52" s="36">
-        <f>SUM(G2:G51)</f>
         <v>4543</v>
       </c>
-      <c r="L52" s="36"/>
-      <c r="M52" s="43"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="L53" s="36"/>
-      <c r="M53" s="43"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J52" s="36"/>
+      <c r="K52" s="43"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E53" s="36">
+        <f>MAX(E2:E51)</f>
+        <v>157.97727272727272</v>
+      </c>
+      <c r="F53" s="54"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="43"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C54" s="37" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E54" s="36"/>
       <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E55" s="36"/>
       <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C56" s="37" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E56" s="36"/>
       <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E57" s="36"/>
       <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="L57" s="36"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J57" s="36"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C58" s="37" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E58" s="36"/>
       <c r="F58" s="36"/>
-      <c r="G58" s="36"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C59" s="37" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E59" s="36"/>
       <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C60" s="37" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E60" s="36"/>
       <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C61" s="37" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E61" s="36"/>
       <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C62" s="37" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E62" s="36"/>
       <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C63" s="37" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E63" s="36"/>
       <c r="F63" s="36"/>
-      <c r="G63" s="36"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C64" s="37" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E64" s="36"/>
       <c r="F64" s="36"/>
-      <c r="G64" s="36"/>
-    </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C65" s="37" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E65" s="36"/>
       <c r="F65" s="36"/>
-      <c r="G65" s="36"/>
-    </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C66" s="37" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E66" s="36"/>
       <c r="F66" s="36"/>
-      <c r="G66" s="36"/>
-    </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E67" s="36"/>
       <c r="F67" s="36"/>
-      <c r="G67" s="36"/>
-    </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C68" s="37" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C69" s="37" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C71" s="37" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E71" s="36"/>
       <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
-    </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C72" s="37" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E72" s="36"/>
       <c r="F72" s="36"/>
-      <c r="G72" s="36"/>
-    </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C73" s="37" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E73" s="36"/>
       <c r="F73" s="36"/>
-      <c r="G73" s="36"/>
-    </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C74" s="37" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E74" s="36"/>
       <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-    </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E75" s="36"/>
       <c r="F75" s="36"/>
-      <c r="G75" s="36"/>
-    </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C76" s="37" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E76" s="36"/>
       <c r="F76" s="36"/>
-      <c r="G76" s="36"/>
-    </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E77" s="36"/>
       <c r="F77" s="36"/>
-      <c r="G77" s="36"/>
-    </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C78" s="37" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E78" s="36"/>
       <c r="F78" s="36"/>
-      <c r="G78" s="36"/>
-    </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E79" s="36"/>
       <c r="F79" s="36"/>
-      <c r="G79" s="36"/>
-    </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E80" s="36"/>
       <c r="F80" s="36"/>
-      <c r="G80" s="36"/>
-    </row>
-    <row r="81" spans="5:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E81" s="36"/>
       <c r="F81" s="36"/>
-      <c r="G81" s="36"/>
-    </row>
-    <row r="82" spans="5:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E82" s="36"/>
       <c r="F82" s="36"/>
-      <c r="G82" s="36"/>
-    </row>
-    <row r="83" spans="5:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E83" s="36"/>
       <c r="F83" s="36"/>
-      <c r="G83" s="36"/>
-    </row>
-    <row r="84" spans="5:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E84" s="36"/>
       <c r="F84" s="36"/>
-      <c r="G84" s="36"/>
-    </row>
-    <row r="85" spans="5:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E85" s="36"/>
       <c r="F85" s="36"/>
-      <c r="G85" s="36"/>
-    </row>
-    <row r="86" spans="5:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E86" s="36"/>
       <c r="F86" s="36"/>
-      <c r="G86" s="36"/>
-    </row>
-    <row r="87" spans="5:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E87" s="36"/>
       <c r="F87" s="36"/>
-      <c r="G87" s="36"/>
-    </row>
-    <row r="88" spans="5:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E88" s="36"/>
       <c r="F88" s="36"/>
-      <c r="G88" s="36"/>
     </row>
   </sheetData>
-  <sortState ref="A3:N51">
-    <sortCondition ref="G3:G51"/>
-    <sortCondition ref="C3:C51"/>
+  <sortState ref="A2:M51">
+    <sortCondition descending="1" ref="B2:B51"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adjusted Sassafras vertical gain
</commit_message>
<xml_diff>
--- a/Walter/TripReports/STATE HIGH POINTS.xlsx
+++ b/Walter/TripReports/STATE HIGH POINTS.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\websites\slnWalter\Walter\TripReports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10306062-2FBE-40F6-ABE0-4BE14862C3B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28632" yWindow="2100" windowWidth="19296" windowHeight="10896" activeTab="1"/>
+    <workbookView xWindow="3225" yWindow="345" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HighPoint Log" sheetId="1" r:id="rId1"/>
     <sheet name="Walter Scale" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -611,7 +617,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
@@ -945,7 +951,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -978,9 +984,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1013,6 +1036,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1188,26 +1228,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" style="36" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="36" customWidth="1"/>
     <col min="3" max="3" width="12" style="12" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" style="12" customWidth="1"/>
-    <col min="10" max="34" width="8.88671875" style="12"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="12" customWidth="1"/>
+    <col min="10" max="34" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>101</v>
       </c>
@@ -1261,7 +1301,7 @@
       <c r="AG1" s="18"/>
       <c r="AH1" s="18"/>
     </row>
-    <row r="2" spans="1:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>16</v>
       </c>
@@ -1290,7 +1330,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>24</v>
       </c>
@@ -1319,7 +1359,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>32</v>
       </c>
@@ -1346,7 +1386,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>21</v>
       </c>
@@ -1373,7 +1413,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>7</v>
       </c>
@@ -1402,7 +1442,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1452,7 +1492,7 @@
       <c r="AG7" s="12"/>
       <c r="AH7" s="12"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>11</v>
       </c>
@@ -1479,7 +1519,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -1506,7 +1546,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>13</v>
       </c>
@@ -1533,7 +1573,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1560,7 +1600,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -1587,7 +1627,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -1614,7 +1654,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1641,7 +1681,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>8</v>
       </c>
@@ -1668,7 +1708,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1695,7 +1735,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1725,7 +1765,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -1777,7 +1817,7 @@
       <c r="AG18" s="12"/>
       <c r="AH18" s="12"/>
     </row>
-    <row r="19" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>20</v>
       </c>
@@ -1831,7 +1871,7 @@
       <c r="AG19" s="12"/>
       <c r="AH19" s="12"/>
     </row>
-    <row r="20" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1881,7 +1921,7 @@
       <c r="AG20" s="12"/>
       <c r="AH20" s="12"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>30</v>
       </c>
@@ -1905,7 +1945,7 @@
       </c>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>22</v>
       </c>
@@ -1935,7 +1975,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>18</v>
       </c>
@@ -1959,7 +1999,7 @@
       </c>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>26</v>
       </c>
@@ -1983,7 +2023,7 @@
       </c>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>31</v>
       </c>
@@ -2007,7 +2047,7 @@
       </c>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>25</v>
       </c>
@@ -2031,7 +2071,7 @@
       </c>
       <c r="H26" s="11"/>
     </row>
-    <row r="27" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>29</v>
       </c>
@@ -2061,7 +2101,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>17</v>
       </c>
@@ -2085,7 +2125,7 @@
       </c>
       <c r="H28" s="11"/>
     </row>
-    <row r="29" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -2109,7 +2149,7 @@
       </c>
       <c r="H29" s="11"/>
     </row>
-    <row r="30" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>19</v>
       </c>
@@ -2133,7 +2173,7 @@
       </c>
       <c r="H30" s="11"/>
     </row>
-    <row r="31" spans="1:34" s="12" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" s="12" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="35"/>
       <c r="D31" s="8"/>
@@ -2142,7 +2182,7 @@
       <c r="G31" s="14"/>
       <c r="H31" s="11"/>
     </row>
-    <row r="32" spans="1:34" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>35</v>
       </c>
@@ -2161,7 +2201,7 @@
       <c r="G32" s="15"/>
       <c r="H32" s="11"/>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>34</v>
       </c>
@@ -2180,7 +2220,7 @@
       <c r="G33" s="15"/>
       <c r="H33" s="11"/>
     </row>
-    <row r="34" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>36</v>
       </c>
@@ -2226,7 +2266,7 @@
       <c r="AG34" s="12"/>
       <c r="AH34" s="12"/>
     </row>
-    <row r="35" spans="1:34" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:34" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>49</v>
       </c>
@@ -2245,7 +2285,7 @@
       <c r="G35" s="15"/>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>51</v>
       </c>
@@ -2291,7 +2331,7 @@
       <c r="AG36" s="12"/>
       <c r="AH36" s="12"/>
     </row>
-    <row r="37" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>6</v>
       </c>
@@ -2337,7 +2377,7 @@
       <c r="AG37" s="12"/>
       <c r="AH37" s="12"/>
     </row>
-    <row r="38" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>45</v>
       </c>
@@ -2383,7 +2423,7 @@
       <c r="AG38" s="12"/>
       <c r="AH38" s="12"/>
     </row>
-    <row r="39" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>44</v>
       </c>
@@ -2429,7 +2469,7 @@
       <c r="AG39" s="12"/>
       <c r="AH39" s="12"/>
     </row>
-    <row r="40" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>42</v>
       </c>
@@ -2475,7 +2515,7 @@
       <c r="AG40" s="12"/>
       <c r="AH40" s="12"/>
     </row>
-    <row r="41" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>28</v>
       </c>
@@ -2521,7 +2561,7 @@
       <c r="AG41" s="12"/>
       <c r="AH41" s="12"/>
     </row>
-    <row r="42" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>48</v>
       </c>
@@ -2567,7 +2607,7 @@
       <c r="AG42" s="12"/>
       <c r="AH42" s="12"/>
     </row>
-    <row r="43" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>38</v>
       </c>
@@ -2613,7 +2653,7 @@
       <c r="AG43" s="12"/>
       <c r="AH43" s="12"/>
     </row>
-    <row r="44" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>37</v>
       </c>
@@ -2659,7 +2699,7 @@
       <c r="AG44" s="12"/>
       <c r="AH44" s="12"/>
     </row>
-    <row r="45" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>47</v>
       </c>
@@ -2705,7 +2745,7 @@
       <c r="AG45" s="12"/>
       <c r="AH45" s="12"/>
     </row>
-    <row r="46" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>41</v>
       </c>
@@ -2751,7 +2791,7 @@
       <c r="AG46" s="12"/>
       <c r="AH46" s="12"/>
     </row>
-    <row r="47" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>40</v>
       </c>
@@ -2797,7 +2837,7 @@
       <c r="AG47" s="12"/>
       <c r="AH47" s="12"/>
     </row>
-    <row r="48" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>43</v>
       </c>
@@ -2843,7 +2883,7 @@
       <c r="AG48" s="12"/>
       <c r="AH48" s="12"/>
     </row>
-    <row r="49" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>23</v>
       </c>
@@ -2889,7 +2929,7 @@
       <c r="AG49" s="12"/>
       <c r="AH49" s="12"/>
     </row>
-    <row r="50" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>33</v>
       </c>
@@ -2935,7 +2975,7 @@
       <c r="AG50" s="12"/>
       <c r="AH50" s="12"/>
     </row>
-    <row r="51" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>46</v>
       </c>
@@ -2981,7 +3021,7 @@
       <c r="AG51" s="12"/>
       <c r="AH51" s="12"/>
     </row>
-    <row r="52" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>39</v>
       </c>
@@ -3027,7 +3067,7 @@
       <c r="AG52" s="12"/>
       <c r="AH52" s="12"/>
     </row>
-    <row r="53" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="35"/>
       <c r="C53" s="12"/>
@@ -3063,151 +3103,151 @@
       <c r="AG53" s="12"/>
       <c r="AH53" s="12"/>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G54" s="13"/>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G55" s="13"/>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G56" s="13"/>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G57" s="13"/>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G58" s="13"/>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G59" s="13"/>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G60" s="13"/>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G61" s="13"/>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G62" s="13"/>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G63" s="13"/>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G64" s="13"/>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G65" s="13"/>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G66" s="13"/>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G67" s="13"/>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G68" s="13"/>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G69" s="13"/>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G70" s="13"/>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G71" s="13"/>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G72" s="13"/>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G73" s="13"/>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G74" s="13"/>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G75" s="13"/>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G76" s="13"/>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G77" s="13"/>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G78" s="13"/>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G79" s="13"/>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G80" s="13"/>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G81" s="13"/>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G82" s="13"/>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G83" s="13"/>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G84" s="13"/>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G85" s="13"/>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G86" s="13"/>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G87" s="13"/>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G88" s="13"/>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G89" s="13"/>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G90" s="13"/>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G91" s="13"/>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G92" s="13"/>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G93" s="13"/>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G94" s="13"/>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G95" s="13"/>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G96" s="13"/>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G97" s="13"/>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G98" s="13"/>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G99" s="13"/>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G100" s="13"/>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G101" s="13"/>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G102" s="13"/>
     </row>
   </sheetData>
@@ -3220,30 +3260,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="62" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="37" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
-    <col min="12" max="12" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="62" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>166</v>
       </c>
@@ -3281,10 +3321,10 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51">
         <f>B2/$B$52</f>
-        <v>0.2201188641866608</v>
+        <v>0.22007042253521128</v>
       </c>
       <c r="B2" s="57">
         <f>ROUND(L2/$L$53*1000,0)</f>
@@ -3306,7 +3346,7 @@
         <v>39</v>
       </c>
       <c r="H2" s="47">
-        <f t="shared" ref="H2:H33" si="0">15*F2/5280</f>
+        <f>15*F2/5280</f>
         <v>53.977272727272727</v>
       </c>
       <c r="I2" s="55">
@@ -3323,10 +3363,10 @@
         <v>157.97727272727272</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="50">
         <f>B3/$B$52</f>
-        <v>0.11138014527845036</v>
+        <v>0.11135563380281691</v>
       </c>
       <c r="B3" s="58">
         <f>ROUND(L3/$L$53*1000,0)</f>
@@ -3363,10 +3403,10 @@
         <v>79.973863636363632</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50">
         <f>B4/$B$52</f>
-        <v>8.1003742020691175E-2</v>
+        <v>8.098591549295775E-2</v>
       </c>
       <c r="B4" s="58">
         <f>ROUND(L4/$L$53*1000,0)</f>
@@ -3403,10 +3443,10 @@
         <v>58.075000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50">
         <f>B5/$B$52</f>
-        <v>8.0563504292317858E-2</v>
+        <v>8.0545774647887328E-2</v>
       </c>
       <c r="B5" s="58">
         <f>ROUND(L5/$L$53*1000,0)</f>
@@ -3445,10 +3485,10 @@
         <v>57.852272727272727</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="50">
         <f>B6/$B$52</f>
-        <v>6.4054589478318297E-2</v>
+        <v>6.4040492957746484E-2</v>
       </c>
       <c r="B6" s="58">
         <f>ROUND(L6/$L$53*1000,0)</f>
@@ -3483,10 +3523,10 @@
         <v>45.998863636363637</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50">
         <f>B7/$B$52</f>
-        <v>5.7891261281091788E-2</v>
+        <v>5.7878521126760563E-2</v>
       </c>
       <c r="B7" s="58">
         <f>ROUND(L7/$L$53*1000,0)</f>
@@ -3521,10 +3561,10 @@
         <v>41.576136363636365</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50">
         <f>B8/$B$52</f>
-        <v>4.8866387849438697E-2</v>
+        <v>4.8855633802816899E-2</v>
       </c>
       <c r="B8" s="58">
         <f>ROUND(L8/$L$53*1000,0)</f>
@@ -3559,10 +3599,10 @@
         <v>35.05681818181818</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50">
         <f>B9/$B$52</f>
-        <v>3.9841514417785606E-2</v>
+        <v>3.9832746478873242E-2</v>
       </c>
       <c r="B9" s="58">
         <f>ROUND(L9/$L$53*1000,0)</f>
@@ -3597,10 +3637,10 @@
         <v>28.567045454545454</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50">
         <f>B10/$B$52</f>
-        <v>3.3237948492185782E-2</v>
+        <v>3.3230633802816899E-2</v>
       </c>
       <c r="B10" s="58">
         <f>ROUND(L10/$L$53*1000,0)</f>
@@ -3631,10 +3671,10 @@
         <v>23.890909090909091</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="50">
         <f>B11/$B$52</f>
-        <v>3.2357473035439135E-2</v>
+        <v>3.2350352112676055E-2</v>
       </c>
       <c r="B11" s="58">
         <f>ROUND(L11/$L$53*1000,0)</f>
@@ -3665,10 +3705,10 @@
         <v>23.204545454545453</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="50">
         <f>B12/$B$52</f>
-        <v>3.1036759850319173E-2</v>
+        <v>3.1029929577464789E-2</v>
       </c>
       <c r="B12" s="58">
         <f>ROUND(L12/$L$53*1000,0)</f>
@@ -3699,10 +3739,10 @@
         <v>22.331818181818182</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="50">
         <f>B13/$B$52</f>
-        <v>2.7734976887519261E-2</v>
+        <v>2.7728873239436621E-2</v>
       </c>
       <c r="B13" s="58">
         <f>ROUND(L13/$L$53*1000,0)</f>
@@ -3733,10 +3773,10 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="50">
         <f>B14/$B$52</f>
-        <v>2.6414263702399295E-2</v>
+        <v>2.6408450704225352E-2</v>
       </c>
       <c r="B14" s="58">
         <f>ROUND(L14/$L$53*1000,0)</f>
@@ -3767,10 +3807,10 @@
         <v>18.94318181818182</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="50">
         <f>B15/$B$52</f>
-        <v>2.3332599603786044E-2</v>
+        <v>2.3327464788732395E-2</v>
       </c>
       <c r="B15" s="58">
         <f>ROUND(L15/$L$53*1000,0)</f>
@@ -3801,10 +3841,10 @@
         <v>16.780681818181819</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50">
         <f>B16/$B$52</f>
-        <v>2.1571648690292759E-2</v>
+        <v>2.1566901408450703E-2</v>
       </c>
       <c r="B16" s="58">
         <f>ROUND(L16/$L$53*1000,0)</f>
@@ -3835,10 +3875,10 @@
         <v>15.432954545454546</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="50">
         <f>B17/$B$52</f>
-        <v>1.7829627999119524E-2</v>
+        <v>1.7825704225352113E-2</v>
       </c>
       <c r="B17" s="58">
         <f>ROUND(L17/$L$53*1000,0)</f>
@@ -3869,10 +3909,10 @@
         <v>12.861363636363636</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50">
         <f>B18/$B$52</f>
-        <v>1.4968082764692935E-2</v>
+        <v>1.4964788732394365E-2</v>
       </c>
       <c r="B18" s="58">
         <f>ROUND(L18/$L$53*1000,0)</f>
@@ -3903,10 +3943,10 @@
         <v>10.801704545454545</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
         <f>B19/$B$52</f>
-        <v>1.408760730794629E-2</v>
+        <v>1.4084507042253521E-2</v>
       </c>
       <c r="B19" s="58">
         <f>ROUND(L19/$L$53*1000,0)</f>
@@ -3937,10 +3977,10 @@
         <v>10.061363636363637</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50">
         <f>B20/$B$52</f>
-        <v>1.2106537530266344E-2</v>
+        <v>1.2103873239436619E-2</v>
       </c>
       <c r="B20" s="58">
         <f>ROUND(L20/$L$53*1000,0)</f>
@@ -3971,10 +4011,10 @@
         <v>8.704545454545455</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="50">
         <f>B21/$B$52</f>
-        <v>6.8236847897864845E-3</v>
+        <v>6.8221830985915489E-3</v>
       </c>
       <c r="B21" s="58">
         <f>ROUND(L21/$L$53*1000,0)</f>
@@ -4005,10 +4045,10 @@
         <v>4.8784090909090914</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="50">
         <f>B22/$B$52</f>
-        <v>6.1633281972265025E-3</v>
+        <v>6.1619718309859151E-3</v>
       </c>
       <c r="B22" s="58">
         <f>ROUND(L22/$L$53*1000,0)</f>
@@ -4039,10 +4079,10 @@
         <v>4.3624999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="50">
         <f>B23/$B$52</f>
-        <v>5.9432093330398419E-3</v>
+        <v>5.9419014084507041E-3</v>
       </c>
       <c r="B23" s="58">
         <f>ROUND(L23/$L$53*1000,0)</f>
@@ -4073,10 +4113,10 @@
         <v>4.3306818181818185</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="50">
         <f>B24/$B$52</f>
-        <v>4.6224961479198771E-3</v>
+        <v>4.6214788732394365E-3</v>
       </c>
       <c r="B24" s="58">
         <f>ROUND(L24/$L$53*1000,0)</f>
@@ -4107,10 +4147,10 @@
         <v>3.28125</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="50">
         <f>B25/$B$52</f>
-        <v>4.4023772837332156E-3</v>
+        <v>4.4014084507042256E-3</v>
       </c>
       <c r="B25" s="58">
         <f>ROUND(L25/$L$53*1000,0)</f>
@@ -4141,10 +4181,10 @@
         <v>3.1363636363636367</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="50">
         <f>B26/$B$52</f>
-        <v>3.0816640986132513E-3</v>
+        <v>3.0809859154929575E-3</v>
       </c>
       <c r="B26" s="58">
         <f>ROUND(L26/$L$53*1000,0)</f>
@@ -4175,10 +4215,10 @@
         <v>2.2261363636363636</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="52">
         <f>B27/$B$52</f>
-        <v>2.6414263702399295E-3</v>
+        <v>2.6408450704225352E-3</v>
       </c>
       <c r="B27" s="59">
         <f>ROUND(L27/$L$53*1000,0)</f>
@@ -4211,10 +4251,10 @@
         <v>1.9375</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="50">
         <f>B28/$B$52</f>
-        <v>2.2011886418666078E-3</v>
+        <v>2.2007042253521128E-3</v>
       </c>
       <c r="B28" s="58">
         <f>ROUND(L28/$L$53*1000,0)</f>
@@ -4245,10 +4285,10 @@
         <v>1.6392045454545454</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="50">
         <f>B29/$B$52</f>
-        <v>1.5408320493066256E-3</v>
+        <v>1.5404929577464788E-3</v>
       </c>
       <c r="B29" s="58">
         <f>ROUND(L29/$L$53*1000,0)</f>
@@ -4279,10 +4319,10 @@
         <v>1.053409090909091</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="50">
         <f>B30/$B$52</f>
-        <v>1.1005943209333039E-3</v>
+        <v>1.1003521126760564E-3</v>
       </c>
       <c r="B30" s="58">
         <f>ROUND(L30/$L$53*1000,0)</f>
@@ -4313,10 +4353,10 @@
         <v>0.74090909090909096</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="50">
         <f>B31/$B$52</f>
-        <v>6.6035659255998238E-4</v>
+        <v>6.6021126760563379E-4</v>
       </c>
       <c r="B31" s="58">
         <f>ROUND(L31/$L$53*1000,0)</f>
@@ -4347,10 +4387,10 @@
         <v>0.48522727272727273</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="50">
         <f>B32/$B$52</f>
-        <v>6.6035659255998238E-4</v>
+        <v>6.6021126760563379E-4</v>
       </c>
       <c r="B32" s="58">
         <f>ROUND(L32/$L$53*1000,0)</f>
@@ -4381,10 +4421,10 @@
         <v>0.48409090909090913</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="50">
         <f>B33/$B$52</f>
-        <v>4.4023772837332157E-4</v>
+        <v>4.4014084507042255E-4</v>
       </c>
       <c r="B33" s="58">
         <f>ROUND(L33/$L$53*1000,0)</f>
@@ -4415,10 +4455,10 @@
         <v>0.35681818181818181</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50">
         <f>B34/$B$52</f>
-        <v>4.4023772837332157E-4</v>
+        <v>4.4014084507042255E-4</v>
       </c>
       <c r="B34" s="58">
         <f>ROUND(L34/$L$53*1000,0)</f>
@@ -4449,10 +4489,10 @@
         <v>0.31363636363636366</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="50">
         <f>B35/$B$52</f>
-        <v>2.2011886418666079E-4</v>
+        <v>2.2007042253521127E-4</v>
       </c>
       <c r="B35" s="58">
         <f>ROUND(L35/$L$53*1000,0)</f>
@@ -4483,10 +4523,10 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="50">
         <f>B36/$B$52</f>
-        <v>2.2011886418666079E-4</v>
+        <v>2.2007042253521127E-4</v>
       </c>
       <c r="B36" s="58">
         <f>ROUND(L36/$L$53*1000,0)</f>
@@ -4517,14 +4557,14 @@
         <v>0.15681818181818183</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50">
         <f>B37/$B$52</f>
-        <v>2.2011886418666079E-4</v>
+        <v>4.4014084507042255E-4</v>
       </c>
       <c r="B37" s="58">
         <f>ROUND(L37/$L$53*1000,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>163</v>
@@ -4536,25 +4576,25 @@
         <v>58</v>
       </c>
       <c r="F37" s="12">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G37" s="12">
         <v>0.1</v>
       </c>
       <c r="H37" s="12">
         <f>15*F37/5280</f>
-        <v>0</v>
+        <v>0.14204545454545456</v>
       </c>
       <c r="I37" s="43"/>
       <c r="L37" s="43">
         <f>H37+G37+I37 + J37*2 + K37</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0.24204545454545456</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50">
         <f>B38/$B$52</f>
-        <v>2.2011886418666079E-4</v>
+        <v>2.2007042253521127E-4</v>
       </c>
       <c r="B38" s="58">
         <f>ROUND(L38/$L$53*1000,0)</f>
@@ -4585,7 +4625,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="53">
         <f>B39/$B$52</f>
         <v>0</v>
@@ -4621,7 +4661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="50">
         <f>B40/$B$52</f>
         <v>0</v>
@@ -4655,7 +4695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="50">
         <f>B41/$B$52</f>
         <v>0</v>
@@ -4674,22 +4714,22 @@
         <v>36</v>
       </c>
       <c r="F41" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G41" s="12">
         <v>0</v>
       </c>
       <c r="H41" s="12">
         <f>15*F41/5280</f>
-        <v>5.6818181818181816E-2</v>
+        <v>0</v>
       </c>
       <c r="I41" s="43"/>
       <c r="L41" s="43">
         <f>H41+G41+I41 + J41*2 + K41</f>
-        <v>5.6818181818181816E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="50">
         <f>B42/$B$52</f>
         <v>0</v>
@@ -4723,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="50">
         <f>B43/$B$52</f>
         <v>0</v>
@@ -4757,7 +4797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="50">
         <f>B44/$B$52</f>
         <v>0</v>
@@ -4791,7 +4831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="50">
         <f>B45/$B$52</f>
         <v>0</v>
@@ -4825,7 +4865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="50">
         <f>B46/$B$52</f>
         <v>0</v>
@@ -4859,7 +4899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="50">
         <f>B47/$B$52</f>
         <v>0</v>
@@ -4893,7 +4933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="50">
         <f>B48/$B$52</f>
         <v>0</v>
@@ -4912,22 +4952,22 @@
         <v>76</v>
       </c>
       <c r="F48" s="12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G48" s="12">
         <v>0</v>
       </c>
       <c r="H48" s="12">
         <f>15*F48/5280</f>
-        <v>2.8409090909090908E-2</v>
+        <v>0</v>
       </c>
       <c r="I48" s="43"/>
       <c r="L48" s="43">
         <f>H48+G48+I48 + J48*2 + K48</f>
-        <v>2.8409090909090908E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="50">
         <f>B49/$B$52</f>
         <v>0</v>
@@ -4961,7 +5001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="50">
         <f>B50/$B$52</f>
         <v>0</v>
@@ -4995,7 +5035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="50">
         <f>B51/$B$52</f>
         <v>0</v>
@@ -5029,19 +5069,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B52" s="61">
         <f>SUM(B2:B51)</f>
-        <v>4543</v>
+        <v>4544</v>
       </c>
       <c r="I52" s="36"/>
       <c r="J52" s="43"/>
       <c r="L52" s="36">
         <f>SUM(L2:L51)</f>
-        <v>717.858522727273</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+        <v>717.91534090909113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B53" s="58"/>
       <c r="I53" s="36"/>
       <c r="J53" s="43"/>
@@ -5050,196 +5090,196 @@
         <v>157.97727272727272</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B54" s="61"/>
       <c r="D54" s="37" t="s">
         <v>169</v>
       </c>
       <c r="L54" s="36"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B55" s="61"/>
       <c r="D55" t="s">
         <v>167</v>
       </c>
       <c r="L55" s="36"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B56" s="61"/>
       <c r="D56" s="37" t="s">
         <v>168</v>
       </c>
       <c r="L56" s="36"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B57" s="61"/>
       <c r="I57" s="36"/>
       <c r="L57" s="36"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B58" s="61"/>
       <c r="D58" s="37" t="s">
         <v>170</v>
       </c>
       <c r="L58" s="36"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B59" s="61"/>
       <c r="D59" s="37" t="s">
         <v>186</v>
       </c>
       <c r="L59" s="36"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B60" s="61"/>
       <c r="D60" s="37" t="s">
         <v>172</v>
       </c>
       <c r="L60" s="36"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B61" s="61"/>
       <c r="D61" s="37" t="s">
         <v>171</v>
       </c>
       <c r="L61" s="36"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B62" s="61"/>
       <c r="D62" s="37" t="s">
         <v>173</v>
       </c>
       <c r="L62" s="36"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B63" s="61"/>
       <c r="D63" s="37" t="s">
         <v>188</v>
       </c>
       <c r="L63" s="36"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B64" s="61"/>
       <c r="D64" s="37" t="s">
         <v>187</v>
       </c>
       <c r="L64" s="36"/>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" s="61"/>
       <c r="D65" s="37" t="s">
         <v>184</v>
       </c>
       <c r="L65" s="36"/>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" s="61"/>
       <c r="D66" s="37" t="s">
         <v>185</v>
       </c>
       <c r="L66" s="36"/>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" s="61"/>
       <c r="L67" s="36"/>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D68" s="37" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D69" s="37" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B71" s="61"/>
       <c r="D71" s="37" t="s">
         <v>174</v>
       </c>
       <c r="L71" s="36"/>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B72" s="61"/>
       <c r="D72" s="37" t="s">
         <v>182</v>
       </c>
       <c r="L72" s="36"/>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B73" s="61"/>
       <c r="D73" s="37" t="s">
         <v>183</v>
       </c>
       <c r="L73" s="36"/>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" s="61"/>
       <c r="D74" s="37" t="s">
         <v>181</v>
       </c>
       <c r="L74" s="36"/>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B75" s="61"/>
       <c r="L75" s="36"/>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" s="61"/>
       <c r="D76" s="37" t="s">
         <v>175</v>
       </c>
       <c r="L76" s="36"/>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B77" s="61"/>
       <c r="L77" s="36"/>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B78" s="61"/>
       <c r="D78" s="37" t="s">
         <v>176</v>
       </c>
       <c r="L78" s="36"/>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B79" s="61"/>
       <c r="L79" s="36"/>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B80" s="61"/>
       <c r="L80" s="36"/>
     </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" s="61"/>
       <c r="L81" s="36"/>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="61"/>
       <c r="L82" s="36"/>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="61"/>
       <c r="L83" s="36"/>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" s="61"/>
       <c r="L84" s="36"/>
     </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" s="61"/>
       <c r="L85" s="36"/>
     </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" s="61"/>
       <c r="L86" s="36"/>
     </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" s="61"/>
       <c r="L87" s="36"/>
     </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" s="61"/>
       <c r="L88" s="36"/>
     </row>
@@ -5253,12 +5293,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new distance for White Butte
</commit_message>
<xml_diff>
--- a/Walter/TripReports/STATE HIGH POINTS.xlsx
+++ b/Walter/TripReports/STATE HIGH POINTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\websites\slnWalter\Walter\TripReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10306062-2FBE-40F6-ABE0-4BE14862C3B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B0DD6F-4BF9-4699-A979-23790E1B7FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="345" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HighPoint Log" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="182">
   <si>
     <t>State</t>
   </si>
@@ -512,9 +512,6 @@
     <t>        2</t>
   </si>
   <si>
-    <t>Walter Scale</t>
-  </si>
-  <si>
     <t>HP</t>
   </si>
   <si>
@@ -533,27 +530,6 @@
     <t xml:space="preserve">Percent Of </t>
   </si>
   <si>
-    <t>The elevation gain is an estimate of all vertical gain (including gain related to undulating terrain) on the least technical standard route. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance is the round-trip distance on the least technical standard route.  </t>
-  </si>
-  <si>
-    <t>The Walter Scale is based on the overall amout of human-only effort required to obtain a US state highpoint by way of the least technical standard route.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Walter Scale assigns effort points to each highpoint.  </t>
-  </si>
-  <si>
-    <t>Truncating  the  ratio of 3/0.189394  the Walter scale estimates it to be 15 times more difficult to climb 1 mile then to walk 1 mile.</t>
-  </si>
-  <si>
-    <t>It is estimaed that 3 miles can be walked in 1 hour, and likewise 1000 vertical feet  (0.189394 miles) can be climbed in one hour.</t>
-  </si>
-  <si>
-    <t>As such the Walter scale awards 1 point for each milage of walking, and 1 point for each 352 feet of gain.</t>
-  </si>
-  <si>
     <t>The Walter Scale reflects the Pareto Principle which states that for most taskes roughly 80% of the results come from 20% of the effort.</t>
   </si>
   <si>
@@ -584,21 +560,6 @@
     <t>The remaining 11 highpoints (aka remaining 22%) require 79.86% of the effort.</t>
   </si>
   <si>
-    <t>Points are normalized to a 1 - 1000 scale, to allow easy comparisons.</t>
-  </si>
-  <si>
-    <t>Walter Scale:  Points = (mileage + 15*(vertical distance in miles) + difficulty + nights + 2*coldDays)/maxScore * 1000</t>
-  </si>
-  <si>
-    <t>Effort points are a combination of total hiking mileage, vertical gain, terrain difficulty, nights required, and days with temperature remaining below.</t>
-  </si>
-  <si>
-    <t>If a highpoint involves roped rock climbing or roped glacier travel an additional 12 bonus miles are awarded.</t>
-  </si>
-  <si>
-    <t>If a highpoint involves climbing with the use of both hands and feet, but not the protection of a rope, an additional 6 bonus miles are awarded.</t>
-  </si>
-  <si>
     <t>Vertical Points</t>
   </si>
   <si>
@@ -612,6 +573,9 @@
   </si>
   <si>
     <t>Days Below Freezing in PM</t>
+  </si>
+  <si>
+    <t>Effort Scale</t>
   </si>
 </sst>
 </file>
@@ -769,7 +733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -883,6 +847,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1231,7 +1202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -3263,8 +3234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3285,53 +3256,53 @@
   <sheetData>
     <row r="1" spans="1:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B1" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>161</v>
-      </c>
       <c r="F1" s="40" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="I1" s="40" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="J1" s="40" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="K1" s="40" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="L1" s="40" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51">
-        <f>B2/$B$52</f>
-        <v>0.22007042253521128</v>
+        <f>B2/$L$56</f>
+        <v>0.21963540522732264</v>
       </c>
       <c r="B2" s="57">
         <f>ROUND(L2/$L$53*1000,0)</f>
         <v>1000</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D2" s="48" t="s">
         <v>1</v>
@@ -3365,15 +3336,15 @@
     </row>
     <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="50">
-        <f>B3/$B$52</f>
-        <v>0.11135563380281691</v>
+        <f>B3/$L$56</f>
+        <v>0.11113551504502525</v>
       </c>
       <c r="B3" s="58">
         <f>ROUND(L3/$L$53*1000,0)</f>
         <v>506</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" s="42" t="s">
         <v>9</v>
@@ -3405,15 +3376,15 @@
     </row>
     <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50">
-        <f>B4/$B$52</f>
-        <v>8.098591549295775E-2</v>
+        <f>B4/$L$56</f>
+        <v>8.0825829123654727E-2</v>
       </c>
       <c r="B4" s="58">
         <f>ROUND(L4/$L$53*1000,0)</f>
         <v>368</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" s="42" t="s">
         <v>19</v>
@@ -3445,15 +3416,15 @@
     </row>
     <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50">
-        <f>B5/$B$52</f>
-        <v>8.0545774647887328E-2</v>
+        <f>B5/$L$56</f>
+        <v>8.0386558313200088E-2</v>
       </c>
       <c r="B5" s="58">
         <f>ROUND(L5/$L$53*1000,0)</f>
         <v>366</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D5" s="42" t="s">
         <v>7</v>
@@ -3487,15 +3458,15 @@
     </row>
     <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="50">
-        <f>B6/$B$52</f>
-        <v>6.4040492957746484E-2</v>
+        <f>B6/$L$56</f>
+        <v>6.3913902921150886E-2</v>
       </c>
       <c r="B6" s="58">
         <f>ROUND(L6/$L$53*1000,0)</f>
         <v>291</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D6" s="42" t="s">
         <v>13</v>
@@ -3525,15 +3496,15 @@
     </row>
     <row r="7" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50">
-        <f>B7/$B$52</f>
-        <v>5.7878521126760563E-2</v>
+        <f>B7/$L$56</f>
+        <v>5.7764111574785858E-2</v>
       </c>
       <c r="B7" s="58">
         <f>ROUND(L7/$L$53*1000,0)</f>
         <v>263</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D7" s="42" t="s">
         <v>3</v>
@@ -3563,15 +3534,15 @@
     </row>
     <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50">
-        <f>B8/$B$52</f>
-        <v>4.8855633802816899E-2</v>
+        <f>B8/$L$56</f>
+        <v>4.8759059960465624E-2</v>
       </c>
       <c r="B8" s="58">
         <f>ROUND(L8/$L$53*1000,0)</f>
         <v>222</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D8" s="42" t="s">
         <v>25</v>
@@ -3601,15 +3572,15 @@
     </row>
     <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50">
-        <f>B9/$B$52</f>
-        <v>3.9832746478873242E-2</v>
+        <f>B9/$L$56</f>
+        <v>3.9754008346145397E-2</v>
       </c>
       <c r="B9" s="58">
         <f>ROUND(L9/$L$53*1000,0)</f>
         <v>181</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D9" s="42" t="s">
         <v>21</v>
@@ -3639,15 +3610,15 @@
     </row>
     <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50">
-        <f>B10/$B$52</f>
-        <v>3.3230633802816899E-2</v>
+        <f>B10/$L$56</f>
+        <v>3.3164946189325722E-2</v>
       </c>
       <c r="B10" s="58">
         <f>ROUND(L10/$L$53*1000,0)</f>
         <v>151</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D10" s="42" t="s">
         <v>41</v>
@@ -3673,15 +3644,15 @@
     </row>
     <row r="11" spans="1:12" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="50">
-        <f>B11/$B$52</f>
-        <v>3.2350352112676055E-2</v>
+        <f>B11/$L$56</f>
+        <v>3.228640456841643E-2</v>
       </c>
       <c r="B11" s="58">
         <f>ROUND(L11/$L$53*1000,0)</f>
         <v>147</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D11" s="42" t="s">
         <v>5</v>
@@ -3707,15 +3678,15 @@
     </row>
     <row r="12" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="50">
-        <f>B12/$B$52</f>
-        <v>3.1029929577464789E-2</v>
+        <f>B12/$L$56</f>
+        <v>3.0968592137052494E-2</v>
       </c>
       <c r="B12" s="58">
         <f>ROUND(L12/$L$53*1000,0)</f>
         <v>141</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D12" s="42" t="s">
         <v>43</v>
@@ -3741,15 +3712,15 @@
     </row>
     <row r="13" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="50">
-        <f>B13/$B$52</f>
-        <v>2.7728873239436621E-2</v>
+        <f>B13/$L$56</f>
+        <v>2.7674061058642653E-2</v>
       </c>
       <c r="B13" s="58">
         <f>ROUND(L13/$L$53*1000,0)</f>
         <v>126</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D13" s="42" t="s">
         <v>17</v>
@@ -3775,15 +3746,15 @@
     </row>
     <row r="14" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="50">
-        <f>B14/$B$52</f>
-        <v>2.6408450704225352E-2</v>
+        <f>B14/$L$56</f>
+        <v>2.6356248627278717E-2</v>
       </c>
       <c r="B14" s="58">
         <f>ROUND(L14/$L$53*1000,0)</f>
         <v>120</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D14" s="42" t="s">
         <v>23</v>
@@ -3809,15 +3780,15 @@
     </row>
     <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="50">
-        <f>B15/$B$52</f>
-        <v>2.3327464788732395E-2</v>
+        <f>B15/$L$56</f>
+        <v>2.32813529540962E-2</v>
       </c>
       <c r="B15" s="58">
         <f>ROUND(L15/$L$53*1000,0)</f>
         <v>106</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D15" s="42" t="s">
         <v>27</v>
@@ -3843,15 +3814,15 @@
     </row>
     <row r="16" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50">
-        <f>B16/$B$52</f>
-        <v>2.1566901408450703E-2</v>
+        <f>B16/$L$56</f>
+        <v>2.1524269712277617E-2</v>
       </c>
       <c r="B16" s="58">
         <f>ROUND(L16/$L$53*1000,0)</f>
         <v>98</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D16" s="42" t="s">
         <v>15</v>
@@ -3877,15 +3848,15 @@
     </row>
     <row r="17" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="50">
-        <f>B17/$B$52</f>
-        <v>1.7825704225352113E-2</v>
+        <f>B17/$L$56</f>
+        <v>1.7790467823413134E-2</v>
       </c>
       <c r="B17" s="58">
         <f>ROUND(L17/$L$53*1000,0)</f>
         <v>81</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D17" s="42" t="s">
         <v>37</v>
@@ -3911,15 +3882,15 @@
     </row>
     <row r="18" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50">
-        <f>B18/$B$52</f>
-        <v>1.4964788732394365E-2</v>
+        <f>B18/$L$56</f>
+        <v>1.4935207555457939E-2</v>
       </c>
       <c r="B18" s="58">
         <f>ROUND(L18/$L$53*1000,0)</f>
         <v>68</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D18" s="42" t="s">
         <v>45</v>
@@ -3945,15 +3916,15 @@
     </row>
     <row r="19" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
-        <f>B19/$B$52</f>
-        <v>1.4084507042253521E-2</v>
+        <f>B19/$L$56</f>
+        <v>1.405666593454865E-2</v>
       </c>
       <c r="B19" s="58">
         <f>ROUND(L19/$L$53*1000,0)</f>
         <v>64</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D19" s="42" t="s">
         <v>29</v>
@@ -3979,15 +3950,15 @@
     </row>
     <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50">
-        <f>B20/$B$52</f>
-        <v>1.2103873239436619E-2</v>
+        <f>B20/$L$56</f>
+        <v>1.2079947287502746E-2</v>
       </c>
       <c r="B20" s="58">
         <f>ROUND(L20/$L$53*1000,0)</f>
         <v>55</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D20" s="42" t="s">
         <v>73</v>
@@ -4013,15 +3984,15 @@
     </row>
     <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="50">
-        <f>B21/$B$52</f>
-        <v>6.8221830985915489E-3</v>
+        <f>B21/$L$56</f>
+        <v>6.8086975620470017E-3</v>
       </c>
       <c r="B21" s="58">
         <f>ROUND(L21/$L$53*1000,0)</f>
         <v>31</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D21" s="42" t="s">
         <v>71</v>
@@ -4045,153 +4016,153 @@
         <v>4.8784090909090914</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50">
-        <f>B22/$B$52</f>
-        <v>6.1619718309859151E-3</v>
-      </c>
-      <c r="B22" s="58">
+    <row r="22" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="63">
+        <f>B22/$L$56</f>
+        <v>6.369426751592357E-3</v>
+      </c>
+      <c r="B22" s="64">
         <f>ROUND(L22/$L$53*1000,0)</f>
-        <v>28</v>
-      </c>
-      <c r="C22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="65" t="s">
         <v>163</v>
       </c>
-      <c r="D22" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="12">
-        <v>550</v>
-      </c>
-      <c r="G22" s="12">
-        <v>2.8</v>
-      </c>
-      <c r="H22" s="12">
+      <c r="D22" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="65">
+        <v>400</v>
+      </c>
+      <c r="G22" s="65">
+        <v>3.4</v>
+      </c>
+      <c r="H22" s="65">
         <f>15*F22/5280</f>
-        <v>1.5625</v>
-      </c>
-      <c r="I22" s="43"/>
-      <c r="L22" s="43">
+        <v>1.1363636363636365</v>
+      </c>
+      <c r="I22" s="67"/>
+      <c r="L22" s="67">
         <f>H22+G22+I22 + J22*2 + K22</f>
-        <v>4.3624999999999998</v>
+        <v>4.5363636363636362</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="50">
-        <f>B23/$B$52</f>
-        <v>5.9419014084507041E-3</v>
+        <f>B23/$L$56</f>
+        <v>6.1497913463650338E-3</v>
       </c>
       <c r="B23" s="58">
         <f>ROUND(L23/$L$53*1000,0)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F23" s="12">
-        <v>750</v>
+        <v>550</v>
       </c>
       <c r="G23" s="12">
-        <v>2.2000000000000002</v>
+        <v>2.8</v>
       </c>
       <c r="H23" s="12">
         <f>15*F23/5280</f>
-        <v>2.1306818181818183</v>
+        <v>1.5625</v>
       </c>
       <c r="I23" s="43"/>
       <c r="L23" s="43">
         <f>H23+G23+I23 + J23*2 + K23</f>
-        <v>4.3306818181818185</v>
+        <v>4.3624999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="50">
-        <f>B24/$B$52</f>
-        <v>4.6214788732394365E-3</v>
+        <f>B24/$L$56</f>
+        <v>5.9301559411377115E-3</v>
       </c>
       <c r="B24" s="58">
         <f>ROUND(L24/$L$53*1000,0)</f>
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F24" s="12">
-        <v>275</v>
+        <v>750</v>
       </c>
       <c r="G24" s="12">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H24" s="12">
         <f>15*F24/5280</f>
-        <v>0.78125</v>
+        <v>2.1306818181818183</v>
       </c>
       <c r="I24" s="43"/>
       <c r="L24" s="43">
         <f>H24+G24+I24 + J24*2 + K24</f>
-        <v>3.28125</v>
+        <v>4.3306818181818185</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="50">
-        <f>B25/$B$52</f>
-        <v>4.4014084507042256E-3</v>
+        <f>B25/$L$56</f>
+        <v>4.6123435097737758E-3</v>
       </c>
       <c r="B25" s="58">
         <f>ROUND(L25/$L$53*1000,0)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F25" s="12">
-        <v>400</v>
+        <v>275</v>
       </c>
       <c r="G25" s="12">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="H25" s="12">
         <f>15*F25/5280</f>
-        <v>1.1363636363636365</v>
+        <v>0.78125</v>
       </c>
       <c r="I25" s="43"/>
       <c r="L25" s="43">
         <f>H25+G25+I25 + J25*2 + K25</f>
-        <v>3.1363636363636367</v>
+        <v>3.28125</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="50">
-        <f>B26/$B$52</f>
-        <v>3.0809859154929575E-3</v>
+        <f>B26/$L$56</f>
+        <v>3.0748956731825169E-3</v>
       </c>
       <c r="B26" s="58">
         <f>ROUND(L26/$L$53*1000,0)</f>
         <v>14</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D26" s="42" t="s">
         <v>95</v>
@@ -4217,15 +4188,15 @@
     </row>
     <row r="27" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="52">
-        <f>B27/$B$52</f>
-        <v>2.6408450704225352E-3</v>
+        <f>B27/$L$56</f>
+        <v>2.6356248627278718E-3</v>
       </c>
       <c r="B27" s="59">
         <f>ROUND(L27/$L$53*1000,0)</f>
         <v>12</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" s="39" t="s">
         <v>33</v>
@@ -4253,15 +4224,15 @@
     </row>
     <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="50">
-        <f>B28/$B$52</f>
-        <v>2.2007042253521128E-3</v>
+        <f>B28/$L$56</f>
+        <v>2.1963540522732263E-3</v>
       </c>
       <c r="B28" s="58">
         <f>ROUND(L28/$L$53*1000,0)</f>
         <v>10</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D28" s="42" t="s">
         <v>67</v>
@@ -4287,15 +4258,15 @@
     </row>
     <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="50">
-        <f>B29/$B$52</f>
-        <v>1.5404929577464788E-3</v>
+        <f>B29/$L$56</f>
+        <v>1.5374478365912585E-3</v>
       </c>
       <c r="B29" s="58">
         <f>ROUND(L29/$L$53*1000,0)</f>
         <v>7</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D29" s="42" t="s">
         <v>11</v>
@@ -4321,15 +4292,15 @@
     </row>
     <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="50">
-        <f>B30/$B$52</f>
-        <v>1.1003521126760564E-3</v>
+        <f>B30/$L$56</f>
+        <v>1.0981770261366132E-3</v>
       </c>
       <c r="B30" s="58">
         <f>ROUND(L30/$L$53*1000,0)</f>
         <v>5</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D30" s="42" t="s">
         <v>77</v>
@@ -4355,15 +4326,15 @@
     </row>
     <row r="31" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="50">
-        <f>B31/$B$52</f>
-        <v>6.6021126760563379E-4</v>
+        <f>B31/$L$56</f>
+        <v>6.5890621568196796E-4</v>
       </c>
       <c r="B31" s="58">
         <f>ROUND(L31/$L$53*1000,0)</f>
         <v>3</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D31" s="42" t="s">
         <v>81</v>
@@ -4389,15 +4360,15 @@
     </row>
     <row r="32" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="50">
-        <f>B32/$B$52</f>
-        <v>6.6021126760563379E-4</v>
+        <f>B32/$L$56</f>
+        <v>6.5890621568196796E-4</v>
       </c>
       <c r="B32" s="58">
         <f>ROUND(L32/$L$53*1000,0)</f>
         <v>3</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D32" s="42" t="s">
         <v>31</v>
@@ -4423,8 +4394,8 @@
     </row>
     <row r="33" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="50">
-        <f>B33/$B$52</f>
-        <v>4.4014084507042255E-4</v>
+        <f>B33/$L$56</f>
+        <v>4.392708104546453E-4</v>
       </c>
       <c r="B33" s="58">
         <f>ROUND(L33/$L$53*1000,0)</f>
@@ -4434,174 +4405,174 @@
         <v>163</v>
       </c>
       <c r="D33" s="42" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="F33" s="12">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G33" s="12">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H33" s="12">
         <f>15*F33/5280</f>
-        <v>5.6818181818181816E-2</v>
+        <v>0.11363636363636363</v>
       </c>
       <c r="I33" s="43"/>
       <c r="L33" s="43">
         <f>H33+G33+I33 + J33*2 + K33</f>
-        <v>0.35681818181818181</v>
+        <v>0.31363636363636366</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50">
-        <f>B34/$B$52</f>
-        <v>4.4014084507042255E-4</v>
+        <f>B34/$L$56</f>
+        <v>4.392708104546453E-4</v>
       </c>
       <c r="B34" s="58">
         <f>ROUND(L34/$L$53*1000,0)</f>
         <v>2</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D34" s="42" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="F34" s="12">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G34" s="12">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="H34" s="12">
         <f>15*F34/5280</f>
-        <v>0.11363636363636363</v>
+        <v>0.14204545454545456</v>
       </c>
       <c r="I34" s="43"/>
       <c r="L34" s="43">
         <f>H34+G34+I34 + J34*2 + K34</f>
-        <v>0.31363636363636366</v>
+        <v>0.29204545454545455</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="50">
-        <f>B35/$B$52</f>
-        <v>2.2007042253521127E-4</v>
+        <f>B35/$L$56</f>
+        <v>4.392708104546453E-4</v>
       </c>
       <c r="B35" s="58">
         <f>ROUND(L35/$L$53*1000,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D35" s="42" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F35" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G35" s="12">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="H35" s="12">
         <f>15*F35/5280</f>
-        <v>0</v>
+        <v>5.6818181818181816E-2</v>
       </c>
       <c r="I35" s="43"/>
       <c r="L35" s="43">
         <f>H35+G35+I35 + J35*2 + K35</f>
-        <v>0.1</v>
+        <v>0.35681818181818181</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="50">
-        <f>B36/$B$52</f>
-        <v>2.2007042253521127E-4</v>
+        <f>B36/$L$56</f>
+        <v>2.1963540522732265E-4</v>
       </c>
       <c r="B36" s="58">
         <f>ROUND(L36/$L$53*1000,0)</f>
         <v>1</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D36" s="42" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E36" s="42" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F36" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G36" s="12">
         <v>0.1</v>
       </c>
       <c r="H36" s="12">
         <f>15*F36/5280</f>
-        <v>5.6818181818181816E-2</v>
+        <v>0</v>
       </c>
       <c r="I36" s="43"/>
       <c r="L36" s="43">
         <f>H36+G36+I36 + J36*2 + K36</f>
-        <v>0.15681818181818183</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50">
-        <f>B37/$B$52</f>
-        <v>4.4014084507042255E-4</v>
+        <f>B37/$L$56</f>
+        <v>2.1963540522732265E-4</v>
       </c>
       <c r="B37" s="58">
         <f>ROUND(L37/$L$53*1000,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D37" s="42" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E37" s="42" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F37" s="12">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G37" s="12">
         <v>0.1</v>
       </c>
       <c r="H37" s="12">
         <f>15*F37/5280</f>
-        <v>0.14204545454545456</v>
+        <v>5.6818181818181816E-2</v>
       </c>
       <c r="I37" s="43"/>
       <c r="L37" s="43">
         <f>H37+G37+I37 + J37*2 + K37</f>
-        <v>0.24204545454545456</v>
+        <v>0.15681818181818183</v>
       </c>
     </row>
     <row r="38" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50">
-        <f>B38/$B$52</f>
-        <v>2.2007042253521127E-4</v>
+        <f>B38/$L$56</f>
+        <v>2.1963540522732265E-4</v>
       </c>
       <c r="B38" s="58">
         <f>ROUND(L38/$L$53*1000,0)</f>
         <v>1</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D38" s="42" t="s">
         <v>91</v>
@@ -4627,7 +4598,7 @@
     </row>
     <row r="39" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="53">
-        <f>B39/$B$52</f>
+        <f>B39/$L$56</f>
         <v>0</v>
       </c>
       <c r="B39" s="60">
@@ -4635,7 +4606,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>69</v>
@@ -4663,7 +4634,7 @@
     </row>
     <row r="40" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="50">
-        <f>B40/$B$52</f>
+        <f>B40/$L$56</f>
         <v>0</v>
       </c>
       <c r="B40" s="58">
@@ -4671,13 +4642,13 @@
         <v>0</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D40" s="42" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="E40" s="42" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="F40" s="12">
         <v>0</v>
@@ -4697,7 +4668,7 @@
     </row>
     <row r="41" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="50">
-        <f>B41/$B$52</f>
+        <f>B41/$L$56</f>
         <v>0</v>
       </c>
       <c r="B41" s="58">
@@ -4705,13 +4676,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D41" s="42" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="E41" s="42" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="F41" s="12">
         <v>0</v>
@@ -4731,7 +4702,7 @@
     </row>
     <row r="42" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="50">
-        <f>B42/$B$52</f>
+        <f>B42/$L$56</f>
         <v>0</v>
       </c>
       <c r="B42" s="58">
@@ -4739,13 +4710,13 @@
         <v>0</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D42" s="42" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="E42" s="42" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="F42" s="12">
         <v>0</v>
@@ -4765,7 +4736,7 @@
     </row>
     <row r="43" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="50">
-        <f>B43/$B$52</f>
+        <f>B43/$L$56</f>
         <v>0</v>
       </c>
       <c r="B43" s="58">
@@ -4773,13 +4744,13 @@
         <v>0</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D43" s="42" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E43" s="42" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F43" s="12">
         <v>0</v>
@@ -4799,7 +4770,7 @@
     </row>
     <row r="44" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="50">
-        <f>B44/$B$52</f>
+        <f>B44/$L$56</f>
         <v>0</v>
       </c>
       <c r="B44" s="58">
@@ -4807,13 +4778,13 @@
         <v>0</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D44" s="42" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E44" s="42" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F44" s="12">
         <v>0</v>
@@ -4833,7 +4804,7 @@
     </row>
     <row r="45" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="50">
-        <f>B45/$B$52</f>
+        <f>B45/$L$56</f>
         <v>0</v>
       </c>
       <c r="B45" s="58">
@@ -4841,13 +4812,13 @@
         <v>0</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D45" s="42" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="E45" s="42" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="F45" s="12">
         <v>0</v>
@@ -4867,7 +4838,7 @@
     </row>
     <row r="46" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="50">
-        <f>B46/$B$52</f>
+        <f>B46/$L$56</f>
         <v>0</v>
       </c>
       <c r="B46" s="58">
@@ -4875,13 +4846,13 @@
         <v>0</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="E46" s="42" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="F46" s="12">
         <v>0</v>
@@ -4901,7 +4872,7 @@
     </row>
     <row r="47" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="50">
-        <f>B47/$B$52</f>
+        <f>B47/$L$56</f>
         <v>0</v>
       </c>
       <c r="B47" s="58">
@@ -4909,13 +4880,13 @@
         <v>0</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D47" s="42" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="E47" s="42" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="F47" s="12">
         <v>0</v>
@@ -4935,7 +4906,7 @@
     </row>
     <row r="48" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="50">
-        <f>B48/$B$52</f>
+        <f>B48/$L$56</f>
         <v>0</v>
       </c>
       <c r="B48" s="58">
@@ -4946,10 +4917,10 @@
         <v>164</v>
       </c>
       <c r="D48" s="42" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="E48" s="42" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="F48" s="12">
         <v>0</v>
@@ -4969,7 +4940,7 @@
     </row>
     <row r="49" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="50">
-        <f>B49/$B$52</f>
+        <f>B49/$L$56</f>
         <v>0</v>
       </c>
       <c r="B49" s="58">
@@ -4977,33 +4948,33 @@
         <v>0</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D49" s="42" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="E49" s="42" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="F49" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G49" s="12">
         <v>0</v>
       </c>
       <c r="H49" s="12">
         <f>15*F49/5280</f>
-        <v>0</v>
+        <v>5.6818181818181816E-2</v>
       </c>
       <c r="I49" s="43"/>
       <c r="L49" s="43">
         <f>H49+G49+I49 + J49*2 + K49</f>
-        <v>0</v>
+        <v>5.6818181818181816E-2</v>
       </c>
     </row>
     <row r="50" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="50">
-        <f>B50/$B$52</f>
+        <f>B50/$L$56</f>
         <v>0</v>
       </c>
       <c r="B50" s="58">
@@ -5011,7 +4982,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D50" s="42" t="s">
         <v>85</v>
@@ -5037,7 +5008,7 @@
     </row>
     <row r="51" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="50">
-        <f>B51/$B$52</f>
+        <f>B51/$L$56</f>
         <v>0</v>
       </c>
       <c r="B51" s="58">
@@ -5045,7 +5016,7 @@
         <v>0</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D51" s="42" t="s">
         <v>65</v>
@@ -5070,15 +5041,12 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="61">
-        <f>SUM(B2:B51)</f>
-        <v>4544</v>
-      </c>
+      <c r="B52" s="61"/>
       <c r="I52" s="36"/>
       <c r="J52" s="43"/>
       <c r="L52" s="36">
         <f>SUM(L2:L51)</f>
-        <v>717.91534090909113</v>
+        <v>719.4221590909093</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -5092,24 +5060,19 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B54" s="61"/>
-      <c r="D54" s="37" t="s">
-        <v>169</v>
-      </c>
       <c r="L54" s="36"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B55" s="61"/>
-      <c r="D55" t="s">
-        <v>167</v>
-      </c>
+      <c r="D55"/>
       <c r="L55" s="36"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B56" s="61"/>
-      <c r="D56" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="L56" s="36"/>
+      <c r="L56" s="36">
+        <f>SUM(B2:B51)</f>
+        <v>4553</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B57" s="61"/>
@@ -5118,65 +5081,38 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B58" s="61"/>
-      <c r="D58" s="37" t="s">
-        <v>170</v>
-      </c>
       <c r="L58" s="36"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B59" s="61"/>
-      <c r="D59" s="37" t="s">
-        <v>186</v>
-      </c>
       <c r="L59" s="36"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B60" s="61"/>
-      <c r="D60" s="37" t="s">
-        <v>172</v>
-      </c>
       <c r="L60" s="36"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B61" s="61"/>
-      <c r="D61" s="37" t="s">
-        <v>171</v>
-      </c>
       <c r="L61" s="36"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B62" s="61"/>
-      <c r="D62" s="37" t="s">
-        <v>173</v>
-      </c>
       <c r="L62" s="36"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B63" s="61"/>
-      <c r="D63" s="37" t="s">
-        <v>188</v>
-      </c>
       <c r="L63" s="36"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B64" s="61"/>
-      <c r="D64" s="37" t="s">
-        <v>187</v>
-      </c>
       <c r="L64" s="36"/>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" s="61"/>
-      <c r="D65" s="37" t="s">
-        <v>184</v>
-      </c>
       <c r="L65" s="36"/>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" s="61"/>
-      <c r="D66" s="37" t="s">
-        <v>185</v>
-      </c>
       <c r="L66" s="36"/>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.25">
@@ -5185,39 +5121,39 @@
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D68" s="37" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D69" s="37" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B71" s="61"/>
       <c r="D71" s="37" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="L71" s="36"/>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B72" s="61"/>
       <c r="D72" s="37" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="L72" s="36"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B73" s="61"/>
       <c r="D73" s="37" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="L73" s="36"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" s="61"/>
       <c r="D74" s="37" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="L74" s="36"/>
     </row>
@@ -5228,7 +5164,7 @@
     <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" s="61"/>
       <c r="D76" s="37" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="L76" s="36"/>
     </row>
@@ -5239,7 +5175,7 @@
     <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B78" s="61"/>
       <c r="D78" s="37" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="L78" s="36"/>
     </row>
@@ -5286,6 +5222,7 @@
   </sheetData>
   <sortState ref="A3:L51">
     <sortCondition descending="1" ref="B3:B51"/>
+    <sortCondition ref="D3:D51"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add page for more Non-Zero summits
</commit_message>
<xml_diff>
--- a/Walter/TripReports/STATE HIGH POINTS.xlsx
+++ b/Walter/TripReports/STATE HIGH POINTS.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\websites\slnWalter\Walter\TripReports\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B0DD6F-4BF9-4699-A979-23790E1B7FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19296" windowHeight="10896" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HighPoint Log" sheetId="1" r:id="rId1"/>
-    <sheet name="Walter Scale" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Effor Scale" sheetId="3" r:id="rId2"/>
+    <sheet name="Less Zeros" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="186">
   <si>
     <t>State</t>
   </si>
@@ -576,12 +570,24 @@
   </si>
   <si>
     <t>Effort Scale</t>
+  </si>
+  <si>
+    <t>Mount Mansfield via Longs Trail</t>
+  </si>
+  <si>
+    <t>Mount Mitchell via Old Mitchell Trail</t>
+  </si>
+  <si>
+    <t>Mount Greylock via AT from Intersection of Rockwell Rd and Summit Rd</t>
+  </si>
+  <si>
+    <t>Mount Washington via Tuckerman Ravine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
@@ -688,7 +694,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -719,6 +725,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -733,7 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -854,6 +866,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -922,7 +936,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -955,26 +969,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1007,23 +1004,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1199,26 +1179,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH102"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="36" customWidth="1"/>
     <col min="3" max="3" width="12" style="12" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" style="12" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="12" customWidth="1"/>
-    <col min="10" max="34" width="8.85546875" style="12"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" style="12" customWidth="1"/>
+    <col min="10" max="34" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>101</v>
       </c>
@@ -1272,7 +1252,7 @@
       <c r="AG1" s="18"/>
       <c r="AH1" s="18"/>
     </row>
-    <row r="2" spans="1:34" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>16</v>
       </c>
@@ -1301,7 +1281,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>24</v>
       </c>
@@ -1330,7 +1310,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>32</v>
       </c>
@@ -1357,7 +1337,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>21</v>
       </c>
@@ -1384,7 +1364,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>7</v>
       </c>
@@ -1413,7 +1393,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1463,7 +1443,7 @@
       <c r="AG7" s="12"/>
       <c r="AH7" s="12"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>11</v>
       </c>
@@ -1490,7 +1470,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -1517,7 +1497,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>13</v>
       </c>
@@ -1544,7 +1524,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1571,7 +1551,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -1598,7 +1578,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -1625,7 +1605,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1652,7 +1632,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>8</v>
       </c>
@@ -1679,7 +1659,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1706,7 +1686,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1736,7 +1716,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -1788,7 +1768,7 @@
       <c r="AG18" s="12"/>
       <c r="AH18" s="12"/>
     </row>
-    <row r="19" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>20</v>
       </c>
@@ -1842,7 +1822,7 @@
       <c r="AG19" s="12"/>
       <c r="AH19" s="12"/>
     </row>
-    <row r="20" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1892,7 +1872,7 @@
       <c r="AG20" s="12"/>
       <c r="AH20" s="12"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>30</v>
       </c>
@@ -1916,7 +1896,7 @@
       </c>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>22</v>
       </c>
@@ -1946,7 +1926,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>18</v>
       </c>
@@ -1970,7 +1950,7 @@
       </c>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>26</v>
       </c>
@@ -1994,7 +1974,7 @@
       </c>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>31</v>
       </c>
@@ -2011,14 +1991,14 @@
         <v>62</v>
       </c>
       <c r="F25" s="10">
-        <v>3487</v>
+        <v>3491</v>
       </c>
       <c r="G25" s="14">
         <v>43707</v>
       </c>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>25</v>
       </c>
@@ -2042,7 +2022,7 @@
       </c>
       <c r="H26" s="11"/>
     </row>
-    <row r="27" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>29</v>
       </c>
@@ -2072,7 +2052,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>17</v>
       </c>
@@ -2096,7 +2076,7 @@
       </c>
       <c r="H28" s="11"/>
     </row>
-    <row r="29" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -2120,7 +2100,7 @@
       </c>
       <c r="H29" s="11"/>
     </row>
-    <row r="30" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>19</v>
       </c>
@@ -2153,7 +2133,7 @@
       <c r="G31" s="14"/>
       <c r="H31" s="11"/>
     </row>
-    <row r="32" spans="1:34" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>35</v>
       </c>
@@ -2172,7 +2152,7 @@
       <c r="G32" s="15"/>
       <c r="H32" s="11"/>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>34</v>
       </c>
@@ -2191,7 +2171,7 @@
       <c r="G33" s="15"/>
       <c r="H33" s="11"/>
     </row>
-    <row r="34" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>36</v>
       </c>
@@ -2237,7 +2217,7 @@
       <c r="AG34" s="12"/>
       <c r="AH34" s="12"/>
     </row>
-    <row r="35" spans="1:34" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>49</v>
       </c>
@@ -2256,7 +2236,7 @@
       <c r="G35" s="15"/>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>51</v>
       </c>
@@ -2302,7 +2282,7 @@
       <c r="AG36" s="12"/>
       <c r="AH36" s="12"/>
     </row>
-    <row r="37" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>6</v>
       </c>
@@ -2348,7 +2328,7 @@
       <c r="AG37" s="12"/>
       <c r="AH37" s="12"/>
     </row>
-    <row r="38" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>45</v>
       </c>
@@ -2394,7 +2374,7 @@
       <c r="AG38" s="12"/>
       <c r="AH38" s="12"/>
     </row>
-    <row r="39" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>44</v>
       </c>
@@ -2440,7 +2420,7 @@
       <c r="AG39" s="12"/>
       <c r="AH39" s="12"/>
     </row>
-    <row r="40" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>42</v>
       </c>
@@ -2486,7 +2466,7 @@
       <c r="AG40" s="12"/>
       <c r="AH40" s="12"/>
     </row>
-    <row r="41" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>28</v>
       </c>
@@ -2532,7 +2512,7 @@
       <c r="AG41" s="12"/>
       <c r="AH41" s="12"/>
     </row>
-    <row r="42" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>48</v>
       </c>
@@ -2578,7 +2558,7 @@
       <c r="AG42" s="12"/>
       <c r="AH42" s="12"/>
     </row>
-    <row r="43" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>38</v>
       </c>
@@ -2624,7 +2604,7 @@
       <c r="AG43" s="12"/>
       <c r="AH43" s="12"/>
     </row>
-    <row r="44" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>37</v>
       </c>
@@ -2670,7 +2650,7 @@
       <c r="AG44" s="12"/>
       <c r="AH44" s="12"/>
     </row>
-    <row r="45" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>47</v>
       </c>
@@ -2716,7 +2696,7 @@
       <c r="AG45" s="12"/>
       <c r="AH45" s="12"/>
     </row>
-    <row r="46" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>41</v>
       </c>
@@ -2762,7 +2742,7 @@
       <c r="AG46" s="12"/>
       <c r="AH46" s="12"/>
     </row>
-    <row r="47" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>40</v>
       </c>
@@ -2808,7 +2788,7 @@
       <c r="AG47" s="12"/>
       <c r="AH47" s="12"/>
     </row>
-    <row r="48" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>43</v>
       </c>
@@ -2854,7 +2834,7 @@
       <c r="AG48" s="12"/>
       <c r="AH48" s="12"/>
     </row>
-    <row r="49" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>23</v>
       </c>
@@ -2900,7 +2880,7 @@
       <c r="AG49" s="12"/>
       <c r="AH49" s="12"/>
     </row>
-    <row r="50" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>33</v>
       </c>
@@ -2946,7 +2926,7 @@
       <c r="AG50" s="12"/>
       <c r="AH50" s="12"/>
     </row>
-    <row r="51" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>46</v>
       </c>
@@ -2992,7 +2972,7 @@
       <c r="AG51" s="12"/>
       <c r="AH51" s="12"/>
     </row>
-    <row r="52" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>39</v>
       </c>
@@ -3038,7 +3018,7 @@
       <c r="AG52" s="12"/>
       <c r="AH52" s="12"/>
     </row>
-    <row r="53" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8"/>
       <c r="B53" s="35"/>
       <c r="C53" s="12"/>
@@ -3074,151 +3054,151 @@
       <c r="AG53" s="12"/>
       <c r="AH53" s="12"/>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G54" s="13"/>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G55" s="13"/>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G56" s="13"/>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G57" s="13"/>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G58" s="13"/>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G59" s="13"/>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G60" s="13"/>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G61" s="13"/>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G62" s="13"/>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G63" s="13"/>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G64" s="13"/>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G65" s="13"/>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G66" s="13"/>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G67" s="13"/>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G68" s="13"/>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G69" s="13"/>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G70" s="13"/>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G71" s="13"/>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G72" s="13"/>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G73" s="13"/>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G74" s="13"/>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G75" s="13"/>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G76" s="13"/>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G77" s="13"/>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G78" s="13"/>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G79" s="13"/>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G80" s="13"/>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G81" s="13"/>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G82" s="13"/>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G83" s="13"/>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G84" s="13"/>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G85" s="13"/>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G86" s="13"/>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G87" s="13"/>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G88" s="13"/>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G89" s="13"/>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G90" s="13"/>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G91" s="13"/>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G92" s="13"/>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G93" s="13"/>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G94" s="13"/>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G95" s="13"/>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G96" s="13"/>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G97" s="13"/>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G98" s="13"/>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G99" s="13"/>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G100" s="13"/>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G101" s="13"/>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G102" s="13"/>
     </row>
   </sheetData>
@@ -3231,30 +3211,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="62" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="37" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="62" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="37" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="37" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>165</v>
       </c>
@@ -3292,13 +3272,13 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="51">
-        <f>B2/$L$56</f>
+        <f t="shared" ref="A2:A33" si="0">B2/$L$56</f>
         <v>0.21963540522732264</v>
       </c>
       <c r="B2" s="57">
-        <f>ROUND(L2/$L$53*1000,0)</f>
+        <f t="shared" ref="B2:B33" si="1">ROUND(L2/$L$53*1000,0)</f>
         <v>1000</v>
       </c>
       <c r="C2" s="47" t="s">
@@ -3317,7 +3297,7 @@
         <v>39</v>
       </c>
       <c r="H2" s="47">
-        <f>15*F2/5280</f>
+        <f t="shared" ref="H2:H33" si="2">15*F2/5280</f>
         <v>53.977272727272727</v>
       </c>
       <c r="I2" s="55">
@@ -3330,17 +3310,17 @@
         <v>17</v>
       </c>
       <c r="L2" s="49">
-        <f>H2+G2+I2 + J2*2 + K2</f>
+        <f t="shared" ref="L2:L33" si="3">H2+G2+I2 + J2*2 + K2</f>
         <v>157.97727272727272</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="50">
-        <f>B3/$L$56</f>
+        <f t="shared" si="0"/>
         <v>0.11113551504502525</v>
       </c>
       <c r="B3" s="58">
-        <f>ROUND(L3/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>506</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -3359,7 +3339,7 @@
         <v>40.4</v>
       </c>
       <c r="H3" s="12">
-        <f>15*F3/5280</f>
+        <f t="shared" si="2"/>
         <v>24.573863636363637</v>
       </c>
       <c r="I3" s="54">
@@ -3370,17 +3350,17 @@
         <v>3</v>
       </c>
       <c r="L3" s="43">
-        <f>H3+G3+I3 + J3*2 + K3</f>
+        <f t="shared" si="3"/>
         <v>79.973863636363632</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="50">
-        <f>B4/$L$56</f>
+        <f t="shared" si="0"/>
         <v>8.0825829123654727E-2</v>
       </c>
       <c r="B4" s="58">
-        <f>ROUND(L4/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>368</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -3399,7 +3379,7 @@
         <v>22.2</v>
       </c>
       <c r="H4" s="12">
-        <f>15*F4/5280</f>
+        <f t="shared" si="2"/>
         <v>21.875</v>
       </c>
       <c r="I4" s="54">
@@ -3410,17 +3390,17 @@
         <v>2</v>
       </c>
       <c r="L4" s="43">
-        <f>H4+G4+I4 + J4*2 + K4</f>
+        <f t="shared" si="3"/>
         <v>58.075000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="50">
-        <f>B5/$L$56</f>
+        <f t="shared" si="0"/>
         <v>8.0386558313200088E-2</v>
       </c>
       <c r="B5" s="58">
-        <f>ROUND(L5/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>366</v>
       </c>
       <c r="C5" s="12" t="s">
@@ -3439,7 +3419,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="12">
-        <f>15*F5/5280</f>
+        <f t="shared" si="2"/>
         <v>25.852272727272727</v>
       </c>
       <c r="I5" s="54">
@@ -3452,17 +3432,17 @@
         <v>2</v>
       </c>
       <c r="L5" s="43">
-        <f>H5+G5+I5 + J5*2 + K5</f>
+        <f t="shared" si="3"/>
         <v>57.852272727272727</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="50">
-        <f>B6/$L$56</f>
+        <f t="shared" si="0"/>
         <v>6.3913902921150886E-2</v>
       </c>
       <c r="B6" s="58">
-        <f>ROUND(L6/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>291</v>
       </c>
       <c r="C6" s="12" t="s">
@@ -3481,7 +3461,7 @@
         <v>28.8</v>
       </c>
       <c r="H6" s="12">
-        <f>15*F6/5280</f>
+        <f t="shared" si="2"/>
         <v>15.198863636363637</v>
       </c>
       <c r="I6" s="54"/>
@@ -3490,17 +3470,17 @@
         <v>2</v>
       </c>
       <c r="L6" s="43">
-        <f>H6+G6+I6 + J6*2 + K6</f>
+        <f t="shared" si="3"/>
         <v>45.998863636363637</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="50">
-        <f>B7/$L$56</f>
+        <f t="shared" si="0"/>
         <v>5.7764111574785858E-2</v>
       </c>
       <c r="B7" s="58">
-        <f>ROUND(L7/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>263</v>
       </c>
       <c r="C7" s="42" t="s">
@@ -3519,7 +3499,7 @@
         <v>21.4</v>
       </c>
       <c r="H7" s="12">
-        <f>15*F7/5280</f>
+        <f t="shared" si="2"/>
         <v>19.176136363636363</v>
       </c>
       <c r="I7" s="54"/>
@@ -3528,17 +3508,17 @@
         <v>1</v>
       </c>
       <c r="L7" s="43">
-        <f>H7+G7+I7 + J7*2 + K7</f>
+        <f t="shared" si="3"/>
         <v>41.576136363636365</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="50">
-        <f>B8/$L$56</f>
+        <f t="shared" si="0"/>
         <v>4.8759059960465624E-2</v>
       </c>
       <c r="B8" s="58">
-        <f>ROUND(L8/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>222</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -3557,7 +3537,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="12">
-        <f>15*F8/5280</f>
+        <f t="shared" si="2"/>
         <v>15.056818181818182</v>
       </c>
       <c r="I8" s="54">
@@ -3566,17 +3546,17 @@
       <c r="J8" s="54"/>
       <c r="K8" s="54"/>
       <c r="L8" s="43">
-        <f>H8+G8+I8 + J8*2 + K8</f>
+        <f t="shared" si="3"/>
         <v>35.05681818181818</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="50">
-        <f>B9/$L$56</f>
+        <f t="shared" si="0"/>
         <v>3.9754008346145397E-2</v>
       </c>
       <c r="B9" s="58">
-        <f>ROUND(L9/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>181</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -3595,7 +3575,7 @@
         <v>6.8</v>
       </c>
       <c r="H9" s="12">
-        <f>15*F9/5280</f>
+        <f t="shared" si="2"/>
         <v>15.767045454545455</v>
       </c>
       <c r="I9" s="54">
@@ -3604,17 +3584,17 @@
       <c r="J9" s="54"/>
       <c r="K9" s="54"/>
       <c r="L9" s="43">
-        <f>H9+G9+I9 + J9*2 + K9</f>
+        <f t="shared" si="3"/>
         <v>28.567045454545454</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="50">
-        <f>B10/$L$56</f>
+        <f t="shared" si="0"/>
         <v>3.3164946189325722E-2</v>
       </c>
       <c r="B10" s="58">
-        <f>ROUND(L10/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>151</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -3633,22 +3613,22 @@
         <v>14.8</v>
       </c>
       <c r="H10" s="12">
-        <f>15*F10/5280</f>
+        <f t="shared" si="2"/>
         <v>9.0909090909090917</v>
       </c>
       <c r="I10" s="43"/>
       <c r="L10" s="43">
-        <f>H10+G10+I10 + J10*2 + K10</f>
+        <f t="shared" si="3"/>
         <v>23.890909090909091</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="50">
-        <f>B11/$L$56</f>
+        <f t="shared" si="0"/>
         <v>3.228640456841643E-2</v>
       </c>
       <c r="B11" s="58">
-        <f>ROUND(L11/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>147</v>
       </c>
       <c r="C11" s="42" t="s">
@@ -3667,22 +3647,22 @@
         <v>9</v>
       </c>
       <c r="H11" s="12">
-        <f>15*F11/5280</f>
+        <f t="shared" si="2"/>
         <v>14.204545454545455</v>
       </c>
       <c r="I11" s="43"/>
       <c r="L11" s="43">
-        <f>H11+G11+I11 + J11*2 + K11</f>
+        <f t="shared" si="3"/>
         <v>23.204545454545453</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="50">
-        <f>B12/$L$56</f>
+        <f t="shared" si="0"/>
         <v>3.0968592137052494E-2</v>
       </c>
       <c r="B12" s="58">
-        <f>ROUND(L12/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>141</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -3701,22 +3681,22 @@
         <v>10.4</v>
       </c>
       <c r="H12" s="12">
-        <f>15*F12/5280</f>
+        <f t="shared" si="2"/>
         <v>11.931818181818182</v>
       </c>
       <c r="I12" s="43"/>
       <c r="L12" s="43">
-        <f>H12+G12+I12 + J12*2 + K12</f>
+        <f t="shared" si="3"/>
         <v>22.331818181818182</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="50">
-        <f>B13/$L$56</f>
+        <f t="shared" si="0"/>
         <v>2.7674061058642653E-2</v>
       </c>
       <c r="B13" s="58">
-        <f>ROUND(L13/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>126</v>
       </c>
       <c r="C13" s="12" t="s">
@@ -3735,22 +3715,22 @@
         <v>7.4</v>
       </c>
       <c r="H13" s="12">
-        <f>15*F13/5280</f>
+        <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
       <c r="I13" s="43"/>
       <c r="L13" s="43">
-        <f>H13+G13+I13 + J13*2 + K13</f>
+        <f t="shared" si="3"/>
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="50">
-        <f>B14/$L$56</f>
+        <f t="shared" si="0"/>
         <v>2.6356248627278717E-2</v>
       </c>
       <c r="B14" s="58">
-        <f>ROUND(L14/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="C14" s="42" t="s">
@@ -3769,22 +3749,22 @@
         <v>9</v>
       </c>
       <c r="H14" s="12">
-        <f>15*F14/5280</f>
+        <f t="shared" si="2"/>
         <v>9.9431818181818183</v>
       </c>
       <c r="I14" s="43"/>
       <c r="L14" s="43">
-        <f>H14+G14+I14 + J14*2 + K14</f>
+        <f t="shared" si="3"/>
         <v>18.94318181818182</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="50">
-        <f>B15/$L$56</f>
+        <f t="shared" si="0"/>
         <v>2.32813529540962E-2</v>
       </c>
       <c r="B15" s="58">
-        <f>ROUND(L15/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>106</v>
       </c>
       <c r="C15" s="12" t="s">
@@ -3803,22 +3783,22 @@
         <v>8.4</v>
       </c>
       <c r="H15" s="12">
-        <f>15*F15/5280</f>
+        <f t="shared" si="2"/>
         <v>8.3806818181818183</v>
       </c>
       <c r="I15" s="43"/>
       <c r="L15" s="43">
-        <f>H15+G15+I15 + J15*2 + K15</f>
+        <f t="shared" si="3"/>
         <v>16.780681818181819</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="50">
-        <f>B16/$L$56</f>
+        <f t="shared" si="0"/>
         <v>2.1524269712277617E-2</v>
       </c>
       <c r="B16" s="58">
-        <f>ROUND(L16/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="C16" s="12" t="s">
@@ -3837,22 +3817,22 @@
         <v>6.2</v>
       </c>
       <c r="H16" s="12">
-        <f>15*F16/5280</f>
+        <f t="shared" si="2"/>
         <v>9.232954545454545</v>
       </c>
       <c r="I16" s="43"/>
       <c r="L16" s="43">
-        <f>H16+G16+I16 + J16*2 + K16</f>
+        <f t="shared" si="3"/>
         <v>15.432954545454546</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="50">
-        <f>B17/$L$56</f>
+        <f t="shared" si="0"/>
         <v>1.7790467823413134E-2</v>
       </c>
       <c r="B17" s="58">
-        <f>ROUND(L17/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -3871,22 +3851,22 @@
         <v>8.6</v>
       </c>
       <c r="H17" s="12">
-        <f>15*F17/5280</f>
+        <f t="shared" si="2"/>
         <v>4.2613636363636367</v>
       </c>
       <c r="I17" s="43"/>
       <c r="L17" s="43">
-        <f>H17+G17+I17 + J17*2 + K17</f>
+        <f t="shared" si="3"/>
         <v>12.861363636363636</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="50">
-        <f>B18/$L$56</f>
+        <f t="shared" si="0"/>
         <v>1.4935207555457939E-2</v>
       </c>
       <c r="B18" s="58">
-        <f>ROUND(L18/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>68</v>
       </c>
       <c r="C18" s="12" t="s">
@@ -3905,22 +3885,22 @@
         <v>8.6</v>
       </c>
       <c r="H18" s="12">
-        <f>15*F18/5280</f>
+        <f t="shared" si="2"/>
         <v>2.2017045454545454</v>
       </c>
       <c r="I18" s="43"/>
       <c r="L18" s="43">
-        <f>H18+G18+I18 + J18*2 + K18</f>
+        <f t="shared" si="3"/>
         <v>10.801704545454545</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
-        <f>B19/$L$56</f>
+        <f t="shared" si="0"/>
         <v>1.405666593454865E-2</v>
       </c>
       <c r="B19" s="58">
-        <f>ROUND(L19/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="C19" s="12" t="s">
@@ -3939,22 +3919,22 @@
         <v>5.8</v>
       </c>
       <c r="H19" s="12">
-        <f>15*F19/5280</f>
+        <f t="shared" si="2"/>
         <v>4.2613636363636367</v>
       </c>
       <c r="I19" s="43"/>
       <c r="L19" s="43">
-        <f>H19+G19+I19 + J19*2 + K19</f>
+        <f t="shared" si="3"/>
         <v>10.061363636363637</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="50">
-        <f>B20/$L$56</f>
+        <f t="shared" si="0"/>
         <v>1.2079947287502746E-2</v>
       </c>
       <c r="B20" s="58">
-        <f>ROUND(L20/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="C20" s="12" t="s">
@@ -3973,22 +3953,22 @@
         <v>7</v>
       </c>
       <c r="H20" s="12">
-        <f>15*F20/5280</f>
+        <f t="shared" si="2"/>
         <v>1.7045454545454546</v>
       </c>
       <c r="I20" s="43"/>
       <c r="L20" s="43">
-        <f>H20+G20+I20 + J20*2 + K20</f>
+        <f t="shared" si="3"/>
         <v>8.704545454545455</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="50">
-        <f>B21/$L$56</f>
+        <f t="shared" si="0"/>
         <v>6.8086975620470017E-3</v>
       </c>
       <c r="B21" s="58">
-        <f>ROUND(L21/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C21" s="12" t="s">
@@ -4007,22 +3987,22 @@
         <v>3.6</v>
       </c>
       <c r="H21" s="12">
-        <f>15*F21/5280</f>
+        <f t="shared" si="2"/>
         <v>1.2784090909090908</v>
       </c>
       <c r="I21" s="43"/>
       <c r="L21" s="43">
-        <f>H21+G21+I21 + J21*2 + K21</f>
+        <f t="shared" si="3"/>
         <v>4.8784090909090914</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="65" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="63">
-        <f>B22/$L$56</f>
+        <f t="shared" si="0"/>
         <v>6.369426751592357E-3</v>
       </c>
       <c r="B22" s="64">
-        <f>ROUND(L22/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C22" s="65" t="s">
@@ -4041,31 +4021,31 @@
         <v>3.4</v>
       </c>
       <c r="H22" s="65">
-        <f>15*F22/5280</f>
+        <f t="shared" si="2"/>
         <v>1.1363636363636365</v>
       </c>
       <c r="I22" s="67"/>
       <c r="L22" s="67">
-        <f>H22+G22+I22 + J22*2 + K22</f>
+        <f t="shared" si="3"/>
         <v>4.5363636363636362</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="50">
-        <f>B23/$L$56</f>
+        <f t="shared" si="0"/>
         <v>6.1497913463650338E-3</v>
       </c>
       <c r="B23" s="58">
-        <f>ROUND(L23/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="68" t="s">
         <v>52</v>
       </c>
       <c r="F23" s="12">
@@ -4075,22 +4055,22 @@
         <v>2.8</v>
       </c>
       <c r="H23" s="12">
-        <f>15*F23/5280</f>
+        <f t="shared" si="2"/>
         <v>1.5625</v>
       </c>
       <c r="I23" s="43"/>
       <c r="L23" s="43">
-        <f>H23+G23+I23 + J23*2 + K23</f>
+        <f t="shared" si="3"/>
         <v>4.3624999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="50">
-        <f>B24/$L$56</f>
+        <f t="shared" si="0"/>
         <v>5.9301559411377115E-3</v>
       </c>
       <c r="B24" s="58">
-        <f>ROUND(L24/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C24" s="12" t="s">
@@ -4109,22 +4089,22 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H24" s="12">
-        <f>15*F24/5280</f>
+        <f t="shared" si="2"/>
         <v>2.1306818181818183</v>
       </c>
       <c r="I24" s="43"/>
       <c r="L24" s="43">
-        <f>H24+G24+I24 + J24*2 + K24</f>
+        <f t="shared" si="3"/>
         <v>4.3306818181818185</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="50">
-        <f>B25/$L$56</f>
+        <f t="shared" si="0"/>
         <v>4.6123435097737758E-3</v>
       </c>
       <c r="B25" s="58">
-        <f>ROUND(L25/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -4143,22 +4123,22 @@
         <v>2.5</v>
       </c>
       <c r="H25" s="12">
-        <f>15*F25/5280</f>
+        <f t="shared" si="2"/>
         <v>0.78125</v>
       </c>
       <c r="I25" s="43"/>
       <c r="L25" s="43">
-        <f>H25+G25+I25 + J25*2 + K25</f>
+        <f t="shared" si="3"/>
         <v>3.28125</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50">
-        <f>B26/$L$56</f>
+        <f t="shared" si="0"/>
         <v>3.0748956731825169E-3</v>
       </c>
       <c r="B26" s="58">
-        <f>ROUND(L26/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C26" s="12" t="s">
@@ -4177,22 +4157,22 @@
         <v>1.8</v>
       </c>
       <c r="H26" s="12">
-        <f>15*F26/5280</f>
+        <f t="shared" si="2"/>
         <v>0.42613636363636365</v>
       </c>
       <c r="I26" s="43"/>
       <c r="L26" s="43">
-        <f>H26+G26+I26 + J26*2 + K26</f>
+        <f t="shared" si="3"/>
         <v>2.2261363636363636</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="52">
-        <f>B27/$L$56</f>
+        <f t="shared" si="0"/>
         <v>2.6356248627278718E-3</v>
       </c>
       <c r="B27" s="59">
-        <f>ROUND(L27/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -4211,24 +4191,24 @@
         <v>1</v>
       </c>
       <c r="H27" s="6">
-        <f>15*F27/5280</f>
+        <f t="shared" si="2"/>
         <v>0.9375</v>
       </c>
       <c r="I27" s="38"/>
       <c r="J27" s="38"/>
       <c r="K27" s="38"/>
       <c r="L27" s="38">
-        <f>H27+G27+I27 + J27*2 + K27</f>
+        <f t="shared" si="3"/>
         <v>1.9375</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="50">
-        <f>B28/$L$56</f>
+        <f t="shared" si="0"/>
         <v>2.1963540522732263E-3</v>
       </c>
       <c r="B28" s="58">
-        <f>ROUND(L28/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C28" s="12" t="s">
@@ -4247,22 +4227,22 @@
         <v>1</v>
       </c>
       <c r="H28" s="12">
-        <f>15*F28/5280</f>
+        <f t="shared" si="2"/>
         <v>0.63920454545454541</v>
       </c>
       <c r="I28" s="43"/>
       <c r="L28" s="43">
-        <f>H28+G28+I28 + J28*2 + K28</f>
+        <f t="shared" si="3"/>
         <v>1.6392045454545454</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="50">
-        <f>B29/$L$56</f>
+        <f t="shared" si="0"/>
         <v>1.5374478365912585E-3</v>
       </c>
       <c r="B29" s="58">
-        <f>ROUND(L29/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C29" s="12" t="s">
@@ -4281,22 +4261,22 @@
         <v>0.4</v>
       </c>
       <c r="H29" s="12">
-        <f>15*F29/5280</f>
+        <f t="shared" si="2"/>
         <v>0.65340909090909094</v>
       </c>
       <c r="I29" s="43"/>
       <c r="L29" s="43">
-        <f>H29+G29+I29 + J29*2 + K29</f>
+        <f t="shared" si="3"/>
         <v>1.053409090909091</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="50">
-        <f>B30/$L$56</f>
+        <f t="shared" si="0"/>
         <v>1.0981770261366132E-3</v>
       </c>
       <c r="B30" s="58">
-        <f>ROUND(L30/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -4315,22 +4295,22 @@
         <v>0.4</v>
       </c>
       <c r="H30" s="12">
-        <f>15*F30/5280</f>
+        <f t="shared" si="2"/>
         <v>0.34090909090909088</v>
       </c>
       <c r="I30" s="43"/>
       <c r="L30" s="43">
-        <f>H30+G30+I30 + J30*2 + K30</f>
+        <f t="shared" si="3"/>
         <v>0.74090909090909096</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="50">
-        <f>B31/$L$56</f>
+        <f t="shared" si="0"/>
         <v>6.5890621568196796E-4</v>
       </c>
       <c r="B31" s="58">
-        <f>ROUND(L31/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C31" s="12" t="s">
@@ -4349,31 +4329,31 @@
         <v>0.4</v>
       </c>
       <c r="H31" s="12">
-        <f>15*F31/5280</f>
+        <f t="shared" si="2"/>
         <v>8.5227272727272721E-2</v>
       </c>
       <c r="I31" s="43"/>
       <c r="L31" s="43">
-        <f>H31+G31+I31 + J31*2 + K31</f>
+        <f t="shared" si="3"/>
         <v>0.48522727272727273</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="50">
-        <f>B32/$L$56</f>
+        <f t="shared" si="0"/>
         <v>6.5890621568196796E-4</v>
       </c>
       <c r="B32" s="58">
-        <f>ROUND(L32/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="42" t="s">
+      <c r="E32" s="68" t="s">
         <v>32</v>
       </c>
       <c r="F32" s="12">
@@ -4383,22 +4363,22 @@
         <v>0.2</v>
       </c>
       <c r="H32" s="12">
-        <f>15*F32/5280</f>
+        <f t="shared" si="2"/>
         <v>0.28409090909090912</v>
       </c>
       <c r="I32" s="43"/>
       <c r="L32" s="43">
-        <f>H32+G32+I32 + J32*2 + K32</f>
+        <f t="shared" si="3"/>
         <v>0.48409090909090913</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="50">
-        <f>B33/$L$56</f>
+        <f t="shared" si="0"/>
         <v>4.392708104546453E-4</v>
       </c>
       <c r="B33" s="58">
-        <f>ROUND(L33/$L$53*1000,0)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C33" s="12" t="s">
@@ -4417,22 +4397,22 @@
         <v>0.2</v>
       </c>
       <c r="H33" s="12">
-        <f>15*F33/5280</f>
+        <f t="shared" si="2"/>
         <v>0.11363636363636363</v>
       </c>
       <c r="I33" s="43"/>
       <c r="L33" s="43">
-        <f>H33+G33+I33 + J33*2 + K33</f>
+        <f t="shared" si="3"/>
         <v>0.31363636363636366</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="50">
-        <f>B34/$L$56</f>
+        <f t="shared" ref="A34:A65" si="4">B34/$L$56</f>
         <v>4.392708104546453E-4</v>
       </c>
       <c r="B34" s="58">
-        <f>ROUND(L34/$L$53*1000,0)</f>
+        <f t="shared" ref="B34:B51" si="5">ROUND(L34/$L$53*1000,0)</f>
         <v>2</v>
       </c>
       <c r="C34" s="12" t="s">
@@ -4451,22 +4431,22 @@
         <v>0.15</v>
       </c>
       <c r="H34" s="12">
-        <f>15*F34/5280</f>
+        <f t="shared" ref="H34:H51" si="6">15*F34/5280</f>
         <v>0.14204545454545456</v>
       </c>
       <c r="I34" s="43"/>
       <c r="L34" s="43">
-        <f>H34+G34+I34 + J34*2 + K34</f>
+        <f t="shared" ref="L34:L65" si="7">H34+G34+I34 + J34*2 + K34</f>
         <v>0.29204545454545455</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="50">
-        <f>B35/$L$56</f>
+        <f t="shared" si="4"/>
         <v>4.392708104546453E-4</v>
       </c>
       <c r="B35" s="58">
-        <f>ROUND(L35/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="C35" s="12" t="s">
@@ -4485,22 +4465,22 @@
         <v>0.3</v>
       </c>
       <c r="H35" s="12">
-        <f>15*F35/5280</f>
+        <f t="shared" si="6"/>
         <v>5.6818181818181816E-2</v>
       </c>
       <c r="I35" s="43"/>
       <c r="L35" s="43">
-        <f>H35+G35+I35 + J35*2 + K35</f>
+        <f t="shared" si="7"/>
         <v>0.35681818181818181</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="50">
-        <f>B36/$L$56</f>
+        <f t="shared" si="4"/>
         <v>2.1963540522732265E-4</v>
       </c>
       <c r="B36" s="58">
-        <f>ROUND(L36/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C36" s="12" t="s">
@@ -4519,31 +4499,31 @@
         <v>0.1</v>
       </c>
       <c r="H36" s="12">
-        <f>15*F36/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I36" s="43"/>
       <c r="L36" s="43">
-        <f>H36+G36+I36 + J36*2 + K36</f>
+        <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="50">
-        <f>B37/$L$56</f>
+        <f t="shared" si="4"/>
         <v>2.1963540522732265E-4</v>
       </c>
       <c r="B37" s="58">
-        <f>ROUND(L37/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="D37" s="42" t="s">
+      <c r="D37" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="E37" s="42" t="s">
+      <c r="E37" s="68" t="s">
         <v>62</v>
       </c>
       <c r="F37" s="12">
@@ -4553,22 +4533,22 @@
         <v>0.1</v>
       </c>
       <c r="H37" s="12">
-        <f>15*F37/5280</f>
+        <f t="shared" si="6"/>
         <v>5.6818181818181816E-2</v>
       </c>
       <c r="I37" s="43"/>
       <c r="L37" s="43">
-        <f>H37+G37+I37 + J37*2 + K37</f>
+        <f t="shared" si="7"/>
         <v>0.15681818181818183</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="50">
-        <f>B38/$L$56</f>
+        <f t="shared" si="4"/>
         <v>2.1963540522732265E-4</v>
       </c>
       <c r="B38" s="58">
-        <f>ROUND(L38/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C38" s="12" t="s">
@@ -4587,22 +4567,22 @@
         <v>0.2</v>
       </c>
       <c r="H38" s="12">
-        <f>15*F38/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I38" s="43"/>
       <c r="L38" s="43">
-        <f>H38+G38+I38 + J38*2 + K38</f>
+        <f t="shared" si="7"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="53">
-        <f>B39/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B39" s="60">
-        <f>ROUND(L39/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C39" s="44" t="s">
@@ -4621,24 +4601,24 @@
         <v>0</v>
       </c>
       <c r="H39" s="44">
-        <f>15*F39/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I39" s="46"/>
       <c r="J39" s="46"/>
       <c r="K39" s="46"/>
       <c r="L39" s="46">
-        <f>H39+G39+I39 + J39*2 + K39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="50">
-        <f>B40/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B40" s="58">
-        <f>ROUND(L40/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C40" s="12" t="s">
@@ -4657,22 +4637,22 @@
         <v>0</v>
       </c>
       <c r="H40" s="12">
-        <f>15*F40/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I40" s="43"/>
       <c r="L40" s="43">
-        <f>H40+G40+I40 + J40*2 + K40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="50">
-        <f>B41/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B41" s="58">
-        <f>ROUND(L41/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C41" s="12" t="s">
@@ -4691,31 +4671,31 @@
         <v>0</v>
       </c>
       <c r="H41" s="12">
-        <f>15*F41/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I41" s="43"/>
       <c r="L41" s="43">
-        <f>H41+G41+I41 + J41*2 + K41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="50">
-        <f>B42/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B42" s="58">
-        <f>ROUND(L42/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="D42" s="42" t="s">
+      <c r="D42" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="42" t="s">
+      <c r="E42" s="68" t="s">
         <v>50</v>
       </c>
       <c r="F42" s="12">
@@ -4725,22 +4705,22 @@
         <v>0</v>
       </c>
       <c r="H42" s="12">
-        <f>15*F42/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I42" s="43"/>
       <c r="L42" s="43">
-        <f>H42+G42+I42 + J42*2 + K42</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="50">
-        <f>B43/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B43" s="58">
-        <f>ROUND(L43/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C43" s="12" t="s">
@@ -4759,22 +4739,22 @@
         <v>0</v>
       </c>
       <c r="H43" s="12">
-        <f>15*F43/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I43" s="43"/>
       <c r="L43" s="43">
-        <f>H43+G43+I43 + J43*2 + K43</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="50">
-        <f>B44/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B44" s="58">
-        <f>ROUND(L44/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C44" s="12" t="s">
@@ -4793,22 +4773,22 @@
         <v>0</v>
       </c>
       <c r="H44" s="12">
-        <f>15*F44/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I44" s="43"/>
       <c r="L44" s="43">
-        <f>H44+G44+I44 + J44*2 + K44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="50">
-        <f>B45/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B45" s="58">
-        <f>ROUND(L45/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C45" s="12" t="s">
@@ -4827,22 +4807,22 @@
         <v>0</v>
       </c>
       <c r="H45" s="12">
-        <f>15*F45/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I45" s="43"/>
       <c r="L45" s="43">
-        <f>H45+G45+I45 + J45*2 + K45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="50">
-        <f>B46/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B46" s="58">
-        <f>ROUND(L46/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C46" s="12" t="s">
@@ -4861,22 +4841,22 @@
         <v>0</v>
       </c>
       <c r="H46" s="12">
-        <f>15*F46/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I46" s="43"/>
       <c r="L46" s="43">
-        <f>H46+G46+I46 + J46*2 + K46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="50">
-        <f>B47/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B47" s="58">
-        <f>ROUND(L47/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C47" s="12" t="s">
@@ -4895,22 +4875,22 @@
         <v>0</v>
       </c>
       <c r="H47" s="12">
-        <f>15*F47/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I47" s="43"/>
       <c r="L47" s="43">
-        <f>H47+G47+I47 + J47*2 + K47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="50">
-        <f>B48/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B48" s="58">
-        <f>ROUND(L48/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C48" s="12" t="s">
@@ -4929,31 +4909,31 @@
         <v>0</v>
       </c>
       <c r="H48" s="12">
-        <f>15*F48/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I48" s="43"/>
       <c r="L48" s="43">
-        <f>H48+G48+I48 + J48*2 + K48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="50">
-        <f>B49/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B49" s="58">
-        <f>ROUND(L49/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="D49" s="42" t="s">
+      <c r="D49" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="E49" s="42" t="s">
+      <c r="E49" s="68" t="s">
         <v>36</v>
       </c>
       <c r="F49" s="12">
@@ -4963,22 +4943,22 @@
         <v>0</v>
       </c>
       <c r="H49" s="12">
-        <f>15*F49/5280</f>
+        <f t="shared" si="6"/>
         <v>5.6818181818181816E-2</v>
       </c>
       <c r="I49" s="43"/>
       <c r="L49" s="43">
-        <f>H49+G49+I49 + J49*2 + K49</f>
+        <f t="shared" si="7"/>
         <v>5.6818181818181816E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="50">
-        <f>B50/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B50" s="58">
-        <f>ROUND(L50/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C50" s="12" t="s">
@@ -4997,22 +4977,22 @@
         <v>0</v>
       </c>
       <c r="H50" s="12">
-        <f>15*F50/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I50" s="43"/>
       <c r="L50" s="43">
-        <f>H50+G50+I50 + J50*2 + K50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="50">
-        <f>B51/$L$56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B51" s="58">
-        <f>ROUND(L51/$L$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C51" s="12" t="s">
@@ -5031,16 +5011,16 @@
         <v>0</v>
       </c>
       <c r="H51" s="12">
-        <f>15*F51/5280</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I51" s="43"/>
       <c r="L51" s="43">
-        <f>H51+G51+I51 + J51*2 + K51</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B52" s="61"/>
       <c r="I52" s="36"/>
       <c r="J52" s="43"/>
@@ -5049,7 +5029,7 @@
         <v>719.4221590909093</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B53" s="58"/>
       <c r="I53" s="36"/>
       <c r="J53" s="43"/>
@@ -5058,164 +5038,164 @@
         <v>157.97727272727272</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B54" s="61"/>
       <c r="L54" s="36"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B55" s="61"/>
       <c r="D55"/>
       <c r="L55" s="36"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B56" s="61"/>
       <c r="L56" s="36">
         <f>SUM(B2:B51)</f>
         <v>4553</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B57" s="61"/>
       <c r="I57" s="36"/>
       <c r="L57" s="36"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B58" s="61"/>
       <c r="L58" s="36"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B59" s="61"/>
       <c r="L59" s="36"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B60" s="61"/>
       <c r="L60" s="36"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B61" s="61"/>
       <c r="L61" s="36"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B62" s="61"/>
       <c r="L62" s="36"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B63" s="61"/>
       <c r="L63" s="36"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B64" s="61"/>
       <c r="L64" s="36"/>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B65" s="61"/>
       <c r="L65" s="36"/>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B66" s="61"/>
       <c r="L66" s="36"/>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B67" s="61"/>
       <c r="L67" s="36"/>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D68" s="37" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D69" s="37" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B71" s="61"/>
       <c r="D71" s="37" t="s">
         <v>166</v>
       </c>
       <c r="L71" s="36"/>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B72" s="61"/>
       <c r="D72" s="37" t="s">
         <v>174</v>
       </c>
       <c r="L72" s="36"/>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B73" s="61"/>
       <c r="D73" s="37" t="s">
         <v>175</v>
       </c>
       <c r="L73" s="36"/>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B74" s="61"/>
       <c r="D74" s="37" t="s">
         <v>173</v>
       </c>
       <c r="L74" s="36"/>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B75" s="61"/>
       <c r="L75" s="36"/>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B76" s="61"/>
       <c r="D76" s="37" t="s">
         <v>167</v>
       </c>
       <c r="L76" s="36"/>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B77" s="61"/>
       <c r="L77" s="36"/>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B78" s="61"/>
       <c r="D78" s="37" t="s">
         <v>168</v>
       </c>
       <c r="L78" s="36"/>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B79" s="61"/>
       <c r="L79" s="36"/>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B80" s="61"/>
       <c r="L80" s="36"/>
     </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B81" s="61"/>
       <c r="L81" s="36"/>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B82" s="61"/>
       <c r="L82" s="36"/>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B83" s="61"/>
       <c r="L83" s="36"/>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B84" s="61"/>
       <c r="L84" s="36"/>
     </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B85" s="61"/>
       <c r="L85" s="36"/>
     </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B86" s="61"/>
       <c r="L86" s="36"/>
     </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B87" s="61"/>
       <c r="L87" s="36"/>
     </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B88" s="61"/>
       <c r="L88" s="36"/>
     </row>
@@ -5230,13 +5210,2003 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="62" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="37" customWidth="1"/>
+    <col min="5" max="5" width="33.88671875" style="37" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="K1" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" s="40" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51">
+        <f t="shared" ref="A2:A51" si="0">B2/$L$56</f>
+        <v>0.20859407592824364</v>
+      </c>
+      <c r="B2" s="57">
+        <f t="shared" ref="B2:B51" si="1">ROUND(L2/$L$53*1000,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="47">
+        <v>19000</v>
+      </c>
+      <c r="G2" s="49">
+        <v>39</v>
+      </c>
+      <c r="H2" s="47">
+        <f t="shared" ref="H2:H51" si="2">15*F2/5280</f>
+        <v>53.977272727272727</v>
+      </c>
+      <c r="I2" s="55">
+        <v>12</v>
+      </c>
+      <c r="J2" s="55">
+        <v>18</v>
+      </c>
+      <c r="K2" s="55">
+        <v>17</v>
+      </c>
+      <c r="L2" s="49">
+        <f t="shared" ref="L2:L51" si="3">H2+G2+I2 + J2*2 + K2</f>
+        <v>157.97727272727272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50">
+        <f>B3/$L$56</f>
+        <v>0.10554860241969129</v>
+      </c>
+      <c r="B3" s="58">
+        <f>ROUND(L3/$L$53*1000,0)</f>
+        <v>506</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="12">
+        <v>8650</v>
+      </c>
+      <c r="G3" s="12">
+        <v>40.4</v>
+      </c>
+      <c r="H3" s="12">
+        <f>15*F3/5280</f>
+        <v>24.573863636363637</v>
+      </c>
+      <c r="I3" s="54">
+        <v>12</v>
+      </c>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54">
+        <v>3</v>
+      </c>
+      <c r="L3" s="43">
+        <f>H3+G3+I3 + J3*2 + K3</f>
+        <v>79.973863636363632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50">
+        <f>B4/$L$56</f>
+        <v>7.6762619941593654E-2</v>
+      </c>
+      <c r="B4" s="58">
+        <f>ROUND(L4/$L$53*1000,0)</f>
+        <v>368</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="12">
+        <v>7700</v>
+      </c>
+      <c r="G4" s="12">
+        <v>22.2</v>
+      </c>
+      <c r="H4" s="12">
+        <f>15*F4/5280</f>
+        <v>21.875</v>
+      </c>
+      <c r="I4" s="54">
+        <v>12</v>
+      </c>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54">
+        <v>2</v>
+      </c>
+      <c r="L4" s="43">
+        <f>H4+G4+I4 + J4*2 + K4</f>
+        <v>58.075000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50">
+        <f>B5/$L$56</f>
+        <v>7.634543178973717E-2</v>
+      </c>
+      <c r="B5" s="58">
+        <f>ROUND(L5/$L$53*1000,0)</f>
+        <v>366</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="12">
+        <v>9100</v>
+      </c>
+      <c r="G5" s="12">
+        <v>16</v>
+      </c>
+      <c r="H5" s="12">
+        <f>15*F5/5280</f>
+        <v>25.852272727272727</v>
+      </c>
+      <c r="I5" s="54">
+        <v>12</v>
+      </c>
+      <c r="J5" s="54">
+        <v>1</v>
+      </c>
+      <c r="K5" s="54">
+        <v>2</v>
+      </c>
+      <c r="L5" s="43">
+        <f>H5+G5+I5 + J5*2 + K5</f>
+        <v>57.852272727272727</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50">
+        <f>B6/$L$56</f>
+        <v>6.07008760951189E-2</v>
+      </c>
+      <c r="B6" s="58">
+        <f>ROUND(L6/$L$53*1000,0)</f>
+        <v>291</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="12">
+        <v>5350</v>
+      </c>
+      <c r="G6" s="12">
+        <v>28.8</v>
+      </c>
+      <c r="H6" s="12">
+        <f>15*F6/5280</f>
+        <v>15.198863636363637</v>
+      </c>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54">
+        <v>2</v>
+      </c>
+      <c r="L6" s="43">
+        <f>H6+G6+I6 + J6*2 + K6</f>
+        <v>45.998863636363637</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="50">
+        <f>B7/$L$56</f>
+        <v>5.4860241969128073E-2</v>
+      </c>
+      <c r="B7" s="58">
+        <f>ROUND(L7/$L$53*1000,0)</f>
+        <v>263</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="12">
+        <v>6750</v>
+      </c>
+      <c r="G7" s="12">
+        <v>21.4</v>
+      </c>
+      <c r="H7" s="12">
+        <f>15*F7/5280</f>
+        <v>19.176136363636363</v>
+      </c>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54">
+        <v>1</v>
+      </c>
+      <c r="L7" s="43">
+        <f>H7+G7+I7 + J7*2 + K7</f>
+        <v>41.576136363636365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="50">
+        <f>B8/$L$56</f>
+        <v>4.630788485607009E-2</v>
+      </c>
+      <c r="B8" s="58">
+        <f>ROUND(L8/$L$53*1000,0)</f>
+        <v>222</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="12">
+        <v>5300</v>
+      </c>
+      <c r="G8" s="12">
+        <v>8</v>
+      </c>
+      <c r="H8" s="12">
+        <f>15*F8/5280</f>
+        <v>15.056818181818182</v>
+      </c>
+      <c r="I8" s="54">
+        <v>12</v>
+      </c>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="43">
+        <f>H8+G8+I8 + J8*2 + K8</f>
+        <v>35.05681818181818</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="50">
+        <f>B9/$L$56</f>
+        <v>3.77555277430121E-2</v>
+      </c>
+      <c r="B9" s="58">
+        <f>ROUND(L9/$L$53*1000,0)</f>
+        <v>181</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="12">
+        <v>5550</v>
+      </c>
+      <c r="G9" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="H9" s="12">
+        <f>15*F9/5280</f>
+        <v>15.767045454545455</v>
+      </c>
+      <c r="I9" s="54">
+        <v>6</v>
+      </c>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="43">
+        <f>H9+G9+I9 + J9*2 + K9</f>
+        <v>28.567045454545454</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="50">
+        <f>B10/$L$56</f>
+        <v>3.1497705465164789E-2</v>
+      </c>
+      <c r="B10" s="58">
+        <f>ROUND(L10/$L$53*1000,0)</f>
+        <v>151</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="12">
+        <v>3200</v>
+      </c>
+      <c r="G10" s="12">
+        <v>14.8</v>
+      </c>
+      <c r="H10" s="12">
+        <f>15*F10/5280</f>
+        <v>9.0909090909090917</v>
+      </c>
+      <c r="I10" s="43"/>
+      <c r="L10" s="43">
+        <f>H10+G10+I10 + J10*2 + K10</f>
+        <v>23.890909090909091</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="50">
+        <f>B11/$L$56</f>
+        <v>3.0663329161451813E-2</v>
+      </c>
+      <c r="B11" s="58">
+        <f>ROUND(L11/$L$53*1000,0)</f>
+        <v>147</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="12">
+        <v>5000</v>
+      </c>
+      <c r="G11" s="12">
+        <v>9</v>
+      </c>
+      <c r="H11" s="12">
+        <f>15*F11/5280</f>
+        <v>14.204545454545455</v>
+      </c>
+      <c r="I11" s="43"/>
+      <c r="L11" s="43">
+        <f>H11+G11+I11 + J11*2 + K11</f>
+        <v>23.204545454545453</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="50">
+        <f>B12/$L$56</f>
+        <v>2.9411764705882353E-2</v>
+      </c>
+      <c r="B12" s="58">
+        <f>ROUND(L12/$L$53*1000,0)</f>
+        <v>141</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="12">
+        <v>4200</v>
+      </c>
+      <c r="G12" s="12">
+        <v>10.4</v>
+      </c>
+      <c r="H12" s="12">
+        <f>15*F12/5280</f>
+        <v>11.931818181818182</v>
+      </c>
+      <c r="I12" s="43"/>
+      <c r="L12" s="43">
+        <f>H12+G12+I12 + J12*2 + K12</f>
+        <v>22.331818181818182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="50">
+        <f>B13/$L$56</f>
+        <v>2.6908635794743431E-2</v>
+      </c>
+      <c r="B13" s="58">
+        <f>ROUND(L13/$L$53*1000,0)</f>
+        <v>129</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="F13" s="69">
+        <v>4300</v>
+      </c>
+      <c r="G13" s="69">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="H13" s="12">
+        <f>15*F13/5280</f>
+        <v>12.215909090909092</v>
+      </c>
+      <c r="I13" s="43"/>
+      <c r="L13" s="43">
+        <f>H13+G13+I13 + J13*2 + K13</f>
+        <v>20.415909090909089</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="50">
+        <f>B14/$L$56</f>
+        <v>2.6282853566958697E-2</v>
+      </c>
+      <c r="B14" s="58">
+        <f>ROUND(L14/$L$53*1000,0)</f>
+        <v>126</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="12">
+        <v>4400</v>
+      </c>
+      <c r="G14" s="12">
+        <v>7.4</v>
+      </c>
+      <c r="H14" s="12">
+        <f>15*F14/5280</f>
+        <v>12.5</v>
+      </c>
+      <c r="I14" s="43"/>
+      <c r="L14" s="43">
+        <f>H14+G14+I14 + J14*2 + K14</f>
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="50">
+        <f>B15/$L$56</f>
+        <v>2.5031289111389236E-2</v>
+      </c>
+      <c r="B15" s="58">
+        <f>ROUND(L15/$L$53*1000,0)</f>
+        <v>120</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="12">
+        <v>3500</v>
+      </c>
+      <c r="G15" s="12">
+        <v>9</v>
+      </c>
+      <c r="H15" s="12">
+        <f>15*F15/5280</f>
+        <v>9.9431818181818183</v>
+      </c>
+      <c r="I15" s="43"/>
+      <c r="L15" s="43">
+        <f>H15+G15+I15 + J15*2 + K15</f>
+        <v>18.94318181818182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="50">
+        <f>B16/$L$56</f>
+        <v>2.2110972048393827E-2</v>
+      </c>
+      <c r="B16" s="58">
+        <f>ROUND(L16/$L$53*1000,0)</f>
+        <v>106</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="12">
+        <v>2950</v>
+      </c>
+      <c r="G16" s="12">
+        <v>8.4</v>
+      </c>
+      <c r="H16" s="12">
+        <f>15*F16/5280</f>
+        <v>8.3806818181818183</v>
+      </c>
+      <c r="I16" s="43"/>
+      <c r="L16" s="43">
+        <f>H16+G16+I16 + J16*2 + K16</f>
+        <v>16.780681818181819</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="50">
+        <f>B17/$L$56</f>
+        <v>2.0442219440967878E-2</v>
+      </c>
+      <c r="B17" s="58">
+        <f>ROUND(L17/$L$53*1000,0)</f>
+        <v>98</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="12">
+        <v>3250</v>
+      </c>
+      <c r="G17" s="12">
+        <v>6.2</v>
+      </c>
+      <c r="H17" s="12">
+        <f>15*F17/5280</f>
+        <v>9.232954545454545</v>
+      </c>
+      <c r="I17" s="43"/>
+      <c r="L17" s="43">
+        <f>H17+G17+I17 + J17*2 + K17</f>
+        <v>15.432954545454546</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="50">
+        <f>B18/$L$56</f>
+        <v>1.6896120150187734E-2</v>
+      </c>
+      <c r="B18" s="58">
+        <f>ROUND(L18/$L$53*1000,0)</f>
+        <v>81</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="12">
+        <v>1500</v>
+      </c>
+      <c r="G18" s="12">
+        <v>8.6</v>
+      </c>
+      <c r="H18" s="12">
+        <f>15*F18/5280</f>
+        <v>4.2613636363636367</v>
+      </c>
+      <c r="I18" s="43"/>
+      <c r="L18" s="43">
+        <f>H18+G18+I18 + J18*2 + K18</f>
+        <v>12.861363636363636</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="50">
+        <f>B19/$L$56</f>
+        <v>1.6478931998331246E-2</v>
+      </c>
+      <c r="B19" s="58">
+        <f>ROUND(L19/$L$53*1000,0)</f>
+        <v>79</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="68" t="s">
+        <v>182</v>
+      </c>
+      <c r="F19" s="69">
+        <v>2800</v>
+      </c>
+      <c r="G19" s="69">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H19" s="12">
+        <f>15*F19/5280</f>
+        <v>7.9545454545454541</v>
+      </c>
+      <c r="I19" s="43"/>
+      <c r="L19" s="43">
+        <f>H19+G19+I19 + J19*2 + K19</f>
+        <v>12.554545454545455</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="50">
+        <f>B20/$L$56</f>
+        <v>1.4184397163120567E-2</v>
+      </c>
+      <c r="B20" s="58">
+        <f>ROUND(L20/$L$53*1000,0)</f>
+        <v>68</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="12">
+        <v>775</v>
+      </c>
+      <c r="G20" s="12">
+        <v>8.6</v>
+      </c>
+      <c r="H20" s="12">
+        <f>15*F20/5280</f>
+        <v>2.2017045454545454</v>
+      </c>
+      <c r="I20" s="43"/>
+      <c r="L20" s="43">
+        <f>H20+G20+I20 + J20*2 + K20</f>
+        <v>10.801704545454545</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="50">
+        <f>B21/$L$56</f>
+        <v>1.3350020859407593E-2</v>
+      </c>
+      <c r="B21" s="58">
+        <f>ROUND(L21/$L$53*1000,0)</f>
+        <v>64</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="12">
+        <v>1500</v>
+      </c>
+      <c r="G21" s="12">
+        <v>5.8</v>
+      </c>
+      <c r="H21" s="12">
+        <f>15*F21/5280</f>
+        <v>4.2613636363636367</v>
+      </c>
+      <c r="I21" s="43"/>
+      <c r="L21" s="43">
+        <f>H21+G21+I21 + J21*2 + K21</f>
+        <v>10.061363636363637</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="50">
+        <f>B22/$L$56</f>
+        <v>1.14726741760534E-2</v>
+      </c>
+      <c r="B22" s="58">
+        <f>ROUND(L22/$L$53*1000,0)</f>
+        <v>55</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="12">
+        <v>600</v>
+      </c>
+      <c r="G22" s="12">
+        <v>7</v>
+      </c>
+      <c r="H22" s="12">
+        <f>15*F22/5280</f>
+        <v>1.7045454545454546</v>
+      </c>
+      <c r="I22" s="43"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="43">
+        <f>H22+G22+I22 + J22*2 + K22</f>
+        <v>8.704545454545455</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="50">
+        <f>B23/$L$56</f>
+        <v>7.3007926574885276E-3</v>
+      </c>
+      <c r="B23" s="58">
+        <f>ROUND(L23/$L$53*1000,0)</f>
+        <v>35</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="68" t="s">
+        <v>183</v>
+      </c>
+      <c r="F23" s="69">
+        <v>700</v>
+      </c>
+      <c r="G23" s="69">
+        <v>3.6</v>
+      </c>
+      <c r="H23" s="12">
+        <f>15*F23/5280</f>
+        <v>1.9886363636363635</v>
+      </c>
+      <c r="I23" s="43"/>
+      <c r="L23" s="43">
+        <f>H23+G23+I23 + J23*2 + K23</f>
+        <v>5.5886363636363638</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="50">
+        <f>B24/$L$56</f>
+        <v>6.4664163537755531E-3</v>
+      </c>
+      <c r="B24" s="58">
+        <f>ROUND(L24/$L$53*1000,0)</f>
+        <v>31</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="12">
+        <v>450</v>
+      </c>
+      <c r="G24" s="12">
+        <v>3.6</v>
+      </c>
+      <c r="H24" s="12">
+        <f>15*F24/5280</f>
+        <v>1.2784090909090908</v>
+      </c>
+      <c r="I24" s="43"/>
+      <c r="L24" s="43">
+        <f>H24+G24+I24 + J24*2 + K24</f>
+        <v>4.8784090909090914</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="63">
+        <f>B25/$L$56</f>
+        <v>6.0492282019190659E-3</v>
+      </c>
+      <c r="B25" s="64">
+        <f>ROUND(L25/$L$53*1000,0)</f>
+        <v>29</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="65">
+        <v>400</v>
+      </c>
+      <c r="G25" s="65">
+        <v>3.4</v>
+      </c>
+      <c r="H25" s="65">
+        <f>15*F25/5280</f>
+        <v>1.1363636363636365</v>
+      </c>
+      <c r="I25" s="67"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="67">
+        <f>H25+G25+I25 + J25*2 + K25</f>
+        <v>4.5363636363636362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="50">
+        <f>B26/$L$56</f>
+        <v>5.6320400500625778E-3</v>
+      </c>
+      <c r="B26" s="58">
+        <f>ROUND(L26/$L$53*1000,0)</f>
+        <v>27</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="12">
+        <v>750</v>
+      </c>
+      <c r="G26" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H26" s="12">
+        <f>15*F26/5280</f>
+        <v>2.1306818181818183</v>
+      </c>
+      <c r="I26" s="43"/>
+      <c r="L26" s="43">
+        <f>H26+G26+I26 + J26*2 + K26</f>
+        <v>4.3306818181818185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="50">
+        <f>B27/$L$56</f>
+        <v>4.3804755944931162E-3</v>
+      </c>
+      <c r="B27" s="58">
+        <f>ROUND(L27/$L$53*1000,0)</f>
+        <v>21</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="12">
+        <v>275</v>
+      </c>
+      <c r="G27" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="H27" s="12">
+        <f>15*F27/5280</f>
+        <v>0.78125</v>
+      </c>
+      <c r="I27" s="43"/>
+      <c r="L27" s="43">
+        <f>H27+G27+I27 + J27*2 + K27</f>
+        <v>3.28125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="50">
+        <f>B28/$L$56</f>
+        <v>3.1289111389236545E-3</v>
+      </c>
+      <c r="B28" s="58">
+        <f>ROUND(L28/$L$53*1000,0)</f>
+        <v>15</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="69">
+        <v>400</v>
+      </c>
+      <c r="G28" s="69">
+        <v>1.2</v>
+      </c>
+      <c r="H28" s="12">
+        <f>15*F28/5280</f>
+        <v>1.1363636363636365</v>
+      </c>
+      <c r="I28" s="43"/>
+      <c r="L28" s="43">
+        <f>H28+G28+I28 + J28*2 + K28</f>
+        <v>2.3363636363636364</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="50">
+        <f>B29/$L$56</f>
+        <v>3.1289111389236545E-3</v>
+      </c>
+      <c r="B29" s="58">
+        <f>ROUND(L29/$L$53*1000,0)</f>
+        <v>15</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="68" t="s">
+        <v>184</v>
+      </c>
+      <c r="F29" s="69">
+        <v>320</v>
+      </c>
+      <c r="G29" s="69">
+        <v>1.5</v>
+      </c>
+      <c r="H29" s="12">
+        <f>15*F29/5280</f>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="I29" s="43"/>
+      <c r="L29" s="43">
+        <f>H29+G29+I29 + J29*2 + K29</f>
+        <v>2.4090909090909092</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="50">
+        <f>B30/$L$56</f>
+        <v>2.9203170629954109E-3</v>
+      </c>
+      <c r="B30" s="58">
+        <f>ROUND(L30/$L$53*1000,0)</f>
+        <v>14</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30" s="12">
+        <v>150</v>
+      </c>
+      <c r="G30" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="H30" s="12">
+        <f>15*F30/5280</f>
+        <v>0.42613636363636365</v>
+      </c>
+      <c r="I30" s="43"/>
+      <c r="L30" s="43">
+        <f>H30+G30+I30 + J30*2 + K30</f>
+        <v>2.2261363636363636</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="52">
+        <f>B31/$L$56</f>
+        <v>2.5031289111389237E-3</v>
+      </c>
+      <c r="B31" s="59">
+        <f>ROUND(L31/$L$53*1000,0)</f>
+        <v>12</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="6">
+        <v>330</v>
+      </c>
+      <c r="G31" s="6">
+        <v>1</v>
+      </c>
+      <c r="H31" s="6">
+        <f>15*F31/5280</f>
+        <v>0.9375</v>
+      </c>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38">
+        <f>H31+G31+I31 + J31*2 + K31</f>
+        <v>1.9375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="50">
+        <f>B32/$L$56</f>
+        <v>2.0859407592824365E-3</v>
+      </c>
+      <c r="B32" s="58">
+        <f>ROUND(L32/$L$53*1000,0)</f>
+        <v>10</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="12">
+        <v>225</v>
+      </c>
+      <c r="G32" s="12">
+        <v>1</v>
+      </c>
+      <c r="H32" s="12">
+        <f>15*F32/5280</f>
+        <v>0.63920454545454541</v>
+      </c>
+      <c r="I32" s="43"/>
+      <c r="L32" s="43">
+        <f>H32+G32+I32 + J32*2 + K32</f>
+        <v>1.6392045454545454</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="50">
+        <f>B33/$L$56</f>
+        <v>1.4601585314977055E-3</v>
+      </c>
+      <c r="B33" s="58">
+        <f>ROUND(L33/$L$53*1000,0)</f>
+        <v>7</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="12">
+        <v>230</v>
+      </c>
+      <c r="G33" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="H33" s="12">
+        <f>15*F33/5280</f>
+        <v>0.65340909090909094</v>
+      </c>
+      <c r="I33" s="43"/>
+      <c r="L33" s="43">
+        <f>H33+G33+I33 + J33*2 + K33</f>
+        <v>1.053409090909091</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="50">
+        <f>B34/$L$56</f>
+        <v>1.0429703796412183E-3</v>
+      </c>
+      <c r="B34" s="58">
+        <f>ROUND(L34/$L$53*1000,0)</f>
+        <v>5</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="12">
+        <v>120</v>
+      </c>
+      <c r="G34" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="H34" s="12">
+        <f>15*F34/5280</f>
+        <v>0.34090909090909088</v>
+      </c>
+      <c r="I34" s="43"/>
+      <c r="L34" s="43">
+        <f>H34+G34+I34 + J34*2 + K34</f>
+        <v>0.74090909090909096</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="50">
+        <f>B35/$L$56</f>
+        <v>6.2578222778473093E-4</v>
+      </c>
+      <c r="B35" s="58">
+        <f>ROUND(L35/$L$53*1000,0)</f>
+        <v>3</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="12">
+        <v>30</v>
+      </c>
+      <c r="G35" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="H35" s="12">
+        <f>15*F35/5280</f>
+        <v>8.5227272727272721E-2</v>
+      </c>
+      <c r="I35" s="43"/>
+      <c r="L35" s="43">
+        <f>H35+G35+I35 + J35*2 + K35</f>
+        <v>0.48522727272727273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="50">
+        <f>B36/$L$56</f>
+        <v>4.1718815185648727E-4</v>
+      </c>
+      <c r="B36" s="58">
+        <f>ROUND(L36/$L$53*1000,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="12">
+        <v>40</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H36" s="12">
+        <f>15*F36/5280</f>
+        <v>0.11363636363636363</v>
+      </c>
+      <c r="I36" s="43"/>
+      <c r="L36" s="43">
+        <f>H36+G36+I36 + J36*2 + K36</f>
+        <v>0.31363636363636366</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="50">
+        <f>B37/$L$56</f>
+        <v>4.1718815185648727E-4</v>
+      </c>
+      <c r="B37" s="58">
+        <f>ROUND(L37/$L$53*1000,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" s="12">
+        <v>50</v>
+      </c>
+      <c r="G37" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="H37" s="12">
+        <f>15*F37/5280</f>
+        <v>0.14204545454545456</v>
+      </c>
+      <c r="I37" s="43"/>
+      <c r="L37" s="43">
+        <f>H37+G37+I37 + J37*2 + K37</f>
+        <v>0.29204545454545455</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="50">
+        <f>B38/$L$56</f>
+        <v>4.1718815185648727E-4</v>
+      </c>
+      <c r="B38" s="58">
+        <f>ROUND(L38/$L$53*1000,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="12">
+        <v>20</v>
+      </c>
+      <c r="G38" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="H38" s="12">
+        <f>15*F38/5280</f>
+        <v>5.6818181818181816E-2</v>
+      </c>
+      <c r="I38" s="43"/>
+      <c r="L38" s="43">
+        <f>H38+G38+I38 + J38*2 + K38</f>
+        <v>0.35681818181818181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="50">
+        <f>B39/$L$56</f>
+        <v>2.0859407592824363E-4</v>
+      </c>
+      <c r="B39" s="58">
+        <f>ROUND(L39/$L$53*1000,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0</v>
+      </c>
+      <c r="G39" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="H39" s="12">
+        <f>15*F39/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="43"/>
+      <c r="L39" s="43">
+        <f>H39+G39+I39 + J39*2 + K39</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="50">
+        <f>B40/$L$56</f>
+        <v>2.0859407592824363E-4</v>
+      </c>
+      <c r="B40" s="58">
+        <f>ROUND(L40/$L$53*1000,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="F40" s="12">
+        <v>0</v>
+      </c>
+      <c r="G40" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H40" s="12">
+        <f>15*F40/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="43"/>
+      <c r="L40" s="43">
+        <f>H40+G40+I40 + J40*2 + K40</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="53">
+        <f>B41/$L$56</f>
+        <v>0</v>
+      </c>
+      <c r="B41" s="60">
+        <f>ROUND(L41/$L$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C41" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" s="44">
+        <v>0</v>
+      </c>
+      <c r="G41" s="44">
+        <v>0</v>
+      </c>
+      <c r="H41" s="44">
+        <f>15*F41/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46">
+        <f>H41+G41+I41 + J41*2 + K41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="50">
+        <f>B42/$L$56</f>
+        <v>0</v>
+      </c>
+      <c r="B42" s="58">
+        <f>ROUND(L42/$L$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D42" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F42" s="12">
+        <v>0</v>
+      </c>
+      <c r="G42" s="12">
+        <v>0</v>
+      </c>
+      <c r="H42" s="12">
+        <f>15*F42/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="43"/>
+      <c r="L42" s="43">
+        <f>H42+G42+I42 + J42*2 + K42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="50">
+        <f>B43/$L$56</f>
+        <v>0</v>
+      </c>
+      <c r="B43" s="58">
+        <f>ROUND(L43/$L$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="E43" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="F43" s="12">
+        <v>0</v>
+      </c>
+      <c r="G43" s="12">
+        <v>0</v>
+      </c>
+      <c r="H43" s="12">
+        <f>15*F43/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="43"/>
+      <c r="L43" s="43">
+        <f>H43+G43+I43 + J43*2 + K43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="50">
+        <f>B44/$L$56</f>
+        <v>0</v>
+      </c>
+      <c r="B44" s="58">
+        <f>ROUND(L44/$L$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" s="12">
+        <v>0</v>
+      </c>
+      <c r="G44" s="12">
+        <v>0</v>
+      </c>
+      <c r="H44" s="12">
+        <f>15*F44/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="43"/>
+      <c r="L44" s="43">
+        <f>H44+G44+I44 + J44*2 + K44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="50">
+        <f>B45/$L$56</f>
+        <v>0</v>
+      </c>
+      <c r="B45" s="58">
+        <f>ROUND(L45/$L$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="12">
+        <v>0</v>
+      </c>
+      <c r="G45" s="12">
+        <v>0</v>
+      </c>
+      <c r="H45" s="12">
+        <f>15*F45/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="43"/>
+      <c r="L45" s="43">
+        <f>H45+G45+I45 + J45*2 + K45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="50">
+        <f>B46/$L$56</f>
+        <v>0</v>
+      </c>
+      <c r="B46" s="58">
+        <f>ROUND(L46/$L$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="F46" s="12">
+        <v>0</v>
+      </c>
+      <c r="G46" s="12">
+        <v>0</v>
+      </c>
+      <c r="H46" s="12">
+        <f>15*F46/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="43"/>
+      <c r="L46" s="43">
+        <f>H46+G46+I46 + J46*2 + K46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="50">
+        <f>B47/$L$56</f>
+        <v>0</v>
+      </c>
+      <c r="B47" s="58">
+        <f>ROUND(L47/$L$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E47" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="F47" s="12">
+        <v>0</v>
+      </c>
+      <c r="G47" s="12">
+        <v>0</v>
+      </c>
+      <c r="H47" s="12">
+        <f>15*F47/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I47" s="43"/>
+      <c r="L47" s="43">
+        <f>H47+G47+I47 + J47*2 + K47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="50">
+        <f>B48/$L$56</f>
+        <v>0</v>
+      </c>
+      <c r="B48" s="58">
+        <f>ROUND(L48/$L$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D48" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="F48" s="12">
+        <v>0</v>
+      </c>
+      <c r="G48" s="12">
+        <v>0</v>
+      </c>
+      <c r="H48" s="12">
+        <f>15*F48/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I48" s="43"/>
+      <c r="L48" s="43">
+        <f>H48+G48+I48 + J48*2 + K48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="50">
+        <f>B49/$L$56</f>
+        <v>0</v>
+      </c>
+      <c r="B49" s="58">
+        <f>ROUND(L49/$L$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="E49" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="12">
+        <v>0</v>
+      </c>
+      <c r="G49" s="12">
+        <v>0</v>
+      </c>
+      <c r="H49" s="12">
+        <f>15*F49/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I49" s="43"/>
+      <c r="L49" s="43">
+        <f>H49+G49+I49 + J49*2 + K49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="50">
+        <f>B50/$L$56</f>
+        <v>0</v>
+      </c>
+      <c r="B50" s="58">
+        <f>ROUND(L50/$L$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E50" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="F50" s="12">
+        <v>0</v>
+      </c>
+      <c r="G50" s="12">
+        <v>0</v>
+      </c>
+      <c r="H50" s="12">
+        <f>15*F50/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I50" s="43"/>
+      <c r="L50" s="43">
+        <f>H50+G50+I50 + J50*2 + K50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="50">
+        <f>B51/$L$56</f>
+        <v>0</v>
+      </c>
+      <c r="B51" s="58">
+        <f>ROUND(L51/$L$53*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E51" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="F51" s="12">
+        <v>0</v>
+      </c>
+      <c r="G51" s="12">
+        <v>0</v>
+      </c>
+      <c r="H51" s="12">
+        <f>15*F51/5280</f>
+        <v>0</v>
+      </c>
+      <c r="I51" s="43"/>
+      <c r="L51" s="43">
+        <f>H51+G51+I51 + J51*2 + K51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B52" s="61"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="43"/>
+      <c r="L52" s="36">
+        <f>SUM(L2:L51)</f>
+        <v>757.66647727272755</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B53" s="58"/>
+      <c r="I53" s="36"/>
+      <c r="J53" s="43"/>
+      <c r="L53" s="36">
+        <f>MAX(L2:L51)</f>
+        <v>157.97727272727272</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B54" s="61"/>
+      <c r="L54" s="36"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B55" s="61"/>
+      <c r="D55"/>
+      <c r="L55" s="36"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B56" s="61"/>
+      <c r="L56" s="36">
+        <f>SUM(B2:B51)</f>
+        <v>4794</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B57" s="61"/>
+      <c r="I57" s="36"/>
+      <c r="L57" s="36"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B58" s="61"/>
+      <c r="L58" s="36"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B59" s="61"/>
+      <c r="L59" s="36"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B60" s="61"/>
+      <c r="L60" s="36"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B61" s="61"/>
+      <c r="L61" s="36"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B62" s="61"/>
+      <c r="L62" s="36"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B63" s="61"/>
+      <c r="L63" s="36"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B64" s="61"/>
+      <c r="L64" s="36"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B65" s="61"/>
+      <c r="L65" s="36"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B66" s="61"/>
+      <c r="L66" s="36"/>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B67" s="61"/>
+      <c r="L67" s="36"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D68" s="37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D69" s="37" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B71" s="61"/>
+      <c r="D71" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="L71" s="36"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B72" s="61"/>
+      <c r="D72" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="L72" s="36"/>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B73" s="61"/>
+      <c r="D73" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="L73" s="36"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B74" s="61"/>
+      <c r="D74" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="L74" s="36"/>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B75" s="61"/>
+      <c r="L75" s="36"/>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B76" s="61"/>
+      <c r="D76" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="L76" s="36"/>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B77" s="61"/>
+      <c r="L77" s="36"/>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B78" s="61"/>
+      <c r="D78" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="L78" s="36"/>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B79" s="61"/>
+      <c r="L79" s="36"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B80" s="61"/>
+      <c r="L80" s="36"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B81" s="61"/>
+      <c r="L81" s="36"/>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B82" s="61"/>
+      <c r="L82" s="36"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B83" s="61"/>
+      <c r="L83" s="36"/>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B84" s="61"/>
+      <c r="L84" s="36"/>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B85" s="61"/>
+      <c r="L85" s="36"/>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B86" s="61"/>
+      <c r="L86" s="36"/>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B87" s="61"/>
+      <c r="L87" s="36"/>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B88" s="61"/>
+      <c r="L88" s="36"/>
+    </row>
+  </sheetData>
+  <sortState ref="A3:L51">
+    <sortCondition descending="1" ref="B3:B51"/>
+    <sortCondition ref="D3:D51"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
non standard route option
</commit_message>
<xml_diff>
--- a/Walter/TripReports/STATE HIGH POINTS.xlsx
+++ b/Walter/TripReports/STATE HIGH POINTS.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19296" windowHeight="10896" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19296" windowHeight="10896" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HighPoint Log" sheetId="1" r:id="rId1"/>
     <sheet name="Effor Scale" sheetId="3" r:id="rId2"/>
     <sheet name="Less Zeros" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="274">
   <si>
     <t>State</t>
   </si>
@@ -582,6 +583,270 @@
   </si>
   <si>
     <t>Mount Washington via Tuckerman Ravine</t>
+  </si>
+  <si>
+    <t>1000&lt;br /&gt;20.86%</t>
+  </si>
+  <si>
+    <t>506&lt;br /&gt;10.55%</t>
+  </si>
+  <si>
+    <t>368&lt;br /&gt;7.68%</t>
+  </si>
+  <si>
+    <t>366&lt;br /&gt;7.63%</t>
+  </si>
+  <si>
+    <t>291&lt;br /&gt;6.07%</t>
+  </si>
+  <si>
+    <t>263&lt;br /&gt;5.49%</t>
+  </si>
+  <si>
+    <t>222&lt;br /&gt;4.63%</t>
+  </si>
+  <si>
+    <t>181&lt;br /&gt;3.78%</t>
+  </si>
+  <si>
+    <t>151&lt;br /&gt;3.15%</t>
+  </si>
+  <si>
+    <t>147&lt;br /&gt;3.07%</t>
+  </si>
+  <si>
+    <t>141&lt;br /&gt;2.94%</t>
+  </si>
+  <si>
+    <t>129&lt;br /&gt;2.69%</t>
+  </si>
+  <si>
+    <t>126&lt;br /&gt;2.63%</t>
+  </si>
+  <si>
+    <t>120&lt;br /&gt;2.50%</t>
+  </si>
+  <si>
+    <t>106&lt;br /&gt;2.21%</t>
+  </si>
+  <si>
+    <t>98&lt;br /&gt;2.04%</t>
+  </si>
+  <si>
+    <t>81&lt;br /&gt;1.69%</t>
+  </si>
+  <si>
+    <t>79&lt;br /&gt;1.65%</t>
+  </si>
+  <si>
+    <t>68&lt;br /&gt;1.42%</t>
+  </si>
+  <si>
+    <t>64&lt;br /&gt;1.34%</t>
+  </si>
+  <si>
+    <t>55&lt;br /&gt;1.15%</t>
+  </si>
+  <si>
+    <t>35&lt;br /&gt;0.73%</t>
+  </si>
+  <si>
+    <t>31&lt;br /&gt;0.65%</t>
+  </si>
+  <si>
+    <t>29&lt;br /&gt;0.60%</t>
+  </si>
+  <si>
+    <t>27&lt;br /&gt;0.56%</t>
+  </si>
+  <si>
+    <t>21&lt;br /&gt;0.44%</t>
+  </si>
+  <si>
+    <t>15&lt;br /&gt;0.31%</t>
+  </si>
+  <si>
+    <t>14&lt;br /&gt;0.29%</t>
+  </si>
+  <si>
+    <t>12&lt;br /&gt;0.25%</t>
+  </si>
+  <si>
+    <t>10&lt;br /&gt;0.21%</t>
+  </si>
+  <si>
+    <t>7&lt;br /&gt;0.15%</t>
+  </si>
+  <si>
+    <t>5&lt;br /&gt;0.10%</t>
+  </si>
+  <si>
+    <t>3&lt;br /&gt;0.06%</t>
+  </si>
+  <si>
+    <t>2&lt;br /&gt;0.04%</t>
+  </si>
+  <si>
+    <t>1&lt;br /&gt;0.02%</t>
+  </si>
+  <si>
+    <t>Highpoint</t>
+  </si>
+  <si>
+    <t>Alaska - Denali</t>
+  </si>
+  <si>
+    <t>Wyoming - Gannett Peak</t>
+  </si>
+  <si>
+    <t>Montana - Granite Peak</t>
+  </si>
+  <si>
+    <t>Washington - Mount Rainier</t>
+  </si>
+  <si>
+    <t>Utah - Kings Peak</t>
+  </si>
+  <si>
+    <t>California - Mount Whitney</t>
+  </si>
+  <si>
+    <t>Oregon - Mount Hood</t>
+  </si>
+  <si>
+    <t>Idaho - Borah Peak</t>
+  </si>
+  <si>
+    <t>New York - Mount Marcy</t>
+  </si>
+  <si>
+    <t>Colorado - Mount Elbert</t>
+  </si>
+  <si>
+    <t>Maine - Katahdin</t>
+  </si>
+  <si>
+    <t>New Hampshire - Mount Washington via Tuckerman Ravine</t>
+  </si>
+  <si>
+    <t>Nevada - Boundary Peak</t>
+  </si>
+  <si>
+    <t>Arizona - Humphreys Peak</t>
+  </si>
+  <si>
+    <t>Texas - Guadalupe Peak</t>
+  </si>
+  <si>
+    <t>New Mexico - Wheeler Peak</t>
+  </si>
+  <si>
+    <t>Virginia - Mount Rogers</t>
+  </si>
+  <si>
+    <t>Vermont - Mount Mansfield via Longs Trail</t>
+  </si>
+  <si>
+    <t>Oklahoma - Black Mesa</t>
+  </si>
+  <si>
+    <t>South Dakota - Black Elk Peak</t>
+  </si>
+  <si>
+    <t>Minnesota - Eagle Mountain</t>
+  </si>
+  <si>
+    <t>North Carolina - Mount Mitchell via Old Mitchell Trail</t>
+  </si>
+  <si>
+    <t>Connecticut - Mount Frissell-South Slope</t>
+  </si>
+  <si>
+    <t>North Dakota - White Butte</t>
+  </si>
+  <si>
+    <t>Maryland - Backbone Mountain</t>
+  </si>
+  <si>
+    <t>Illinois - Charles Mound</t>
+  </si>
+  <si>
+    <t>Georgia - Brasstown Bald</t>
+  </si>
+  <si>
+    <t>Massachusetts - Mount Greylock via AT from Intersection of Rockwell Rd and Summit Rd</t>
+  </si>
+  <si>
+    <t>Louisiana - Driskill Mountain</t>
+  </si>
+  <si>
+    <t>Tennessee - Clingmans Dome</t>
+  </si>
+  <si>
+    <t>Arkansas - Magazine Mountain</t>
+  </si>
+  <si>
+    <t>Hawaii - Mauna Kea</t>
+  </si>
+  <si>
+    <t>Wisconsin - Timms Hill</t>
+  </si>
+  <si>
+    <t>Missouri - Taum Sauk Mountain</t>
+  </si>
+  <si>
+    <t>New Jersey - High Point</t>
+  </si>
+  <si>
+    <t>South Carolina - Sassafras Mountain</t>
+  </si>
+  <si>
+    <t>West Virginia - Spruce Knob</t>
+  </si>
+  <si>
+    <t>Kentucky - Black Mountain</t>
+  </si>
+  <si>
+    <t>Rhode Island - Jerimoth Hill</t>
+  </si>
+  <si>
+    <t>Alabama - Cheaha Mountain</t>
+  </si>
+  <si>
+    <t>Delaware - Ebright Azimuth</t>
+  </si>
+  <si>
+    <t>Florida - Britton Hill</t>
+  </si>
+  <si>
+    <t>Indiana - Hoosier Hill</t>
+  </si>
+  <si>
+    <t>Iowa - Hawkeye Point</t>
+  </si>
+  <si>
+    <t>Kansas - Mount Sunflower</t>
+  </si>
+  <si>
+    <t>Michigan - Mount Arvon</t>
+  </si>
+  <si>
+    <t>Mississippi - Woodall Mountain</t>
+  </si>
+  <si>
+    <t>Nebraska - Panorama Point</t>
+  </si>
+  <si>
+    <t>Ohio - Campbell Hill</t>
+  </si>
+  <si>
+    <t>Pennsylvania - Mount Davis</t>
+  </si>
+  <si>
+    <t>Vertical Gain (ft)</t>
+  </si>
+  <si>
+    <t>Round-Trip (miles)</t>
   </si>
 </sst>
 </file>
@@ -4408,7 +4673,7 @@
     </row>
     <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="50">
-        <f t="shared" ref="A34:A65" si="4">B34/$L$56</f>
+        <f t="shared" ref="A34:A51" si="4">B34/$L$56</f>
         <v>4.392708104546453E-4</v>
       </c>
       <c r="B34" s="58">
@@ -4436,7 +4701,7 @@
       </c>
       <c r="I34" s="43"/>
       <c r="L34" s="43">
-        <f t="shared" ref="L34:L65" si="7">H34+G34+I34 + J34*2 + K34</f>
+        <f t="shared" ref="L34:L51" si="7">H34+G34+I34 + J34*2 + K34</f>
         <v>0.29204545454545455</v>
       </c>
     </row>
@@ -5211,29 +5476,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection sqref="A1:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" style="62" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="33.88671875" style="37" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
-    <col min="12" max="12" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="37" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" style="37" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" customWidth="1"/>
+    <col min="11" max="11" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>165</v>
       </c>
@@ -5241,1972 +5505,2555 @@
         <v>181</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>161</v>
+        <v>0</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="F1" s="40" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="I1" s="40" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J1" s="40" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="K1" s="40" t="s">
-        <v>169</v>
-      </c>
-      <c r="L1" s="40" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="51">
-        <f t="shared" ref="A2:A51" si="0">B2/$L$56</f>
+        <f>B2/$K$56</f>
         <v>0.20859407592824364</v>
       </c>
       <c r="B2" s="57">
-        <f t="shared" ref="B2:B51" si="1">ROUND(L2/$L$53*1000,0)</f>
+        <f t="shared" ref="B2" si="0">ROUND(K2/$K$53*1000,0)</f>
         <v>1000</v>
       </c>
-      <c r="C2" s="47" t="s">
-        <v>162</v>
+      <c r="C2" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="D2" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="47">
+        <v>19000</v>
+      </c>
+      <c r="F2" s="49">
+        <v>39</v>
+      </c>
+      <c r="G2" s="47">
+        <f t="shared" ref="G2" si="1">15*E2/5280</f>
+        <v>53.977272727272727</v>
+      </c>
+      <c r="H2" s="55">
+        <v>12</v>
+      </c>
+      <c r="I2" s="55">
+        <v>18</v>
+      </c>
+      <c r="J2" s="55">
+        <v>17</v>
+      </c>
+      <c r="K2" s="49">
+        <f t="shared" ref="K2" si="2">G2+F2+H2 + I2*2 + J2</f>
+        <v>157.97727272727272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50">
+        <f>B3/$K$56</f>
+        <v>0.10554860241969129</v>
+      </c>
+      <c r="B3" s="58">
+        <f t="shared" ref="B3:B34" si="3">ROUND(K3/$K$53*1000,0)</f>
+        <v>506</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="12">
+        <v>8650</v>
+      </c>
+      <c r="F3" s="12">
+        <v>40.4</v>
+      </c>
+      <c r="G3" s="12">
+        <f t="shared" ref="G3:G34" si="4">15*E3/5280</f>
+        <v>24.573863636363637</v>
+      </c>
+      <c r="H3" s="54">
+        <v>12</v>
+      </c>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54">
+        <v>3</v>
+      </c>
+      <c r="K3" s="43">
+        <f t="shared" ref="K3:K34" si="5">G3+F3+H3 + I3*2 + J3</f>
+        <v>79.973863636363632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50">
+        <f>B4/$K$56</f>
+        <v>7.6762619941593654E-2</v>
+      </c>
+      <c r="B4" s="58">
+        <f t="shared" si="3"/>
+        <v>368</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="12">
+        <v>7700</v>
+      </c>
+      <c r="F4" s="12">
+        <v>22.2</v>
+      </c>
+      <c r="G4" s="12">
+        <f t="shared" si="4"/>
+        <v>21.875</v>
+      </c>
+      <c r="H4" s="54">
+        <v>12</v>
+      </c>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54">
+        <v>2</v>
+      </c>
+      <c r="K4" s="43">
+        <f t="shared" si="5"/>
+        <v>58.075000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50">
+        <f>B5/$K$56</f>
+        <v>7.634543178973717E-2</v>
+      </c>
+      <c r="B5" s="58">
+        <f t="shared" si="3"/>
+        <v>366</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="12">
+        <v>9100</v>
+      </c>
+      <c r="F5" s="12">
+        <v>16</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" si="4"/>
+        <v>25.852272727272727</v>
+      </c>
+      <c r="H5" s="54">
+        <v>12</v>
+      </c>
+      <c r="I5" s="54">
         <v>1</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="J5" s="54">
         <v>2</v>
       </c>
-      <c r="F2" s="47">
-        <v>19000</v>
-      </c>
-      <c r="G2" s="49">
-        <v>39</v>
-      </c>
-      <c r="H2" s="47">
-        <f t="shared" ref="H2:H51" si="2">15*F2/5280</f>
-        <v>53.977272727272727</v>
-      </c>
-      <c r="I2" s="55">
+      <c r="K5" s="43">
+        <f t="shared" si="5"/>
+        <v>57.852272727272727</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50">
+        <f>B6/$K$56</f>
+        <v>6.07008760951189E-2</v>
+      </c>
+      <c r="B6" s="58">
+        <f t="shared" si="3"/>
+        <v>291</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="12">
+        <v>5350</v>
+      </c>
+      <c r="F6" s="12">
+        <v>28.8</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" si="4"/>
+        <v>15.198863636363637</v>
+      </c>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54">
+        <v>2</v>
+      </c>
+      <c r="K6" s="43">
+        <f t="shared" si="5"/>
+        <v>45.998863636363637</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="50">
+        <f>B7/$K$56</f>
+        <v>5.4860241969128073E-2</v>
+      </c>
+      <c r="B7" s="58">
+        <f t="shared" si="3"/>
+        <v>263</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="12">
+        <v>6750</v>
+      </c>
+      <c r="F7" s="12">
+        <v>21.4</v>
+      </c>
+      <c r="G7" s="12">
+        <f t="shared" si="4"/>
+        <v>19.176136363636363</v>
+      </c>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54">
+        <v>1</v>
+      </c>
+      <c r="K7" s="43">
+        <f t="shared" si="5"/>
+        <v>41.576136363636365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="50">
+        <f>B8/$K$56</f>
+        <v>4.630788485607009E-2</v>
+      </c>
+      <c r="B8" s="58">
+        <f t="shared" si="3"/>
+        <v>222</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="12">
+        <v>5300</v>
+      </c>
+      <c r="F8" s="12">
+        <v>8</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="4"/>
+        <v>15.056818181818182</v>
+      </c>
+      <c r="H8" s="54">
         <v>12</v>
       </c>
-      <c r="J2" s="55">
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="43">
+        <f t="shared" si="5"/>
+        <v>35.05681818181818</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="50">
+        <f>B9/$K$56</f>
+        <v>3.77555277430121E-2</v>
+      </c>
+      <c r="B9" s="58">
+        <f t="shared" si="3"/>
+        <v>181</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="12">
+        <v>5550</v>
+      </c>
+      <c r="F9" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" si="4"/>
+        <v>15.767045454545455</v>
+      </c>
+      <c r="H9" s="54">
+        <v>6</v>
+      </c>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="43">
+        <f t="shared" si="5"/>
+        <v>28.567045454545454</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="50">
+        <f>B10/$K$56</f>
+        <v>3.1497705465164789E-2</v>
+      </c>
+      <c r="B10" s="58">
+        <f t="shared" si="3"/>
+        <v>151</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="12">
+        <v>3200</v>
+      </c>
+      <c r="F10" s="12">
+        <v>14.8</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="4"/>
+        <v>9.0909090909090917</v>
+      </c>
+      <c r="H10" s="43"/>
+      <c r="K10" s="43">
+        <f t="shared" si="5"/>
+        <v>23.890909090909091</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="50">
+        <f>B11/$K$56</f>
+        <v>3.0663329161451813E-2</v>
+      </c>
+      <c r="B11" s="58">
+        <f t="shared" si="3"/>
+        <v>147</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="12">
+        <v>5000</v>
+      </c>
+      <c r="F11" s="12">
+        <v>9</v>
+      </c>
+      <c r="G11" s="12">
+        <f t="shared" si="4"/>
+        <v>14.204545454545455</v>
+      </c>
+      <c r="H11" s="43"/>
+      <c r="K11" s="43">
+        <f t="shared" si="5"/>
+        <v>23.204545454545453</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="50">
+        <f>B12/$K$56</f>
+        <v>2.9411764705882353E-2</v>
+      </c>
+      <c r="B12" s="58">
+        <f t="shared" si="3"/>
+        <v>141</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="12">
+        <v>4200</v>
+      </c>
+      <c r="F12" s="12">
+        <v>10.4</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="4"/>
+        <v>11.931818181818182</v>
+      </c>
+      <c r="H12" s="43"/>
+      <c r="K12" s="43">
+        <f t="shared" si="5"/>
+        <v>22.331818181818182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="50">
+        <f>B13/$K$56</f>
+        <v>2.6908635794743431E-2</v>
+      </c>
+      <c r="B13" s="58">
+        <f t="shared" si="3"/>
+        <v>129</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" s="69">
+        <v>4300</v>
+      </c>
+      <c r="F13" s="69">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" si="4"/>
+        <v>12.215909090909092</v>
+      </c>
+      <c r="H13" s="43"/>
+      <c r="K13" s="43">
+        <f t="shared" si="5"/>
+        <v>20.415909090909089</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="50">
+        <f>B14/$K$56</f>
+        <v>2.6282853566958697E-2</v>
+      </c>
+      <c r="B14" s="58">
+        <f t="shared" si="3"/>
+        <v>126</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="55">
-        <v>17</v>
-      </c>
-      <c r="L2" s="49">
-        <f t="shared" ref="L2:L51" si="3">H2+G2+I2 + J2*2 + K2</f>
-        <v>157.97727272727272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50">
-        <f>B3/$L$56</f>
-        <v>0.10554860241969129</v>
-      </c>
-      <c r="B3" s="58">
-        <f>ROUND(L3/$L$53*1000,0)</f>
-        <v>506</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D3" s="42" t="s">
+      <c r="E14" s="12">
+        <v>4400</v>
+      </c>
+      <c r="F14" s="12">
+        <v>7.4</v>
+      </c>
+      <c r="G14" s="12">
+        <f t="shared" si="4"/>
+        <v>12.5</v>
+      </c>
+      <c r="H14" s="43"/>
+      <c r="K14" s="43">
+        <f t="shared" si="5"/>
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="50">
+        <f>B15/$K$56</f>
+        <v>2.5031289111389236E-2</v>
+      </c>
+      <c r="B15" s="58">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="12">
+        <v>3500</v>
+      </c>
+      <c r="F15" s="12">
         <v>9</v>
       </c>
-      <c r="E3" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="12">
-        <v>8650</v>
-      </c>
-      <c r="G3" s="12">
-        <v>40.4</v>
-      </c>
-      <c r="H3" s="12">
-        <f>15*F3/5280</f>
-        <v>24.573863636363637</v>
-      </c>
-      <c r="I3" s="54">
+      <c r="G15" s="12">
+        <f t="shared" si="4"/>
+        <v>9.9431818181818183</v>
+      </c>
+      <c r="H15" s="43"/>
+      <c r="K15" s="43">
+        <f t="shared" si="5"/>
+        <v>18.94318181818182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="50">
+        <f>B16/$K$56</f>
+        <v>2.2110972048393827E-2</v>
+      </c>
+      <c r="B16" s="58">
+        <f t="shared" si="3"/>
+        <v>106</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="12">
+        <v>2950</v>
+      </c>
+      <c r="F16" s="12">
+        <v>8.4</v>
+      </c>
+      <c r="G16" s="12">
+        <f t="shared" si="4"/>
+        <v>8.3806818181818183</v>
+      </c>
+      <c r="H16" s="43"/>
+      <c r="K16" s="43">
+        <f t="shared" si="5"/>
+        <v>16.780681818181819</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="50">
+        <f>B17/$K$56</f>
+        <v>2.0442219440967878E-2</v>
+      </c>
+      <c r="B17" s="58">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="12">
+        <v>3250</v>
+      </c>
+      <c r="F17" s="12">
+        <v>6.2</v>
+      </c>
+      <c r="G17" s="12">
+        <f t="shared" si="4"/>
+        <v>9.232954545454545</v>
+      </c>
+      <c r="H17" s="43"/>
+      <c r="K17" s="43">
+        <f t="shared" si="5"/>
+        <v>15.432954545454546</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="50">
+        <f>B18/$K$56</f>
+        <v>1.6896120150187734E-2</v>
+      </c>
+      <c r="B18" s="58">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1500</v>
+      </c>
+      <c r="F18" s="12">
+        <v>8.6</v>
+      </c>
+      <c r="G18" s="12">
+        <f t="shared" si="4"/>
+        <v>4.2613636363636367</v>
+      </c>
+      <c r="H18" s="43"/>
+      <c r="K18" s="43">
+        <f t="shared" si="5"/>
+        <v>12.861363636363636</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="50">
+        <f>B19/$K$56</f>
+        <v>1.6478931998331246E-2</v>
+      </c>
+      <c r="B19" s="58">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="C19" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="68" t="s">
+        <v>182</v>
+      </c>
+      <c r="E19" s="69">
+        <v>2800</v>
+      </c>
+      <c r="F19" s="69">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G19" s="12">
+        <f t="shared" si="4"/>
+        <v>7.9545454545454541</v>
+      </c>
+      <c r="H19" s="43"/>
+      <c r="K19" s="43">
+        <f t="shared" si="5"/>
+        <v>12.554545454545455</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="50">
+        <f>B20/$K$56</f>
+        <v>1.4184397163120567E-2</v>
+      </c>
+      <c r="B20" s="58">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="12">
+        <v>775</v>
+      </c>
+      <c r="F20" s="12">
+        <v>8.6</v>
+      </c>
+      <c r="G20" s="12">
+        <f t="shared" si="4"/>
+        <v>2.2017045454545454</v>
+      </c>
+      <c r="H20" s="43"/>
+      <c r="K20" s="43">
+        <f t="shared" si="5"/>
+        <v>10.801704545454545</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="50">
+        <f>B21/$K$56</f>
+        <v>1.3350020859407593E-2</v>
+      </c>
+      <c r="B21" s="58">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="12">
+        <v>1500</v>
+      </c>
+      <c r="F21" s="12">
+        <v>5.8</v>
+      </c>
+      <c r="G21" s="12">
+        <f t="shared" si="4"/>
+        <v>4.2613636363636367</v>
+      </c>
+      <c r="H21" s="43"/>
+      <c r="K21" s="43">
+        <f t="shared" si="5"/>
+        <v>10.061363636363637</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="65" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="50">
+        <f>B22/$K$56</f>
+        <v>1.14726741760534E-2</v>
+      </c>
+      <c r="B22" s="58">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="12">
+        <v>600</v>
+      </c>
+      <c r="F22" s="12">
+        <v>7</v>
+      </c>
+      <c r="G22" s="12">
+        <f t="shared" si="4"/>
+        <v>1.7045454545454546</v>
+      </c>
+      <c r="H22" s="43"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="43">
+        <f t="shared" si="5"/>
+        <v>8.704545454545455</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="50">
+        <f>B23/$K$56</f>
+        <v>7.3007926574885276E-3</v>
+      </c>
+      <c r="B23" s="58">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="C23" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>183</v>
+      </c>
+      <c r="E23" s="69">
+        <v>700</v>
+      </c>
+      <c r="F23" s="69">
+        <v>3.6</v>
+      </c>
+      <c r="G23" s="12">
+        <f t="shared" si="4"/>
+        <v>1.9886363636363635</v>
+      </c>
+      <c r="H23" s="43"/>
+      <c r="K23" s="43">
+        <f t="shared" si="5"/>
+        <v>5.5886363636363638</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="50">
+        <f>B24/$K$56</f>
+        <v>6.4664163537755531E-3</v>
+      </c>
+      <c r="B24" s="58">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="12">
+        <v>450</v>
+      </c>
+      <c r="F24" s="12">
+        <v>3.6</v>
+      </c>
+      <c r="G24" s="12">
+        <f t="shared" si="4"/>
+        <v>1.2784090909090908</v>
+      </c>
+      <c r="H24" s="43"/>
+      <c r="K24" s="43">
+        <f t="shared" si="5"/>
+        <v>4.8784090909090914</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="63">
+        <f>B25/$K$56</f>
+        <v>6.0492282019190659E-3</v>
+      </c>
+      <c r="B25" s="64">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="C25" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="65">
+        <v>400</v>
+      </c>
+      <c r="F25" s="65">
+        <v>3.4</v>
+      </c>
+      <c r="G25" s="65">
+        <f t="shared" si="4"/>
+        <v>1.1363636363636365</v>
+      </c>
+      <c r="H25" s="67"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="67">
+        <f t="shared" si="5"/>
+        <v>4.5363636363636362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="50">
+        <f>B26/$K$56</f>
+        <v>5.6320400500625778E-3</v>
+      </c>
+      <c r="B26" s="58">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="12">
+        <v>750</v>
+      </c>
+      <c r="F26" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G26" s="12">
+        <f t="shared" si="4"/>
+        <v>2.1306818181818183</v>
+      </c>
+      <c r="H26" s="43"/>
+      <c r="K26" s="43">
+        <f t="shared" si="5"/>
+        <v>4.3306818181818185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="50">
+        <f>B27/$K$56</f>
+        <v>4.3804755944931162E-3</v>
+      </c>
+      <c r="B27" s="58">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="12">
+        <v>275</v>
+      </c>
+      <c r="F27" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G27" s="12">
+        <f t="shared" si="4"/>
+        <v>0.78125</v>
+      </c>
+      <c r="H27" s="43"/>
+      <c r="K27" s="43">
+        <f t="shared" si="5"/>
+        <v>3.28125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="50">
+        <f>B28/$K$56</f>
+        <v>3.1289111389236545E-3</v>
+      </c>
+      <c r="B28" s="58">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="C28" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="69">
+        <v>400</v>
+      </c>
+      <c r="F28" s="69">
+        <v>1.2</v>
+      </c>
+      <c r="G28" s="12">
+        <f t="shared" si="4"/>
+        <v>1.1363636363636365</v>
+      </c>
+      <c r="H28" s="43"/>
+      <c r="K28" s="43">
+        <f t="shared" si="5"/>
+        <v>2.3363636363636364</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="50">
+        <f>B29/$K$56</f>
+        <v>3.1289111389236545E-3</v>
+      </c>
+      <c r="B29" s="58">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="C29" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="68" t="s">
+        <v>184</v>
+      </c>
+      <c r="E29" s="69">
+        <v>320</v>
+      </c>
+      <c r="F29" s="69">
+        <v>1.5</v>
+      </c>
+      <c r="G29" s="12">
+        <f t="shared" si="4"/>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="H29" s="43"/>
+      <c r="K29" s="43">
+        <f t="shared" si="5"/>
+        <v>2.4090909090909092</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="50">
+        <f>B30/$K$56</f>
+        <v>2.9203170629954109E-3</v>
+      </c>
+      <c r="B30" s="58">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="12">
+        <v>150</v>
+      </c>
+      <c r="F30" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="G30" s="12">
+        <f t="shared" si="4"/>
+        <v>0.42613636363636365</v>
+      </c>
+      <c r="H30" s="43"/>
+      <c r="K30" s="43">
+        <f t="shared" si="5"/>
+        <v>2.2261363636363636</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="52">
+        <f>B31/$K$56</f>
+        <v>2.5031289111389237E-3</v>
+      </c>
+      <c r="B31" s="59">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54">
-        <v>3</v>
-      </c>
-      <c r="L3" s="43">
-        <f>H3+G3+I3 + J3*2 + K3</f>
-        <v>79.973863636363632</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50">
-        <f>B4/$L$56</f>
-        <v>7.6762619941593654E-2</v>
-      </c>
-      <c r="B4" s="58">
-        <f>ROUND(L4/$L$53*1000,0)</f>
-        <v>368</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="12">
-        <v>7700</v>
-      </c>
-      <c r="G4" s="12">
-        <v>22.2</v>
-      </c>
-      <c r="H4" s="12">
-        <f>15*F4/5280</f>
-        <v>21.875</v>
-      </c>
-      <c r="I4" s="54">
-        <v>12</v>
-      </c>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54">
-        <v>2</v>
-      </c>
-      <c r="L4" s="43">
-        <f>H4+G4+I4 + J4*2 + K4</f>
-        <v>58.075000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50">
-        <f>B5/$L$56</f>
-        <v>7.634543178973717E-2</v>
-      </c>
-      <c r="B5" s="58">
-        <f>ROUND(L5/$L$53*1000,0)</f>
-        <v>366</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="12">
-        <v>9100</v>
-      </c>
-      <c r="G5" s="12">
-        <v>16</v>
-      </c>
-      <c r="H5" s="12">
-        <f>15*F5/5280</f>
-        <v>25.852272727272727</v>
-      </c>
-      <c r="I5" s="54">
-        <v>12</v>
-      </c>
-      <c r="J5" s="54">
+      <c r="C31" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="6">
+        <v>330</v>
+      </c>
+      <c r="F31" s="6">
         <v>1</v>
       </c>
-      <c r="K5" s="54">
-        <v>2</v>
-      </c>
-      <c r="L5" s="43">
-        <f>H5+G5+I5 + J5*2 + K5</f>
-        <v>57.852272727272727</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50">
-        <f>B6/$L$56</f>
-        <v>6.07008760951189E-2</v>
-      </c>
-      <c r="B6" s="58">
-        <f>ROUND(L6/$L$53*1000,0)</f>
-        <v>291</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="12">
-        <v>5350</v>
-      </c>
-      <c r="G6" s="12">
-        <v>28.8</v>
-      </c>
-      <c r="H6" s="12">
-        <f>15*F6/5280</f>
-        <v>15.198863636363637</v>
-      </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54">
-        <v>2</v>
-      </c>
-      <c r="L6" s="43">
-        <f>H6+G6+I6 + J6*2 + K6</f>
-        <v>45.998863636363637</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50">
-        <f>B7/$L$56</f>
-        <v>5.4860241969128073E-2</v>
-      </c>
-      <c r="B7" s="58">
-        <f>ROUND(L7/$L$53*1000,0)</f>
-        <v>263</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="12">
-        <v>6750</v>
-      </c>
-      <c r="G7" s="12">
-        <v>21.4</v>
-      </c>
-      <c r="H7" s="12">
-        <f>15*F7/5280</f>
-        <v>19.176136363636363</v>
-      </c>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54">
-        <v>1</v>
-      </c>
-      <c r="L7" s="43">
-        <f>H7+G7+I7 + J7*2 + K7</f>
-        <v>41.576136363636365</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50">
-        <f>B8/$L$56</f>
-        <v>4.630788485607009E-2</v>
-      </c>
-      <c r="B8" s="58">
-        <f>ROUND(L8/$L$53*1000,0)</f>
-        <v>222</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="12">
-        <v>5300</v>
-      </c>
-      <c r="G8" s="12">
-        <v>8</v>
-      </c>
-      <c r="H8" s="12">
-        <f>15*F8/5280</f>
-        <v>15.056818181818182</v>
-      </c>
-      <c r="I8" s="54">
-        <v>12</v>
-      </c>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="43">
-        <f>H8+G8+I8 + J8*2 + K8</f>
-        <v>35.05681818181818</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50">
-        <f>B9/$L$56</f>
-        <v>3.77555277430121E-2</v>
-      </c>
-      <c r="B9" s="58">
-        <f>ROUND(L9/$L$53*1000,0)</f>
-        <v>181</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="12">
-        <v>5550</v>
-      </c>
-      <c r="G9" s="12">
-        <v>6.8</v>
-      </c>
-      <c r="H9" s="12">
-        <f>15*F9/5280</f>
-        <v>15.767045454545455</v>
-      </c>
-      <c r="I9" s="54">
-        <v>6</v>
-      </c>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="43">
-        <f>H9+G9+I9 + J9*2 + K9</f>
-        <v>28.567045454545454</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50">
-        <f>B10/$L$56</f>
-        <v>3.1497705465164789E-2</v>
-      </c>
-      <c r="B10" s="58">
-        <f>ROUND(L10/$L$53*1000,0)</f>
-        <v>151</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="12">
-        <v>3200</v>
-      </c>
-      <c r="G10" s="12">
-        <v>14.8</v>
-      </c>
-      <c r="H10" s="12">
-        <f>15*F10/5280</f>
-        <v>9.0909090909090917</v>
-      </c>
-      <c r="I10" s="43"/>
-      <c r="L10" s="43">
-        <f>H10+G10+I10 + J10*2 + K10</f>
-        <v>23.890909090909091</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50">
-        <f>B11/$L$56</f>
-        <v>3.0663329161451813E-2</v>
-      </c>
-      <c r="B11" s="58">
-        <f>ROUND(L11/$L$53*1000,0)</f>
-        <v>147</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="12">
-        <v>5000</v>
-      </c>
-      <c r="G11" s="12">
-        <v>9</v>
-      </c>
-      <c r="H11" s="12">
-        <f>15*F11/5280</f>
-        <v>14.204545454545455</v>
-      </c>
-      <c r="I11" s="43"/>
-      <c r="L11" s="43">
-        <f>H11+G11+I11 + J11*2 + K11</f>
-        <v>23.204545454545453</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50">
-        <f>B12/$L$56</f>
-        <v>2.9411764705882353E-2</v>
-      </c>
-      <c r="B12" s="58">
-        <f>ROUND(L12/$L$53*1000,0)</f>
-        <v>141</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="12">
-        <v>4200</v>
-      </c>
-      <c r="G12" s="12">
-        <v>10.4</v>
-      </c>
-      <c r="H12" s="12">
-        <f>15*F12/5280</f>
-        <v>11.931818181818182</v>
-      </c>
-      <c r="I12" s="43"/>
-      <c r="L12" s="43">
-        <f>H12+G12+I12 + J12*2 + K12</f>
-        <v>22.331818181818182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50">
-        <f>B13/$L$56</f>
-        <v>2.6908635794743431E-2</v>
-      </c>
-      <c r="B13" s="58">
-        <f>ROUND(L13/$L$53*1000,0)</f>
-        <v>129</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D13" s="68" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="68" t="s">
-        <v>185</v>
-      </c>
-      <c r="F13" s="69">
-        <v>4300</v>
-      </c>
-      <c r="G13" s="69">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H13" s="12">
-        <f>15*F13/5280</f>
-        <v>12.215909090909092</v>
-      </c>
-      <c r="I13" s="43"/>
-      <c r="L13" s="43">
-        <f>H13+G13+I13 + J13*2 + K13</f>
-        <v>20.415909090909089</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50">
-        <f>B14/$L$56</f>
-        <v>2.6282853566958697E-2</v>
-      </c>
-      <c r="B14" s="58">
-        <f>ROUND(L14/$L$53*1000,0)</f>
-        <v>126</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="12">
-        <v>4400</v>
-      </c>
-      <c r="G14" s="12">
-        <v>7.4</v>
-      </c>
-      <c r="H14" s="12">
-        <f>15*F14/5280</f>
-        <v>12.5</v>
-      </c>
-      <c r="I14" s="43"/>
-      <c r="L14" s="43">
-        <f>H14+G14+I14 + J14*2 + K14</f>
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50">
-        <f>B15/$L$56</f>
-        <v>2.5031289111389236E-2</v>
-      </c>
-      <c r="B15" s="58">
-        <f>ROUND(L15/$L$53*1000,0)</f>
-        <v>120</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="12">
-        <v>3500</v>
-      </c>
-      <c r="G15" s="12">
-        <v>9</v>
-      </c>
-      <c r="H15" s="12">
-        <f>15*F15/5280</f>
-        <v>9.9431818181818183</v>
-      </c>
-      <c r="I15" s="43"/>
-      <c r="L15" s="43">
-        <f>H15+G15+I15 + J15*2 + K15</f>
-        <v>18.94318181818182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50">
-        <f>B16/$L$56</f>
-        <v>2.2110972048393827E-2</v>
-      </c>
-      <c r="B16" s="58">
-        <f>ROUND(L16/$L$53*1000,0)</f>
-        <v>106</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="12">
-        <v>2950</v>
-      </c>
-      <c r="G16" s="12">
-        <v>8.4</v>
-      </c>
-      <c r="H16" s="12">
-        <f>15*F16/5280</f>
-        <v>8.3806818181818183</v>
-      </c>
-      <c r="I16" s="43"/>
-      <c r="L16" s="43">
-        <f>H16+G16+I16 + J16*2 + K16</f>
-        <v>16.780681818181819</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50">
-        <f>B17/$L$56</f>
-        <v>2.0442219440967878E-2</v>
-      </c>
-      <c r="B17" s="58">
-        <f>ROUND(L17/$L$53*1000,0)</f>
-        <v>98</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="12">
-        <v>3250</v>
-      </c>
-      <c r="G17" s="12">
-        <v>6.2</v>
-      </c>
-      <c r="H17" s="12">
-        <f>15*F17/5280</f>
-        <v>9.232954545454545</v>
-      </c>
-      <c r="I17" s="43"/>
-      <c r="L17" s="43">
-        <f>H17+G17+I17 + J17*2 + K17</f>
-        <v>15.432954545454546</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50">
-        <f>B18/$L$56</f>
-        <v>1.6896120150187734E-2</v>
-      </c>
-      <c r="B18" s="58">
-        <f>ROUND(L18/$L$53*1000,0)</f>
-        <v>81</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="12">
-        <v>1500</v>
-      </c>
-      <c r="G18" s="12">
-        <v>8.6</v>
-      </c>
-      <c r="H18" s="12">
-        <f>15*F18/5280</f>
-        <v>4.2613636363636367</v>
-      </c>
-      <c r="I18" s="43"/>
-      <c r="L18" s="43">
-        <f>H18+G18+I18 + J18*2 + K18</f>
-        <v>12.861363636363636</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="50">
-        <f>B19/$L$56</f>
-        <v>1.6478931998331246E-2</v>
-      </c>
-      <c r="B19" s="58">
-        <f>ROUND(L19/$L$53*1000,0)</f>
-        <v>79</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D19" s="68" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="68" t="s">
-        <v>182</v>
-      </c>
-      <c r="F19" s="69">
-        <v>2800</v>
-      </c>
-      <c r="G19" s="69">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H19" s="12">
-        <f>15*F19/5280</f>
-        <v>7.9545454545454541</v>
-      </c>
-      <c r="I19" s="43"/>
-      <c r="L19" s="43">
-        <f>H19+G19+I19 + J19*2 + K19</f>
-        <v>12.554545454545455</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50">
-        <f>B20/$L$56</f>
-        <v>1.4184397163120567E-2</v>
-      </c>
-      <c r="B20" s="58">
-        <f>ROUND(L20/$L$53*1000,0)</f>
-        <v>68</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="12">
-        <v>775</v>
-      </c>
-      <c r="G20" s="12">
-        <v>8.6</v>
-      </c>
-      <c r="H20" s="12">
-        <f>15*F20/5280</f>
-        <v>2.2017045454545454</v>
-      </c>
-      <c r="I20" s="43"/>
-      <c r="L20" s="43">
-        <f>H20+G20+I20 + J20*2 + K20</f>
-        <v>10.801704545454545</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50">
-        <f>B21/$L$56</f>
-        <v>1.3350020859407593E-2</v>
-      </c>
-      <c r="B21" s="58">
-        <f>ROUND(L21/$L$53*1000,0)</f>
-        <v>64</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="12">
-        <v>1500</v>
-      </c>
-      <c r="G21" s="12">
-        <v>5.8</v>
-      </c>
-      <c r="H21" s="12">
-        <f>15*F21/5280</f>
-        <v>4.2613636363636367</v>
-      </c>
-      <c r="I21" s="43"/>
-      <c r="L21" s="43">
-        <f>H21+G21+I21 + J21*2 + K21</f>
-        <v>10.061363636363637</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="50">
-        <f>B22/$L$56</f>
-        <v>1.14726741760534E-2</v>
-      </c>
-      <c r="B22" s="58">
-        <f>ROUND(L22/$L$53*1000,0)</f>
-        <v>55</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D22" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="12">
-        <v>600</v>
-      </c>
-      <c r="G22" s="12">
-        <v>7</v>
-      </c>
-      <c r="H22" s="12">
-        <f>15*F22/5280</f>
-        <v>1.7045454545454546</v>
-      </c>
-      <c r="I22" s="43"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="43">
-        <f>H22+G22+I22 + J22*2 + K22</f>
-        <v>8.704545454545455</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="50">
-        <f>B23/$L$56</f>
-        <v>7.3007926574885276E-3</v>
-      </c>
-      <c r="B23" s="58">
-        <f>ROUND(L23/$L$53*1000,0)</f>
-        <v>35</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D23" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="68" t="s">
-        <v>183</v>
-      </c>
-      <c r="F23" s="69">
-        <v>700</v>
-      </c>
-      <c r="G23" s="69">
-        <v>3.6</v>
-      </c>
-      <c r="H23" s="12">
-        <f>15*F23/5280</f>
-        <v>1.9886363636363635</v>
-      </c>
-      <c r="I23" s="43"/>
-      <c r="L23" s="43">
-        <f>H23+G23+I23 + J23*2 + K23</f>
-        <v>5.5886363636363638</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50">
-        <f>B24/$L$56</f>
-        <v>6.4664163537755531E-3</v>
-      </c>
-      <c r="B24" s="58">
-        <f>ROUND(L24/$L$53*1000,0)</f>
-        <v>31</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="12">
-        <v>450</v>
-      </c>
-      <c r="G24" s="12">
-        <v>3.6</v>
-      </c>
-      <c r="H24" s="12">
-        <f>15*F24/5280</f>
-        <v>1.2784090909090908</v>
-      </c>
-      <c r="I24" s="43"/>
-      <c r="L24" s="43">
-        <f>H24+G24+I24 + J24*2 + K24</f>
-        <v>4.8784090909090914</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="63">
-        <f>B25/$L$56</f>
-        <v>6.0492282019190659E-3</v>
-      </c>
-      <c r="B25" s="64">
-        <f>ROUND(L25/$L$53*1000,0)</f>
-        <v>29</v>
-      </c>
-      <c r="C25" s="65" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="65">
-        <v>400</v>
-      </c>
-      <c r="G25" s="65">
-        <v>3.4</v>
-      </c>
-      <c r="H25" s="65">
-        <f>15*F25/5280</f>
-        <v>1.1363636363636365</v>
-      </c>
-      <c r="I25" s="67"/>
-      <c r="J25" s="65"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="67">
-        <f>H25+G25+I25 + J25*2 + K25</f>
-        <v>4.5363636363636362</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50">
-        <f>B26/$L$56</f>
-        <v>5.6320400500625778E-3</v>
-      </c>
-      <c r="B26" s="58">
-        <f>ROUND(L26/$L$53*1000,0)</f>
-        <v>27</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="12">
-        <v>750</v>
-      </c>
-      <c r="G26" s="12">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H26" s="12">
-        <f>15*F26/5280</f>
-        <v>2.1306818181818183</v>
-      </c>
-      <c r="I26" s="43"/>
-      <c r="L26" s="43">
-        <f>H26+G26+I26 + J26*2 + K26</f>
-        <v>4.3306818181818185</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="50">
-        <f>B27/$L$56</f>
-        <v>4.3804755944931162E-3</v>
-      </c>
-      <c r="B27" s="58">
-        <f>ROUND(L27/$L$53*1000,0)</f>
-        <v>21</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="F27" s="12">
-        <v>275</v>
-      </c>
-      <c r="G27" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="H27" s="12">
-        <f>15*F27/5280</f>
-        <v>0.78125</v>
-      </c>
-      <c r="I27" s="43"/>
-      <c r="L27" s="43">
-        <f>H27+G27+I27 + J27*2 + K27</f>
-        <v>3.28125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="50">
-        <f>B28/$L$56</f>
-        <v>3.1289111389236545E-3</v>
-      </c>
-      <c r="B28" s="58">
-        <f>ROUND(L28/$L$53*1000,0)</f>
-        <v>15</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D28" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="69">
-        <v>400</v>
-      </c>
-      <c r="G28" s="69">
-        <v>1.2</v>
-      </c>
-      <c r="H28" s="12">
-        <f>15*F28/5280</f>
-        <v>1.1363636363636365</v>
-      </c>
-      <c r="I28" s="43"/>
-      <c r="L28" s="43">
-        <f>H28+G28+I28 + J28*2 + K28</f>
-        <v>2.3363636363636364</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="50">
-        <f>B29/$L$56</f>
-        <v>3.1289111389236545E-3</v>
-      </c>
-      <c r="B29" s="58">
-        <f>ROUND(L29/$L$53*1000,0)</f>
-        <v>15</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D29" s="68" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="68" t="s">
-        <v>184</v>
-      </c>
-      <c r="F29" s="69">
-        <v>320</v>
-      </c>
-      <c r="G29" s="69">
-        <v>1.5</v>
-      </c>
-      <c r="H29" s="12">
-        <f>15*F29/5280</f>
-        <v>0.90909090909090906</v>
-      </c>
-      <c r="I29" s="43"/>
-      <c r="L29" s="43">
-        <f>H29+G29+I29 + J29*2 + K29</f>
-        <v>2.4090909090909092</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="50">
-        <f>B30/$L$56</f>
-        <v>2.9203170629954109E-3</v>
-      </c>
-      <c r="B30" s="58">
-        <f>ROUND(L30/$L$53*1000,0)</f>
-        <v>14</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="E30" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="F30" s="12">
-        <v>150</v>
-      </c>
-      <c r="G30" s="12">
-        <v>1.8</v>
-      </c>
-      <c r="H30" s="12">
-        <f>15*F30/5280</f>
-        <v>0.42613636363636365</v>
-      </c>
-      <c r="I30" s="43"/>
-      <c r="L30" s="43">
-        <f>H30+G30+I30 + J30*2 + K30</f>
-        <v>2.2261363636363636</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="52">
-        <f>B31/$L$56</f>
-        <v>2.5031289111389237E-3</v>
-      </c>
-      <c r="B31" s="59">
-        <f>ROUND(L31/$L$53*1000,0)</f>
-        <v>12</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D31" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="6">
-        <v>330</v>
-      </c>
       <c r="G31" s="6">
-        <v>1</v>
-      </c>
-      <c r="H31" s="6">
-        <f>15*F31/5280</f>
+        <f t="shared" si="4"/>
         <v>0.9375</v>
       </c>
+      <c r="H31" s="38"/>
       <c r="I31" s="38"/>
       <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38">
-        <f>H31+G31+I31 + J31*2 + K31</f>
+      <c r="K31" s="38">
+        <f t="shared" si="5"/>
         <v>1.9375</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="50">
-        <f>B32/$L$56</f>
+        <f>B32/$K$56</f>
         <v>2.0859407592824365E-3</v>
       </c>
       <c r="B32" s="58">
-        <f>ROUND(L32/$L$53*1000,0)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>162</v>
+      <c r="C32" s="42" t="s">
+        <v>67</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="42" t="s">
         <v>68</v>
       </c>
+      <c r="E32" s="12">
+        <v>225</v>
+      </c>
       <c r="F32" s="12">
-        <v>225</v>
+        <v>1</v>
       </c>
       <c r="G32" s="12">
+        <f t="shared" si="4"/>
+        <v>0.63920454545454541</v>
+      </c>
+      <c r="H32" s="43"/>
+      <c r="K32" s="43">
+        <f t="shared" si="5"/>
+        <v>1.6392045454545454</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="50">
+        <f>B33/$K$56</f>
+        <v>1.4601585314977055E-3</v>
+      </c>
+      <c r="B33" s="58">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="12">
+        <v>230</v>
+      </c>
+      <c r="F33" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="G33" s="12">
+        <f t="shared" si="4"/>
+        <v>0.65340909090909094</v>
+      </c>
+      <c r="H33" s="43"/>
+      <c r="K33" s="43">
+        <f t="shared" si="5"/>
+        <v>1.053409090909091</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="50">
+        <f>B34/$K$56</f>
+        <v>1.0429703796412183E-3</v>
+      </c>
+      <c r="B34" s="58">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="12">
+        <v>120</v>
+      </c>
+      <c r="F34" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="G34" s="12">
+        <f t="shared" si="4"/>
+        <v>0.34090909090909088</v>
+      </c>
+      <c r="H34" s="43"/>
+      <c r="K34" s="43">
+        <f t="shared" si="5"/>
+        <v>0.74090909090909096</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="50">
+        <f>B35/$K$56</f>
+        <v>6.2578222778473093E-4</v>
+      </c>
+      <c r="B35" s="58">
+        <f t="shared" ref="B35:B51" si="6">ROUND(K35/$K$53*1000,0)</f>
+        <v>3</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="12">
+        <v>30</v>
+      </c>
+      <c r="F35" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="G35" s="12">
+        <f t="shared" ref="G35:G51" si="7">15*E35/5280</f>
+        <v>8.5227272727272721E-2</v>
+      </c>
+      <c r="H35" s="43"/>
+      <c r="K35" s="43">
+        <f t="shared" ref="K35:K66" si="8">G35+F35+H35 + I35*2 + J35</f>
+        <v>0.48522727272727273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="50">
+        <f>B36/$K$56</f>
+        <v>4.1718815185648727E-4</v>
+      </c>
+      <c r="B36" s="58">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="12">
+        <v>40</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="G36" s="12">
+        <f t="shared" si="7"/>
+        <v>0.11363636363636363</v>
+      </c>
+      <c r="H36" s="43"/>
+      <c r="K36" s="43">
+        <f t="shared" si="8"/>
+        <v>0.31363636363636366</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="50">
+        <f>B37/$K$56</f>
+        <v>4.1718815185648727E-4</v>
+      </c>
+      <c r="B37" s="58">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="12">
+        <v>50</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="G37" s="12">
+        <f t="shared" si="7"/>
+        <v>0.14204545454545456</v>
+      </c>
+      <c r="H37" s="43"/>
+      <c r="K37" s="43">
+        <f t="shared" si="8"/>
+        <v>0.29204545454545455</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="50">
+        <f>B38/$K$56</f>
+        <v>4.1718815185648727E-4</v>
+      </c>
+      <c r="B38" s="58">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" s="12">
+        <v>20</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="G38" s="12">
+        <f t="shared" si="7"/>
+        <v>5.6818181818181816E-2</v>
+      </c>
+      <c r="H38" s="43"/>
+      <c r="K38" s="43">
+        <f t="shared" si="8"/>
+        <v>0.35681818181818181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="50">
+        <f>B39/$K$56</f>
+        <v>2.0859407592824363E-4</v>
+      </c>
+      <c r="B39" s="58">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="H32" s="12">
-        <f>15*F32/5280</f>
-        <v>0.63920454545454541</v>
-      </c>
-      <c r="I32" s="43"/>
-      <c r="L32" s="43">
-        <f>H32+G32+I32 + J32*2 + K32</f>
-        <v>1.6392045454545454</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="50">
-        <f>B33/$L$56</f>
-        <v>1.4601585314977055E-3</v>
-      </c>
-      <c r="B33" s="58">
-        <f>ROUND(L33/$L$53*1000,0)</f>
-        <v>7</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="12">
-        <v>230</v>
-      </c>
-      <c r="G33" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="H33" s="12">
-        <f>15*F33/5280</f>
-        <v>0.65340909090909094</v>
-      </c>
-      <c r="I33" s="43"/>
-      <c r="L33" s="43">
-        <f>H33+G33+I33 + J33*2 + K33</f>
-        <v>1.053409090909091</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="50">
-        <f>B34/$L$56</f>
-        <v>1.0429703796412183E-3</v>
-      </c>
-      <c r="B34" s="58">
-        <f>ROUND(L34/$L$53*1000,0)</f>
-        <v>5</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="D34" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="F34" s="12">
-        <v>120</v>
-      </c>
-      <c r="G34" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="H34" s="12">
-        <f>15*F34/5280</f>
-        <v>0.34090909090909088</v>
-      </c>
-      <c r="I34" s="43"/>
-      <c r="L34" s="43">
-        <f>H34+G34+I34 + J34*2 + K34</f>
-        <v>0.74090909090909096</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="50">
-        <f>B35/$L$56</f>
-        <v>6.2578222778473093E-4</v>
-      </c>
-      <c r="B35" s="58">
-        <f>ROUND(L35/$L$53*1000,0)</f>
-        <v>3</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D35" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="E35" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="F35" s="12">
-        <v>30</v>
-      </c>
-      <c r="G35" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="H35" s="12">
-        <f>15*F35/5280</f>
-        <v>8.5227272727272721E-2</v>
-      </c>
-      <c r="I35" s="43"/>
-      <c r="L35" s="43">
-        <f>H35+G35+I35 + J35*2 + K35</f>
-        <v>0.48522727272727273</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="50">
-        <f>B36/$L$56</f>
-        <v>4.1718815185648727E-4</v>
-      </c>
-      <c r="B36" s="58">
-        <f>ROUND(L36/$L$53*1000,0)</f>
-        <v>2</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="D36" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="F36" s="12">
-        <v>40</v>
-      </c>
-      <c r="G36" s="12">
+      <c r="C39" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="12">
+        <v>0</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="G39" s="12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="43"/>
+      <c r="K39" s="43">
+        <f t="shared" si="8"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="50">
+        <f>B40/$K$56</f>
+        <v>2.0859407592824363E-4</v>
+      </c>
+      <c r="B40" s="58">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="12">
+        <v>0</v>
+      </c>
+      <c r="F40" s="12">
         <v>0.2</v>
       </c>
-      <c r="H36" s="12">
-        <f>15*F36/5280</f>
-        <v>0.11363636363636363</v>
-      </c>
-      <c r="I36" s="43"/>
-      <c r="L36" s="43">
-        <f>H36+G36+I36 + J36*2 + K36</f>
-        <v>0.31363636363636366</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="50">
-        <f>B37/$L$56</f>
-        <v>4.1718815185648727E-4</v>
-      </c>
-      <c r="B37" s="58">
-        <f>ROUND(L37/$L$53*1000,0)</f>
-        <v>2</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D37" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="F37" s="12">
-        <v>50</v>
-      </c>
-      <c r="G37" s="12">
-        <v>0.15</v>
-      </c>
-      <c r="H37" s="12">
-        <f>15*F37/5280</f>
-        <v>0.14204545454545456</v>
-      </c>
-      <c r="I37" s="43"/>
-      <c r="L37" s="43">
-        <f>H37+G37+I37 + J37*2 + K37</f>
-        <v>0.29204545454545455</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="50">
-        <f>B38/$L$56</f>
-        <v>4.1718815185648727E-4</v>
-      </c>
-      <c r="B38" s="58">
-        <f>ROUND(L38/$L$53*1000,0)</f>
-        <v>2</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D38" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="12">
-        <v>20</v>
-      </c>
-      <c r="G38" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="H38" s="12">
-        <f>15*F38/5280</f>
-        <v>5.6818181818181816E-2</v>
-      </c>
-      <c r="I38" s="43"/>
-      <c r="L38" s="43">
-        <f>H38+G38+I38 + J38*2 + K38</f>
-        <v>0.35681818181818181</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="50">
-        <f>B39/$L$56</f>
-        <v>2.0859407592824363E-4</v>
-      </c>
-      <c r="B39" s="58">
-        <f>ROUND(L39/$L$53*1000,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D39" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="E39" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="F39" s="12">
-        <v>0</v>
-      </c>
-      <c r="G39" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="H39" s="12">
-        <f>15*F39/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I39" s="43"/>
-      <c r="L39" s="43">
-        <f>H39+G39+I39 + J39*2 + K39</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="50">
-        <f>B40/$L$56</f>
-        <v>2.0859407592824363E-4</v>
-      </c>
-      <c r="B40" s="58">
-        <f>ROUND(L40/$L$53*1000,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D40" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="E40" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="F40" s="12">
-        <v>0</v>
-      </c>
       <c r="G40" s="12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="43"/>
+      <c r="K40" s="43">
+        <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
-      <c r="H40" s="12">
-        <f>15*F40/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="43"/>
-      <c r="L40" s="43">
-        <f>H40+G40+I40 + J40*2 + K40</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="53">
-        <f>B41/$L$56</f>
+        <f>B41/$K$56</f>
         <v>0</v>
       </c>
       <c r="B41" s="60">
-        <f>ROUND(L41/$L$53*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C41" s="44" t="s">
-        <v>162</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C41" s="45" t="s">
+        <v>69</v>
       </c>
       <c r="D41" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="45" t="s">
         <v>70</v>
       </c>
+      <c r="E41" s="44">
+        <v>0</v>
+      </c>
       <c r="F41" s="44">
         <v>0</v>
       </c>
       <c r="G41" s="44">
-        <v>0</v>
-      </c>
-      <c r="H41" s="44">
-        <f>15*F41/5280</f>
-        <v>0</v>
-      </c>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H41" s="46"/>
       <c r="I41" s="46"/>
       <c r="J41" s="46"/>
-      <c r="K41" s="46"/>
-      <c r="L41" s="46">
-        <f>H41+G41+I41 + J41*2 + K41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K41" s="46">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="50">
-        <f>B42/$L$56</f>
+        <f>B42/$K$56</f>
         <v>0</v>
       </c>
       <c r="B42" s="58">
-        <f>ROUND(L42/$L$53*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>164</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C42" s="42" t="s">
+        <v>97</v>
       </c>
       <c r="D42" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="E42" s="42" t="s">
         <v>98</v>
       </c>
+      <c r="E42" s="12">
+        <v>0</v>
+      </c>
       <c r="F42" s="12">
         <v>0</v>
       </c>
       <c r="G42" s="12">
-        <v>0</v>
-      </c>
-      <c r="H42" s="12">
-        <f>15*F42/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I42" s="43"/>
-      <c r="L42" s="43">
-        <f>H42+G42+I42 + J42*2 + K42</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H42" s="43"/>
+      <c r="K42" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="50">
-        <f>B43/$L$56</f>
+        <f>B43/$K$56</f>
         <v>0</v>
       </c>
       <c r="B43" s="58">
-        <f>ROUND(L43/$L$53*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>164</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C43" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="D43" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="E43" s="42" t="s">
         <v>100</v>
       </c>
+      <c r="E43" s="12">
+        <v>0</v>
+      </c>
       <c r="F43" s="12">
         <v>0</v>
       </c>
       <c r="G43" s="12">
-        <v>0</v>
-      </c>
-      <c r="H43" s="12">
-        <f>15*F43/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I43" s="43"/>
-      <c r="L43" s="43">
-        <f>H43+G43+I43 + J43*2 + K43</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="43"/>
+      <c r="K43" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="50">
-        <f>B44/$L$56</f>
+        <f>B44/$K$56</f>
         <v>0</v>
       </c>
       <c r="B44" s="58">
-        <f>ROUND(L44/$L$53*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>164</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C44" s="42" t="s">
+        <v>87</v>
       </c>
       <c r="D44" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="E44" s="42" t="s">
         <v>88</v>
       </c>
+      <c r="E44" s="12">
+        <v>0</v>
+      </c>
       <c r="F44" s="12">
         <v>0</v>
       </c>
       <c r="G44" s="12">
-        <v>0</v>
-      </c>
-      <c r="H44" s="12">
-        <f>15*F44/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I44" s="43"/>
-      <c r="L44" s="43">
-        <f>H44+G44+I44 + J44*2 + K44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="43"/>
+      <c r="K44" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="50">
-        <f>B45/$L$56</f>
+        <f>B45/$K$56</f>
         <v>0</v>
       </c>
       <c r="B45" s="58">
-        <f>ROUND(L45/$L$53*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>164</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>83</v>
       </c>
       <c r="D45" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="E45" s="42" t="s">
         <v>84</v>
       </c>
+      <c r="E45" s="12">
+        <v>0</v>
+      </c>
       <c r="F45" s="12">
         <v>0</v>
       </c>
       <c r="G45" s="12">
-        <v>0</v>
-      </c>
-      <c r="H45" s="12">
-        <f>15*F45/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I45" s="43"/>
-      <c r="L45" s="43">
-        <f>H45+G45+I45 + J45*2 + K45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H45" s="43"/>
+      <c r="K45" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="50">
-        <f>B46/$L$56</f>
+        <f>B46/$K$56</f>
         <v>0</v>
       </c>
       <c r="B46" s="58">
-        <f>ROUND(L46/$L$53*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>164</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C46" s="42" t="s">
+        <v>55</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="E46" s="42" t="s">
         <v>56</v>
       </c>
+      <c r="E46" s="12">
+        <v>0</v>
+      </c>
       <c r="F46" s="12">
         <v>0</v>
       </c>
       <c r="G46" s="12">
-        <v>0</v>
-      </c>
-      <c r="H46" s="12">
-        <f>15*F46/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I46" s="43"/>
-      <c r="L46" s="43">
-        <f>H46+G46+I46 + J46*2 + K46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H46" s="43"/>
+      <c r="K46" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="50">
-        <f>B47/$L$56</f>
+        <f>B47/$K$56</f>
         <v>0</v>
       </c>
       <c r="B47" s="58">
-        <f>ROUND(L47/$L$53*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>163</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C47" s="42" t="s">
+        <v>75</v>
       </c>
       <c r="D47" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="E47" s="42" t="s">
         <v>76</v>
       </c>
+      <c r="E47" s="12">
+        <v>0</v>
+      </c>
       <c r="F47" s="12">
         <v>0</v>
       </c>
       <c r="G47" s="12">
-        <v>0</v>
-      </c>
-      <c r="H47" s="12">
-        <f>15*F47/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I47" s="43"/>
-      <c r="L47" s="43">
-        <f>H47+G47+I47 + J47*2 + K47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H47" s="43"/>
+      <c r="K47" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="50">
-        <f>B48/$L$56</f>
+        <f>B48/$K$56</f>
         <v>0</v>
       </c>
       <c r="B48" s="58">
-        <f>ROUND(L48/$L$53*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>163</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C48" s="42" t="s">
+        <v>93</v>
       </c>
       <c r="D48" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="E48" s="42" t="s">
         <v>94</v>
       </c>
+      <c r="E48" s="12">
+        <v>0</v>
+      </c>
       <c r="F48" s="12">
         <v>0</v>
       </c>
       <c r="G48" s="12">
-        <v>0</v>
-      </c>
-      <c r="H48" s="12">
-        <f>15*F48/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I48" s="43"/>
-      <c r="L48" s="43">
-        <f>H48+G48+I48 + J48*2 + K48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H48" s="43"/>
+      <c r="K48" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="50">
-        <f>B49/$L$56</f>
+        <f>B49/$K$56</f>
         <v>0</v>
       </c>
       <c r="B49" s="58">
-        <f>ROUND(L49/$L$53*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>164</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C49" s="42" t="s">
+        <v>39</v>
       </c>
       <c r="D49" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="E49" s="42" t="s">
         <v>40</v>
       </c>
+      <c r="E49" s="12">
+        <v>0</v>
+      </c>
       <c r="F49" s="12">
         <v>0</v>
       </c>
       <c r="G49" s="12">
-        <v>0</v>
-      </c>
-      <c r="H49" s="12">
-        <f>15*F49/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I49" s="43"/>
-      <c r="L49" s="43">
-        <f>H49+G49+I49 + J49*2 + K49</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H49" s="43"/>
+      <c r="K49" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="50">
-        <f>B50/$L$56</f>
+        <f>B50/$K$56</f>
         <v>0</v>
       </c>
       <c r="B50" s="58">
-        <f>ROUND(L50/$L$53*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>163</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>85</v>
       </c>
       <c r="D50" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="E50" s="42" t="s">
         <v>86</v>
       </c>
+      <c r="E50" s="12">
+        <v>0</v>
+      </c>
       <c r="F50" s="12">
         <v>0</v>
       </c>
       <c r="G50" s="12">
-        <v>0</v>
-      </c>
-      <c r="H50" s="12">
-        <f>15*F50/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I50" s="43"/>
-      <c r="L50" s="43">
-        <f>H50+G50+I50 + J50*2 + K50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H50" s="43"/>
+      <c r="K50" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="50">
-        <f>B51/$L$56</f>
+        <f>B51/$K$56</f>
         <v>0</v>
       </c>
       <c r="B51" s="58">
-        <f>ROUND(L51/$L$53*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>163</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C51" s="42" t="s">
+        <v>65</v>
       </c>
       <c r="D51" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="E51" s="42" t="s">
         <v>66</v>
       </c>
+      <c r="E51" s="12">
+        <v>0</v>
+      </c>
       <c r="F51" s="12">
         <v>0</v>
       </c>
       <c r="G51" s="12">
-        <v>0</v>
-      </c>
-      <c r="H51" s="12">
-        <f>15*F51/5280</f>
-        <v>0</v>
-      </c>
-      <c r="I51" s="43"/>
-      <c r="L51" s="43">
-        <f>H51+G51+I51 + J51*2 + K51</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H51" s="43"/>
+      <c r="K51" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B52" s="61"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="43"/>
-      <c r="L52" s="36">
-        <f>SUM(L2:L51)</f>
+      <c r="H52" s="36"/>
+      <c r="I52" s="43"/>
+      <c r="K52" s="36">
+        <f>SUM(K2:K51)</f>
         <v>757.66647727272755</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B53" s="58"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="43"/>
-      <c r="L53" s="36">
-        <f>MAX(L2:L51)</f>
+      <c r="H53" s="36"/>
+      <c r="I53" s="43"/>
+      <c r="K53" s="36">
+        <f>MAX(K2:K51)</f>
         <v>157.97727272727272</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B54" s="61"/>
-      <c r="L54" s="36"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K54" s="36"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B55" s="61"/>
-      <c r="D55"/>
-      <c r="L55" s="36"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C55"/>
+      <c r="K55" s="36"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B56" s="61"/>
-      <c r="L56" s="36">
+      <c r="K56" s="36">
         <f>SUM(B2:B51)</f>
         <v>4794</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B57" s="61"/>
-      <c r="I57" s="36"/>
-      <c r="L57" s="36"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H57" s="36"/>
+      <c r="K57" s="36"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B58" s="61"/>
-      <c r="L58" s="36"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K58" s="36"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B59" s="61"/>
-      <c r="L59" s="36"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K59" s="36"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B60" s="61"/>
-      <c r="L60" s="36"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K60" s="36"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B61" s="61"/>
-      <c r="L61" s="36"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K61" s="36"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B62" s="61"/>
-      <c r="L62" s="36"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K62" s="36"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B63" s="61"/>
-      <c r="L63" s="36"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K63" s="36"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B64" s="61"/>
-      <c r="L64" s="36"/>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K64" s="36"/>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B65" s="61"/>
-      <c r="L65" s="36"/>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K65" s="36"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B66" s="61"/>
-      <c r="L66" s="36"/>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K66" s="36"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B67" s="61"/>
-      <c r="L67" s="36"/>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="D68" s="37" t="s">
+      <c r="K67" s="36"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C68" s="37" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="D69" s="37" t="s">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C69" s="37" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B71" s="61"/>
-      <c r="D71" s="37" t="s">
+      <c r="C71" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L71" s="36"/>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K71" s="36"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B72" s="61"/>
-      <c r="D72" s="37" t="s">
+      <c r="C72" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="L72" s="36"/>
-    </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K72" s="36"/>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B73" s="61"/>
-      <c r="D73" s="37" t="s">
+      <c r="C73" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="L73" s="36"/>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K73" s="36"/>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B74" s="61"/>
-      <c r="D74" s="37" t="s">
+      <c r="C74" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="L74" s="36"/>
-    </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K74" s="36"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B75" s="61"/>
-      <c r="L75" s="36"/>
-    </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K75" s="36"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B76" s="61"/>
-      <c r="D76" s="37" t="s">
+      <c r="C76" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="L76" s="36"/>
-    </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K76" s="36"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B77" s="61"/>
-      <c r="L77" s="36"/>
-    </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K77" s="36"/>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B78" s="61"/>
-      <c r="D78" s="37" t="s">
+      <c r="C78" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="L78" s="36"/>
-    </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K78" s="36"/>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B79" s="61"/>
-      <c r="L79" s="36"/>
-    </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K79" s="36"/>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B80" s="61"/>
-      <c r="L80" s="36"/>
-    </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K80" s="36"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B81" s="61"/>
-      <c r="L81" s="36"/>
-    </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K81" s="36"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B82" s="61"/>
-      <c r="L82" s="36"/>
-    </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K82" s="36"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B83" s="61"/>
-      <c r="L83" s="36"/>
-    </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K83" s="36"/>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B84" s="61"/>
-      <c r="L84" s="36"/>
-    </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K84" s="36"/>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B85" s="61"/>
-      <c r="L85" s="36"/>
-    </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K85" s="36"/>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B86" s="61"/>
-      <c r="L86" s="36"/>
-    </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K86" s="36"/>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B87" s="61"/>
-      <c r="L87" s="36"/>
-    </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K87" s="36"/>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B88" s="61"/>
-      <c r="L88" s="36"/>
+      <c r="K88" s="36"/>
     </row>
   </sheetData>
   <sortState ref="A3:L51">
     <sortCondition descending="1" ref="B3:B51"/>
-    <sortCondition ref="D3:D51"/>
+    <sortCondition ref="C3:C51"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2">
+        <v>19000</v>
+      </c>
+      <c r="D2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3">
+        <v>8650</v>
+      </c>
+      <c r="D3">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4">
+        <v>7700</v>
+      </c>
+      <c r="D4">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5">
+        <v>9100</v>
+      </c>
+      <c r="D5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6">
+        <v>5350</v>
+      </c>
+      <c r="D6">
+        <v>28.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7">
+        <v>6750</v>
+      </c>
+      <c r="D7">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8">
+        <v>5300</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9">
+        <v>5550</v>
+      </c>
+      <c r="D9">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C10">
+        <v>3200</v>
+      </c>
+      <c r="D10">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11">
+        <v>5000</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12">
+        <v>4200</v>
+      </c>
+      <c r="D12">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C13">
+        <v>4300</v>
+      </c>
+      <c r="D13">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B14" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14">
+        <v>4400</v>
+      </c>
+      <c r="D14">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15">
+        <v>3500</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16">
+        <v>2950</v>
+      </c>
+      <c r="D16">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" t="s">
+        <v>237</v>
+      </c>
+      <c r="C17">
+        <v>3250</v>
+      </c>
+      <c r="D17">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B18" t="s">
+        <v>238</v>
+      </c>
+      <c r="C18">
+        <v>1500</v>
+      </c>
+      <c r="D18">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>203</v>
+      </c>
+      <c r="B19" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19">
+        <v>2800</v>
+      </c>
+      <c r="D19">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>204</v>
+      </c>
+      <c r="B20" t="s">
+        <v>240</v>
+      </c>
+      <c r="C20">
+        <v>775</v>
+      </c>
+      <c r="D20">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C21">
+        <v>1500</v>
+      </c>
+      <c r="D21">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22">
+        <v>600</v>
+      </c>
+      <c r="D22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" t="s">
+        <v>243</v>
+      </c>
+      <c r="C23">
+        <v>700</v>
+      </c>
+      <c r="D23">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>208</v>
+      </c>
+      <c r="B24" t="s">
+        <v>244</v>
+      </c>
+      <c r="C24">
+        <v>450</v>
+      </c>
+      <c r="D24">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>209</v>
+      </c>
+      <c r="B25" t="s">
+        <v>245</v>
+      </c>
+      <c r="C25">
+        <v>400</v>
+      </c>
+      <c r="D25">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B26" t="s">
+        <v>246</v>
+      </c>
+      <c r="C26">
+        <v>750</v>
+      </c>
+      <c r="D26">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" t="s">
+        <v>247</v>
+      </c>
+      <c r="C27">
+        <v>275</v>
+      </c>
+      <c r="D27">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" t="s">
+        <v>248</v>
+      </c>
+      <c r="C28">
+        <v>400</v>
+      </c>
+      <c r="D28">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" t="s">
+        <v>249</v>
+      </c>
+      <c r="C29">
+        <v>320</v>
+      </c>
+      <c r="D29">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>213</v>
+      </c>
+      <c r="B30" t="s">
+        <v>250</v>
+      </c>
+      <c r="C30">
+        <v>150</v>
+      </c>
+      <c r="D30">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>214</v>
+      </c>
+      <c r="B31" t="s">
+        <v>251</v>
+      </c>
+      <c r="C31">
+        <v>330</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>215</v>
+      </c>
+      <c r="B32" t="s">
+        <v>252</v>
+      </c>
+      <c r="C32">
+        <v>225</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C33">
+        <v>230</v>
+      </c>
+      <c r="D33">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>217</v>
+      </c>
+      <c r="B34" t="s">
+        <v>254</v>
+      </c>
+      <c r="C34">
+        <v>120</v>
+      </c>
+      <c r="D34">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>218</v>
+      </c>
+      <c r="B35" t="s">
+        <v>255</v>
+      </c>
+      <c r="C35">
+        <v>30</v>
+      </c>
+      <c r="D35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>219</v>
+      </c>
+      <c r="B36" t="s">
+        <v>256</v>
+      </c>
+      <c r="C36">
+        <v>40</v>
+      </c>
+      <c r="D36">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>219</v>
+      </c>
+      <c r="B37" t="s">
+        <v>257</v>
+      </c>
+      <c r="C37">
+        <v>50</v>
+      </c>
+      <c r="D37">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>219</v>
+      </c>
+      <c r="B38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C38">
+        <v>20</v>
+      </c>
+      <c r="D38">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>220</v>
+      </c>
+      <c r="B39" t="s">
+        <v>259</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>220</v>
+      </c>
+      <c r="B40" t="s">
+        <v>260</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>261</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>262</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>263</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>264</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>265</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>266</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>267</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>268</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>269</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>270</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>271</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
KS and OK trip cost
</commit_message>
<xml_diff>
--- a/Walter/TripReports/STATE HIGH POINTS.xlsx
+++ b/Walter/TripReports/STATE HIGH POINTS.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\websites\slnWalter\Walter\TripReports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D852B3A4-2428-47D0-9C35-347858489855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2028" windowWidth="19296" windowHeight="10896"/>
+    <workbookView xWindow="3930" yWindow="2040" windowWidth="21600" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HighPoint Log" sheetId="1" r:id="rId1"/>
     <sheet name="Effort Scale" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="170">
   <si>
     <t>State</t>
   </si>
@@ -525,12 +531,21 @@
   </si>
   <si>
     <t>HP#09</t>
+  </si>
+  <si>
+    <t>with OK</t>
+  </si>
+  <si>
+    <t>HP#30</t>
+  </si>
+  <si>
+    <t>HP#31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
@@ -909,7 +924,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -942,9 +957,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -977,6 +1009,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1152,25 +1201,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="12" customWidth="1"/>
-    <col min="9" max="33" width="8.88671875" style="12"/>
+    <col min="2" max="2" width="16.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" style="12" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="12" customWidth="1"/>
+    <col min="9" max="33" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>101</v>
       </c>
@@ -1247,7 +1296,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="70">
         <v>24</v>
       </c>
@@ -1273,7 +1322,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>32</v>
       </c>
@@ -1297,7 +1346,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>21</v>
       </c>
@@ -1347,7 +1396,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1394,7 +1443,7 @@
       <c r="AF7" s="12"/>
       <c r="AG7" s="12"/>
     </row>
-    <row r="8" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>11</v>
       </c>
@@ -1418,7 +1467,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -1442,7 +1491,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>13</v>
       </c>
@@ -1466,7 +1515,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1490,7 +1539,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -1514,7 +1563,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -1538,7 +1587,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1562,7 +1611,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>8</v>
       </c>
@@ -1586,7 +1635,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1610,7 +1659,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1637,7 +1686,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:33" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -1686,7 +1735,7 @@
       <c r="AF18" s="12"/>
       <c r="AG18" s="12"/>
     </row>
-    <row r="19" spans="1:33" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>20</v>
       </c>
@@ -1737,7 +1786,7 @@
       <c r="AF19" s="12"/>
       <c r="AG19" s="12"/>
     </row>
-    <row r="20" spans="1:33" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1784,7 +1833,7 @@
       <c r="AF20" s="12"/>
       <c r="AG20" s="12"/>
     </row>
-    <row r="21" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>30</v>
       </c>
@@ -1805,7 +1854,7 @@
       </c>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>22</v>
       </c>
@@ -1832,7 +1881,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>18</v>
       </c>
@@ -1853,7 +1902,7 @@
       </c>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>26</v>
       </c>
@@ -1874,7 +1923,7 @@
       </c>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>31</v>
       </c>
@@ -1895,7 +1944,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>29</v>
       </c>
@@ -1922,7 +1971,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>25</v>
       </c>
@@ -1943,7 +1992,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>17</v>
       </c>
@@ -1964,7 +2013,7 @@
       </c>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -1985,7 +2034,7 @@
       </c>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>19</v>
       </c>
@@ -2006,10 +2055,13 @@
       </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>28</v>
       </c>
+      <c r="B31" s="12" t="s">
+        <v>168</v>
+      </c>
       <c r="C31" s="8" t="s">
         <v>55</v>
       </c>
@@ -2023,11 +2075,20 @@
         <v>43822</v>
       </c>
       <c r="G31" s="11"/>
-    </row>
-    <row r="32" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="19">
+        <v>699</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>23</v>
       </c>
+      <c r="B32" s="12" t="s">
+        <v>169</v>
+      </c>
       <c r="C32" s="8" t="s">
         <v>45</v>
       </c>
@@ -2042,7 +2103,7 @@
       </c>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="1:33" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:33" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>35</v>
       </c>
@@ -2058,7 +2119,7 @@
       <c r="F33" s="15"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>34</v>
       </c>
@@ -2074,7 +2135,7 @@
       <c r="F34" s="15"/>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>36</v>
       </c>
@@ -2117,7 +2178,7 @@
       <c r="AF35" s="12"/>
       <c r="AG35" s="12"/>
     </row>
-    <row r="36" spans="1:33" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:33" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>49</v>
       </c>
@@ -2133,7 +2194,7 @@
       <c r="F36" s="15"/>
       <c r="G36" s="11"/>
     </row>
-    <row r="37" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>51</v>
       </c>
@@ -2176,7 +2237,7 @@
       <c r="AF37" s="12"/>
       <c r="AG37" s="12"/>
     </row>
-    <row r="38" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>6</v>
       </c>
@@ -2219,7 +2280,7 @@
       <c r="AF38" s="12"/>
       <c r="AG38" s="12"/>
     </row>
-    <row r="39" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>45</v>
       </c>
@@ -2262,7 +2323,7 @@
       <c r="AF39" s="12"/>
       <c r="AG39" s="12"/>
     </row>
-    <row r="40" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>44</v>
       </c>
@@ -2305,7 +2366,7 @@
       <c r="AF40" s="12"/>
       <c r="AG40" s="12"/>
     </row>
-    <row r="41" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>42</v>
       </c>
@@ -2348,7 +2409,7 @@
       <c r="AF41" s="12"/>
       <c r="AG41" s="12"/>
     </row>
-    <row r="43" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>48</v>
       </c>
@@ -2391,7 +2452,7 @@
       <c r="AF43" s="12"/>
       <c r="AG43" s="12"/>
     </row>
-    <row r="44" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>38</v>
       </c>
@@ -2434,7 +2495,7 @@
       <c r="AF44" s="12"/>
       <c r="AG44" s="12"/>
     </row>
-    <row r="45" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>37</v>
       </c>
@@ -2477,7 +2538,7 @@
       <c r="AF45" s="12"/>
       <c r="AG45" s="12"/>
     </row>
-    <row r="46" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>47</v>
       </c>
@@ -2520,7 +2581,7 @@
       <c r="AF46" s="12"/>
       <c r="AG46" s="12"/>
     </row>
-    <row r="47" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>41</v>
       </c>
@@ -2563,7 +2624,7 @@
       <c r="AF47" s="12"/>
       <c r="AG47" s="12"/>
     </row>
-    <row r="48" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>40</v>
       </c>
@@ -2606,7 +2667,7 @@
       <c r="AF48" s="12"/>
       <c r="AG48" s="12"/>
     </row>
-    <row r="49" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>43</v>
       </c>
@@ -2649,7 +2710,7 @@
       <c r="AF49" s="12"/>
       <c r="AG49" s="12"/>
     </row>
-    <row r="51" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>33</v>
       </c>
@@ -2692,7 +2753,7 @@
       <c r="AF51" s="12"/>
       <c r="AG51" s="12"/>
     </row>
-    <row r="52" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>46</v>
       </c>
@@ -2735,7 +2796,7 @@
       <c r="AF52" s="12"/>
       <c r="AG52" s="12"/>
     </row>
-    <row r="53" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="65">
         <v>39</v>
       </c>
@@ -2778,7 +2839,7 @@
       <c r="AF53" s="12"/>
       <c r="AG53" s="12"/>
     </row>
-    <row r="54" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="12"/>
       <c r="C54" s="8"/>
@@ -2813,151 +2874,151 @@
       <c r="AF54" s="12"/>
       <c r="AG54" s="12"/>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F55" s="13"/>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F56" s="13"/>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F57" s="13"/>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F58" s="13"/>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F59" s="13"/>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F60" s="13"/>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F61" s="13"/>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F62" s="13"/>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F63" s="13"/>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F64" s="13"/>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F65" s="13"/>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F66" s="13"/>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F67" s="13"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F68" s="13"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F69" s="13"/>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F70" s="13"/>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F71" s="13"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F72" s="13"/>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F73" s="13"/>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F74" s="13"/>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F75" s="13"/>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F76" s="13"/>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F77" s="13"/>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F78" s="13"/>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F79" s="13"/>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F80" s="13"/>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F81" s="13"/>
     </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F82" s="13"/>
     </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F83" s="13"/>
     </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F84" s="13"/>
     </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F85" s="13"/>
     </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F86" s="13"/>
     </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F87" s="13"/>
     </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F88" s="13"/>
     </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F89" s="13"/>
     </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F90" s="13"/>
     </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F91" s="13"/>
     </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F92" s="13"/>
     </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F93" s="13"/>
     </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F94" s="13"/>
     </row>
-    <row r="95" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F95" s="13"/>
     </row>
-    <row r="96" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F96" s="13"/>
     </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F97" s="13"/>
     </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F98" s="13"/>
     </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F99" s="13"/>
     </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F100" s="13"/>
     </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F101" s="13"/>
     </row>
-    <row r="102" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F102" s="13"/>
     </row>
-    <row r="103" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F103" s="13"/>
     </row>
   </sheetData>
@@ -2970,30 +3031,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="59" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="34" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="34" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
-    <col min="12" max="12" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="59" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="34" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="38" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>141</v>
       </c>
@@ -3031,7 +3092,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48">
         <f t="shared" ref="A2:A33" si="0">B2/$L$56</f>
         <v>0.21963540522732264</v>
@@ -3073,7 +3134,7 @@
         <v>157.97727272727272</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="47">
         <f t="shared" si="0"/>
         <v>0.11113551504502525</v>
@@ -3113,7 +3174,7 @@
         <v>79.973863636363632</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47">
         <f t="shared" si="0"/>
         <v>8.0825829123654727E-2</v>
@@ -3153,7 +3214,7 @@
         <v>58.075000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47">
         <f t="shared" si="0"/>
         <v>8.0386558313200088E-2</v>
@@ -3195,7 +3256,7 @@
         <v>57.852272727272727</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47">
         <f t="shared" si="0"/>
         <v>6.3913902921150886E-2</v>
@@ -3233,7 +3294,7 @@
         <v>45.998863636363637</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47">
         <f t="shared" si="0"/>
         <v>5.7764111574785858E-2</v>
@@ -3271,7 +3332,7 @@
         <v>41.576136363636365</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47">
         <f t="shared" si="0"/>
         <v>4.8759059960465624E-2</v>
@@ -3309,7 +3370,7 @@
         <v>35.05681818181818</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47">
         <f t="shared" si="0"/>
         <v>3.9754008346145397E-2</v>
@@ -3347,7 +3408,7 @@
         <v>28.567045454545454</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="47">
         <f t="shared" si="0"/>
         <v>3.3164946189325722E-2</v>
@@ -3415,7 +3476,7 @@
         <v>23.204545454545453</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47">
         <f t="shared" si="0"/>
         <v>3.0968592137052494E-2</v>
@@ -3449,7 +3510,7 @@
         <v>22.331818181818182</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47">
         <f t="shared" si="0"/>
         <v>2.7674061058642653E-2</v>
@@ -3483,7 +3544,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47">
         <f t="shared" si="0"/>
         <v>2.6356248627278717E-2</v>
@@ -3517,7 +3578,7 @@
         <v>18.94318181818182</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47">
         <f t="shared" si="0"/>
         <v>2.32813529540962E-2</v>
@@ -3551,7 +3612,7 @@
         <v>16.780681818181819</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47">
         <f t="shared" si="0"/>
         <v>2.1524269712277617E-2</v>
@@ -3585,7 +3646,7 @@
         <v>15.432954545454546</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="47">
         <f t="shared" si="0"/>
         <v>1.7790467823413134E-2</v>
@@ -3619,7 +3680,7 @@
         <v>12.861363636363636</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47">
         <f t="shared" si="0"/>
         <v>1.4935207555457939E-2</v>
@@ -3653,7 +3714,7 @@
         <v>10.801704545454545</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47">
         <f t="shared" si="0"/>
         <v>1.405666593454865E-2</v>
@@ -3687,7 +3748,7 @@
         <v>10.061363636363637</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47">
         <f t="shared" si="0"/>
         <v>1.2079947287502746E-2</v>
@@ -3721,7 +3782,7 @@
         <v>8.704545454545455</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47">
         <f t="shared" si="0"/>
         <v>6.8086975620470017E-3</v>
@@ -3755,7 +3816,7 @@
         <v>4.8784090909090914</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="60">
         <f t="shared" si="0"/>
         <v>6.369426751592357E-3</v>
@@ -3789,7 +3850,7 @@
         <v>4.5363636363636362</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47">
         <f t="shared" si="0"/>
         <v>6.1497913463650338E-3</v>
@@ -3823,7 +3884,7 @@
         <v>4.3624999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47">
         <f t="shared" si="0"/>
         <v>5.9301559411377115E-3</v>
@@ -3857,7 +3918,7 @@
         <v>4.3306818181818185</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47">
         <f t="shared" si="0"/>
         <v>4.6123435097737758E-3</v>
@@ -3891,7 +3952,7 @@
         <v>3.28125</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="47">
         <f t="shared" si="0"/>
         <v>3.0748956731825169E-3</v>
@@ -3925,7 +3986,7 @@
         <v>2.2261363636363636</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="49">
         <f t="shared" si="0"/>
         <v>2.6356248627278718E-3</v>
@@ -3961,7 +4022,7 @@
         <v>1.9375</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47">
         <f t="shared" si="0"/>
         <v>2.1963540522732263E-3</v>
@@ -3995,7 +4056,7 @@
         <v>1.6392045454545454</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47">
         <f t="shared" si="0"/>
         <v>1.5374478365912585E-3</v>
@@ -4029,7 +4090,7 @@
         <v>1.053409090909091</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="47">
         <f t="shared" si="0"/>
         <v>1.0981770261366132E-3</v>
@@ -4063,7 +4124,7 @@
         <v>0.74090909090909096</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="47">
         <f t="shared" si="0"/>
         <v>6.5890621568196796E-4</v>
@@ -4097,7 +4158,7 @@
         <v>0.48522727272727273</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="47">
         <f t="shared" si="0"/>
         <v>6.5890621568196796E-4</v>
@@ -4131,7 +4192,7 @@
         <v>0.48409090909090913</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="47">
         <f t="shared" si="0"/>
         <v>4.392708104546453E-4</v>
@@ -4165,7 +4226,7 @@
         <v>0.31363636363636366</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="47">
         <f t="shared" ref="A34:A51" si="4">B34/$L$56</f>
         <v>4.392708104546453E-4</v>
@@ -4199,7 +4260,7 @@
         <v>0.29204545454545455</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="47">
         <f t="shared" si="4"/>
         <v>4.392708104546453E-4</v>
@@ -4233,7 +4294,7 @@
         <v>0.35681818181818181</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="47">
         <f t="shared" si="4"/>
         <v>2.1963540522732265E-4</v>
@@ -4267,7 +4328,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="47">
         <f t="shared" si="4"/>
         <v>2.1963540522732265E-4</v>
@@ -4301,7 +4362,7 @@
         <v>0.15681818181818183</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="47">
         <f t="shared" si="4"/>
         <v>2.1963540522732265E-4</v>
@@ -4335,7 +4396,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="50">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4371,7 +4432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4405,7 +4466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4439,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4473,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4507,7 +4568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4541,7 +4602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4575,7 +4636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4609,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4643,7 +4704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4677,7 +4738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4711,7 +4772,7 @@
         <v>5.6818181818181816E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4745,7 +4806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -4779,7 +4840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B52" s="58"/>
       <c r="I52" s="33"/>
       <c r="J52" s="40"/>
@@ -4788,7 +4849,7 @@
         <v>719.4221590909093</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B53" s="55"/>
       <c r="I53" s="33"/>
       <c r="J53" s="40"/>
@@ -4797,164 +4858,164 @@
         <v>157.97727272727272</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B54" s="58"/>
       <c r="L54" s="33"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B55" s="58"/>
       <c r="D55"/>
       <c r="L55" s="33"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B56" s="58"/>
       <c r="L56" s="33">
         <f>SUM(B2:B51)</f>
         <v>4553</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B57" s="58"/>
       <c r="I57" s="33"/>
       <c r="L57" s="33"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B58" s="58"/>
       <c r="L58" s="33"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B59" s="58"/>
       <c r="L59" s="33"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B60" s="58"/>
       <c r="L60" s="33"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B61" s="58"/>
       <c r="L61" s="33"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B62" s="58"/>
       <c r="L62" s="33"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B63" s="58"/>
       <c r="L63" s="33"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B64" s="58"/>
       <c r="L64" s="33"/>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" s="58"/>
       <c r="L65" s="33"/>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" s="58"/>
       <c r="L66" s="33"/>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" s="58"/>
       <c r="L67" s="33"/>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D68" s="34" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D69" s="34" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B71" s="58"/>
       <c r="D71" s="34" t="s">
         <v>142</v>
       </c>
       <c r="L71" s="33"/>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B72" s="58"/>
       <c r="D72" s="34" t="s">
         <v>150</v>
       </c>
       <c r="L72" s="33"/>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B73" s="58"/>
       <c r="D73" s="34" t="s">
         <v>151</v>
       </c>
       <c r="L73" s="33"/>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" s="58"/>
       <c r="D74" s="34" t="s">
         <v>149</v>
       </c>
       <c r="L74" s="33"/>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B75" s="58"/>
       <c r="L75" s="33"/>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" s="58"/>
       <c r="D76" s="34" t="s">
         <v>143</v>
       </c>
       <c r="L76" s="33"/>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B77" s="58"/>
       <c r="L77" s="33"/>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B78" s="58"/>
       <c r="D78" s="34" t="s">
         <v>144</v>
       </c>
       <c r="L78" s="33"/>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B79" s="58"/>
       <c r="L79" s="33"/>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B80" s="58"/>
       <c r="L80" s="33"/>
     </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" s="58"/>
       <c r="L81" s="33"/>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="58"/>
       <c r="L82" s="33"/>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="58"/>
       <c r="L83" s="33"/>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" s="58"/>
       <c r="L84" s="33"/>
     </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" s="58"/>
       <c r="L85" s="33"/>
     </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" s="58"/>
       <c r="L86" s="33"/>
     </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" s="58"/>
       <c r="L87" s="33"/>
     </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" s="58"/>
       <c r="L88" s="33"/>
     </row>
@@ -4969,12 +5030,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adjusted ks ok expenses
</commit_message>
<xml_diff>
--- a/Walter/TripReports/STATE HIGH POINTS.xlsx
+++ b/Walter/TripReports/STATE HIGH POINTS.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\websites\slnWalter\Walter\TripReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057E83E3-636A-4F6A-B761-A369EE9C2A62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="HighPoint Log" sheetId="1" r:id="rId1"/>
     <sheet name="Effort Scale" sheetId="3" r:id="rId2"/>
     <sheet name="graph by year" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -545,9 +544,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
@@ -715,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -856,6 +856,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="14" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -882,7 +883,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1012,7 +1013,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1163,7 +1164,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BDDB-4219-875C-4207839544B0}"/>
             </c:ext>
@@ -1179,11 +1180,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="515953920"/>
-        <c:axId val="515955888"/>
+        <c:axId val="392223368"/>
+        <c:axId val="392224152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="515953920"/>
+        <c:axId val="392223368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1226,7 +1227,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515955888"/>
+        <c:crossAx val="392224152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1234,7 +1235,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="515955888"/>
+        <c:axId val="392224152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1270,7 +1271,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="515953920"/>
+        <c:crossAx val="392223368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1965,7 +1966,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B90CE593-94B9-4A8C-A64E-B77DDB75BC6E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B90CE593-94B9-4A8C-A64E-B77DDB75BC6E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2062,23 +2063,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2114,23 +2098,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2306,11 +2273,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3182,8 +3149,9 @@
         <v>43822</v>
       </c>
       <c r="G31" s="11"/>
-      <c r="H31" s="19">
-        <v>699</v>
+      <c r="H31" s="76">
+        <f>699-57.72</f>
+        <v>641.28</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>166</v>
@@ -4138,7 +4106,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6137,7 +6105,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6165,7 +6133,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A27" si="0">A2+1</f>
+        <f t="shared" ref="A3:A19" si="0">A2+1</f>
         <v>2003</v>
       </c>
       <c r="B3">

</xml_diff>

<commit_message>
note about marshall not going to Ebright Azimuth.  and costs of trip
</commit_message>
<xml_diff>
--- a/Walter/TripReports/STATE HIGH POINTS.xlsx
+++ b/Walter/TripReports/STATE HIGH POINTS.xlsx
@@ -950,7 +950,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1085,7 +1084,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1334,7 +1332,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1502,11 +1499,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="407178784"/>
-        <c:axId val="407181528"/>
+        <c:axId val="363114208"/>
+        <c:axId val="363111464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="407178784"/>
+        <c:axId val="363114208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1548,7 +1545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="407181528"/>
+        <c:crossAx val="363111464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1556,7 +1553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="407181528"/>
+        <c:axId val="363111464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,7 +1603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="407178784"/>
+        <c:crossAx val="363114208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1620,7 +1617,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2558,7 +2554,7 @@
   <dimension ref="A1:AH90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4001,7 +3997,8 @@
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="17">
-        <v>1300</v>
+        <f>1335.79+7.95</f>
+        <v>1343.74</v>
       </c>
       <c r="J44" s="10" t="s">
         <v>182</v>
@@ -4449,11 +4446,11 @@
     </row>
     <row r="2" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="46">
-        <f t="shared" ref="A2:A33" si="0">B2/$M$56</f>
+        <f t="shared" ref="A2" si="0">B2/$M$56</f>
         <v>0.21963540522732264</v>
       </c>
       <c r="B2" s="52">
-        <f t="shared" ref="B2:B33" si="1">ROUND(M2/$M$53*1000,0)</f>
+        <f t="shared" ref="B2" si="1">ROUND(M2/$M$53*1000,0)</f>
         <v>1000</v>
       </c>
       <c r="C2" s="42" t="s">
@@ -4475,7 +4472,7 @@
         <v>39</v>
       </c>
       <c r="I2" s="42">
-        <f t="shared" ref="I2:I33" si="2">15*G2/5280</f>
+        <f t="shared" ref="I2" si="2">15*G2/5280</f>
         <v>53.977272727272727</v>
       </c>
       <c r="J2" s="50">
@@ -4488,17 +4485,17 @@
         <v>17</v>
       </c>
       <c r="M2" s="44">
-        <f t="shared" ref="M2:M33" si="3">I2+H2+J2 + K2*2 + L2</f>
+        <f t="shared" ref="M2" si="3">I2+H2+J2 + K2*2 + L2</f>
         <v>157.97727272727272</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="45">
-        <f>B3/$M$56</f>
+        <f t="shared" ref="A3:A34" si="4">B3/$M$56</f>
         <v>0.11113551504502525</v>
       </c>
       <c r="B3" s="53">
-        <f>ROUND(M3/$M$53*1000,0)</f>
+        <f t="shared" ref="B3:B34" si="5">ROUND(M3/$M$53*1000,0)</f>
         <v>506</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -4520,7 +4517,7 @@
         <v>40.4</v>
       </c>
       <c r="I3" s="10">
-        <f>15*G3/5280</f>
+        <f t="shared" ref="I3:I34" si="6">15*G3/5280</f>
         <v>24.573863636363637</v>
       </c>
       <c r="J3" s="49">
@@ -4531,17 +4528,17 @@
         <v>3</v>
       </c>
       <c r="M3" s="38">
-        <f>I3+H3+J3 + K3*2 + L3</f>
+        <f t="shared" ref="M3:M34" si="7">I3+H3+J3 + K3*2 + L3</f>
         <v>79.973863636363632</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45">
-        <f>B4/$M$56</f>
+        <f t="shared" si="4"/>
         <v>8.0825829123654727E-2</v>
       </c>
       <c r="B4" s="53">
-        <f>ROUND(M4/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>368</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -4563,7 +4560,7 @@
         <v>22.2</v>
       </c>
       <c r="I4" s="10">
-        <f>15*G4/5280</f>
+        <f t="shared" si="6"/>
         <v>21.875</v>
       </c>
       <c r="J4" s="49">
@@ -4574,17 +4571,17 @@
         <v>2</v>
       </c>
       <c r="M4" s="38">
-        <f>I4+H4+J4 + K4*2 + L4</f>
+        <f t="shared" si="7"/>
         <v>58.075000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="45">
-        <f>B5/$M$56</f>
+        <f t="shared" si="4"/>
         <v>8.0386558313200088E-2</v>
       </c>
       <c r="B5" s="53">
-        <f>ROUND(M5/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>366</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -4606,7 +4603,7 @@
         <v>16</v>
       </c>
       <c r="I5" s="10">
-        <f>15*G5/5280</f>
+        <f t="shared" si="6"/>
         <v>25.852272727272727</v>
       </c>
       <c r="J5" s="49">
@@ -4619,17 +4616,17 @@
         <v>2</v>
       </c>
       <c r="M5" s="38">
-        <f>I5+H5+J5 + K5*2 + L5</f>
+        <f t="shared" si="7"/>
         <v>57.852272727272727</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45">
-        <f>B6/$M$56</f>
+        <f t="shared" si="4"/>
         <v>6.3913902921150886E-2</v>
       </c>
       <c r="B6" s="53">
-        <f>ROUND(M6/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>291</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -4651,7 +4648,7 @@
         <v>28.8</v>
       </c>
       <c r="I6" s="10">
-        <f>15*G6/5280</f>
+        <f t="shared" si="6"/>
         <v>15.198863636363637</v>
       </c>
       <c r="J6" s="49"/>
@@ -4660,17 +4657,17 @@
         <v>2</v>
       </c>
       <c r="M6" s="38">
-        <f>I6+H6+J6 + K6*2 + L6</f>
+        <f t="shared" si="7"/>
         <v>45.998863636363637</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="45">
-        <f>B7/$M$56</f>
+        <f t="shared" si="4"/>
         <v>5.7764111574785858E-2</v>
       </c>
       <c r="B7" s="53">
-        <f>ROUND(M7/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>263</v>
       </c>
       <c r="C7" s="37" t="s">
@@ -4692,7 +4689,7 @@
         <v>21.4</v>
       </c>
       <c r="I7" s="10">
-        <f>15*G7/5280</f>
+        <f t="shared" si="6"/>
         <v>19.176136363636363</v>
       </c>
       <c r="J7" s="49"/>
@@ -4701,17 +4698,17 @@
         <v>1</v>
       </c>
       <c r="M7" s="38">
-        <f>I7+H7+J7 + K7*2 + L7</f>
+        <f t="shared" si="7"/>
         <v>41.576136363636365</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45">
-        <f>B8/$M$56</f>
+        <f t="shared" si="4"/>
         <v>4.8759059960465624E-2</v>
       </c>
       <c r="B8" s="53">
-        <f>ROUND(M8/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>222</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -4733,7 +4730,7 @@
         <v>8</v>
       </c>
       <c r="I8" s="10">
-        <f>15*G8/5280</f>
+        <f t="shared" si="6"/>
         <v>15.056818181818182</v>
       </c>
       <c r="J8" s="49">
@@ -4742,17 +4739,17 @@
       <c r="K8" s="49"/>
       <c r="L8" s="49"/>
       <c r="M8" s="38">
-        <f>I8+H8+J8 + K8*2 + L8</f>
+        <f t="shared" si="7"/>
         <v>35.05681818181818</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="45">
-        <f>B9/$M$56</f>
+        <f t="shared" si="4"/>
         <v>3.9754008346145397E-2</v>
       </c>
       <c r="B9" s="53">
-        <f>ROUND(M9/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>181</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -4774,7 +4771,7 @@
         <v>6.8</v>
       </c>
       <c r="I9" s="10">
-        <f>15*G9/5280</f>
+        <f t="shared" si="6"/>
         <v>15.767045454545455</v>
       </c>
       <c r="J9" s="49">
@@ -4783,17 +4780,17 @@
       <c r="K9" s="49"/>
       <c r="L9" s="49"/>
       <c r="M9" s="38">
-        <f>I9+H9+J9 + K9*2 + L9</f>
+        <f t="shared" si="7"/>
         <v>28.567045454545454</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45">
-        <f>B10/$M$56</f>
+        <f t="shared" si="4"/>
         <v>3.3164946189325722E-2</v>
       </c>
       <c r="B10" s="53">
-        <f>ROUND(M10/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>151</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -4815,22 +4812,22 @@
         <v>14.8</v>
       </c>
       <c r="I10" s="10">
-        <f>15*G10/5280</f>
+        <f t="shared" si="6"/>
         <v>9.0909090909090917</v>
       </c>
       <c r="J10" s="38"/>
       <c r="M10" s="38">
-        <f>I10+H10+J10 + K10*2 + L10</f>
+        <f t="shared" si="7"/>
         <v>23.890909090909091</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="45">
-        <f>B11/$M$56</f>
+        <f t="shared" si="4"/>
         <v>3.228640456841643E-2</v>
       </c>
       <c r="B11" s="53">
-        <f>ROUND(M11/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>147</v>
       </c>
       <c r="C11" s="37" t="s">
@@ -4852,22 +4849,22 @@
         <v>9</v>
       </c>
       <c r="I11" s="10">
-        <f>15*G11/5280</f>
+        <f t="shared" si="6"/>
         <v>14.204545454545455</v>
       </c>
       <c r="J11" s="38"/>
       <c r="M11" s="38">
-        <f>I11+H11+J11 + K11*2 + L11</f>
+        <f t="shared" si="7"/>
         <v>23.204545454545453</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="45">
-        <f>B12/$M$56</f>
+        <f t="shared" si="4"/>
         <v>3.0968592137052494E-2</v>
       </c>
       <c r="B12" s="53">
-        <f>ROUND(M12/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>141</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -4889,22 +4886,22 @@
         <v>10.4</v>
       </c>
       <c r="I12" s="10">
-        <f>15*G12/5280</f>
+        <f t="shared" si="6"/>
         <v>11.931818181818182</v>
       </c>
       <c r="J12" s="38"/>
       <c r="M12" s="38">
-        <f>I12+H12+J12 + K12*2 + L12</f>
+        <f t="shared" si="7"/>
         <v>22.331818181818182</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="45">
-        <f>B13/$M$56</f>
+        <f t="shared" si="4"/>
         <v>2.7674061058642653E-2</v>
       </c>
       <c r="B13" s="53">
-        <f>ROUND(M13/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>126</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -4926,22 +4923,22 @@
         <v>7.4</v>
       </c>
       <c r="I13" s="10">
-        <f>15*G13/5280</f>
+        <f t="shared" si="6"/>
         <v>12.5</v>
       </c>
       <c r="J13" s="38"/>
       <c r="M13" s="38">
-        <f>I13+H13+J13 + K13*2 + L13</f>
+        <f t="shared" si="7"/>
         <v>19.899999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="45">
-        <f>B14/$M$56</f>
+        <f t="shared" si="4"/>
         <v>2.6356248627278717E-2</v>
       </c>
       <c r="B14" s="53">
-        <f>ROUND(M14/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
       <c r="C14" s="37" t="s">
@@ -4963,22 +4960,22 @@
         <v>9</v>
       </c>
       <c r="I14" s="10">
-        <f>15*G14/5280</f>
+        <f t="shared" si="6"/>
         <v>9.9431818181818183</v>
       </c>
       <c r="J14" s="38"/>
       <c r="M14" s="38">
-        <f>I14+H14+J14 + K14*2 + L14</f>
+        <f t="shared" si="7"/>
         <v>18.94318181818182</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="45">
-        <f>B15/$M$56</f>
+        <f t="shared" si="4"/>
         <v>2.32813529540962E-2</v>
       </c>
       <c r="B15" s="53">
-        <f>ROUND(M15/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>106</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -5000,22 +4997,22 @@
         <v>8.4</v>
       </c>
       <c r="I15" s="10">
-        <f>15*G15/5280</f>
+        <f t="shared" si="6"/>
         <v>8.3806818181818183</v>
       </c>
       <c r="J15" s="38"/>
       <c r="M15" s="38">
-        <f>I15+H15+J15 + K15*2 + L15</f>
+        <f t="shared" si="7"/>
         <v>16.780681818181819</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="45">
-        <f>B16/$M$56</f>
+        <f t="shared" si="4"/>
         <v>2.1524269712277617E-2</v>
       </c>
       <c r="B16" s="53">
-        <f>ROUND(M16/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>98</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -5037,22 +5034,22 @@
         <v>6.2</v>
       </c>
       <c r="I16" s="10">
-        <f>15*G16/5280</f>
+        <f t="shared" si="6"/>
         <v>9.232954545454545</v>
       </c>
       <c r="J16" s="38"/>
       <c r="M16" s="38">
-        <f>I16+H16+J16 + K16*2 + L16</f>
+        <f t="shared" si="7"/>
         <v>15.432954545454546</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="45">
-        <f>B17/$M$56</f>
+        <f t="shared" si="4"/>
         <v>1.7790467823413134E-2</v>
       </c>
       <c r="B17" s="53">
-        <f>ROUND(M17/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -5074,22 +5071,22 @@
         <v>8.6</v>
       </c>
       <c r="I17" s="10">
-        <f>15*G17/5280</f>
+        <f t="shared" si="6"/>
         <v>4.2613636363636367</v>
       </c>
       <c r="J17" s="38"/>
       <c r="M17" s="38">
-        <f>I17+H17+J17 + K17*2 + L17</f>
+        <f t="shared" si="7"/>
         <v>12.861363636363636</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="45">
-        <f>B18/$M$56</f>
+        <f t="shared" si="4"/>
         <v>1.4935207555457939E-2</v>
       </c>
       <c r="B18" s="53">
-        <f>ROUND(M18/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>68</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -5111,22 +5108,22 @@
         <v>8.6</v>
       </c>
       <c r="I18" s="10">
-        <f>15*G18/5280</f>
+        <f t="shared" si="6"/>
         <v>2.2017045454545454</v>
       </c>
       <c r="J18" s="38"/>
       <c r="M18" s="38">
-        <f>I18+H18+J18 + K18*2 + L18</f>
+        <f t="shared" si="7"/>
         <v>10.801704545454545</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="45">
-        <f>B19/$M$56</f>
+        <f t="shared" si="4"/>
         <v>1.405666593454865E-2</v>
       </c>
       <c r="B19" s="53">
-        <f>ROUND(M19/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>64</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -5148,22 +5145,22 @@
         <v>5.8</v>
       </c>
       <c r="I19" s="10">
-        <f>15*G19/5280</f>
+        <f t="shared" si="6"/>
         <v>4.2613636363636367</v>
       </c>
       <c r="J19" s="38"/>
       <c r="M19" s="38">
-        <f>I19+H19+J19 + K19*2 + L19</f>
+        <f t="shared" si="7"/>
         <v>10.061363636363637</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="45">
-        <f>B20/$M$56</f>
+        <f t="shared" si="4"/>
         <v>1.2079947287502746E-2</v>
       </c>
       <c r="B20" s="53">
-        <f>ROUND(M20/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>55</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -5185,22 +5182,22 @@
         <v>7</v>
       </c>
       <c r="I20" s="10">
-        <f>15*G20/5280</f>
+        <f t="shared" si="6"/>
         <v>1.7045454545454546</v>
       </c>
       <c r="J20" s="38"/>
       <c r="M20" s="38">
-        <f>I20+H20+J20 + K20*2 + L20</f>
+        <f t="shared" si="7"/>
         <v>8.704545454545455</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="45">
-        <f>B21/$M$56</f>
+        <f t="shared" si="4"/>
         <v>6.8086975620470017E-3</v>
       </c>
       <c r="B21" s="53">
-        <f>ROUND(M21/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -5222,22 +5219,22 @@
         <v>3.6</v>
       </c>
       <c r="I21" s="10">
-        <f>15*G21/5280</f>
+        <f t="shared" si="6"/>
         <v>1.2784090909090908</v>
       </c>
       <c r="J21" s="38"/>
       <c r="M21" s="38">
-        <f>I21+H21+J21 + K21*2 + L21</f>
+        <f t="shared" si="7"/>
         <v>4.8784090909090914</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="58">
-        <f>B22/$M$56</f>
+        <f t="shared" si="4"/>
         <v>6.369426751592357E-3</v>
       </c>
       <c r="B22" s="59">
-        <f>ROUND(M22/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="C22" s="60" t="s">
@@ -5259,22 +5256,22 @@
         <v>3.4</v>
       </c>
       <c r="I22" s="60">
-        <f>15*G22/5280</f>
+        <f t="shared" si="6"/>
         <v>1.1363636363636365</v>
       </c>
       <c r="J22" s="62"/>
       <c r="M22" s="62">
-        <f>I22+H22+J22 + K22*2 + L22</f>
+        <f t="shared" si="7"/>
         <v>4.5363636363636362</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="45">
-        <f>B23/$M$56</f>
+        <f t="shared" si="4"/>
         <v>6.1497913463650338E-3</v>
       </c>
       <c r="B23" s="53">
-        <f>ROUND(M23/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -5296,22 +5293,22 @@
         <v>2.8</v>
       </c>
       <c r="I23" s="10">
-        <f>15*G23/5280</f>
+        <f t="shared" si="6"/>
         <v>1.5625</v>
       </c>
       <c r="J23" s="38"/>
       <c r="M23" s="38">
-        <f>I23+H23+J23 + K23*2 + L23</f>
+        <f t="shared" si="7"/>
         <v>4.3624999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="45">
-        <f>B24/$M$56</f>
+        <f t="shared" si="4"/>
         <v>5.9301559411377115E-3</v>
       </c>
       <c r="B24" s="53">
-        <f>ROUND(M24/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -5333,22 +5330,22 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="I24" s="10">
-        <f>15*G24/5280</f>
+        <f t="shared" si="6"/>
         <v>2.1306818181818183</v>
       </c>
       <c r="J24" s="38"/>
       <c r="M24" s="38">
-        <f>I24+H24+J24 + K24*2 + L24</f>
+        <f t="shared" si="7"/>
         <v>4.3306818181818185</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="45">
-        <f>B25/$M$56</f>
+        <f t="shared" si="4"/>
         <v>4.6123435097737758E-3</v>
       </c>
       <c r="B25" s="53">
-        <f>ROUND(M25/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -5370,22 +5367,22 @@
         <v>2.5</v>
       </c>
       <c r="I25" s="10">
-        <f>15*G25/5280</f>
+        <f t="shared" si="6"/>
         <v>0.78125</v>
       </c>
       <c r="J25" s="38"/>
       <c r="M25" s="38">
-        <f>I25+H25+J25 + K25*2 + L25</f>
+        <f t="shared" si="7"/>
         <v>3.28125</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="45">
-        <f>B26/$M$56</f>
+        <f t="shared" si="4"/>
         <v>3.0748956731825169E-3</v>
       </c>
       <c r="B26" s="53">
-        <f>ROUND(M26/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -5407,22 +5404,22 @@
         <v>1.8</v>
       </c>
       <c r="I26" s="10">
-        <f>15*G26/5280</f>
+        <f t="shared" si="6"/>
         <v>0.42613636363636365</v>
       </c>
       <c r="J26" s="38"/>
       <c r="M26" s="38">
-        <f>I26+H26+J26 + K26*2 + L26</f>
+        <f t="shared" si="7"/>
         <v>2.2261363636363636</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="47">
-        <f>B27/$M$56</f>
+        <f t="shared" si="4"/>
         <v>2.6356248627278718E-3</v>
       </c>
       <c r="B27" s="54">
-        <f>ROUND(M27/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -5444,24 +5441,24 @@
         <v>1</v>
       </c>
       <c r="I27" s="6">
-        <f>15*G27/5280</f>
+        <f t="shared" si="6"/>
         <v>0.9375</v>
       </c>
       <c r="J27" s="33"/>
       <c r="K27" s="33"/>
       <c r="L27" s="33"/>
       <c r="M27" s="33">
-        <f>I27+H27+J27 + K27*2 + L27</f>
+        <f t="shared" si="7"/>
         <v>1.9375</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="45">
-        <f>B28/$M$56</f>
+        <f t="shared" si="4"/>
         <v>2.1963540522732263E-3</v>
       </c>
       <c r="B28" s="53">
-        <f>ROUND(M28/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -5483,22 +5480,22 @@
         <v>1</v>
       </c>
       <c r="I28" s="10">
-        <f>15*G28/5280</f>
+        <f t="shared" si="6"/>
         <v>0.63920454545454541</v>
       </c>
       <c r="J28" s="38"/>
       <c r="M28" s="38">
-        <f>I28+H28+J28 + K28*2 + L28</f>
+        <f t="shared" si="7"/>
         <v>1.6392045454545454</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="45">
-        <f>B29/$M$56</f>
+        <f t="shared" si="4"/>
         <v>1.5374478365912585E-3</v>
       </c>
       <c r="B29" s="53">
-        <f>ROUND(M29/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="C29" s="10" t="s">
@@ -5517,22 +5514,22 @@
         <v>0.4</v>
       </c>
       <c r="I29" s="10">
-        <f>15*G29/5280</f>
+        <f t="shared" si="6"/>
         <v>0.65340909090909094</v>
       </c>
       <c r="J29" s="38"/>
       <c r="M29" s="38">
-        <f>I29+H29+J29 + K29*2 + L29</f>
+        <f t="shared" si="7"/>
         <v>1.053409090909091</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="45">
-        <f>B30/$M$56</f>
+        <f t="shared" si="4"/>
         <v>1.0981770261366132E-3</v>
       </c>
       <c r="B30" s="53">
-        <f>ROUND(M30/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -5554,22 +5551,22 @@
         <v>0.4</v>
       </c>
       <c r="I30" s="10">
-        <f>15*G30/5280</f>
+        <f t="shared" si="6"/>
         <v>0.34090909090909088</v>
       </c>
       <c r="J30" s="38"/>
       <c r="M30" s="38">
-        <f>I30+H30+J30 + K30*2 + L30</f>
+        <f t="shared" si="7"/>
         <v>0.74090909090909096</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="45">
-        <f>B31/$M$56</f>
+        <f t="shared" si="4"/>
         <v>6.5890621568196796E-4</v>
       </c>
       <c r="B31" s="53">
-        <f>ROUND(M31/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C31" s="10" t="s">
@@ -5591,22 +5588,22 @@
         <v>0.2</v>
       </c>
       <c r="I31" s="10">
-        <f>15*G31/5280</f>
+        <f t="shared" si="6"/>
         <v>0.28409090909090912</v>
       </c>
       <c r="J31" s="38"/>
       <c r="M31" s="38">
-        <f>I31+H31+J31 + K31*2 + L31</f>
+        <f t="shared" si="7"/>
         <v>0.48409090909090913</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="45">
-        <f>B32/$M$56</f>
+        <f t="shared" si="4"/>
         <v>6.5890621568196796E-4</v>
       </c>
       <c r="B32" s="53">
-        <f>ROUND(M32/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C32" s="10" t="s">
@@ -5628,22 +5625,22 @@
         <v>0.4</v>
       </c>
       <c r="I32" s="10">
-        <f>15*G32/5280</f>
+        <f t="shared" si="6"/>
         <v>8.5227272727272721E-2</v>
       </c>
       <c r="J32" s="38"/>
       <c r="M32" s="38">
-        <f>I32+H32+J32 + K32*2 + L32</f>
+        <f t="shared" si="7"/>
         <v>0.48522727272727273</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="45">
-        <f>B33/$M$56</f>
+        <f t="shared" si="4"/>
         <v>4.392708104546453E-4</v>
       </c>
       <c r="B33" s="53">
-        <f>ROUND(M33/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="C33" s="10" t="s">
@@ -5665,22 +5662,22 @@
         <v>0.3</v>
       </c>
       <c r="I33" s="10">
-        <f>15*G33/5280</f>
+        <f t="shared" si="6"/>
         <v>5.6818181818181816E-2</v>
       </c>
       <c r="J33" s="38"/>
       <c r="M33" s="38">
-        <f>I33+H33+J33 + K33*2 + L33</f>
+        <f t="shared" si="7"/>
         <v>0.35681818181818181</v>
       </c>
     </row>
     <row r="34" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="45">
-        <f>B34/$M$56</f>
+        <f t="shared" si="4"/>
         <v>4.392708104546453E-4</v>
       </c>
       <c r="B34" s="53">
-        <f>ROUND(M34/$M$53*1000,0)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="C34" s="10" t="s">
@@ -5702,22 +5699,22 @@
         <v>0.15</v>
       </c>
       <c r="I34" s="10">
-        <f>15*G34/5280</f>
+        <f t="shared" si="6"/>
         <v>0.14204545454545456</v>
       </c>
       <c r="J34" s="38"/>
       <c r="M34" s="38">
-        <f>I34+H34+J34 + K34*2 + L34</f>
+        <f t="shared" si="7"/>
         <v>0.29204545454545455</v>
       </c>
     </row>
     <row r="35" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="45">
-        <f>B35/$M$56</f>
+        <f t="shared" ref="A35:A66" si="8">B35/$M$56</f>
         <v>4.392708104546453E-4</v>
       </c>
       <c r="B35" s="53">
-        <f>ROUND(M35/$M$53*1000,0)</f>
+        <f t="shared" ref="B35:B51" si="9">ROUND(M35/$M$53*1000,0)</f>
         <v>2</v>
       </c>
       <c r="C35" s="10" t="s">
@@ -5739,22 +5736,22 @@
         <v>0.2</v>
       </c>
       <c r="I35" s="10">
-        <f>15*G35/5280</f>
+        <f t="shared" ref="I35:I51" si="10">15*G35/5280</f>
         <v>0.11363636363636363</v>
       </c>
       <c r="J35" s="38"/>
       <c r="M35" s="38">
-        <f>I35+H35+J35 + K35*2 + L35</f>
+        <f t="shared" ref="M35:M66" si="11">I35+H35+J35 + K35*2 + L35</f>
         <v>0.31363636363636366</v>
       </c>
     </row>
     <row r="36" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="45">
-        <f>B36/$M$56</f>
+        <f t="shared" si="8"/>
         <v>2.1963540522732265E-4</v>
       </c>
       <c r="B36" s="53">
-        <f>ROUND(M36/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="C36" s="10" t="s">
@@ -5776,22 +5773,22 @@
         <v>0.1</v>
       </c>
       <c r="I36" s="10">
-        <f>15*G36/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J36" s="38"/>
       <c r="M36" s="38">
-        <f>I36+H36+J36 + K36*2 + L36</f>
+        <f t="shared" si="11"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="45">
-        <f>B37/$M$56</f>
+        <f t="shared" si="8"/>
         <v>2.1963540522732265E-4</v>
       </c>
       <c r="B37" s="53">
-        <f>ROUND(M37/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="C37" s="10" t="s">
@@ -5813,22 +5810,22 @@
         <v>0.1</v>
       </c>
       <c r="I37" s="10">
-        <f>15*G37/5280</f>
+        <f t="shared" si="10"/>
         <v>5.6818181818181816E-2</v>
       </c>
       <c r="J37" s="38"/>
       <c r="M37" s="38">
-        <f>I37+H37+J37 + K37*2 + L37</f>
+        <f t="shared" si="11"/>
         <v>0.15681818181818183</v>
       </c>
     </row>
     <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="45">
-        <f>B38/$M$56</f>
+        <f t="shared" si="8"/>
         <v>2.1963540522732265E-4</v>
       </c>
       <c r="B38" s="53">
-        <f>ROUND(M38/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="C38" s="10" t="s">
@@ -5850,22 +5847,22 @@
         <v>0.2</v>
       </c>
       <c r="I38" s="10">
-        <f>15*G38/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J38" s="38"/>
       <c r="M38" s="38">
-        <f>I38+H38+J38 + K38*2 + L38</f>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="45">
-        <f>B39/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B39" s="53">
-        <f>ROUND(M39/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C39" s="10" t="s">
@@ -5887,22 +5884,22 @@
         <v>0</v>
       </c>
       <c r="I39" s="10">
-        <f>15*G39/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J39" s="38"/>
       <c r="M39" s="38">
-        <f>I39+H39+J39 + K39*2 + L39</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="45">
-        <f>B40/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B40" s="53">
-        <f>ROUND(M40/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C40" s="10" t="s">
@@ -5924,22 +5921,22 @@
         <v>0</v>
       </c>
       <c r="I40" s="10">
-        <f>15*G40/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J40" s="38"/>
       <c r="M40" s="38">
-        <f>I40+H40+J40 + K40*2 + L40</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="45">
-        <f>B41/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B41" s="53">
-        <f>ROUND(M41/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C41" s="10" t="s">
@@ -5961,22 +5958,22 @@
         <v>0</v>
       </c>
       <c r="I41" s="10">
-        <f>15*G41/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J41" s="38"/>
       <c r="M41" s="38">
-        <f>I41+H41+J41 + K41*2 + L41</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="45">
-        <f>B42/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B42" s="53">
-        <f>ROUND(M42/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C42" s="10" t="s">
@@ -5998,22 +5995,22 @@
         <v>0</v>
       </c>
       <c r="I42" s="10">
-        <f>15*G42/5280</f>
+        <f t="shared" si="10"/>
         <v>5.6818181818181816E-2</v>
       </c>
       <c r="J42" s="38"/>
       <c r="M42" s="38">
-        <f>I42+H42+J42 + K42*2 + L42</f>
+        <f t="shared" si="11"/>
         <v>5.6818181818181816E-2</v>
       </c>
     </row>
     <row r="43" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="48">
-        <f>B43/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B43" s="55">
-        <f>ROUND(M43/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C43" s="39" t="s">
@@ -6035,24 +6032,24 @@
         <v>0</v>
       </c>
       <c r="I43" s="39">
-        <f>15*G43/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J43" s="41"/>
       <c r="K43" s="41"/>
       <c r="L43" s="41"/>
       <c r="M43" s="41">
-        <f>I43+H43+J43 + K43*2 + L43</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="45">
-        <f>B44/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B44" s="53">
-        <f>ROUND(M44/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C44" s="10" t="s">
@@ -6074,22 +6071,22 @@
         <v>0</v>
       </c>
       <c r="I44" s="10">
-        <f>15*G44/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J44" s="38"/>
       <c r="M44" s="38">
-        <f>I44+H44+J44 + K44*2 + L44</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="45">
-        <f>B45/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B45" s="53">
-        <f>ROUND(M45/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C45" s="10" t="s">
@@ -6111,22 +6108,22 @@
         <v>0</v>
       </c>
       <c r="I45" s="10">
-        <f>15*G45/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J45" s="38"/>
       <c r="M45" s="38">
-        <f>I45+H45+J45 + K45*2 + L45</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="45">
-        <f>B46/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B46" s="53">
-        <f>ROUND(M46/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C46" s="10" t="s">
@@ -6148,22 +6145,22 @@
         <v>0</v>
       </c>
       <c r="I46" s="10">
-        <f>15*G46/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J46" s="38"/>
       <c r="M46" s="38">
-        <f>I46+H46+J46 + K46*2 + L46</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="45">
-        <f>B47/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B47" s="53">
-        <f>ROUND(M47/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C47" s="10" t="s">
@@ -6185,22 +6182,22 @@
         <v>0</v>
       </c>
       <c r="I47" s="10">
-        <f>15*G47/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J47" s="38"/>
       <c r="M47" s="38">
-        <f>I47+H47+J47 + K47*2 + L47</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="45">
-        <f>B48/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B48" s="53">
-        <f>ROUND(M48/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C48" s="10" t="s">
@@ -6222,22 +6219,22 @@
         <v>0</v>
       </c>
       <c r="I48" s="10">
-        <f>15*G48/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J48" s="38"/>
       <c r="M48" s="38">
-        <f>I48+H48+J48 + K48*2 + L48</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="45">
-        <f>B49/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B49" s="53">
-        <f>ROUND(M49/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C49" s="10" t="s">
@@ -6259,22 +6256,22 @@
         <v>0</v>
       </c>
       <c r="I49" s="10">
-        <f>15*G49/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J49" s="38"/>
       <c r="M49" s="38">
-        <f>I49+H49+J49 + K49*2 + L49</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="45">
-        <f>B50/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B50" s="53">
-        <f>ROUND(M50/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C50" s="10" t="s">
@@ -6296,22 +6293,22 @@
         <v>0</v>
       </c>
       <c r="I50" s="10">
-        <f>15*G50/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J50" s="38"/>
       <c r="M50" s="38">
-        <f>I50+H50+J50 + K50*2 + L50</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="45">
-        <f>B51/$M$56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B51" s="53">
-        <f>ROUND(M51/$M$53*1000,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C51" s="10" t="s">
@@ -6333,12 +6330,12 @@
         <v>0</v>
       </c>
       <c r="I51" s="10">
-        <f>15*G51/5280</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J51" s="38"/>
       <c r="M51" s="38">
-        <f>I51+H51+J51 + K51*2 + L51</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6570,7 +6567,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A21" si="0">A2+1</f>
         <v>2002</v>
       </c>
       <c r="B3">
@@ -6582,7 +6579,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>A3+1</f>
+        <f t="shared" si="0"/>
         <v>2003</v>
       </c>
       <c r="B4">
@@ -6594,7 +6591,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>2004</v>
       </c>
       <c r="B5">
@@ -6606,7 +6603,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>2005</v>
       </c>
       <c r="B6">
@@ -6618,7 +6615,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>2006</v>
       </c>
       <c r="B7">
@@ -6630,7 +6627,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>2007</v>
       </c>
       <c r="B8">
@@ -6642,7 +6639,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>2008</v>
       </c>
       <c r="B9">
@@ -6654,7 +6651,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>2009</v>
       </c>
       <c r="B10">
@@ -6666,7 +6663,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>2010</v>
       </c>
       <c r="B11">
@@ -6678,7 +6675,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>2011</v>
       </c>
       <c r="B12">
@@ -6690,7 +6687,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>2012</v>
       </c>
       <c r="B13">
@@ -6702,7 +6699,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>2013</v>
       </c>
       <c r="B14">
@@ -6714,7 +6711,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>A14+1</f>
+        <f t="shared" si="0"/>
         <v>2014</v>
       </c>
       <c r="B15">
@@ -6726,7 +6723,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>A15+1</f>
+        <f t="shared" si="0"/>
         <v>2015</v>
       </c>
       <c r="B16">
@@ -6738,7 +6735,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>2016</v>
       </c>
       <c r="B17">
@@ -6750,7 +6747,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>A17+1</f>
+        <f t="shared" si="0"/>
         <v>2017</v>
       </c>
       <c r="B18">
@@ -6762,7 +6759,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>A18+1</f>
+        <f t="shared" si="0"/>
         <v>2018</v>
       </c>
       <c r="B19">
@@ -6774,7 +6771,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>A19+1</f>
+        <f t="shared" si="0"/>
         <v>2019</v>
       </c>
       <c r="B20">
@@ -6786,7 +6783,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>A20+1</f>
+        <f t="shared" si="0"/>
         <v>2020</v>
       </c>
       <c r="B21">

</xml_diff>